<commit_message>
pierwsze podjęcia zadań przez realizatorów
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
   <si>
     <t>Id</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Słonek</t>
+  </si>
+  <si>
+    <t>Słonka</t>
   </si>
 </sst>
 </file>
@@ -550,7 +556,7 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -581,7 +587,8 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -612,7 +619,7 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -626,6 +633,23 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -661,23 +685,6 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -949,7 +956,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F21" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A4:F21"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Id" dataDxfId="5"/>
@@ -1831,10 +1838,12 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2"/>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
@@ -1848,10 +1857,12 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2"/>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="D6" s="9">
         <v>1</v>
       </c>
@@ -1865,7 +1876,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C7" s="2"/>
@@ -1882,7 +1893,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2"/>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="2"/>
@@ -1896,7 +1907,7 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C9" s="2"/>
@@ -1910,10 +1921,12 @@
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2"/>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="D10" s="9">
         <v>2</v>
       </c>
@@ -1924,7 +1937,7 @@
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="2"/>
@@ -1938,7 +1951,7 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="2"/>
@@ -1952,7 +1965,7 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C13" s="2"/>
@@ -1966,7 +1979,7 @@
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2"/>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="2"/>
@@ -1980,7 +1993,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C15" s="2"/>
@@ -1994,7 +2007,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C16" s="2"/>
@@ -2008,7 +2021,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="2"/>
@@ -2022,7 +2035,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="2"/>
@@ -2036,7 +2049,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C19" s="2"/>
@@ -2050,7 +2063,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="2"/>
@@ -2064,7 +2077,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>

</xml_diff>

<commit_message>
dodanie wykresu burndown, update tasków
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>Słonka</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>pozostało [h]</t>
+  </si>
+  <si>
+    <t>SUMA</t>
   </si>
 </sst>
 </file>
@@ -409,7 +418,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -442,6 +451,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -938,6 +948,257 @@
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pl-PL"/>
+              <a:t>burndown</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Sprint1</c:v>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'01_SprintBacklog'!$A$30:$A$65</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>41273</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41274</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41275</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41276</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41277</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41278</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41279</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41280</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41281</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41282</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41283</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41284</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41285</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41286</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41287</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41288</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41289</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41290</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41291</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41292</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41293</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41294</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41295</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41296</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41297</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>41298</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>41299</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>41300</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41301</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>41302</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>41303</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>41304</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41305</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>41306</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41307</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'01_SprintBacklog'!$B$30:$B$65</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
+                <c:pt idx="0">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="51869952"/>
+        <c:axId val="67297280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="51869952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="67297280"/>
+        <c:crosses val="autoZero"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="67297280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="81"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51869952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1047750</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Wykres 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1786,16 +2047,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="9.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.75" style="1" customWidth="1"/>
     <col min="4" max="4" width="19.875" style="1" customWidth="1"/>
     <col min="5" max="5" width="16.5" style="1" customWidth="1"/>
@@ -1837,9 +2098,11 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
       <c r="B5" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>79</v>
@@ -1847,7 +2110,9 @@
       <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>59</v>
       </c>
@@ -1856,9 +2121,11 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
       <c r="B6" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>79</v>
@@ -1866,7 +2133,9 @@
       <c r="D6" s="9">
         <v>1</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
       <c r="F6" s="2" t="s">
         <v>60</v>
       </c>
@@ -1875,7 +2144,9 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2"/>
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
       <c r="B7" s="9" t="s">
         <v>76</v>
       </c>
@@ -1883,7 +2154,9 @@
       <c r="D7" s="9">
         <v>2.5</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F7" s="2" t="s">
         <v>61</v>
       </c>
@@ -1892,7 +2165,9 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
       <c r="B8" s="9" t="s">
         <v>76</v>
       </c>
@@ -1900,13 +2175,17 @@
       <c r="D8" s="9">
         <v>2.5</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>2.5</v>
+      </c>
       <c r="F8" s="2" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="2"/>
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
       <c r="B9" s="9" t="s">
         <v>76</v>
       </c>
@@ -1914,15 +2193,19 @@
       <c r="D9" s="9">
         <v>2</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
       <c r="F9" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="2"/>
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
       <c r="B10" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>80</v>
@@ -1930,41 +2213,53 @@
       <c r="D10" s="9">
         <v>2</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>0.5</v>
+      </c>
       <c r="F10" s="2" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="2"/>
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
       <c r="B11" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="9">
-        <v>10</v>
-      </c>
-      <c r="E11" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="E11" s="2">
+        <v>20</v>
+      </c>
       <c r="F11" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="2"/>
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
       <c r="B12" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="9">
-        <v>10</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="E12" s="2">
+        <v>20</v>
+      </c>
       <c r="F12" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="2"/>
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
       <c r="B13" s="9" t="s">
         <v>76</v>
       </c>
@@ -1972,27 +2267,35 @@
       <c r="D13" s="9">
         <v>2</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="2">
+        <v>2</v>
+      </c>
       <c r="F13" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
       <c r="B14" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="9">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10</v>
+      </c>
       <c r="F14" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
       <c r="B15" s="9" t="s">
         <v>76</v>
       </c>
@@ -2000,13 +2303,17 @@
       <c r="D15" s="9">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
       <c r="F15" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="2"/>
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
       <c r="B16" s="9" t="s">
         <v>76</v>
       </c>
@@ -2014,27 +2321,35 @@
       <c r="D16" s="9">
         <v>0.5</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2">
+        <v>0.5</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="2"/>
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
       <c r="B17" s="9" t="s">
         <v>76</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="9">
-        <v>4.5</v>
-      </c>
-      <c r="E17" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>9</v>
+      </c>
       <c r="F17" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="2"/>
+      <c r="A18" s="2">
+        <v>14</v>
+      </c>
       <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
@@ -2042,13 +2357,17 @@
       <c r="D18" s="9">
         <v>2</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2">
+        <v>2</v>
+      </c>
       <c r="F18" s="2" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="2"/>
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
       <c r="B19" s="9" t="s">
         <v>76</v>
       </c>
@@ -2056,13 +2375,17 @@
       <c r="D19" s="9">
         <v>4</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2">
+        <v>4</v>
+      </c>
       <c r="F19" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2"/>
+      <c r="A20" s="2">
+        <v>16</v>
+      </c>
       <c r="B20" s="9" t="s">
         <v>76</v>
       </c>
@@ -2070,22 +2393,226 @@
       <c r="D20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
       <c r="F20" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>83</v>
+      </c>
       <c r="B21" s="9"/>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="D21" s="2">
+        <f>SUM(D5:D20)</f>
+        <v>80.5</v>
+      </c>
+      <c r="E21" s="2">
+        <f>SUM(E5:E20)</f>
+        <v>79</v>
+      </c>
       <c r="F21" s="2"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="16">
+        <v>41273</v>
+      </c>
+      <c r="B30" s="1">
+        <v>80.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="16">
+        <v>41274</v>
+      </c>
+      <c r="B31" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="16">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="16">
+        <v>41276</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="16">
+        <v>41277</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="16">
+        <v>41278</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="16">
+        <v>41279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="16">
+        <v>41280</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="16">
+        <v>41281</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="16">
+        <v>41282</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="16">
+        <v>41283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="16">
+        <v>41284</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="16">
+        <v>41285</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="16">
+        <v>41286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="16">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="16">
+        <v>41288</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="16">
+        <v>41289</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="16">
+        <v>41290</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="16">
+        <v>41291</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="16">
+        <v>41292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="16">
+        <v>41293</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="16">
+        <v>41294</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="16">
+        <v>41295</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="16">
+        <v>41296</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="16">
+        <v>41297</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="16">
+        <v>41298</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="16">
+        <v>41299</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="16">
+        <v>41300</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="16">
+        <v>41301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="16">
+        <v>41302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="16">
+        <v>41303</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="16">
+        <v>41304</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="16">
+        <v>41305</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="16">
+        <v>41306</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="16">
+        <v>41307</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="16">
+        <v>41308</v>
       </c>
     </row>
   </sheetData>
@@ -2096,8 +2623,9 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update backloga, edycja rankingu rekuperatorow
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>Id</t>
   </si>
@@ -327,9 +327,6 @@
   </si>
   <si>
     <t>SUMA</t>
-  </si>
-  <si>
-    <t>planowane zużycie h</t>
   </si>
   <si>
     <t>Umówić się na spotkanie z czterema przedstawicielami</t>
@@ -1079,10 +1076,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13448840769903767"/>
+          <c:x val="0.13448840769903775"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.7144142607174101"/>
-          <c:h val="0.49521580635753876"/>
+          <c:w val="0.71441426071740988"/>
+          <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1090,9 +1087,47 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>spalanie</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:name>trend</c:name>
+            <c:spPr>
+              <a:ln w="12700">
+                <a:gradFill>
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:srgbClr val="000082"/>
+                    </a:gs>
+                    <a:gs pos="30000">
+                      <a:srgbClr val="66008F"/>
+                    </a:gs>
+                    <a:gs pos="64999">
+                      <a:srgbClr val="BA0066"/>
+                    </a:gs>
+                    <a:gs pos="89999">
+                      <a:srgbClr val="FF0000"/>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:srgbClr val="FF8200"/>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="0"/>
+                </a:gradFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+          </c:trendline>
           <c:cat>
             <c:numRef>
               <c:f>'01_SprintBacklog'!$A$42:$A$76</c:f>
@@ -1222,264 +1257,32 @@
                 <c:pt idx="2">
                   <c:v>76.5</c:v>
                 </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>'01_SprintBacklog'!$A$42:$A$76</c:f>
-              <c:numCache>
-                <c:formatCode>yyyy/mm/dd</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>41273</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>41274</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>41275</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>41276</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>41277</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>41278</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41279</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>41280</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>41281</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>41282</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>41283</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>41284</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>41285</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>41286</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>41287</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>41288</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>41289</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41290</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>41291</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>41292</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>41293</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41294</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>41295</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>41296</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>41297</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>41298</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>41299</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>41300</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>41301</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>41302</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>41303</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>41304</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>41305</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>41306</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>41307</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'01_SprintBacklog'!$C$42:$C$76</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="35"/>
-                <c:pt idx="0">
-                  <c:v>80.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>75.900000000000006</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>73.599999999999994</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>71.3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>69</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>66.7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>64.400000000000006</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>62.1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>59.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>57.5</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55.2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>52.9</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>50.6</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>48.3</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>43.7</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41.4</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>39.1</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>36.799999999999997</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>34.5</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>32.200000000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>29.9</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>27.6</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25.3</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>20.7</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>18.399999999999999</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>16.100000000000001</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>13.8</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>11.5</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>9.1999999999999993</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>6.9</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.5999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.2999999999999998</c:v>
+                  <c:v>75.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62990592"/>
-        <c:axId val="63004672"/>
+        <c:axId val="73114368"/>
+        <c:axId val="73115904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62990592"/>
+        <c:axId val="73114368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63004672"/>
+        <c:crossAx val="73115904"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63004672"/>
+        <c:axId val="73115904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -1489,20 +1292,29 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62990592"/>
+        <c:crossAx val="73114368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.86438523325287864"/>
+          <c:y val="0.29353966170895313"/>
+          <c:w val="0.11894812645906698"/>
+          <c:h val="0.22334823203957854"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1513,15 +1325,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>95249</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1381125</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2391,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2659,17 +2471,19 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C16" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D16" s="9">
         <v>0.5</v>
       </c>
       <c r="E16" s="2">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2720,7 +2534,7 @@
         <v>4</v>
       </c>
       <c r="E19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>70</v>
@@ -2756,351 +2570,208 @@
       </c>
       <c r="E21" s="2">
         <f>SUM(E5:E20)</f>
-        <v>76.5</v>
+        <v>75.25</v>
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" s="16">
         <v>41273</v>
       </c>
       <c r="B42" s="1">
         <v>80.5</v>
       </c>
-      <c r="C42" s="1">
-        <v>80.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" s="16">
         <v>41274</v>
       </c>
       <c r="B43" s="1">
         <v>79</v>
       </c>
-      <c r="C43" s="1">
-        <f>ROUND(C42-2.3,2)</f>
-        <v>78.2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" s="16">
         <v>41275</v>
       </c>
       <c r="B44" s="1">
         <v>76.5</v>
       </c>
-      <c r="C44" s="1">
-        <f t="shared" ref="C44:C77" si="0">ROUND(C43-2.3,2)</f>
-        <v>75.900000000000006</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" s="16">
         <v>41276</v>
       </c>
-      <c r="C45" s="1">
-        <f t="shared" si="0"/>
-        <v>73.599999999999994</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="B45" s="1">
+        <v>75.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" s="16">
         <v>41277</v>
       </c>
-      <c r="C46" s="1">
-        <f t="shared" si="0"/>
-        <v>71.3</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" s="16">
         <v>41278</v>
       </c>
-      <c r="C47" s="1">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" s="16">
         <v>41279</v>
       </c>
-      <c r="C48" s="1">
-        <f t="shared" si="0"/>
-        <v>66.7</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+    </row>
+    <row r="49" spans="1:1">
       <c r="A49" s="16">
         <v>41280</v>
       </c>
-      <c r="C49" s="1">
-        <f t="shared" si="0"/>
-        <v>64.400000000000006</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+    </row>
+    <row r="50" spans="1:1">
       <c r="A50" s="16">
         <v>41281</v>
       </c>
-      <c r="C50" s="1">
-        <f t="shared" si="0"/>
-        <v>62.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+    </row>
+    <row r="51" spans="1:1">
       <c r="A51" s="16">
         <v>41282</v>
       </c>
-      <c r="C51" s="1">
-        <f t="shared" si="0"/>
-        <v>59.8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+    </row>
+    <row r="52" spans="1:1">
       <c r="A52" s="16">
         <v>41283</v>
       </c>
-      <c r="C52" s="1">
-        <f t="shared" si="0"/>
-        <v>57.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+    </row>
+    <row r="53" spans="1:1">
       <c r="A53" s="16">
         <v>41284</v>
       </c>
-      <c r="C53" s="1">
-        <f t="shared" si="0"/>
-        <v>55.2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+    </row>
+    <row r="54" spans="1:1">
       <c r="A54" s="16">
         <v>41285</v>
       </c>
-      <c r="C54" s="1">
-        <f t="shared" si="0"/>
-        <v>52.9</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+    </row>
+    <row r="55" spans="1:1">
       <c r="A55" s="16">
         <v>41286</v>
       </c>
-      <c r="C55" s="1">
-        <f t="shared" si="0"/>
-        <v>50.6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+    </row>
+    <row r="56" spans="1:1">
       <c r="A56" s="16">
         <v>41287</v>
       </c>
-      <c r="C56" s="1">
-        <f t="shared" si="0"/>
-        <v>48.3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+    </row>
+    <row r="57" spans="1:1">
       <c r="A57" s="16">
         <v>41288</v>
       </c>
-      <c r="C57" s="1">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+    </row>
+    <row r="58" spans="1:1">
       <c r="A58" s="16">
         <v>41289</v>
       </c>
-      <c r="C58" s="1">
-        <f t="shared" si="0"/>
-        <v>43.7</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+    </row>
+    <row r="59" spans="1:1">
       <c r="A59" s="16">
         <v>41290</v>
       </c>
-      <c r="C59" s="1">
-        <f t="shared" si="0"/>
-        <v>41.4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+    </row>
+    <row r="60" spans="1:1">
       <c r="A60" s="16">
         <v>41291</v>
       </c>
-      <c r="C60" s="1">
-        <f t="shared" si="0"/>
-        <v>39.1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+    </row>
+    <row r="61" spans="1:1">
       <c r="A61" s="16">
         <v>41292</v>
       </c>
-      <c r="C61" s="1">
-        <f t="shared" si="0"/>
-        <v>36.799999999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+    </row>
+    <row r="62" spans="1:1">
       <c r="A62" s="16">
         <v>41293</v>
       </c>
-      <c r="C62" s="1">
-        <f t="shared" si="0"/>
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+    </row>
+    <row r="63" spans="1:1">
       <c r="A63" s="16">
         <v>41294</v>
       </c>
-      <c r="C63" s="1">
-        <f t="shared" si="0"/>
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+    </row>
+    <row r="64" spans="1:1">
       <c r="A64" s="16">
         <v>41295</v>
       </c>
-      <c r="C64" s="1">
-        <f t="shared" si="0"/>
-        <v>29.9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+    </row>
+    <row r="65" spans="1:1">
       <c r="A65" s="16">
         <v>41296</v>
       </c>
-      <c r="C65" s="1">
-        <f t="shared" si="0"/>
-        <v>27.6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+    </row>
+    <row r="66" spans="1:1">
       <c r="A66" s="16">
         <v>41297</v>
       </c>
-      <c r="C66" s="1">
-        <f t="shared" si="0"/>
-        <v>25.3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+    </row>
+    <row r="67" spans="1:1">
       <c r="A67" s="16">
         <v>41298</v>
       </c>
-      <c r="C67" s="1">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+    </row>
+    <row r="68" spans="1:1">
       <c r="A68" s="16">
         <v>41299</v>
       </c>
-      <c r="C68" s="1">
-        <f t="shared" si="0"/>
-        <v>20.7</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+    </row>
+    <row r="69" spans="1:1">
       <c r="A69" s="16">
         <v>41300</v>
       </c>
-      <c r="C69" s="1">
-        <f t="shared" si="0"/>
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+    </row>
+    <row r="70" spans="1:1">
       <c r="A70" s="16">
         <v>41301</v>
       </c>
-      <c r="C70" s="1">
-        <f t="shared" si="0"/>
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+    </row>
+    <row r="71" spans="1:1">
       <c r="A71" s="16">
         <v>41302</v>
       </c>
-      <c r="C71" s="1">
-        <f t="shared" si="0"/>
-        <v>13.8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+    </row>
+    <row r="72" spans="1:1">
       <c r="A72" s="16">
         <v>41303</v>
       </c>
-      <c r="C72" s="1">
-        <f t="shared" si="0"/>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+    </row>
+    <row r="73" spans="1:1">
       <c r="A73" s="16">
         <v>41304</v>
       </c>
-      <c r="C73" s="1">
-        <f t="shared" si="0"/>
-        <v>9.1999999999999993</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+    </row>
+    <row r="74" spans="1:1">
       <c r="A74" s="16">
         <v>41305</v>
       </c>
-      <c r="C74" s="1">
-        <f t="shared" si="0"/>
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+    </row>
+    <row r="75" spans="1:1">
       <c r="A75" s="16">
         <v>41306</v>
       </c>
-      <c r="C75" s="1">
-        <f t="shared" si="0"/>
-        <v>4.5999999999999996</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+    </row>
+    <row r="76" spans="1:1">
       <c r="A76" s="16">
         <v>41307</v>
       </c>
-      <c r="C76" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+    </row>
+    <row r="77" spans="1:1">
       <c r="A77" s="16">
         <v>41308</v>
-      </c>
-      <c r="C77" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ranking firm od WM, update backlog
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -299,9 +299,6 @@
     <t>Zestawienie i ranking ofert firm WM</t>
   </si>
   <si>
-    <t>Znaleźć trzecią firme WM</t>
-  </si>
-  <si>
     <t>Zamówienie projektu w wybranej firmie</t>
   </si>
   <si>
@@ -333,6 +330,9 @@
   </si>
   <si>
     <t>S+S</t>
+  </si>
+  <si>
+    <t>Znaleźć trzecią i czwartą firme WM</t>
   </si>
 </sst>
 </file>
@@ -1079,9 +1079,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13448840769903778"/>
+          <c:x val="0.1344884076990378"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740977"/>
+          <c:w val="0.71441426071740965"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -1264,31 +1264,37 @@
                   <c:v>75.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73.5</c:v>
+                  <c:v>70.45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70.45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="70916736"/>
-        <c:axId val="70930816"/>
+        <c:axId val="62917248"/>
+        <c:axId val="62927232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="70916736"/>
+        <c:axId val="62917248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70930816"/>
+        <c:crossAx val="62927232"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="70930816"/>
+        <c:axId val="62927232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -1298,7 +1304,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70916736"/>
+        <c:crossAx val="62917248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1309,8 +1315,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325287875"/>
-          <c:y val="0.29353966170895324"/>
+          <c:x val="0.86438523325287886"/>
+          <c:y val="0.29353966170895335"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -1320,7 +1326,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2209,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2262,10 +2268,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
@@ -2277,7 +2283,7 @@
         <v>59</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -2285,10 +2291,10 @@
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -2300,7 +2306,7 @@
         <v>60</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2308,7 +2314,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="9">
@@ -2321,7 +2327,7 @@
         <v>61</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2329,7 +2335,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="9">
@@ -2347,7 +2353,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="9">
@@ -2365,10 +2371,10 @@
         <v>6</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="18">
         <v>2</v>
@@ -2385,7 +2391,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="9">
@@ -2403,7 +2409,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="9">
@@ -2421,7 +2427,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="9">
@@ -2439,7 +2445,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="9">
@@ -2457,10 +2463,10 @@
         <v>11</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="18">
         <v>1</v>
@@ -2469,7 +2475,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2477,10 +2483,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="9">
         <v>0.5</v>
@@ -2489,7 +2495,7 @@
         <v>0.25</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2497,16 +2503,16 @@
         <v>13</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D17" s="9">
         <v>9</v>
       </c>
       <c r="E17" s="2">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>69</v>
@@ -2519,12 +2525,14 @@
       <c r="B18" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D18" s="9">
         <v>2</v>
       </c>
       <c r="E18" s="2">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>71</v>
@@ -2537,7 +2545,9 @@
       <c r="B19" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="D19" s="9">
         <v>4</v>
       </c>
@@ -2553,7 +2563,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="9">
@@ -2563,12 +2573,12 @@
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="2"/>
@@ -2578,16 +2588,16 @@
       </c>
       <c r="E21" s="2">
         <f>SUM(E5:E20)</f>
-        <v>73.45</v>
+        <v>69.95</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2627,17 +2637,23 @@
         <v>41277</v>
       </c>
       <c r="B46" s="1">
-        <v>73.5</v>
+        <v>70.45</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" s="16">
         <v>41278</v>
       </c>
+      <c r="B47" s="1">
+        <v>70.45</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" s="16">
         <v>41279</v>
+      </c>
+      <c r="B48" s="1">
+        <v>69.95</v>
       </c>
     </row>
     <row r="49" spans="1:1">

</xml_diff>

<commit_message>
ranking firm od WM cd., update backlog
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -339,7 +339,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,13 +363,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF92D050"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -385,9 +378,8 @@
       <charset val="238"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FF92D050"/>
+      <color rgb="FF00B050"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
@@ -513,7 +505,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -547,11 +539,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1079,9 +1070,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1344884076990378"/>
+          <c:x val="0.13448840769903783"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740965"/>
+          <c:w val="0.71441426071740943"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -1272,29 +1263,32 @@
                 <c:pt idx="6">
                   <c:v>69.95</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>69.75</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62917248"/>
-        <c:axId val="62927232"/>
+        <c:axId val="62921344"/>
+        <c:axId val="62935424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62917248"/>
+        <c:axId val="62921344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62927232"/>
+        <c:crossAx val="62935424"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62927232"/>
+        <c:axId val="62935424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -1304,7 +1298,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62917248"/>
+        <c:crossAx val="62921344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1315,8 +1309,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325287886"/>
-          <c:y val="0.29353966170895335"/>
+          <c:x val="0.86438523325287908"/>
+          <c:y val="0.2935396617089534"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -1326,7 +1320,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2215,8 +2209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2264,22 +2258,22 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="2">
+      <c r="A5" s="17">
         <v>1</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="18">
         <v>1</v>
       </c>
-      <c r="E5" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>59</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -2287,22 +2281,22 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="2">
+      <c r="A6" s="17">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="18">
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="17">
+        <v>0</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>60</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -2382,7 +2376,7 @@
       <c r="E10" s="17">
         <v>0</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="17" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2474,7 +2468,7 @@
       <c r="E15" s="17">
         <v>0</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="F15" s="17" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2588,7 +2582,7 @@
       </c>
       <c r="E21" s="2">
         <f>SUM(E5:E20)</f>
-        <v>69.95</v>
+        <v>69.75</v>
       </c>
       <c r="F21" s="2"/>
     </row>
@@ -2656,82 +2650,85 @@
         <v>69.95</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:2">
       <c r="A49" s="16">
         <v>41280</v>
       </c>
-    </row>
-    <row r="50" spans="1:1">
+      <c r="B49" s="1">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" s="16">
         <v>41281</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:2">
       <c r="A51" s="16">
         <v>41282</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:2">
       <c r="A52" s="16">
         <v>41283</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:2">
       <c r="A53" s="16">
         <v>41284</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:2">
       <c r="A54" s="16">
         <v>41285</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:2">
       <c r="A55" s="16">
         <v>41286</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:2">
       <c r="A56" s="16">
         <v>41287</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:2">
       <c r="A57" s="16">
         <v>41288</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:2">
       <c r="A58" s="16">
         <v>41289</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:2">
       <c r="A59" s="16">
         <v>41290</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:2">
       <c r="A60" s="16">
         <v>41291</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:2">
       <c r="A61" s="16">
         <v>41292</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:2">
       <c r="A62" s="16">
         <v>41293</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:2">
       <c r="A63" s="16">
         <v>41294</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:2">
       <c r="A64" s="16">
         <v>41295</v>
       </c>

</xml_diff>

<commit_message>
zakończenie pierwszej iteracji, rozpoczęcie trzeciej
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -5317,8 +5317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>

</xml_diff>

<commit_message>
zakonczenie sprintu2, nowy sprint4
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
     <sheet name="01_SprintBacklog" sheetId="2" r:id="rId2"/>
     <sheet name="02_SprintBacklog" sheetId="3" r:id="rId3"/>
     <sheet name="03_SprintBacklog" sheetId="4" r:id="rId4"/>
+    <sheet name="04_Sprint" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -82,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="148">
   <si>
     <t>Id</t>
   </si>
@@ -517,6 +518,15 @@
   </si>
   <si>
     <t>Mieszkanie - optymalne spłacenie kredytu walutowego.</t>
+  </si>
+  <si>
+    <t>Kolumna1</t>
+  </si>
+  <si>
+    <t>SPRINT 04</t>
+  </si>
+  <si>
+    <t>Dokończenie zadań z zakresu zbrojenia działki.</t>
   </si>
 </sst>
 </file>
@@ -617,7 +627,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -736,11 +746,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -814,11 +833,682 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="45">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1057,7 +1747,7 @@
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1067,7 +1757,11 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1120,7 +1814,7 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1130,7 +1824,11 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1183,36 +1881,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1228,161 +1896,6 @@
         </bottom>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1983,6 +2496,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -1992,7 +2506,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740721"/>
+          <c:w val="0.7144142607174071"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -2272,24 +2786,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64958848"/>
-        <c:axId val="64960384"/>
+        <c:axId val="66447616"/>
+        <c:axId val="66785280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64958848"/>
+        <c:axId val="66447616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64960384"/>
+        <c:crossAx val="66785280"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64960384"/>
+        <c:axId val="66785280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -2299,7 +2813,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64958848"/>
+        <c:crossAx val="66447616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2310,8 +2824,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288308"/>
-          <c:y val="0.29353966170895468"/>
+          <c:x val="0.8643852332528833"/>
+          <c:y val="0.29353966170895474"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -2321,7 +2835,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2521,29 +3035,38 @@
                 <c:pt idx="24">
                   <c:v>16</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>15</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64895616"/>
-        <c:axId val="64917888"/>
+        <c:axId val="66814720"/>
+        <c:axId val="66816256"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64895616"/>
+        <c:axId val="66814720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64917888"/>
+        <c:crossAx val="66816256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64917888"/>
+        <c:axId val="66816256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -2553,7 +3076,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64895616"/>
+        <c:crossAx val="66814720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2566,7 +3089,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2715,29 +3238,38 @@
                 <c:pt idx="10">
                   <c:v>68</c:v>
                 </c:pt>
+                <c:pt idx="11">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>58</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65250432"/>
-        <c:axId val="65251968"/>
+        <c:axId val="79281152"/>
+        <c:axId val="79282944"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="65250432"/>
+        <c:axId val="79281152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65251968"/>
+        <c:crossAx val="79282944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="65251968"/>
+        <c:axId val="79282944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -2747,7 +3279,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65250432"/>
+        <c:crossAx val="79281152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2760,7 +3292,161 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="pl-PL"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'04_Sprint'!$A$19:$A$43</c:f>
+              <c:numCache>
+                <c:formatCode>yyyy/mm/dd</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>41321</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41322</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41323</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41325</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>41326</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>41327</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>41328</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>41329</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41330</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41331</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>41332</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>41333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41334</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41335</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41336</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41337</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41338</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41339</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41340</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41341</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41342</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41343</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41344</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>41345</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'04_Sprint'!$B$19:$B$43</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="94628480"/>
+        <c:axId val="94651904"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="94628480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
+        <c:majorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94651904"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="94651904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="94628480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2871,67 +3557,117 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>790575</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1790700</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Wykres 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="61" dataDxfId="59" headerRowBorderDxfId="60" tableBorderDxfId="58" totalsRowBorderDxfId="57">
   <autoFilter ref="A1:F43"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="39"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="38"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="37"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="36"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="35"/>
-    <tableColumn id="6" name="Aby" dataDxfId="34"/>
+    <tableColumn id="1" name="Id" dataDxfId="56"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="55"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="54"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="53"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="52"/>
+    <tableColumn id="6" name="Aby" dataDxfId="51"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
   <autoFilter ref="A4:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="31"/>
-    <tableColumn id="2" name="Status" dataDxfId="30"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="29"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="28"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="27"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="26"/>
+    <tableColumn id="1" name="Id" dataDxfId="48"/>
+    <tableColumn id="2" name="Status" dataDxfId="47"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="46"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="45"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="44"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="25" dataDxfId="24" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="42" dataDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A4:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="2" name="Status" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="18" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="39" totalsRowDxfId="22"/>
+    <tableColumn id="2" name="Status" dataDxfId="38" totalsRowDxfId="21"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="37" totalsRowDxfId="20"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="19">
       <totalsRowFormula>SUM([Rozmiar początkowy '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="14" totalsRowDxfId="13">
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="18">
       <totalsRowFormula>SUM([Pozostało '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Zadanie" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="34" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="A6:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="5"/>
-    <tableColumn id="2" name="Status" dataDxfId="4"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="3"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="2"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="1"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="0"/>
+    <tableColumn id="1" name="Id" dataDxfId="28"/>
+    <tableColumn id="2" name="Status" dataDxfId="27"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="26"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="25"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="24"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6" headerRowBorderDxfId="15" tableBorderDxfId="16" totalsRowBorderDxfId="14">
+  <autoFilter ref="A5:F16"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Kolumna1" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="11" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="8" totalsRowDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3943,7 +4679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:F14"/>
     </sheetView>
   </sheetViews>
@@ -4630,8 +5366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5089,7 +5825,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="26" t="s">
         <v>118</v>
@@ -5155,7 +5891,7 @@
       </c>
       <c r="E24" s="27">
         <f>SUM([Pozostało '[h']])</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F24" s="26"/>
       <c r="G24" s="1"/>
@@ -5379,19 +6115,25 @@
       <c r="A56" s="28">
         <v>41319</v>
       </c>
-      <c r="B56" s="29"/>
+      <c r="B56" s="29">
+        <v>16</v>
+      </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="28">
         <v>41320</v>
       </c>
-      <c r="B57" s="29"/>
+      <c r="B57" s="29">
+        <v>16</v>
+      </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="28">
         <v>41321</v>
       </c>
-      <c r="B58" s="29"/>
+      <c r="B58" s="29">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5412,8 +6154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I58"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5485,93 +6227,93 @@
       <c r="F6" s="25" t="s">
         <v>12</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="2">
+      <c r="A7" s="39">
         <v>1</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="38">
+        <v>2</v>
+      </c>
+      <c r="E7" s="38">
+        <v>0</v>
+      </c>
+      <c r="F7" s="39" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="9">
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="39">
         <v>2</v>
       </c>
-      <c r="E7" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="2">
+      <c r="B8" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="D8" s="38">
         <v>2</v>
       </c>
-      <c r="B8" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="E8" s="38">
+        <v>0</v>
+      </c>
+      <c r="F8" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="39">
+        <v>3</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1.5</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="2">
-        <v>3</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="38">
+        <v>20</v>
+      </c>
+      <c r="E9" s="38">
+        <v>0</v>
+      </c>
+      <c r="F9" s="39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="39">
+        <v>4</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="9">
-        <v>20</v>
-      </c>
-      <c r="E9" s="9">
-        <v>2</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="2">
-        <v>4</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="D10" s="38">
         <v>10</v>
       </c>
-      <c r="E10" s="9">
-        <v>6</v>
-      </c>
-      <c r="F10" s="2" t="s">
+      <c r="E10" s="38">
+        <v>0</v>
+      </c>
+      <c r="F10" s="39" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5579,7 +6321,7 @@
       <c r="A11" s="34">
         <v>5</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -5599,7 +6341,7 @@
       <c r="A12" s="34">
         <v>6</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -5619,7 +6361,7 @@
       <c r="A13" s="34">
         <v>7</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C13" s="2"/>
@@ -5637,7 +6379,7 @@
       <c r="A14" s="37">
         <v>8</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C14" s="39" t="s">
@@ -5657,7 +6399,7 @@
       <c r="A15" s="34">
         <v>9</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C15" s="2"/>
@@ -5675,7 +6417,7 @@
       <c r="A16" s="34">
         <v>10</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="2"/>
@@ -5693,7 +6435,7 @@
       <c r="A17" s="34">
         <v>11</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C17" s="2"/>
@@ -5711,7 +6453,7 @@
       <c r="A18" s="37">
         <v>12</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="9" t="s">
         <v>71</v>
       </c>
       <c r="C18" s="39" t="s">
@@ -5731,7 +6473,7 @@
       <c r="A19" s="34">
         <v>13</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C19" s="2"/>
@@ -5749,7 +6491,7 @@
       <c r="A20" s="34">
         <v>14</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C20" s="13"/>
@@ -5767,7 +6509,7 @@
       <c r="A21" s="34">
         <v>15</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C21" s="2"/>
@@ -5785,7 +6527,7 @@
       <c r="A22" s="34">
         <v>16</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="9" t="s">
         <v>70</v>
       </c>
       <c r="C22" s="13" t="s">
@@ -5805,7 +6547,7 @@
       <c r="A23" s="34">
         <v>17</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C23" s="2"/>
@@ -5823,7 +6565,7 @@
       <c r="A24" s="34">
         <v>18</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C24" s="13"/>
@@ -5841,7 +6583,7 @@
       <c r="A25" s="34">
         <v>19</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="13"/>
@@ -5859,7 +6601,7 @@
       <c r="A26" s="34">
         <v>20</v>
       </c>
-      <c r="B26" s="24" t="s">
+      <c r="B26" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C26" s="2"/>
@@ -5877,7 +6619,7 @@
       <c r="A27" s="34">
         <v>21</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="9" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="2"/>
@@ -5908,7 +6650,7 @@
       <c r="D29" s="13"/>
       <c r="E29" s="13">
         <f>SUBTOTAL(109,E7:E28)</f>
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F29" s="14"/>
     </row>
@@ -6020,19 +6762,25 @@
       <c r="A43" s="28">
         <v>41319</v>
       </c>
-      <c r="B43" s="29"/>
+      <c r="B43" s="29">
+        <v>68</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="28">
         <v>41320</v>
       </c>
-      <c r="B44" s="29"/>
+      <c r="B44" s="29">
+        <v>68</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="28">
         <v>41321</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="29">
+        <v>58</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="28">
@@ -6113,11 +6861,8 @@
       <c r="B58" s="29"/>
     </row>
   </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11:B27">
-      <formula1>$I$7:$I$9</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B10">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B27">
       <formula1>$I$6:$I$8</formula1>
     </dataValidation>
   </dataValidations>
@@ -6127,4 +6872,408 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:F43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="71.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" s="33"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="42">
+        <v>1</v>
+      </c>
+      <c r="B6" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="44"/>
+      <c r="D6" s="43">
+        <v>1</v>
+      </c>
+      <c r="E6" s="44">
+        <v>1</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="42">
+        <v>2</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="E7" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="42">
+        <v>3</v>
+      </c>
+      <c r="B8" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="42">
+        <v>4</v>
+      </c>
+      <c r="B9" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="46">
+        <v>0.5</v>
+      </c>
+      <c r="F9" s="45" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="42">
+        <v>5</v>
+      </c>
+      <c r="B10" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="42">
+        <v>6</v>
+      </c>
+      <c r="B11" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="43">
+        <v>1</v>
+      </c>
+      <c r="E11" s="44">
+        <v>1</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="42">
+        <v>7</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="44"/>
+      <c r="D12" s="43">
+        <v>2</v>
+      </c>
+      <c r="E12" s="44">
+        <v>2</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="42">
+        <v>8</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="46"/>
+      <c r="D13" s="47">
+        <v>6</v>
+      </c>
+      <c r="E13" s="46">
+        <v>6</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="42">
+        <v>9</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="43">
+        <v>2</v>
+      </c>
+      <c r="E14" s="44">
+        <v>2</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="49">
+        <v>10</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47">
+        <v>2</v>
+      </c>
+      <c r="E15" s="46">
+        <v>1</v>
+      </c>
+      <c r="F15" s="48" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="49"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47">
+        <f>SUBTOTAL(109,[Rozmiar początkowy '[h']])</f>
+        <v>16</v>
+      </c>
+      <c r="E16" s="46">
+        <f>SUBTOTAL(109,[Pozostało '[h']])</f>
+        <v>15</v>
+      </c>
+      <c r="F16" s="48"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="28">
+        <v>41321</v>
+      </c>
+      <c r="B19" s="29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="28">
+        <v>41322</v>
+      </c>
+      <c r="B20" s="29"/>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="28">
+        <v>41323</v>
+      </c>
+      <c r="B21" s="29"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="28">
+        <v>41324</v>
+      </c>
+      <c r="B22" s="29"/>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="28">
+        <v>41325</v>
+      </c>
+      <c r="B23" s="29"/>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="28">
+        <v>41326</v>
+      </c>
+      <c r="B24" s="29"/>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="28">
+        <v>41327</v>
+      </c>
+      <c r="B25" s="29"/>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="28">
+        <v>41328</v>
+      </c>
+      <c r="B26" s="29"/>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="28">
+        <v>41329</v>
+      </c>
+      <c r="B27" s="29"/>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="28">
+        <v>41330</v>
+      </c>
+      <c r="B28" s="29"/>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="28">
+        <v>41331</v>
+      </c>
+      <c r="B29" s="29"/>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="28">
+        <v>41332</v>
+      </c>
+      <c r="B30" s="29"/>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="28">
+        <v>41333</v>
+      </c>
+      <c r="B31" s="29"/>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="28">
+        <v>41334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="28">
+        <v>41335</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="28">
+        <v>41336</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="28">
+        <v>41337</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="28">
+        <v>41338</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="28">
+        <v>41339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="28">
+        <v>41340</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="28">
+        <v>41341</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="28">
+        <v>41342</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="28">
+        <v>41343</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="28">
+        <v>41344</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="28">
+        <v>41345</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B15">
+      <formula1>$I$7:$I$10</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
plan uruchomienia transzy eb
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="03_Sprint" sheetId="4" r:id="rId4"/>
     <sheet name="04_Sprint" sheetId="5" r:id="rId5"/>
     <sheet name="05_Sprint" sheetId="6" r:id="rId6"/>
+    <sheet name="Notatki5" sheetId="7" r:id="rId7"/>
+    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -84,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="285">
   <si>
     <t>Id</t>
   </si>
@@ -617,13 +619,337 @@
   <si>
     <t>Pozo-
 stało [h]</t>
+  </si>
+  <si>
+    <t>Pospółka i kliniec - Wrocław</t>
+  </si>
+  <si>
+    <t>http://allegro.pl/piasek-rzeczny-piach-pospolka-wroclaw-i3065577322.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Zakład Przetwórstwa Kruszyw MARGO</t>
+  </si>
+  <si>
+    <t>http://www.kruszywa-margo.pl/</t>
+  </si>
+  <si>
+    <t>Mietków</t>
+  </si>
+  <si>
+    <t>698-942-703</t>
+  </si>
+  <si>
+    <t>http://wroclaw.olx.pl/wroclaw-piaskownia-zwirownia-piasek-zwir-pospolka-zwir-drenazowy-transport-wywrotka-iid-318919317</t>
+  </si>
+  <si>
+    <t>http://www.jft.com.pl/materialy-budowlane.htm</t>
+  </si>
+  <si>
+    <t>Wrocław, Wędkarzy</t>
+  </si>
+  <si>
+    <t>Wrocław, ?</t>
+  </si>
+  <si>
+    <t>http://www.hydrokrusz.pl/kruszywa/cennik.html</t>
+  </si>
+  <si>
+    <t>Wrocław, Centrun</t>
+  </si>
+  <si>
+    <t>71 343 22 55</t>
+  </si>
+  <si>
+    <t>średnica</t>
+  </si>
+  <si>
+    <t>długość [mm]</t>
+  </si>
+  <si>
+    <t>ilość</t>
+  </si>
+  <si>
+    <t>razem śr12</t>
+  </si>
+  <si>
+    <t>razem śr10</t>
+  </si>
+  <si>
+    <t>razem śr8</t>
+  </si>
+  <si>
+    <t>Masa 1m [kg/m]</t>
+  </si>
+  <si>
+    <t>Długość razem [m]</t>
+  </si>
+  <si>
+    <t>Masa   [kg]</t>
+  </si>
+  <si>
+    <t>lp</t>
+  </si>
+  <si>
+    <t>Drut stal.okrągły miękki fi 0,5-0,8mm</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Kotwy stalowe</t>
+  </si>
+  <si>
+    <t>szt</t>
+  </si>
+  <si>
+    <t>Pręty okr.gład.do zbr.bet. fi do 7mm</t>
+  </si>
+  <si>
+    <t>Prętyżebr.skoś.do zbr.bet. fi 12-14mm</t>
+  </si>
+  <si>
+    <t>Fundamenty z projektu</t>
+  </si>
+  <si>
+    <t>Stal do stropu</t>
+  </si>
+  <si>
+    <t>razem</t>
+  </si>
+  <si>
+    <t>Stal do płyty</t>
+  </si>
+  <si>
+    <t>srednica</t>
+  </si>
+  <si>
+    <t>długosc</t>
+  </si>
+  <si>
+    <t>fi 6</t>
+  </si>
+  <si>
+    <t>fi 14</t>
+  </si>
+  <si>
+    <t>fi 18</t>
+  </si>
+  <si>
+    <t>dlugosc razem</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>masa 1m</t>
+  </si>
+  <si>
+    <t>masa</t>
+  </si>
+  <si>
+    <t>masa razem</t>
+  </si>
+  <si>
+    <t>266,54kg</t>
+  </si>
+  <si>
+    <t>Zestawienie stali wg projektu, rys K5</t>
+  </si>
+  <si>
+    <t>Zestawienie stali wg projektu, rys K6</t>
+  </si>
+  <si>
+    <t>Geodeta</t>
+  </si>
+  <si>
+    <t>Harmonogram</t>
+  </si>
+  <si>
+    <t>Ile dni od rozpoczęcia robót trzeba go zawołać</t>
+  </si>
+  <si>
+    <t>Kliniec</t>
+  </si>
+  <si>
+    <t>Pospółka</t>
+  </si>
+  <si>
+    <t>Stal</t>
+  </si>
+  <si>
+    <t>Na kiedy trzeba dostarczyć stal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beton </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kto zamawia beton. </t>
+  </si>
+  <si>
+    <t>Czy warto zamówić stal na całą budowę (płyta + strop)</t>
+  </si>
+  <si>
+    <t>Kominek</t>
+  </si>
+  <si>
+    <t>Kanalizacja</t>
+  </si>
+  <si>
+    <t>Gdzie będzie przebiegać rura z poddasza (bo pierwotnie idzie w kominie)</t>
+  </si>
+  <si>
+    <t>Projekt wod-kan</t>
+  </si>
+  <si>
+    <t>Uzgodnić kanalizację w płycie</t>
+  </si>
+  <si>
+    <t>Ile potrzeba stali na cały budynek. Czy stal kupuje się w gotowych formach do stropu.</t>
+  </si>
+  <si>
+    <t>Kiedy po rozpoczęciu robót potrzebne jest dostarczenie klińca</t>
+  </si>
+  <si>
+    <t>Kiedy po rozpoczęciu robót potrzebne jest dostarczenie pospółki</t>
+  </si>
+  <si>
+    <t>Geodeta - kiedy</t>
+  </si>
+  <si>
+    <t>Beton i Stal</t>
+  </si>
+  <si>
+    <t>Czy można zamówić w Manexie (i czy warto)</t>
+  </si>
+  <si>
+    <t>Okna</t>
+  </si>
+  <si>
+    <t>Uzgodnić zestawienie</t>
+  </si>
+  <si>
+    <t>Czy doprowadzenie powietrza do kominka z zamkniętą komora spalania idzie przez płytę? Jeśli tak to trzeba to uwzglednić.</t>
+  </si>
+  <si>
+    <t>Temat</t>
+  </si>
+  <si>
+    <t>Pytanie</t>
+  </si>
+  <si>
+    <t>Ustalenie</t>
+  </si>
+  <si>
+    <t>Wykop</t>
+  </si>
+  <si>
+    <t>Kiedy zaczyna się i kończy wykopy</t>
+  </si>
+  <si>
+    <t>Piaskarnie</t>
+  </si>
+  <si>
+    <t>Kliniec - opis</t>
+  </si>
+  <si>
+    <t>Kliniec - cena za całość</t>
+  </si>
+  <si>
+    <t>Pospółka - opis</t>
+  </si>
+  <si>
+    <t>Pospółka - cena za całość</t>
+  </si>
+  <si>
+    <t>Jan Familien Trans</t>
+  </si>
+  <si>
+    <t>Dane firmy</t>
+  </si>
+  <si>
+    <t>5-31,5mm, 30m3=50ton</t>
+  </si>
+  <si>
+    <t>Piasek na podsypkę, 110m3=187ton</t>
+  </si>
+  <si>
+    <t>www.kruszywa-margo.pl</t>
+  </si>
+  <si>
+    <t>Margo Mietków</t>
+  </si>
+  <si>
+    <t>3auta po 20ton</t>
+  </si>
+  <si>
+    <t>10 aut po 20 ton</t>
+  </si>
+  <si>
+    <t>Maligrand</t>
+  </si>
+  <si>
+    <t>850zł za samochód 22t</t>
+  </si>
+  <si>
+    <t>440 za samochod 22t</t>
+  </si>
+  <si>
+    <t>Razem koszt surowca z dostawą</t>
+  </si>
+  <si>
+    <t>Hydrokrusz</t>
+  </si>
+  <si>
+    <t>3000,00 (bez dostawy)</t>
+  </si>
+  <si>
+    <t>1tona 60zł - wg cennika na www</t>
+  </si>
+  <si>
+    <t>3553,00 (bez dostawy)</t>
+  </si>
+  <si>
+    <t>Najtańsza mieszanka piaskowo-żwirowa 1t=19zł, wg cennika na www</t>
+  </si>
+  <si>
+    <t>Podpisanie umowy</t>
+  </si>
+  <si>
+    <t>Planowany termin wykonania</t>
+  </si>
+  <si>
+    <t>Zbieranie kasy</t>
+  </si>
+  <si>
+    <t>2013-05-31 do 2013-06-01</t>
+  </si>
+  <si>
+    <t>Zbieramy wyrok</t>
+  </si>
+  <si>
+    <t>Wniosek o wpis do hipoteki</t>
+  </si>
+  <si>
+    <t>Spłata-nadpłata</t>
+  </si>
+  <si>
+    <t>Przewalutowanie</t>
+  </si>
+  <si>
+    <t>Zaświadczenie mbank (terminowej spłaty kredytu i rachunek)</t>
+  </si>
+  <si>
+    <t>Dyspozycja całkowitej spłaty mbank</t>
+  </si>
+  <si>
+    <t>Dyspozycja wypłaty transzy EB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,8 +1046,39 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,8 +1103,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -875,11 +1238,187 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1004,11 +1543,139 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="79">
+  <dxfs count="84">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1065,6 +1732,75 @@
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -1135,6 +1871,77 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1206,238 +2013,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -1484,10 +2059,102 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3132,7 +3799,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout>
@@ -3142,7 +3808,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740699"/>
+          <c:w val="0.71441426071740621"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -3422,24 +4088,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62966784"/>
-        <c:axId val="62989056"/>
+        <c:axId val="63017344"/>
+        <c:axId val="63018880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62966784"/>
+        <c:axId val="63017344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62989056"/>
+        <c:crossAx val="63018880"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62989056"/>
+        <c:axId val="63018880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -3449,7 +4115,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62966784"/>
+        <c:crossAx val="63017344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3460,8 +4126,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288352"/>
-          <c:y val="0.29353966170895485"/>
+          <c:x val="0.86438523325288485"/>
+          <c:y val="0.29353966170895524"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -3471,7 +4137,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3481,9 +4147,7 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="pl-PL"/>
   <c:chart>
-    <c:title>
-      <c:layout/>
-    </c:title>
+    <c:title/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -3685,24 +4349,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63034880"/>
-        <c:axId val="63036416"/>
+        <c:axId val="63044224"/>
+        <c:axId val="63914368"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63034880"/>
+        <c:axId val="63044224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63036416"/>
+        <c:crossAx val="63914368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63036416"/>
+        <c:axId val="63914368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -3712,20 +4376,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63034880"/>
+        <c:crossAx val="63044224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3888,24 +4551,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64167936"/>
-        <c:axId val="64169472"/>
+        <c:axId val="64009344"/>
+        <c:axId val="64010880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64167936"/>
+        <c:axId val="64009344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64169472"/>
+        <c:crossAx val="64010880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64169472"/>
+        <c:axId val="64010880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -3915,20 +4578,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64167936"/>
+        <c:crossAx val="64009344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4043,11 +4705,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64259200"/>
-        <c:axId val="64260736"/>
+        <c:axId val="64346368"/>
+        <c:axId val="64348160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64259200"/>
+        <c:axId val="64346368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4055,13 +4717,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64260736"/>
+        <c:crossAx val="64348160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64260736"/>
+        <c:axId val="64348160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4069,20 +4731,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64259200"/>
+        <c:crossAx val="64346368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4098,10 +4759,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961919"/>
-          <c:y val="3.2882035578885971E-2"/>
-          <c:w val="0.65643820838184697"/>
-          <c:h val="0.63861876640419946"/>
+          <c:x val="0.171815628309619"/>
+          <c:y val="3.2882035578886026E-2"/>
+          <c:w val="0.65643820838184763"/>
+          <c:h val="0.63861876640420068"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4172,16 +4833,37 @@
                 <c:pt idx="1">
                   <c:v>27</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="66648320"/>
-        <c:axId val="69672960"/>
+        <c:axId val="64396672"/>
+        <c:axId val="64439424"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="66648320"/>
+        <c:axId val="64396672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4189,13 +4871,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69672960"/>
+        <c:crossAx val="64439424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="69672960"/>
+        <c:axId val="64439424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4204,7 +4886,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66648320"/>
+        <c:crossAx val="64396672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4217,7 +4899,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4399,96 +5081,108 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75" totalsRowBorderDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
   <autoFilter ref="A1:F43"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="73"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="72"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="71"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="70"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="69"/>
-    <tableColumn id="6" name="Aby" dataDxfId="68"/>
+    <tableColumn id="1" name="Id" dataDxfId="78"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="77"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="76"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="75"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="74"/>
+    <tableColumn id="6" name="Aby" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="67" dataDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A4:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="65"/>
-    <tableColumn id="2" name="Status" dataDxfId="64"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="63"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="62"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="61"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="60"/>
+    <tableColumn id="1" name="Id" dataDxfId="70"/>
+    <tableColumn id="2" name="Status" dataDxfId="69"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="68"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="67"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="66"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="65"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="59" dataDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
   <autoFilter ref="A4:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="2" name="Status" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="49">
+    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="2" name="Status" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
       <totalsRowFormula>SUM([Rozmiar początkowy '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="48" totalsRowDxfId="47">
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <totalsRowFormula>SUM([Pozostało '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Zadanie" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="51" totalsRowDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
   <autoFilter ref="A6:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="39"/>
-    <tableColumn id="2" name="Status" dataDxfId="38"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="37"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="36"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="35"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="34"/>
+    <tableColumn id="1" name="Id" dataDxfId="44"/>
+    <tableColumn id="2" name="Status" dataDxfId="43"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="42"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="41"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="40"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
   <autoFilter ref="A5:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="20" totalsRowDxfId="19"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="33" totalsRowDxfId="32"/>
+    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="23" totalsRowDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
   <autoFilter ref="A5:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="16" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Status" dataDxfId="15" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="14" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="6" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="12" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="2" name="Status" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="6" totalsRowDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B135:D152" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B135:D152"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Temat" dataDxfId="2"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -8107,18 +8801,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
     <col min="2" max="2" width="10.88671875" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" customWidth="1"/>
     <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="70.21875" customWidth="1"/>
+    <col min="6" max="6" width="73.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -8219,20 +8913,20 @@
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="42">
+      <c r="A9" s="85">
         <v>4</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="43">
+      <c r="B9" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="90"/>
+      <c r="D9" s="88">
         <v>0.5</v>
       </c>
-      <c r="E9" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="F9" s="45" t="s">
+      <c r="E9" s="88">
+        <v>0</v>
+      </c>
+      <c r="F9" s="89" t="s">
         <v>152</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -8240,20 +8934,20 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="42">
+      <c r="A10" s="85">
         <v>5</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="43">
+      <c r="B10" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="87"/>
+      <c r="D10" s="88">
         <v>0.5</v>
       </c>
-      <c r="E10" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="F10" s="45" t="s">
+      <c r="E10" s="88">
+        <v>0</v>
+      </c>
+      <c r="F10" s="89" t="s">
         <v>153</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -8338,22 +9032,22 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="42">
+      <c r="A15" s="85">
         <v>10</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15" s="46" t="s">
+      <c r="B15" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="D15" s="47">
+      <c r="D15" s="91">
         <v>2</v>
       </c>
-      <c r="E15" s="47">
-        <v>2</v>
-      </c>
-      <c r="F15" s="48" t="s">
+      <c r="E15" s="91">
+        <v>0</v>
+      </c>
+      <c r="F15" s="92" t="s">
         <v>172</v>
       </c>
     </row>
@@ -8486,22 +9180,22 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="42">
+      <c r="A23" s="85">
         <v>18</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="46" t="s">
+      <c r="B23" s="86" t="s">
+        <v>71</v>
+      </c>
+      <c r="C23" s="90" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="47">
+      <c r="D23" s="91">
         <v>2</v>
       </c>
-      <c r="E23" s="47">
-        <v>2</v>
-      </c>
-      <c r="F23" s="48" t="s">
+      <c r="E23" s="91">
+        <v>0</v>
+      </c>
+      <c r="F23" s="92" t="s">
         <v>164</v>
       </c>
     </row>
@@ -8627,7 +9321,7 @@
       <c r="E30" s="46">
         <f>SUBTOTAL(109,[Pozo-
 stało '[h']])</f>
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F30" s="48"/>
     </row>
@@ -8667,43 +9361,57 @@
       <c r="A35" s="28">
         <v>41409</v>
       </c>
-      <c r="B35" s="29"/>
+      <c r="B35" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="28">
         <v>41410</v>
       </c>
-      <c r="B36" s="29"/>
+      <c r="B36" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="28">
         <v>41411</v>
       </c>
-      <c r="B37" s="29"/>
+      <c r="B37" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="28">
         <v>41412</v>
       </c>
-      <c r="B38" s="29"/>
+      <c r="B38" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="28">
         <v>41413</v>
       </c>
-      <c r="B39" s="29"/>
+      <c r="B39" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="28">
         <v>41414</v>
       </c>
-      <c r="B40" s="29"/>
+      <c r="B40" s="29">
+        <v>27</v>
+      </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="28">
         <v>41415</v>
       </c>
-      <c r="B41" s="29"/>
+      <c r="B41" s="29">
+        <v>26</v>
+      </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="28">
@@ -8780,4 +9488,1713 @@
     <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L152"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.5546875" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="98"/>
+      <c r="B1" s="98"/>
+      <c r="C1" s="98"/>
+      <c r="D1" s="98"/>
+      <c r="E1" s="98"/>
+      <c r="F1" s="98"/>
+      <c r="G1" s="98"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="98"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+    </row>
+    <row r="2" spans="1:11" ht="21" customHeight="1">
+      <c r="A2" s="98"/>
+      <c r="B2" s="99" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="99" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" s="99" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="99" t="s">
+        <v>255</v>
+      </c>
+      <c r="F2" s="99" t="s">
+        <v>256</v>
+      </c>
+      <c r="G2" s="99" t="s">
+        <v>268</v>
+      </c>
+      <c r="H2" s="99" t="s">
+        <v>258</v>
+      </c>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+    </row>
+    <row r="3" spans="1:11" ht="32.25">
+      <c r="A3" s="98"/>
+      <c r="B3" s="100" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="100" t="s">
+        <v>259</v>
+      </c>
+      <c r="D3" s="101">
+        <v>2499</v>
+      </c>
+      <c r="E3" s="100" t="s">
+        <v>260</v>
+      </c>
+      <c r="F3" s="101">
+        <v>3740</v>
+      </c>
+      <c r="G3" s="102">
+        <f>F3+D3</f>
+        <v>6239</v>
+      </c>
+      <c r="H3" s="100" t="s">
+        <v>184</v>
+      </c>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+    </row>
+    <row r="4" spans="1:11" ht="21.75">
+      <c r="A4" s="98"/>
+      <c r="B4" s="100" t="s">
+        <v>262</v>
+      </c>
+      <c r="C4" s="100" t="s">
+        <v>263</v>
+      </c>
+      <c r="D4" s="101">
+        <v>3900</v>
+      </c>
+      <c r="E4" s="100" t="s">
+        <v>264</v>
+      </c>
+      <c r="F4" s="101">
+        <v>13000</v>
+      </c>
+      <c r="G4" s="102">
+        <f t="shared" ref="G4:G5" si="0">F4+D4</f>
+        <v>16900</v>
+      </c>
+      <c r="H4" s="100" t="s">
+        <v>261</v>
+      </c>
+      <c r="I4" s="98"/>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="98"/>
+      <c r="B5" s="100" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="100" t="s">
+        <v>266</v>
+      </c>
+      <c r="D5" s="101">
+        <v>2550</v>
+      </c>
+      <c r="E5" s="100" t="s">
+        <v>267</v>
+      </c>
+      <c r="F5" s="101">
+        <v>3960</v>
+      </c>
+      <c r="G5" s="102">
+        <f t="shared" si="0"/>
+        <v>6510</v>
+      </c>
+      <c r="H5" s="100"/>
+      <c r="I5" s="98"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="98"/>
+    </row>
+    <row r="6" spans="1:11" ht="32.25">
+      <c r="A6" s="98"/>
+      <c r="B6" s="100" t="s">
+        <v>269</v>
+      </c>
+      <c r="C6" s="100" t="s">
+        <v>271</v>
+      </c>
+      <c r="D6" s="101" t="s">
+        <v>270</v>
+      </c>
+      <c r="E6" s="100" t="s">
+        <v>273</v>
+      </c>
+      <c r="F6" s="101" t="s">
+        <v>272</v>
+      </c>
+      <c r="G6" s="102">
+        <v>6553</v>
+      </c>
+      <c r="H6" s="100" t="s">
+        <v>187</v>
+      </c>
+      <c r="I6" s="98"/>
+      <c r="J6" s="98"/>
+      <c r="K6" s="98"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="98"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="98"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="98"/>
+      <c r="H7" s="98"/>
+      <c r="I7" s="98"/>
+      <c r="J7" s="98"/>
+      <c r="K7" s="98"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="98"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="98"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="98"/>
+      <c r="H8" s="98"/>
+      <c r="I8" s="98"/>
+      <c r="J8" s="98"/>
+      <c r="K8" s="98"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="98"/>
+      <c r="B9" s="98"/>
+      <c r="C9" s="98"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="98"/>
+      <c r="H9" s="98"/>
+      <c r="I9" s="98"/>
+      <c r="J9" s="98"/>
+      <c r="K9" s="98"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="98"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
+      <c r="F10" s="98"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
+      <c r="I10" s="98"/>
+      <c r="J10" s="98"/>
+      <c r="K10" s="98"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="98"/>
+      <c r="B11" s="98"/>
+      <c r="C11" s="98"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="98"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="98"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="98"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="98"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="98"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="98"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="98"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="98"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="98"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="98"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="98"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="98"/>
+      <c r="H14" s="98"/>
+      <c r="I14" s="98"/>
+      <c r="J14" s="98"/>
+      <c r="K14" s="98"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="98"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="98"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="98"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+    </row>
+    <row r="21" spans="2:12">
+      <c r="B21" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12">
+      <c r="B22">
+        <v>602632659</v>
+      </c>
+      <c r="C22" t="s">
+        <v>186</v>
+      </c>
+      <c r="D22" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12">
+      <c r="B23">
+        <v>713169022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>181</v>
+      </c>
+      <c r="D23" s="67" t="s">
+        <v>179</v>
+      </c>
+      <c r="H23" s="66" t="s">
+        <v>180</v>
+      </c>
+      <c r="L23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12">
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12">
+      <c r="B25" s="68">
+        <v>600939523</v>
+      </c>
+      <c r="C25" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="66" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12">
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" t="s">
+        <v>188</v>
+      </c>
+      <c r="D26" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="15" thickBot="1"/>
+    <row r="34" spans="2:8">
+      <c r="B34" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C34" s="72" t="s">
+        <v>190</v>
+      </c>
+      <c r="D34" s="72" t="s">
+        <v>191</v>
+      </c>
+      <c r="E34" s="79" t="s">
+        <v>192</v>
+      </c>
+      <c r="F34" s="71" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="72" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="73" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8">
+      <c r="B35" s="74">
+        <v>1</v>
+      </c>
+      <c r="C35" s="69">
+        <v>8</v>
+      </c>
+      <c r="D35" s="69">
+        <v>9640</v>
+      </c>
+      <c r="E35" s="80">
+        <v>16</v>
+      </c>
+      <c r="F35" s="74">
+        <f>E35*D35/1000</f>
+        <v>154.24</v>
+      </c>
+      <c r="G35" s="69"/>
+      <c r="H35" s="75"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" s="74">
+        <v>2</v>
+      </c>
+      <c r="C36" s="69">
+        <v>8</v>
+      </c>
+      <c r="D36" s="69">
+        <v>6870</v>
+      </c>
+      <c r="E36" s="80">
+        <v>116</v>
+      </c>
+      <c r="F36" s="74">
+        <f t="shared" ref="F36:F47" si="1">E36*D36/1000</f>
+        <v>796.92</v>
+      </c>
+      <c r="G36" s="69"/>
+      <c r="H36" s="75"/>
+    </row>
+    <row r="37" spans="2:8">
+      <c r="B37" s="74">
+        <v>3</v>
+      </c>
+      <c r="C37" s="69">
+        <v>8</v>
+      </c>
+      <c r="D37" s="69">
+        <v>7970</v>
+      </c>
+      <c r="E37" s="80">
+        <v>28</v>
+      </c>
+      <c r="F37" s="74">
+        <f t="shared" si="1"/>
+        <v>223.16</v>
+      </c>
+      <c r="G37" s="69"/>
+      <c r="H37" s="75"/>
+    </row>
+    <row r="38" spans="2:8">
+      <c r="B38" s="74">
+        <v>4</v>
+      </c>
+      <c r="C38" s="69">
+        <v>8</v>
+      </c>
+      <c r="D38" s="69">
+        <v>7540</v>
+      </c>
+      <c r="E38" s="80">
+        <v>8</v>
+      </c>
+      <c r="F38" s="74">
+        <f t="shared" si="1"/>
+        <v>60.32</v>
+      </c>
+      <c r="G38" s="69"/>
+      <c r="H38" s="75"/>
+    </row>
+    <row r="39" spans="2:8">
+      <c r="B39" s="74">
+        <v>5</v>
+      </c>
+      <c r="C39" s="69">
+        <v>8</v>
+      </c>
+      <c r="D39" s="69">
+        <v>3180</v>
+      </c>
+      <c r="E39" s="80">
+        <v>10</v>
+      </c>
+      <c r="F39" s="74">
+        <f t="shared" si="1"/>
+        <v>31.8</v>
+      </c>
+      <c r="G39" s="69"/>
+      <c r="H39" s="75"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="74">
+        <v>6</v>
+      </c>
+      <c r="C40" s="69">
+        <v>8</v>
+      </c>
+      <c r="D40" s="69">
+        <v>9140</v>
+      </c>
+      <c r="E40" s="80">
+        <v>54</v>
+      </c>
+      <c r="F40" s="74">
+        <f t="shared" si="1"/>
+        <v>493.56</v>
+      </c>
+      <c r="G40" s="69"/>
+      <c r="H40" s="75"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="74">
+        <v>7</v>
+      </c>
+      <c r="C41" s="69">
+        <v>8</v>
+      </c>
+      <c r="D41" s="69">
+        <v>10040</v>
+      </c>
+      <c r="E41" s="80">
+        <v>36</v>
+      </c>
+      <c r="F41" s="74">
+        <f t="shared" si="1"/>
+        <v>361.44</v>
+      </c>
+      <c r="G41" s="69"/>
+      <c r="H41" s="75"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="74">
+        <v>8</v>
+      </c>
+      <c r="C42" s="69">
+        <v>8</v>
+      </c>
+      <c r="D42" s="69">
+        <v>8340</v>
+      </c>
+      <c r="E42" s="80">
+        <v>34</v>
+      </c>
+      <c r="F42" s="74">
+        <f t="shared" si="1"/>
+        <v>283.56</v>
+      </c>
+      <c r="G42" s="69"/>
+      <c r="H42" s="75"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="74">
+        <v>9</v>
+      </c>
+      <c r="C43" s="69">
+        <v>8</v>
+      </c>
+      <c r="D43" s="69">
+        <v>2500</v>
+      </c>
+      <c r="E43" s="80">
+        <v>83</v>
+      </c>
+      <c r="F43" s="74">
+        <f t="shared" si="1"/>
+        <v>207.5</v>
+      </c>
+      <c r="G43" s="69"/>
+      <c r="H43" s="75"/>
+    </row>
+    <row r="44" spans="2:8">
+      <c r="B44" s="74">
+        <v>10</v>
+      </c>
+      <c r="C44" s="69">
+        <v>10</v>
+      </c>
+      <c r="D44" s="69">
+        <v>970</v>
+      </c>
+      <c r="E44" s="80">
+        <v>38</v>
+      </c>
+      <c r="F44" s="74"/>
+      <c r="G44" s="69">
+        <f>E44*D44/1000</f>
+        <v>36.86</v>
+      </c>
+      <c r="H44" s="75"/>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="74">
+        <v>11</v>
+      </c>
+      <c r="C45" s="69">
+        <v>8</v>
+      </c>
+      <c r="D45" s="69">
+        <v>1780</v>
+      </c>
+      <c r="E45" s="80">
+        <v>240</v>
+      </c>
+      <c r="F45" s="74">
+        <f t="shared" si="1"/>
+        <v>427.2</v>
+      </c>
+      <c r="G45" s="69"/>
+      <c r="H45" s="75"/>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="74">
+        <v>12</v>
+      </c>
+      <c r="C46" s="69">
+        <v>12</v>
+      </c>
+      <c r="D46" s="69">
+        <v>78000</v>
+      </c>
+      <c r="E46" s="80">
+        <v>4</v>
+      </c>
+      <c r="F46" s="74"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="75">
+        <f>E46*D46/1000</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="74">
+        <v>13</v>
+      </c>
+      <c r="C47" s="69">
+        <v>8</v>
+      </c>
+      <c r="D47" s="69">
+        <v>880</v>
+      </c>
+      <c r="E47" s="80">
+        <v>220</v>
+      </c>
+      <c r="F47" s="74">
+        <f t="shared" si="1"/>
+        <v>193.6</v>
+      </c>
+      <c r="G47" s="69"/>
+      <c r="H47" s="75"/>
+    </row>
+    <row r="48" spans="2:8" ht="15" thickBot="1">
+      <c r="B48" s="76">
+        <v>14</v>
+      </c>
+      <c r="C48" s="77">
+        <v>12</v>
+      </c>
+      <c r="D48" s="77">
+        <v>4200</v>
+      </c>
+      <c r="E48" s="81">
+        <v>8</v>
+      </c>
+      <c r="F48" s="76"/>
+      <c r="G48" s="77"/>
+      <c r="H48" s="78">
+        <f t="shared" ref="H48" si="2">E48*D48/1000</f>
+        <v>33.6</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="C49" s="70"/>
+      <c r="D49" s="70"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="83">
+        <f>SUM(F35:F48)</f>
+        <v>3233.2999999999993</v>
+      </c>
+      <c r="G49" s="70">
+        <f t="shared" ref="G49:H49" si="3">SUM(G35:G48)</f>
+        <v>36.86</v>
+      </c>
+      <c r="H49" s="84">
+        <f t="shared" si="3"/>
+        <v>345.6</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8">
+      <c r="B50" s="69" t="s">
+        <v>196</v>
+      </c>
+      <c r="C50" s="69"/>
+      <c r="D50" s="69"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="74">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="G50" s="69">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="H50" s="75">
+        <v>0.88800000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="15" thickBot="1">
+      <c r="B51" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="C51" s="69"/>
+      <c r="D51" s="69"/>
+      <c r="E51" s="80"/>
+      <c r="F51" s="76">
+        <f>ROUND(F49*F50,0)</f>
+        <v>1277</v>
+      </c>
+      <c r="G51" s="77">
+        <f t="shared" ref="G51:H51" si="4">ROUND(G49*G50,0)</f>
+        <v>23</v>
+      </c>
+      <c r="H51" s="78">
+        <f t="shared" si="4"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8">
+      <c r="B52" s="69"/>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="70"/>
+      <c r="G52" s="70"/>
+      <c r="H52" s="70"/>
+    </row>
+    <row r="58" spans="2:8" ht="57">
+      <c r="B58" s="93" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58">
+        <v>0.68</v>
+      </c>
+      <c r="E58" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8">
+      <c r="B59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D59">
+        <v>242</v>
+      </c>
+      <c r="E59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8">
+      <c r="B60" t="s">
+        <v>204</v>
+      </c>
+      <c r="D60">
+        <v>220</v>
+      </c>
+      <c r="E60" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" t="s">
+        <v>205</v>
+      </c>
+      <c r="D61">
+        <v>1418</v>
+      </c>
+      <c r="E61" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" ht="15">
+      <c r="B63" t="s">
+        <v>206</v>
+      </c>
+      <c r="D63" s="94">
+        <v>1035</v>
+      </c>
+      <c r="E63" t="s">
+        <v>201</v>
+      </c>
+      <c r="F63" t="s">
+        <v>209</v>
+      </c>
+      <c r="G63">
+        <v>1607</v>
+      </c>
+      <c r="H63" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" t="s">
+        <v>207</v>
+      </c>
+      <c r="D64">
+        <v>266</v>
+      </c>
+      <c r="E64" t="s">
+        <v>201</v>
+      </c>
+      <c r="F64" t="s">
+        <v>207</v>
+      </c>
+      <c r="G64">
+        <v>577</v>
+      </c>
+      <c r="H64" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="D65">
+        <v>138</v>
+      </c>
+      <c r="E65" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="D66">
+        <v>173</v>
+      </c>
+      <c r="E66" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="15">
+      <c r="D67" s="94">
+        <f>D64+D65+D66</f>
+        <v>577</v>
+      </c>
+      <c r="E67" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" ht="15">
+      <c r="D69" s="94">
+        <f>D63+D67</f>
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B75" s="94" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C76" s="72" t="s">
+        <v>210</v>
+      </c>
+      <c r="D76" s="72" t="s">
+        <v>211</v>
+      </c>
+      <c r="E76" s="72" t="s">
+        <v>203</v>
+      </c>
+      <c r="F76" s="72" t="s">
+        <v>212</v>
+      </c>
+      <c r="G76" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="H76" s="73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="B77" s="74">
+        <v>1</v>
+      </c>
+      <c r="C77" s="69">
+        <v>18</v>
+      </c>
+      <c r="D77" s="69">
+        <v>9.74</v>
+      </c>
+      <c r="E77" s="69">
+        <v>4</v>
+      </c>
+      <c r="F77" s="69"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="75">
+        <v>39.1</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="74">
+        <v>2</v>
+      </c>
+      <c r="C78" s="69">
+        <v>18</v>
+      </c>
+      <c r="D78" s="69">
+        <v>3.27</v>
+      </c>
+      <c r="E78" s="69">
+        <v>4</v>
+      </c>
+      <c r="F78" s="69"/>
+      <c r="G78" s="69"/>
+      <c r="H78" s="75">
+        <v>13.1</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="74">
+        <v>3</v>
+      </c>
+      <c r="C79" s="69">
+        <v>14</v>
+      </c>
+      <c r="D79" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="E79" s="69">
+        <v>2</v>
+      </c>
+      <c r="F79" s="69"/>
+      <c r="G79" s="69">
+        <v>6.6</v>
+      </c>
+      <c r="H79" s="75"/>
+    </row>
+    <row r="80" spans="2:8">
+      <c r="B80" s="74">
+        <v>4</v>
+      </c>
+      <c r="C80" s="69">
+        <v>14</v>
+      </c>
+      <c r="D80" s="69">
+        <v>3.58</v>
+      </c>
+      <c r="E80" s="69">
+        <v>2</v>
+      </c>
+      <c r="F80" s="69"/>
+      <c r="G80" s="69">
+        <v>7.2</v>
+      </c>
+      <c r="H80" s="75"/>
+    </row>
+    <row r="81" spans="2:8">
+      <c r="B81" s="74">
+        <v>5</v>
+      </c>
+      <c r="C81" s="69">
+        <v>6</v>
+      </c>
+      <c r="D81" s="69">
+        <v>1.3</v>
+      </c>
+      <c r="E81" s="69">
+        <v>17</v>
+      </c>
+      <c r="F81" s="69">
+        <v>22.1</v>
+      </c>
+      <c r="G81" s="69"/>
+      <c r="H81" s="75"/>
+    </row>
+    <row r="82" spans="2:8">
+      <c r="B82" s="74">
+        <v>6</v>
+      </c>
+      <c r="C82" s="69">
+        <v>6</v>
+      </c>
+      <c r="D82" s="69">
+        <v>1.64</v>
+      </c>
+      <c r="E82" s="69">
+        <v>23</v>
+      </c>
+      <c r="F82" s="69">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G82" s="69"/>
+      <c r="H82" s="75"/>
+    </row>
+    <row r="83" spans="2:8">
+      <c r="B83" s="74">
+        <v>7</v>
+      </c>
+      <c r="C83" s="69">
+        <v>18</v>
+      </c>
+      <c r="D83" s="69">
+        <v>7.2</v>
+      </c>
+      <c r="E83" s="69">
+        <v>4</v>
+      </c>
+      <c r="F83" s="69"/>
+      <c r="G83" s="69"/>
+      <c r="H83" s="75">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8">
+      <c r="B84" s="74">
+        <v>8</v>
+      </c>
+      <c r="C84" s="69">
+        <v>14</v>
+      </c>
+      <c r="D84" s="69">
+        <v>6.52</v>
+      </c>
+      <c r="E84" s="69">
+        <v>2</v>
+      </c>
+      <c r="F84" s="69"/>
+      <c r="G84" s="69">
+        <v>13</v>
+      </c>
+      <c r="H84" s="75"/>
+    </row>
+    <row r="85" spans="2:8">
+      <c r="B85" s="74">
+        <v>9</v>
+      </c>
+      <c r="C85" s="69">
+        <v>6</v>
+      </c>
+      <c r="D85" s="69">
+        <v>1.64</v>
+      </c>
+      <c r="E85" s="69">
+        <v>35</v>
+      </c>
+      <c r="F85" s="69">
+        <v>57.4</v>
+      </c>
+      <c r="G85" s="69"/>
+      <c r="H85" s="75"/>
+    </row>
+    <row r="86" spans="2:8">
+      <c r="B86" s="74">
+        <v>10</v>
+      </c>
+      <c r="C86" s="69">
+        <v>14</v>
+      </c>
+      <c r="D86" s="69">
+        <v>5.67</v>
+      </c>
+      <c r="E86" s="69">
+        <v>2</v>
+      </c>
+      <c r="F86" s="69"/>
+      <c r="G86" s="69">
+        <v>11.3</v>
+      </c>
+      <c r="H86" s="75"/>
+    </row>
+    <row r="87" spans="2:8">
+      <c r="B87" s="74">
+        <v>11</v>
+      </c>
+      <c r="C87" s="69">
+        <v>14</v>
+      </c>
+      <c r="D87" s="69">
+        <v>4.63</v>
+      </c>
+      <c r="E87" s="69">
+        <v>4</v>
+      </c>
+      <c r="F87" s="69"/>
+      <c r="G87" s="69">
+        <v>18.5</v>
+      </c>
+      <c r="H87" s="75"/>
+    </row>
+    <row r="88" spans="2:8" ht="15" thickBot="1">
+      <c r="B88" s="76">
+        <v>12</v>
+      </c>
+      <c r="C88" s="77">
+        <v>6</v>
+      </c>
+      <c r="D88" s="77">
+        <v>1.64</v>
+      </c>
+      <c r="E88" s="77">
+        <v>29</v>
+      </c>
+      <c r="F88" s="77">
+        <v>47.6</v>
+      </c>
+      <c r="G88" s="77"/>
+      <c r="H88" s="78"/>
+    </row>
+    <row r="89" spans="2:8">
+      <c r="B89" s="70"/>
+      <c r="C89" s="70"/>
+      <c r="D89" s="70" t="s">
+        <v>215</v>
+      </c>
+      <c r="E89" s="70" t="s">
+        <v>216</v>
+      </c>
+      <c r="F89" s="70">
+        <v>164.8</v>
+      </c>
+      <c r="G89" s="70">
+        <v>56.7</v>
+      </c>
+      <c r="H89" s="70">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="69"/>
+      <c r="C90" s="69"/>
+      <c r="D90" s="69" t="s">
+        <v>217</v>
+      </c>
+      <c r="E90" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="F90" s="69">
+        <v>0.222</v>
+      </c>
+      <c r="G90" s="69">
+        <v>1.208</v>
+      </c>
+      <c r="H90" s="69">
+        <v>1.998</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8">
+      <c r="B91" s="69"/>
+      <c r="C91" s="69"/>
+      <c r="D91" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="E91" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="F91" s="69">
+        <v>36.6</v>
+      </c>
+      <c r="G91" s="69">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H91" s="69">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" ht="15">
+      <c r="B92" s="69"/>
+      <c r="C92" s="69"/>
+      <c r="D92" s="95" t="s">
+        <v>219</v>
+      </c>
+      <c r="E92" s="95" t="s">
+        <v>220</v>
+      </c>
+      <c r="F92" s="69"/>
+      <c r="G92" s="69"/>
+      <c r="H92" s="69"/>
+    </row>
+    <row r="93" spans="2:8">
+      <c r="B93" s="69"/>
+      <c r="C93" s="69"/>
+      <c r="D93" s="69"/>
+      <c r="E93" s="69"/>
+      <c r="F93" s="69"/>
+      <c r="G93" s="69"/>
+      <c r="H93" s="69"/>
+    </row>
+    <row r="94" spans="2:8" ht="15">
+      <c r="B94" s="94" t="s">
+        <v>222</v>
+      </c>
+      <c r="C94" s="69"/>
+      <c r="D94" s="69"/>
+      <c r="E94" s="69"/>
+      <c r="F94" s="69"/>
+      <c r="G94" s="69"/>
+      <c r="H94" s="69"/>
+    </row>
+    <row r="95" spans="2:8">
+      <c r="B95" s="69"/>
+      <c r="C95" s="69"/>
+      <c r="D95" s="69"/>
+      <c r="E95" s="69"/>
+      <c r="F95" s="69"/>
+      <c r="G95" s="69"/>
+      <c r="H95" s="69"/>
+    </row>
+    <row r="96" spans="2:8">
+      <c r="B96" s="69"/>
+      <c r="C96" s="69"/>
+      <c r="D96" s="69"/>
+      <c r="E96" s="69"/>
+      <c r="F96" s="69"/>
+      <c r="G96" s="69"/>
+      <c r="H96" s="69"/>
+    </row>
+    <row r="97" spans="2:8">
+      <c r="B97" s="69"/>
+      <c r="C97" s="69"/>
+      <c r="D97" s="69"/>
+      <c r="E97" s="69"/>
+      <c r="F97" s="69"/>
+      <c r="G97" s="69"/>
+      <c r="H97" s="69"/>
+    </row>
+    <row r="98" spans="2:8">
+      <c r="B98" s="69"/>
+      <c r="C98" s="69"/>
+      <c r="D98" s="69"/>
+      <c r="E98" s="69"/>
+      <c r="F98" s="69"/>
+      <c r="G98" s="69"/>
+      <c r="H98" s="69"/>
+    </row>
+    <row r="99" spans="2:8">
+      <c r="B99" s="69"/>
+      <c r="C99" s="69"/>
+      <c r="D99" s="69"/>
+      <c r="E99" s="69"/>
+      <c r="F99" s="69"/>
+      <c r="G99" s="69"/>
+      <c r="H99" s="69"/>
+    </row>
+    <row r="100" spans="2:8">
+      <c r="B100" s="69"/>
+      <c r="C100" s="69"/>
+      <c r="D100" s="69"/>
+      <c r="E100" s="69"/>
+      <c r="F100" s="69"/>
+      <c r="G100" s="69"/>
+      <c r="H100" s="69"/>
+    </row>
+    <row r="101" spans="2:8">
+      <c r="B101" s="69"/>
+      <c r="C101" s="69"/>
+      <c r="D101" s="69"/>
+      <c r="E101" s="69"/>
+      <c r="F101" s="69"/>
+      <c r="G101" s="69"/>
+      <c r="H101" s="69"/>
+    </row>
+    <row r="102" spans="2:8">
+      <c r="B102" s="69"/>
+      <c r="C102" s="69"/>
+      <c r="D102" s="69"/>
+      <c r="E102" s="69"/>
+      <c r="F102" s="69"/>
+      <c r="G102" s="69"/>
+      <c r="H102" s="69"/>
+    </row>
+    <row r="103" spans="2:8">
+      <c r="B103" s="69"/>
+      <c r="C103" s="69"/>
+      <c r="D103" s="69"/>
+      <c r="E103" s="69"/>
+      <c r="F103" s="69"/>
+      <c r="G103" s="69"/>
+      <c r="H103" s="69"/>
+    </row>
+    <row r="104" spans="2:8">
+      <c r="B104" s="69"/>
+      <c r="C104" s="69"/>
+      <c r="D104" s="69"/>
+      <c r="E104" s="69"/>
+      <c r="F104" s="69"/>
+      <c r="G104" s="69"/>
+      <c r="H104" s="69"/>
+    </row>
+    <row r="105" spans="2:8">
+      <c r="B105" s="69"/>
+      <c r="C105" s="69"/>
+      <c r="D105" s="69"/>
+      <c r="E105" s="69"/>
+      <c r="F105" s="69"/>
+      <c r="G105" s="69"/>
+      <c r="H105" s="69"/>
+    </row>
+    <row r="106" spans="2:8">
+      <c r="B106" s="69"/>
+      <c r="C106" s="69"/>
+      <c r="D106" s="69"/>
+      <c r="E106" s="69"/>
+      <c r="F106" s="69"/>
+      <c r="G106" s="69"/>
+      <c r="H106" s="69"/>
+    </row>
+    <row r="107" spans="2:8">
+      <c r="B107" s="69"/>
+      <c r="C107" s="69"/>
+      <c r="D107" s="69"/>
+      <c r="E107" s="69"/>
+      <c r="F107" s="69"/>
+      <c r="G107" s="69"/>
+      <c r="H107" s="69"/>
+    </row>
+    <row r="108" spans="2:8">
+      <c r="B108" s="69"/>
+      <c r="C108" s="69"/>
+      <c r="D108" s="69"/>
+      <c r="E108" s="69"/>
+      <c r="F108" s="69"/>
+      <c r="G108" s="69"/>
+      <c r="H108" s="69"/>
+    </row>
+    <row r="109" spans="2:8">
+      <c r="B109" s="69"/>
+      <c r="C109" s="69"/>
+      <c r="D109" s="69"/>
+      <c r="E109" s="69"/>
+      <c r="F109" s="69"/>
+      <c r="G109" s="69"/>
+      <c r="H109" s="69"/>
+    </row>
+    <row r="110" spans="2:8">
+      <c r="B110" s="69"/>
+      <c r="C110" s="69"/>
+      <c r="D110" s="69"/>
+      <c r="E110" s="69"/>
+      <c r="F110" s="69"/>
+      <c r="G110" s="69"/>
+      <c r="H110" s="69"/>
+    </row>
+    <row r="111" spans="2:8">
+      <c r="B111" s="69"/>
+      <c r="C111" s="69"/>
+      <c r="D111" s="69"/>
+      <c r="E111" s="69"/>
+      <c r="F111" s="69"/>
+      <c r="G111" s="69"/>
+      <c r="H111" s="69"/>
+    </row>
+    <row r="112" spans="2:8">
+      <c r="B112" s="69"/>
+      <c r="C112" s="69"/>
+      <c r="D112" s="69"/>
+      <c r="E112" s="69"/>
+      <c r="F112" s="69"/>
+      <c r="G112" s="69"/>
+      <c r="H112" s="69"/>
+    </row>
+    <row r="113" spans="2:8">
+      <c r="B113" s="69"/>
+      <c r="C113" s="69"/>
+      <c r="D113" s="69"/>
+      <c r="E113" s="69"/>
+      <c r="F113" s="69"/>
+      <c r="G113" s="69"/>
+      <c r="H113" s="69"/>
+    </row>
+    <row r="114" spans="2:8">
+      <c r="B114" s="69"/>
+      <c r="C114" s="69"/>
+      <c r="D114" s="69"/>
+      <c r="E114" s="69"/>
+      <c r="F114" s="69"/>
+      <c r="G114" s="69"/>
+      <c r="H114" s="69"/>
+    </row>
+    <row r="115" spans="2:8">
+      <c r="B115" s="69"/>
+      <c r="C115" s="69"/>
+      <c r="D115" s="69"/>
+      <c r="E115" s="69"/>
+      <c r="F115" s="69"/>
+      <c r="G115" s="69"/>
+      <c r="H115" s="69"/>
+    </row>
+    <row r="116" spans="2:8">
+      <c r="B116" s="69"/>
+      <c r="C116" s="69"/>
+      <c r="D116" s="69"/>
+      <c r="E116" s="69"/>
+      <c r="F116" s="69"/>
+      <c r="G116" s="69"/>
+      <c r="H116" s="69"/>
+    </row>
+    <row r="117" spans="2:8">
+      <c r="B117" s="69"/>
+      <c r="C117" s="69"/>
+      <c r="D117" s="69"/>
+      <c r="E117" s="69"/>
+      <c r="F117" s="69"/>
+      <c r="G117" s="69"/>
+      <c r="H117" s="69"/>
+    </row>
+    <row r="118" spans="2:8">
+      <c r="B118" s="69"/>
+      <c r="C118" s="69"/>
+      <c r="D118" s="69"/>
+      <c r="E118" s="69"/>
+      <c r="F118" s="69"/>
+      <c r="G118" s="69"/>
+      <c r="H118" s="69"/>
+    </row>
+    <row r="119" spans="2:8">
+      <c r="B119" s="69"/>
+      <c r="C119" s="69"/>
+      <c r="D119" s="69"/>
+      <c r="E119" s="69"/>
+      <c r="F119" s="69"/>
+      <c r="G119" s="69"/>
+      <c r="H119" s="69"/>
+    </row>
+    <row r="120" spans="2:8">
+      <c r="B120" s="69"/>
+      <c r="C120" s="69"/>
+      <c r="D120" s="69"/>
+      <c r="E120" s="69"/>
+      <c r="F120" s="69"/>
+      <c r="G120" s="69"/>
+      <c r="H120" s="69"/>
+    </row>
+    <row r="121" spans="2:8">
+      <c r="B121" s="69"/>
+      <c r="C121" s="69"/>
+      <c r="D121" s="69"/>
+      <c r="E121" s="69"/>
+      <c r="F121" s="69"/>
+      <c r="G121" s="69"/>
+      <c r="H121" s="69"/>
+    </row>
+    <row r="135" spans="2:10">
+      <c r="B135" t="s">
+        <v>247</v>
+      </c>
+      <c r="C135" t="s">
+        <v>248</v>
+      </c>
+      <c r="D135" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="136" spans="2:10" ht="30" customHeight="1">
+      <c r="B136" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="C136" s="69"/>
+      <c r="D136" s="69"/>
+    </row>
+    <row r="137" spans="2:10" ht="30" customHeight="1">
+      <c r="B137" s="96" t="s">
+        <v>223</v>
+      </c>
+      <c r="C137" s="96" t="s">
+        <v>225</v>
+      </c>
+      <c r="D137" s="96"/>
+      <c r="J137" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="138" spans="2:10" ht="30" customHeight="1">
+      <c r="B138" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="C138" s="96" t="s">
+        <v>251</v>
+      </c>
+      <c r="D138" s="96"/>
+    </row>
+    <row r="139" spans="2:10" ht="30" customHeight="1">
+      <c r="B139" s="96" t="s">
+        <v>226</v>
+      </c>
+      <c r="C139" s="96" t="s">
+        <v>239</v>
+      </c>
+      <c r="D139" s="96"/>
+    </row>
+    <row r="140" spans="2:10" ht="30" customHeight="1">
+      <c r="B140" s="96" t="s">
+        <v>227</v>
+      </c>
+      <c r="C140" s="96" t="s">
+        <v>240</v>
+      </c>
+      <c r="D140" s="96"/>
+    </row>
+    <row r="141" spans="2:10" ht="30" customHeight="1">
+      <c r="B141" s="96" t="s">
+        <v>228</v>
+      </c>
+      <c r="C141" s="96" t="s">
+        <v>229</v>
+      </c>
+      <c r="D141" s="96"/>
+    </row>
+    <row r="142" spans="2:10" ht="5.25" customHeight="1">
+      <c r="B142" s="96"/>
+      <c r="C142" s="96"/>
+      <c r="D142" s="96"/>
+    </row>
+    <row r="143" spans="2:10" ht="30" customHeight="1">
+      <c r="B143" s="96" t="s">
+        <v>230</v>
+      </c>
+      <c r="C143" s="96" t="s">
+        <v>231</v>
+      </c>
+      <c r="D143" s="96"/>
+    </row>
+    <row r="144" spans="2:10" ht="30" customHeight="1">
+      <c r="B144" s="96" t="s">
+        <v>228</v>
+      </c>
+      <c r="C144" s="96" t="s">
+        <v>232</v>
+      </c>
+      <c r="D144" s="96"/>
+    </row>
+    <row r="145" spans="2:4" ht="30" customHeight="1">
+      <c r="B145" s="96" t="s">
+        <v>228</v>
+      </c>
+      <c r="C145" s="96" t="s">
+        <v>238</v>
+      </c>
+      <c r="D145" s="96"/>
+    </row>
+    <row r="146" spans="2:4" ht="30" customHeight="1">
+      <c r="B146" s="96" t="s">
+        <v>242</v>
+      </c>
+      <c r="C146" s="96" t="s">
+        <v>243</v>
+      </c>
+      <c r="D146" s="96"/>
+    </row>
+    <row r="147" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B147" s="96"/>
+      <c r="C147" s="96"/>
+      <c r="D147" s="96"/>
+    </row>
+    <row r="148" spans="2:4" ht="30" customHeight="1">
+      <c r="B148" s="96" t="s">
+        <v>233</v>
+      </c>
+      <c r="C148" s="96" t="s">
+        <v>246</v>
+      </c>
+      <c r="D148" s="96"/>
+    </row>
+    <row r="149" spans="2:4" ht="30" customHeight="1">
+      <c r="B149" s="96" t="s">
+        <v>234</v>
+      </c>
+      <c r="C149" s="96" t="s">
+        <v>235</v>
+      </c>
+      <c r="D149" s="96"/>
+    </row>
+    <row r="150" spans="2:4" ht="30" customHeight="1">
+      <c r="B150" s="96" t="s">
+        <v>236</v>
+      </c>
+      <c r="C150" s="96" t="s">
+        <v>237</v>
+      </c>
+      <c r="D150" s="96"/>
+    </row>
+    <row r="151" spans="2:4" ht="4.5" customHeight="1">
+      <c r="B151" s="96"/>
+      <c r="C151" s="96"/>
+      <c r="D151" s="96"/>
+    </row>
+    <row r="152" spans="2:4" ht="30" customHeight="1">
+      <c r="B152" s="97" t="s">
+        <v>244</v>
+      </c>
+      <c r="C152" s="97" t="s">
+        <v>245</v>
+      </c>
+      <c r="D152" s="97"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H23" r:id="rId1"/>
+    <hyperlink ref="D24" r:id="rId2"/>
+    <hyperlink ref="D25" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="103">
+        <v>41442</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>278</v>
+      </c>
+      <c r="D5" s="103">
+        <v>41426</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D6" s="103">
+        <v>41425</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4">
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="103">
+        <v>41427</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4">
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D8" s="103">
+        <v>41428</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4">
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4">
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4">
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update baclog, za i przeciw budowie w czerwcu
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -13,7 +13,7 @@
     <sheet name="03_Sprint" sheetId="4" r:id="rId4"/>
     <sheet name="04_Sprint" sheetId="5" r:id="rId5"/>
     <sheet name="05_Sprint" sheetId="6" r:id="rId6"/>
-    <sheet name="Notatki5" sheetId="7" r:id="rId7"/>
+    <sheet name="Piasek i stal" sheetId="7" r:id="rId7"/>
     <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="293">
   <si>
     <t>Id</t>
   </si>
@@ -621,42 +621,12 @@
 stało [h]</t>
   </si>
   <si>
-    <t>Pospółka i kliniec - Wrocław</t>
-  </si>
-  <si>
-    <t>http://allegro.pl/piasek-rzeczny-piach-pospolka-wroclaw-i3065577322.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Zakład Przetwórstwa Kruszyw MARGO</t>
-  </si>
-  <si>
-    <t>http://www.kruszywa-margo.pl/</t>
-  </si>
-  <si>
-    <t>Mietków</t>
-  </si>
-  <si>
-    <t>698-942-703</t>
-  </si>
-  <si>
-    <t>http://wroclaw.olx.pl/wroclaw-piaskownia-zwirownia-piasek-zwir-pospolka-zwir-drenazowy-transport-wywrotka-iid-318919317</t>
-  </si>
-  <si>
     <t>http://www.jft.com.pl/materialy-budowlane.htm</t>
   </si>
   <si>
-    <t>Wrocław, Wędkarzy</t>
-  </si>
-  <si>
-    <t>Wrocław, ?</t>
-  </si>
-  <si>
     <t>http://www.hydrokrusz.pl/kruszywa/cennik.html</t>
   </si>
   <si>
-    <t>Wrocław, Centrun</t>
-  </si>
-  <si>
     <t>71 343 22 55</t>
   </si>
   <si>
@@ -813,9 +783,6 @@
     <t>Kiedy po rozpoczęciu robót potrzebne jest dostarczenie pospółki</t>
   </si>
   <si>
-    <t>Geodeta - kiedy</t>
-  </si>
-  <si>
     <t>Beton i Stal</t>
   </si>
   <si>
@@ -949,6 +916,57 @@
   </si>
   <si>
     <t>Czy wykonane</t>
+  </si>
+  <si>
+    <t>Kontakt</t>
+  </si>
+  <si>
+    <t>Zestawienie stali na płytę</t>
+  </si>
+  <si>
+    <t>Zestawienie stali z projektu Mati</t>
+  </si>
+  <si>
+    <t>Gotowość do pracy Wykonawcy</t>
+  </si>
+  <si>
+    <t>Wykorzystanie dobrej pogody</t>
+  </si>
+  <si>
+    <t>Szybszy koniec budowy</t>
+  </si>
+  <si>
+    <t>Większa szansa na zakończenie stanu zamkniętego przed zimą.</t>
+  </si>
+  <si>
+    <t>Brak spełnionych warunków uruchomienia kredytu</t>
+  </si>
+  <si>
+    <t>Niekorzystne warunki refinansowania kredytu na działkę.</t>
+  </si>
+  <si>
+    <t>Kurs euro dużo wyższy niż zakładany w kwocie refinansowania (koniecznośc dopłaty)</t>
+  </si>
+  <si>
+    <t>Mamy środki jedynie na ok. 10 dni pracy Wykonawcy</t>
+  </si>
+  <si>
+    <t>Mniejsze opcje uniknięcia spreadu walutowego.</t>
+  </si>
+  <si>
+    <t>Zmiany w umowie</t>
+  </si>
+  <si>
+    <t>Umowa z EB</t>
+  </si>
+  <si>
+    <t>DLA NOWAKA</t>
+  </si>
+  <si>
+    <t>Wakacje Dorotki do 25.VI</t>
+  </si>
+  <si>
+    <t>Niepewna sytuacja prawna Marcina (do 19.VI)</t>
   </si>
 </sst>
 </file>
@@ -1053,14 +1071,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Czcionka tekstu podstawowego"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,6 +1092,10 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1417,14 +1431,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1549,9 +1559,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
@@ -1582,11 +1589,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1596,7 +1600,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1605,13 +1609,35 @@
     <xf numFmtId="2" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="84">
@@ -3814,7 +3840,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.7144142607174061"/>
+          <c:w val="0.71441426071740588"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4094,24 +4120,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63275776"/>
-        <c:axId val="63277312"/>
+        <c:axId val="63279872"/>
+        <c:axId val="63281408"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63275776"/>
+        <c:axId val="63279872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63277312"/>
+        <c:crossAx val="63281408"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63277312"/>
+        <c:axId val="63281408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -4121,7 +4147,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63275776"/>
+        <c:crossAx val="63279872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4132,8 +4158,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288497"/>
-          <c:y val="0.29353966170895535"/>
+          <c:x val="0.86438523325288541"/>
+          <c:y val="0.29353966170895546"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -4143,7 +4169,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000444" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000444" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4355,24 +4381,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63302656"/>
-        <c:axId val="63054592"/>
+        <c:axId val="63306752"/>
+        <c:axId val="64172800"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63302656"/>
+        <c:axId val="63306752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63054592"/>
+        <c:crossAx val="64172800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63054592"/>
+        <c:axId val="64172800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -4382,7 +4408,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63302656"/>
+        <c:crossAx val="63306752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4394,7 +4420,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4557,24 +4583,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64194048"/>
-        <c:axId val="64195584"/>
+        <c:axId val="63415808"/>
+        <c:axId val="63417344"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64194048"/>
+        <c:axId val="63415808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64195584"/>
+        <c:crossAx val="63417344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64195584"/>
+        <c:axId val="63417344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -4584,7 +4610,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64194048"/>
+        <c:crossAx val="63415808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4596,7 +4622,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4711,11 +4737,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64277120"/>
-        <c:axId val="64278912"/>
+        <c:axId val="64543360"/>
+        <c:axId val="64545152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64277120"/>
+        <c:axId val="64543360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4723,13 +4749,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64278912"/>
+        <c:crossAx val="64545152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64278912"/>
+        <c:axId val="64545152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4737,7 +4763,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64277120"/>
+        <c:crossAx val="64543360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4749,7 +4775,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4765,10 +4791,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961897"/>
-          <c:y val="3.2882035578886033E-2"/>
+          <c:x val="0.17181562830961888"/>
+          <c:y val="3.2882035578886047E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420079"/>
+          <c:h val="0.63861876640420101"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -4778,10 +4804,10 @@
           <c:order val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'05_Sprint'!$A$33:$A$46</c:f>
+              <c:f>'05_Sprint'!$A$33:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>yyyy/mm/dd</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>41407</c:v>
                 </c:pt>
@@ -4823,16 +4849,46 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>41420</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>41421</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41422</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>41423</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41424</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>41425</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>41426</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>41427</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>41428</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>41429</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>41430</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'05_Sprint'!$B$33:$B$46</c:f>
+              <c:f>'05_Sprint'!$B$33:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="24"/>
                 <c:pt idx="0">
                   <c:v>31</c:v>
                 </c:pt>
@@ -4859,17 +4915,53 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64368640"/>
-        <c:axId val="64370176"/>
+        <c:axId val="64631552"/>
+        <c:axId val="64633088"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64368640"/>
+        <c:axId val="64631552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4877,13 +4969,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64370176"/>
+        <c:crossAx val="64633088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64370176"/>
+        <c:axId val="64633088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -4892,7 +4984,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64368640"/>
+        <c:crossAx val="64631552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4904,7 +4996,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5180,8 +5272,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B135:D152" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B135:D152"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B116:D133" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B116:D133"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Temat" dataDxfId="2"/>
     <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
@@ -8806,8 +8898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -8864,74 +8956,74 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="42">
+      <c r="A6" s="82">
         <v>1</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="43">
+      <c r="B6" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="87"/>
+      <c r="D6" s="85">
         <v>0.5</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="85">
+        <v>0</v>
+      </c>
+      <c r="F6" s="86" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="82">
+        <v>2</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="87"/>
+      <c r="D7" s="85">
         <v>0.5</v>
       </c>
-      <c r="F6" s="45" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="42">
+      <c r="E7" s="85">
+        <v>0</v>
+      </c>
+      <c r="F7" s="86" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="82">
+        <v>3</v>
+      </c>
+      <c r="B8" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="87"/>
+      <c r="D8" s="85">
         <v>2</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="43">
+      <c r="E8" s="85">
+        <v>0</v>
+      </c>
+      <c r="F8" s="86" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="82">
+        <v>4</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="87"/>
+      <c r="D9" s="85">
         <v>0.5</v>
       </c>
-      <c r="E7" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="F7" s="45" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="42">
-        <v>3</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="43">
-        <v>2</v>
-      </c>
-      <c r="E8" s="43">
-        <v>2</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" s="85">
-        <v>4</v>
-      </c>
-      <c r="B9" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="88">
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="88">
+      <c r="E9" s="85">
         <v>0</v>
       </c>
-      <c r="F9" s="89" t="s">
+      <c r="F9" s="86" t="s">
         <v>152</v>
       </c>
       <c r="H9" s="1" t="s">
@@ -8939,20 +9031,20 @@
       </c>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="85">
+      <c r="A10" s="82">
         <v>5</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="87"/>
-      <c r="D10" s="88">
+      <c r="C10" s="84"/>
+      <c r="D10" s="85">
         <v>0.5</v>
       </c>
-      <c r="E10" s="88">
+      <c r="E10" s="85">
         <v>0</v>
       </c>
-      <c r="F10" s="89" t="s">
+      <c r="F10" s="86" t="s">
         <v>153</v>
       </c>
       <c r="H10" s="1" t="s">
@@ -9001,94 +9093,94 @@
       </c>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="42">
+      <c r="A13" s="82">
         <v>8</v>
       </c>
-      <c r="B13" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="43">
+      <c r="B13" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="84"/>
+      <c r="D13" s="85">
         <v>1</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="85">
+        <v>0</v>
+      </c>
+      <c r="F13" s="86" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="82">
+        <v>9</v>
+      </c>
+      <c r="B14" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="84"/>
+      <c r="D14" s="85">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="85">
+        <v>0</v>
+      </c>
+      <c r="F14" s="86" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="82">
+        <v>10</v>
+      </c>
+      <c r="B15" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="D15" s="88">
+        <v>2</v>
+      </c>
+      <c r="E15" s="88">
+        <v>0</v>
+      </c>
+      <c r="F15" s="89" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="82">
+        <v>11</v>
+      </c>
+      <c r="B16" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="87"/>
+      <c r="D16" s="88">
+        <v>2</v>
+      </c>
+      <c r="E16" s="88">
+        <v>0</v>
+      </c>
+      <c r="F16" s="89" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="82">
+        <v>12</v>
+      </c>
+      <c r="B17" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="87"/>
+      <c r="D17" s="88">
         <v>1</v>
       </c>
-      <c r="F13" s="48" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="42">
-        <v>9</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="E14" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="48" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="85">
-        <v>10</v>
-      </c>
-      <c r="B15" s="86" t="s">
-        <v>71</v>
-      </c>
-      <c r="C15" s="90" t="s">
-        <v>174</v>
-      </c>
-      <c r="D15" s="91">
-        <v>2</v>
-      </c>
-      <c r="E15" s="91">
+      <c r="E17" s="88">
         <v>0</v>
       </c>
-      <c r="F15" s="92" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="42">
-        <v>11</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="47">
-        <v>2</v>
-      </c>
-      <c r="E16" s="47">
-        <v>2</v>
-      </c>
-      <c r="F16" s="48" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="42">
-        <v>12</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47">
-        <v>1</v>
-      </c>
-      <c r="E17" s="47">
-        <v>1</v>
-      </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="89" t="s">
         <v>158</v>
       </c>
     </row>
@@ -9129,20 +9221,20 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="42">
+      <c r="A20" s="82">
         <v>15</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="47">
+      <c r="B20" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" s="87"/>
+      <c r="D20" s="88">
         <v>1</v>
       </c>
-      <c r="E20" s="47">
-        <v>1</v>
-      </c>
-      <c r="F20" s="48" t="s">
+      <c r="E20" s="88">
+        <v>0</v>
+      </c>
+      <c r="F20" s="89" t="s">
         <v>161</v>
       </c>
     </row>
@@ -9158,49 +9250,49 @@
         <v>5</v>
       </c>
       <c r="E21" s="47">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F21" s="48" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="42">
+      <c r="A22" s="82">
         <v>17</v>
       </c>
-      <c r="B22" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="46" t="s">
+      <c r="B22" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="87" t="s">
         <v>73</v>
       </c>
-      <c r="D22" s="47">
+      <c r="D22" s="88">
         <v>1</v>
       </c>
-      <c r="E22" s="47">
-        <v>1</v>
-      </c>
-      <c r="F22" s="48" t="s">
+      <c r="E22" s="88">
+        <v>0</v>
+      </c>
+      <c r="F22" s="89" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="85">
+      <c r="A23" s="82">
         <v>18</v>
       </c>
-      <c r="B23" s="86" t="s">
+      <c r="B23" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="90" t="s">
+      <c r="C23" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="D23" s="91">
+      <c r="D23" s="88">
         <v>2</v>
       </c>
-      <c r="E23" s="91">
+      <c r="E23" s="88">
         <v>0</v>
       </c>
-      <c r="F23" s="92" t="s">
+      <c r="F23" s="89" t="s">
         <v>164</v>
       </c>
     </row>
@@ -9259,76 +9351,76 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="42">
+      <c r="A27" s="82">
         <v>22</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C27" s="46" t="s">
+      <c r="B27" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="87" t="s">
         <v>174</v>
       </c>
-      <c r="D27" s="47">
+      <c r="D27" s="88">
         <v>2</v>
       </c>
-      <c r="E27" s="47">
+      <c r="E27" s="88">
+        <v>0</v>
+      </c>
+      <c r="F27" s="89" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="82">
+        <v>23</v>
+      </c>
+      <c r="B28" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="87"/>
+      <c r="D28" s="88">
         <v>2</v>
       </c>
-      <c r="F27" s="48" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
-      <c r="A28" s="42">
-        <v>23</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="47">
-        <v>2</v>
-      </c>
-      <c r="E28" s="47">
-        <v>2</v>
-      </c>
-      <c r="F28" s="48" t="s">
+      <c r="E28" s="88">
+        <v>0</v>
+      </c>
+      <c r="F28" s="89" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="42">
+      <c r="A29" s="82">
         <v>24</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C29" s="46"/>
-      <c r="D29" s="47">
+      <c r="B29" s="83" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="87"/>
+      <c r="D29" s="88">
         <v>1</v>
       </c>
-      <c r="E29" s="47">
-        <v>1</v>
-      </c>
-      <c r="F29" s="48" t="s">
+      <c r="E29" s="88">
+        <v>0</v>
+      </c>
+      <c r="F29" s="89" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="49"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="46"/>
-      <c r="D30" s="47">
+      <c r="A30" s="100"/>
+      <c r="B30" s="101"/>
+      <c r="C30" s="102"/>
+      <c r="D30" s="101">
         <f>SUBTOTAL(109,[Rozmiar 
 początkowy '[h']])</f>
         <v>31</v>
       </c>
-      <c r="E30" s="46">
+      <c r="E30" s="102">
         <f>SUBTOTAL(109,[Pozo-
 stało '[h']])</f>
-        <v>26</v>
-      </c>
-      <c r="F30" s="48"/>
+        <v>7.5</v>
+      </c>
+      <c r="F30" s="103"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="61"/>
@@ -9422,62 +9514,114 @@
       <c r="A42" s="28">
         <v>41416</v>
       </c>
-      <c r="B42" s="29"/>
+      <c r="B42" s="29">
+        <v>22</v>
+      </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" s="28">
         <v>41417</v>
       </c>
-      <c r="B43" s="29"/>
+      <c r="B43" s="29">
+        <v>21</v>
+      </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" s="28">
         <v>41418</v>
       </c>
-      <c r="B44" s="29"/>
+      <c r="B44" s="29">
+        <v>19</v>
+      </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" s="28">
         <v>41419</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="29">
+        <v>16</v>
+      </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="28">
         <v>41420</v>
       </c>
+      <c r="B46" s="29">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:2">
-      <c r="A47" s="28"/>
+      <c r="A47" s="28">
+        <v>41421</v>
+      </c>
+      <c r="B47" s="29">
+        <v>14</v>
+      </c>
     </row>
     <row r="48" spans="1:2">
-      <c r="A48" s="28"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="28"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="28"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="28"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="28"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="28"/>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="28"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="28"/>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="28"/>
-    </row>
-    <row r="57" spans="1:1">
+      <c r="A48" s="28">
+        <v>41422</v>
+      </c>
+      <c r="B48" s="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="28">
+        <v>41423</v>
+      </c>
+      <c r="B49" s="29">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="28">
+        <v>41424</v>
+      </c>
+      <c r="B50" s="29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="28">
+        <v>41425</v>
+      </c>
+      <c r="B51" s="29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="28">
+        <v>41426</v>
+      </c>
+      <c r="B52" s="29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="28">
+        <v>41427</v>
+      </c>
+      <c r="B53" s="29">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="28">
+        <v>41428</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="28">
+        <v>41429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="28">
+        <v>41430</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" s="28"/>
     </row>
   </sheetData>
@@ -9497,10 +9641,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L152"/>
+  <dimension ref="A1:K133"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9512,1721 +9656,1702 @@
     <col min="6" max="6" width="11.109375" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="98"/>
-      <c r="B1" s="98"/>
-      <c r="C1" s="98"/>
-      <c r="D1" s="98"/>
-      <c r="E1" s="98"/>
-      <c r="F1" s="98"/>
-      <c r="G1" s="98"/>
-      <c r="H1" s="98"/>
-      <c r="I1" s="98"/>
-      <c r="J1" s="98"/>
-      <c r="K1" s="98"/>
+      <c r="A1" s="94"/>
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
     </row>
     <row r="2" spans="1:11" ht="21" customHeight="1">
-      <c r="A2" s="98"/>
-      <c r="B2" s="99" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" s="99" t="s">
-        <v>253</v>
-      </c>
-      <c r="D2" s="99" t="s">
-        <v>254</v>
-      </c>
-      <c r="E2" s="99" t="s">
-        <v>255</v>
-      </c>
-      <c r="F2" s="99" t="s">
-        <v>256</v>
-      </c>
-      <c r="G2" s="99" t="s">
-        <v>268</v>
-      </c>
-      <c r="H2" s="99" t="s">
-        <v>258</v>
-      </c>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
+      <c r="A2" s="94"/>
+      <c r="B2" s="95" t="s">
+        <v>241</v>
+      </c>
+      <c r="C2" s="95" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="95" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" s="95" t="s">
+        <v>244</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>245</v>
+      </c>
+      <c r="G2" s="95" t="s">
+        <v>257</v>
+      </c>
+      <c r="H2" s="95" t="s">
+        <v>247</v>
+      </c>
+      <c r="I2" s="95" t="s">
+        <v>276</v>
+      </c>
+      <c r="J2" s="94"/>
+      <c r="K2" s="94"/>
     </row>
     <row r="3" spans="1:11" ht="32.25">
-      <c r="A3" s="98"/>
-      <c r="B3" s="100" t="s">
-        <v>257</v>
-      </c>
-      <c r="C3" s="100" t="s">
-        <v>259</v>
-      </c>
-      <c r="D3" s="101">
+      <c r="A3" s="94"/>
+      <c r="B3" s="104" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="104" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" s="105">
         <v>2499</v>
       </c>
-      <c r="E3" s="100" t="s">
-        <v>260</v>
-      </c>
-      <c r="F3" s="101">
+      <c r="E3" s="104" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="105">
         <v>3740</v>
       </c>
-      <c r="G3" s="102">
+      <c r="G3" s="106">
         <f>F3+D3</f>
         <v>6239</v>
       </c>
-      <c r="H3" s="100" t="s">
-        <v>184</v>
-      </c>
-      <c r="I3" s="98"/>
-      <c r="J3" s="98"/>
-      <c r="K3" s="98"/>
+      <c r="H3" s="104" t="s">
+        <v>177</v>
+      </c>
+      <c r="I3" s="104">
+        <v>600939523</v>
+      </c>
+      <c r="J3" s="94"/>
+      <c r="K3" s="94"/>
     </row>
     <row r="4" spans="1:11" ht="21.75">
-      <c r="A4" s="98"/>
-      <c r="B4" s="100" t="s">
-        <v>262</v>
-      </c>
-      <c r="C4" s="100" t="s">
-        <v>263</v>
-      </c>
-      <c r="D4" s="101">
+      <c r="A4" s="94"/>
+      <c r="B4" s="96" t="s">
+        <v>251</v>
+      </c>
+      <c r="C4" s="96" t="s">
+        <v>252</v>
+      </c>
+      <c r="D4" s="97">
         <v>3900</v>
       </c>
-      <c r="E4" s="100" t="s">
-        <v>264</v>
-      </c>
-      <c r="F4" s="101">
+      <c r="E4" s="96" t="s">
+        <v>253</v>
+      </c>
+      <c r="F4" s="97">
         <v>13000</v>
       </c>
-      <c r="G4" s="102">
+      <c r="G4" s="98">
         <f t="shared" ref="G4:G5" si="0">F4+D4</f>
         <v>16900</v>
       </c>
-      <c r="H4" s="100" t="s">
-        <v>261</v>
-      </c>
-      <c r="I4" s="98"/>
-      <c r="J4" s="98"/>
-      <c r="K4" s="98"/>
+      <c r="H4" s="96" t="s">
+        <v>250</v>
+      </c>
+      <c r="I4" s="96">
+        <v>713169022</v>
+      </c>
+      <c r="J4" s="94"/>
+      <c r="K4" s="94"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="98"/>
-      <c r="B5" s="100" t="s">
-        <v>265</v>
-      </c>
-      <c r="C5" s="100" t="s">
-        <v>266</v>
-      </c>
-      <c r="D5" s="101">
+      <c r="A5" s="94"/>
+      <c r="B5" s="96" t="s">
+        <v>254</v>
+      </c>
+      <c r="C5" s="96" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="97">
         <v>2550</v>
       </c>
-      <c r="E5" s="100" t="s">
-        <v>267</v>
-      </c>
-      <c r="F5" s="101">
+      <c r="E5" s="96" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="97">
         <v>3960</v>
       </c>
-      <c r="G5" s="102">
+      <c r="G5" s="98">
         <f t="shared" si="0"/>
         <v>6510</v>
       </c>
-      <c r="H5" s="100"/>
-      <c r="I5" s="98"/>
-      <c r="J5" s="98"/>
-      <c r="K5" s="98"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96">
+        <v>508870624</v>
+      </c>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
     </row>
     <row r="6" spans="1:11" ht="32.25">
-      <c r="A6" s="98"/>
-      <c r="B6" s="100" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" s="100" t="s">
-        <v>271</v>
-      </c>
-      <c r="D6" s="101" t="s">
-        <v>270</v>
-      </c>
-      <c r="E6" s="100" t="s">
-        <v>273</v>
-      </c>
-      <c r="F6" s="101" t="s">
-        <v>272</v>
-      </c>
-      <c r="G6" s="102">
+      <c r="A6" s="94"/>
+      <c r="B6" s="96" t="s">
+        <v>258</v>
+      </c>
+      <c r="C6" s="96" t="s">
+        <v>260</v>
+      </c>
+      <c r="D6" s="97" t="s">
+        <v>259</v>
+      </c>
+      <c r="E6" s="96" t="s">
+        <v>262</v>
+      </c>
+      <c r="F6" s="97" t="s">
+        <v>261</v>
+      </c>
+      <c r="G6" s="98">
         <v>6553</v>
       </c>
-      <c r="H6" s="100" t="s">
-        <v>187</v>
-      </c>
-      <c r="I6" s="98"/>
-      <c r="J6" s="98"/>
-      <c r="K6" s="98"/>
+      <c r="H6" s="96" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="96" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="94"/>
+      <c r="K6" s="94"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="98"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="98"/>
-      <c r="H7" s="98"/>
-      <c r="I7" s="98"/>
-      <c r="J7" s="98"/>
-      <c r="K7" s="98"/>
+      <c r="A7" s="94"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="94"/>
+      <c r="J7" s="94"/>
+      <c r="K7" s="94"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="98"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="98"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="98"/>
-      <c r="D9" s="98"/>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98"/>
-      <c r="H9" s="98"/>
-      <c r="I9" s="98"/>
-      <c r="J9" s="98"/>
-      <c r="K9" s="98"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="98"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="98"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="98"/>
-      <c r="I10" s="98"/>
-      <c r="J10" s="98"/>
-      <c r="K10" s="98"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="98"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
-      <c r="I11" s="98"/>
-      <c r="J11" s="98"/>
-      <c r="K11" s="98"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="98"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="98"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="98"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="94"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="94"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="94"/>
+      <c r="J8" s="94"/>
+      <c r="K8" s="94"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="98"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98"/>
-      <c r="H13" s="98"/>
-      <c r="I13" s="98"/>
-      <c r="J13" s="98"/>
-      <c r="K13" s="98"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="98"/>
-      <c r="B14" s="98"/>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98"/>
-      <c r="H14" s="98"/>
-      <c r="I14" s="98"/>
-      <c r="J14" s="98"/>
-      <c r="K14" s="98"/>
-    </row>
+      <c r="B13" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1"/>
     <row r="15" spans="1:11">
-      <c r="A15" s="98"/>
-      <c r="B15" s="98"/>
-      <c r="C15" s="98"/>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98"/>
-      <c r="H15" s="98"/>
-      <c r="I15" s="98"/>
-      <c r="J15" s="98"/>
-      <c r="K15" s="98"/>
-    </row>
-    <row r="21" spans="2:12">
-      <c r="B21" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12">
-      <c r="B22">
-        <v>602632659</v>
-      </c>
-      <c r="C22" t="s">
-        <v>186</v>
-      </c>
-      <c r="D22" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12">
-      <c r="B23">
-        <v>713169022</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B15" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="C15" s="69" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="D23" s="67" t="s">
-        <v>179</v>
-      </c>
-      <c r="H23" s="66" t="s">
-        <v>180</v>
-      </c>
-      <c r="L23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="2:12">
-      <c r="B24" t="s">
+      <c r="E15" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="C24" t="s">
-        <v>186</v>
-      </c>
-      <c r="D24" s="66" t="s">
+      <c r="F15" s="68" t="s">
+        <v>185</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>184</v>
+      </c>
+      <c r="H15" s="70" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="2:12">
-      <c r="B25" s="68">
-        <v>600939523</v>
-      </c>
-      <c r="C25" t="s">
-        <v>185</v>
-      </c>
-      <c r="D25" s="66" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="26" spans="2:12">
-      <c r="B26" t="s">
-        <v>189</v>
-      </c>
-      <c r="C26" t="s">
-        <v>188</v>
-      </c>
-      <c r="D26" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="15" thickBot="1"/>
-    <row r="34" spans="2:8">
-      <c r="B34" s="71" t="s">
-        <v>199</v>
-      </c>
-      <c r="C34" s="72" t="s">
-        <v>190</v>
-      </c>
-      <c r="D34" s="72" t="s">
-        <v>191</v>
-      </c>
-      <c r="E34" s="79" t="s">
-        <v>192</v>
-      </c>
-      <c r="F34" s="71" t="s">
-        <v>195</v>
-      </c>
-      <c r="G34" s="72" t="s">
-        <v>194</v>
-      </c>
-      <c r="H34" s="73" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8">
-      <c r="B35" s="74">
+    <row r="16" spans="1:11">
+      <c r="B16" s="71">
         <v>1</v>
       </c>
-      <c r="C35" s="69">
+      <c r="C16" s="66">
         <v>8</v>
       </c>
-      <c r="D35" s="69">
+      <c r="D16" s="66">
         <v>9640</v>
       </c>
-      <c r="E35" s="80">
+      <c r="E16" s="77">
         <v>16</v>
       </c>
-      <c r="F35" s="74">
-        <f>E35*D35/1000</f>
+      <c r="F16" s="71">
+        <f>E16*D16/1000</f>
         <v>154.24</v>
       </c>
-      <c r="G35" s="69"/>
-      <c r="H35" s="75"/>
-    </row>
-    <row r="36" spans="2:8">
-      <c r="B36" s="74">
+      <c r="G16" s="66"/>
+      <c r="H16" s="72"/>
+    </row>
+    <row r="17" spans="2:8">
+      <c r="B17" s="71">
         <v>2</v>
       </c>
-      <c r="C36" s="69">
+      <c r="C17" s="66">
         <v>8</v>
       </c>
-      <c r="D36" s="69">
+      <c r="D17" s="66">
         <v>6870</v>
       </c>
-      <c r="E36" s="80">
+      <c r="E17" s="77">
         <v>116</v>
       </c>
-      <c r="F36" s="74">
-        <f t="shared" ref="F36:F47" si="1">E36*D36/1000</f>
+      <c r="F17" s="71">
+        <f t="shared" ref="F17:F28" si="1">E17*D17/1000</f>
         <v>796.92</v>
       </c>
-      <c r="G36" s="69"/>
-      <c r="H36" s="75"/>
-    </row>
-    <row r="37" spans="2:8">
-      <c r="B37" s="74">
+      <c r="G17" s="66"/>
+      <c r="H17" s="72"/>
+    </row>
+    <row r="18" spans="2:8">
+      <c r="B18" s="71">
         <v>3</v>
       </c>
-      <c r="C37" s="69">
+      <c r="C18" s="66">
         <v>8</v>
       </c>
-      <c r="D37" s="69">
+      <c r="D18" s="66">
         <v>7970</v>
       </c>
-      <c r="E37" s="80">
+      <c r="E18" s="77">
         <v>28</v>
       </c>
-      <c r="F37" s="74">
+      <c r="F18" s="71">
         <f t="shared" si="1"/>
         <v>223.16</v>
       </c>
-      <c r="G37" s="69"/>
-      <c r="H37" s="75"/>
-    </row>
-    <row r="38" spans="2:8">
-      <c r="B38" s="74">
+      <c r="G18" s="66"/>
+      <c r="H18" s="72"/>
+    </row>
+    <row r="19" spans="2:8">
+      <c r="B19" s="71">
         <v>4</v>
       </c>
-      <c r="C38" s="69">
+      <c r="C19" s="66">
         <v>8</v>
       </c>
-      <c r="D38" s="69">
+      <c r="D19" s="66">
         <v>7540</v>
       </c>
-      <c r="E38" s="80">
+      <c r="E19" s="77">
         <v>8</v>
       </c>
-      <c r="F38" s="74">
+      <c r="F19" s="71">
         <f t="shared" si="1"/>
         <v>60.32</v>
       </c>
-      <c r="G38" s="69"/>
-      <c r="H38" s="75"/>
-    </row>
-    <row r="39" spans="2:8">
-      <c r="B39" s="74">
+      <c r="G19" s="66"/>
+      <c r="H19" s="72"/>
+    </row>
+    <row r="20" spans="2:8">
+      <c r="B20" s="71">
         <v>5</v>
       </c>
-      <c r="C39" s="69">
+      <c r="C20" s="66">
         <v>8</v>
       </c>
-      <c r="D39" s="69">
+      <c r="D20" s="66">
         <v>3180</v>
       </c>
-      <c r="E39" s="80">
+      <c r="E20" s="77">
         <v>10</v>
       </c>
-      <c r="F39" s="74">
+      <c r="F20" s="71">
         <f t="shared" si="1"/>
         <v>31.8</v>
       </c>
-      <c r="G39" s="69"/>
-      <c r="H39" s="75"/>
-    </row>
-    <row r="40" spans="2:8">
-      <c r="B40" s="74">
+      <c r="G20" s="66"/>
+      <c r="H20" s="72"/>
+    </row>
+    <row r="21" spans="2:8">
+      <c r="B21" s="71">
         <v>6</v>
       </c>
-      <c r="C40" s="69">
+      <c r="C21" s="66">
         <v>8</v>
       </c>
-      <c r="D40" s="69">
+      <c r="D21" s="66">
         <v>9140</v>
       </c>
-      <c r="E40" s="80">
+      <c r="E21" s="77">
         <v>54</v>
       </c>
-      <c r="F40" s="74">
+      <c r="F21" s="71">
         <f t="shared" si="1"/>
         <v>493.56</v>
       </c>
-      <c r="G40" s="69"/>
-      <c r="H40" s="75"/>
-    </row>
-    <row r="41" spans="2:8">
-      <c r="B41" s="74">
+      <c r="G21" s="66"/>
+      <c r="H21" s="72"/>
+    </row>
+    <row r="22" spans="2:8">
+      <c r="B22" s="71">
         <v>7</v>
       </c>
-      <c r="C41" s="69">
+      <c r="C22" s="66">
         <v>8</v>
       </c>
-      <c r="D41" s="69">
+      <c r="D22" s="66">
         <v>10040</v>
       </c>
-      <c r="E41" s="80">
+      <c r="E22" s="77">
         <v>36</v>
       </c>
-      <c r="F41" s="74">
+      <c r="F22" s="71">
         <f t="shared" si="1"/>
         <v>361.44</v>
       </c>
-      <c r="G41" s="69"/>
-      <c r="H41" s="75"/>
-    </row>
-    <row r="42" spans="2:8">
-      <c r="B42" s="74">
+      <c r="G22" s="66"/>
+      <c r="H22" s="72"/>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="71">
         <v>8</v>
       </c>
-      <c r="C42" s="69">
+      <c r="C23" s="66">
         <v>8</v>
       </c>
-      <c r="D42" s="69">
+      <c r="D23" s="66">
         <v>8340</v>
       </c>
-      <c r="E42" s="80">
+      <c r="E23" s="77">
         <v>34</v>
       </c>
-      <c r="F42" s="74">
+      <c r="F23" s="71">
         <f t="shared" si="1"/>
         <v>283.56</v>
       </c>
-      <c r="G42" s="69"/>
-      <c r="H42" s="75"/>
-    </row>
-    <row r="43" spans="2:8">
-      <c r="B43" s="74">
+      <c r="G23" s="66"/>
+      <c r="H23" s="72"/>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="71">
         <v>9</v>
       </c>
-      <c r="C43" s="69">
+      <c r="C24" s="66">
         <v>8</v>
       </c>
-      <c r="D43" s="69">
+      <c r="D24" s="66">
         <v>2500</v>
       </c>
-      <c r="E43" s="80">
+      <c r="E24" s="77">
         <v>83</v>
       </c>
-      <c r="F43" s="74">
+      <c r="F24" s="71">
         <f t="shared" si="1"/>
         <v>207.5</v>
       </c>
-      <c r="G43" s="69"/>
-      <c r="H43" s="75"/>
-    </row>
-    <row r="44" spans="2:8">
-      <c r="B44" s="74">
+      <c r="G24" s="66"/>
+      <c r="H24" s="72"/>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="71">
         <v>10</v>
       </c>
-      <c r="C44" s="69">
+      <c r="C25" s="66">
         <v>10</v>
       </c>
-      <c r="D44" s="69">
+      <c r="D25" s="66">
         <v>970</v>
       </c>
-      <c r="E44" s="80">
+      <c r="E25" s="77">
         <v>38</v>
       </c>
-      <c r="F44" s="74"/>
-      <c r="G44" s="69">
-        <f>E44*D44/1000</f>
+      <c r="F25" s="71"/>
+      <c r="G25" s="66">
+        <f>E25*D25/1000</f>
         <v>36.86</v>
       </c>
-      <c r="H44" s="75"/>
-    </row>
-    <row r="45" spans="2:8">
-      <c r="B45" s="74">
+      <c r="H25" s="72"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="71">
         <v>11</v>
       </c>
-      <c r="C45" s="69">
+      <c r="C26" s="66">
         <v>8</v>
       </c>
-      <c r="D45" s="69">
+      <c r="D26" s="66">
         <v>1780</v>
       </c>
-      <c r="E45" s="80">
+      <c r="E26" s="77">
         <v>240</v>
       </c>
-      <c r="F45" s="74">
+      <c r="F26" s="71">
         <f t="shared" si="1"/>
         <v>427.2</v>
       </c>
-      <c r="G45" s="69"/>
-      <c r="H45" s="75"/>
-    </row>
-    <row r="46" spans="2:8">
-      <c r="B46" s="74">
+      <c r="G26" s="66"/>
+      <c r="H26" s="72"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="71">
         <v>12</v>
       </c>
-      <c r="C46" s="69">
+      <c r="C27" s="66">
         <v>12</v>
       </c>
-      <c r="D46" s="69">
+      <c r="D27" s="66">
         <v>78000</v>
       </c>
-      <c r="E46" s="80">
+      <c r="E27" s="77">
         <v>4</v>
       </c>
-      <c r="F46" s="74"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="75">
-        <f>E46*D46/1000</f>
+      <c r="F27" s="71"/>
+      <c r="G27" s="66"/>
+      <c r="H27" s="72">
+        <f>E27*D27/1000</f>
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="2:8">
-      <c r="B47" s="74">
+    <row r="28" spans="2:8">
+      <c r="B28" s="71">
         <v>13</v>
       </c>
-      <c r="C47" s="69">
+      <c r="C28" s="66">
         <v>8</v>
       </c>
-      <c r="D47" s="69">
+      <c r="D28" s="66">
         <v>880</v>
       </c>
-      <c r="E47" s="80">
+      <c r="E28" s="77">
         <v>220</v>
       </c>
-      <c r="F47" s="74">
+      <c r="F28" s="71">
         <f t="shared" si="1"/>
         <v>193.6</v>
       </c>
-      <c r="G47" s="69"/>
-      <c r="H47" s="75"/>
-    </row>
-    <row r="48" spans="2:8" ht="15" thickBot="1">
-      <c r="B48" s="76">
+      <c r="G28" s="66"/>
+      <c r="H28" s="72"/>
+    </row>
+    <row r="29" spans="2:8" ht="15" thickBot="1">
+      <c r="B29" s="73">
         <v>14</v>
       </c>
-      <c r="C48" s="77">
+      <c r="C29" s="74">
         <v>12</v>
       </c>
-      <c r="D48" s="77">
+      <c r="D29" s="74">
         <v>4200</v>
       </c>
-      <c r="E48" s="81">
+      <c r="E29" s="78">
         <v>8</v>
       </c>
-      <c r="F48" s="76"/>
-      <c r="G48" s="77"/>
-      <c r="H48" s="78">
-        <f t="shared" ref="H48" si="2">E48*D48/1000</f>
+      <c r="F29" s="73"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="75">
+        <f t="shared" ref="H29" si="2">E29*D29/1000</f>
         <v>33.6</v>
       </c>
     </row>
-    <row r="49" spans="2:8">
-      <c r="B49" s="70" t="s">
-        <v>197</v>
-      </c>
-      <c r="C49" s="70"/>
-      <c r="D49" s="70"/>
-      <c r="E49" s="82"/>
-      <c r="F49" s="83">
-        <f>SUM(F35:F48)</f>
+    <row r="30" spans="2:8">
+      <c r="B30" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="C30" s="67"/>
+      <c r="D30" s="67"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="80">
+        <f>SUM(F16:F29)</f>
         <v>3233.2999999999993</v>
       </c>
-      <c r="G49" s="70">
-        <f t="shared" ref="G49:H49" si="3">SUM(G35:G48)</f>
+      <c r="G30" s="67">
+        <f t="shared" ref="G30:H30" si="3">SUM(G16:G29)</f>
         <v>36.86</v>
       </c>
-      <c r="H49" s="84">
+      <c r="H30" s="81">
         <f t="shared" si="3"/>
         <v>345.6</v>
       </c>
     </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="69" t="s">
-        <v>196</v>
-      </c>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="80"/>
-      <c r="F50" s="74">
+    <row r="31" spans="2:8">
+      <c r="B31" s="66" t="s">
+        <v>186</v>
+      </c>
+      <c r="C31" s="66"/>
+      <c r="D31" s="66"/>
+      <c r="E31" s="77"/>
+      <c r="F31" s="71">
         <v>0.39500000000000002</v>
       </c>
-      <c r="G50" s="69">
+      <c r="G31" s="66">
         <v>0.61699999999999999</v>
       </c>
-      <c r="H50" s="75">
+      <c r="H31" s="72">
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="15" thickBot="1">
-      <c r="B51" s="69" t="s">
-        <v>198</v>
-      </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="69"/>
-      <c r="E51" s="80"/>
-      <c r="F51" s="76">
-        <f>ROUND(F49*F50,0)</f>
+    <row r="32" spans="2:8" ht="15" thickBot="1">
+      <c r="B32" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="73">
+        <f>ROUND(F30*F31,0)</f>
         <v>1277</v>
       </c>
-      <c r="G51" s="77">
-        <f t="shared" ref="G51:H51" si="4">ROUND(G49*G50,0)</f>
+      <c r="G32" s="74">
+        <f t="shared" ref="G32:H32" si="4">ROUND(G30*G31,0)</f>
         <v>23</v>
       </c>
-      <c r="H51" s="78">
+      <c r="H32" s="75">
         <f t="shared" si="4"/>
         <v>307</v>
       </c>
     </row>
-    <row r="52" spans="2:8">
-      <c r="B52" s="69"/>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
-    </row>
-    <row r="58" spans="2:8" ht="57">
-      <c r="B58" s="93" t="s">
+    <row r="33" spans="2:8">
+      <c r="B33" s="66"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="66"/>
+      <c r="E33" s="66"/>
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+    </row>
+    <row r="36" spans="2:8">
+      <c r="B36" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" ht="57">
+      <c r="B39" s="92" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66">
+        <v>0.68</v>
+      </c>
+      <c r="E39" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+    </row>
+    <row r="40" spans="2:8">
+      <c r="B40" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="C40" s="66"/>
+      <c r="D40" s="66">
+        <v>242</v>
+      </c>
+      <c r="E40" s="66" t="s">
+        <v>193</v>
+      </c>
+      <c r="F40" s="66"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="66"/>
+    </row>
+    <row r="41" spans="2:8">
+      <c r="B41" s="66" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66">
+        <v>220</v>
+      </c>
+      <c r="E41" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" s="66"/>
+      <c r="G41" s="66"/>
+      <c r="H41" s="66"/>
+    </row>
+    <row r="42" spans="2:8">
+      <c r="B42" s="66" t="s">
+        <v>195</v>
+      </c>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66">
+        <v>1418</v>
+      </c>
+      <c r="E42" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F42" s="66"/>
+      <c r="G42" s="66"/>
+      <c r="H42" s="66"/>
+    </row>
+    <row r="43" spans="2:8">
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="66"/>
+      <c r="G43" s="66"/>
+      <c r="H43" s="66"/>
+    </row>
+    <row r="44" spans="2:8" ht="15">
+      <c r="B44" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C44" s="66"/>
+      <c r="D44" s="91">
+        <v>1035</v>
+      </c>
+      <c r="E44" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F44" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="G44" s="66">
+        <v>1607</v>
+      </c>
+      <c r="H44" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8">
+      <c r="B45" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C45" s="66"/>
+      <c r="D45" s="66">
+        <v>266</v>
+      </c>
+      <c r="E45" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F45" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="66">
+        <v>577</v>
+      </c>
+      <c r="H45" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8">
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66">
+        <v>138</v>
+      </c>
+      <c r="E46" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" s="66"/>
+      <c r="G46" s="66"/>
+      <c r="H46" s="66"/>
+    </row>
+    <row r="47" spans="2:8">
+      <c r="B47" s="66"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="66">
+        <v>173</v>
+      </c>
+      <c r="E47" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F47" s="66"/>
+      <c r="G47" s="66"/>
+      <c r="H47" s="66"/>
+    </row>
+    <row r="48" spans="2:8" ht="15">
+      <c r="B48" s="66"/>
+      <c r="C48" s="66"/>
+      <c r="D48" s="91">
+        <f>D45+D46+D47</f>
+        <v>577</v>
+      </c>
+      <c r="E48" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="F48" s="66"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="66"/>
+    </row>
+    <row r="49" spans="2:8">
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+    </row>
+    <row r="50" spans="2:8" ht="15">
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="91">
+        <f>D44+D48</f>
+        <v>1612</v>
+      </c>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+    </row>
+    <row r="56" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B56" s="90" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8">
+      <c r="B57" s="68" t="s">
+        <v>189</v>
+      </c>
+      <c r="C57" s="69" t="s">
         <v>200</v>
       </c>
-      <c r="D58">
-        <v>0.68</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="D57" s="69" t="s">
         <v>201</v>
       </c>
+      <c r="E57" s="69" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="G57" s="69" t="s">
+        <v>203</v>
+      </c>
+      <c r="H57" s="70" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8">
+      <c r="B58" s="71">
+        <v>1</v>
+      </c>
+      <c r="C58" s="66">
+        <v>18</v>
+      </c>
+      <c r="D58" s="66">
+        <v>9.74</v>
+      </c>
+      <c r="E58" s="66">
+        <v>4</v>
+      </c>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="72">
+        <v>39.1</v>
+      </c>
     </row>
     <row r="59" spans="2:8">
-      <c r="B59" t="s">
-        <v>202</v>
-      </c>
-      <c r="D59">
-        <v>242</v>
-      </c>
-      <c r="E59" t="s">
-        <v>203</v>
+      <c r="B59" s="71">
+        <v>2</v>
+      </c>
+      <c r="C59" s="66">
+        <v>18</v>
+      </c>
+      <c r="D59" s="66">
+        <v>3.27</v>
+      </c>
+      <c r="E59" s="66">
+        <v>4</v>
+      </c>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="72">
+        <v>13.1</v>
       </c>
     </row>
     <row r="60" spans="2:8">
-      <c r="B60" t="s">
-        <v>204</v>
-      </c>
-      <c r="D60">
+      <c r="B60" s="71">
+        <v>3</v>
+      </c>
+      <c r="C60" s="66">
+        <v>14</v>
+      </c>
+      <c r="D60" s="66">
+        <v>3.3</v>
+      </c>
+      <c r="E60" s="66">
+        <v>2</v>
+      </c>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66">
+        <v>6.6</v>
+      </c>
+      <c r="H60" s="72"/>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" s="71">
+        <v>4</v>
+      </c>
+      <c r="C61" s="66">
+        <v>14</v>
+      </c>
+      <c r="D61" s="66">
+        <v>3.58</v>
+      </c>
+      <c r="E61" s="66">
+        <v>2</v>
+      </c>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66">
+        <v>7.2</v>
+      </c>
+      <c r="H61" s="72"/>
+    </row>
+    <row r="62" spans="2:8">
+      <c r="B62" s="71">
+        <v>5</v>
+      </c>
+      <c r="C62" s="66">
+        <v>6</v>
+      </c>
+      <c r="D62" s="66">
+        <v>1.3</v>
+      </c>
+      <c r="E62" s="66">
+        <v>17</v>
+      </c>
+      <c r="F62" s="66">
+        <v>22.1</v>
+      </c>
+      <c r="G62" s="66"/>
+      <c r="H62" s="72"/>
+    </row>
+    <row r="63" spans="2:8">
+      <c r="B63" s="71">
+        <v>6</v>
+      </c>
+      <c r="C63" s="66">
+        <v>6</v>
+      </c>
+      <c r="D63" s="66">
+        <v>1.64</v>
+      </c>
+      <c r="E63" s="66">
+        <v>23</v>
+      </c>
+      <c r="F63" s="66">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G63" s="66"/>
+      <c r="H63" s="72"/>
+    </row>
+    <row r="64" spans="2:8">
+      <c r="B64" s="71">
+        <v>7</v>
+      </c>
+      <c r="C64" s="66">
+        <v>18</v>
+      </c>
+      <c r="D64" s="66">
+        <v>7.2</v>
+      </c>
+      <c r="E64" s="66">
+        <v>4</v>
+      </c>
+      <c r="F64" s="66"/>
+      <c r="G64" s="66"/>
+      <c r="H64" s="72">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="71">
+        <v>8</v>
+      </c>
+      <c r="C65" s="66">
+        <v>14</v>
+      </c>
+      <c r="D65" s="66">
+        <v>6.52</v>
+      </c>
+      <c r="E65" s="66">
+        <v>2</v>
+      </c>
+      <c r="F65" s="66"/>
+      <c r="G65" s="66">
+        <v>13</v>
+      </c>
+      <c r="H65" s="72"/>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="71">
+        <v>9</v>
+      </c>
+      <c r="C66" s="66">
+        <v>6</v>
+      </c>
+      <c r="D66" s="66">
+        <v>1.64</v>
+      </c>
+      <c r="E66" s="66">
+        <v>35</v>
+      </c>
+      <c r="F66" s="66">
+        <v>57.4</v>
+      </c>
+      <c r="G66" s="66"/>
+      <c r="H66" s="72"/>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="71">
+        <v>10</v>
+      </c>
+      <c r="C67" s="66">
+        <v>14</v>
+      </c>
+      <c r="D67" s="66">
+        <v>5.67</v>
+      </c>
+      <c r="E67" s="66">
+        <v>2</v>
+      </c>
+      <c r="F67" s="66"/>
+      <c r="G67" s="66">
+        <v>11.3</v>
+      </c>
+      <c r="H67" s="72"/>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="71">
+        <v>11</v>
+      </c>
+      <c r="C68" s="66">
+        <v>14</v>
+      </c>
+      <c r="D68" s="66">
+        <v>4.63</v>
+      </c>
+      <c r="E68" s="66">
+        <v>4</v>
+      </c>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66">
+        <v>18.5</v>
+      </c>
+      <c r="H68" s="72"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" thickBot="1">
+      <c r="B69" s="73">
+        <v>12</v>
+      </c>
+      <c r="C69" s="74">
+        <v>6</v>
+      </c>
+      <c r="D69" s="74">
+        <v>1.64</v>
+      </c>
+      <c r="E69" s="74">
+        <v>29</v>
+      </c>
+      <c r="F69" s="74">
+        <v>47.6</v>
+      </c>
+      <c r="G69" s="74"/>
+      <c r="H69" s="75"/>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" s="67"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="67" t="s">
+        <v>205</v>
+      </c>
+      <c r="E70" s="67" t="s">
+        <v>206</v>
+      </c>
+      <c r="F70" s="67">
+        <v>164.8</v>
+      </c>
+      <c r="G70" s="67">
+        <v>56.7</v>
+      </c>
+      <c r="H70" s="67">
+        <v>80.8</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" s="66"/>
+      <c r="C71" s="66"/>
+      <c r="D71" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="E71" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F71" s="66">
+        <v>0.222</v>
+      </c>
+      <c r="G71" s="66">
+        <v>1.208</v>
+      </c>
+      <c r="H71" s="66">
+        <v>1.998</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8">
+      <c r="B72" s="66"/>
+      <c r="C72" s="66"/>
+      <c r="D72" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E72" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F72" s="66">
+        <v>36.6</v>
+      </c>
+      <c r="G72" s="66">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H72" s="66">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="15">
+      <c r="B73" s="66"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E73" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66"/>
+      <c r="H73" s="66"/>
+    </row>
+    <row r="74" spans="2:8">
+      <c r="B74" s="66"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="66"/>
+      <c r="E74" s="66"/>
+      <c r="F74" s="66"/>
+      <c r="G74" s="66"/>
+      <c r="H74" s="66"/>
+    </row>
+    <row r="75" spans="2:8" ht="15">
+      <c r="B75" s="90" t="s">
+        <v>212</v>
+      </c>
+      <c r="C75" s="66"/>
+      <c r="D75" s="66"/>
+      <c r="E75" s="66"/>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66"/>
+      <c r="H75" s="66"/>
+    </row>
+    <row r="76" spans="2:8">
+      <c r="B76" s="66"/>
+      <c r="C76" s="66"/>
+      <c r="D76" s="66"/>
+      <c r="E76" s="66"/>
+      <c r="F76" s="66"/>
+      <c r="G76" s="66"/>
+      <c r="H76" s="66"/>
+    </row>
+    <row r="77" spans="2:8">
+      <c r="B77" s="66"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="66"/>
+      <c r="E77" s="66"/>
+      <c r="F77" s="66"/>
+      <c r="G77" s="66"/>
+      <c r="H77" s="66"/>
+    </row>
+    <row r="78" spans="2:8">
+      <c r="B78" s="66"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="66"/>
+      <c r="H78" s="66"/>
+    </row>
+    <row r="79" spans="2:8">
+      <c r="B79" s="66"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
+      <c r="H79" s="66"/>
+    </row>
+    <row r="80" spans="2:8">
+      <c r="B80" s="66"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="66"/>
+      <c r="E80" s="66"/>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66"/>
+      <c r="H80" s="66"/>
+    </row>
+    <row r="81" spans="2:8">
+      <c r="B81" s="66"/>
+      <c r="C81" s="66"/>
+      <c r="D81" s="66"/>
+      <c r="E81" s="66"/>
+      <c r="F81" s="66"/>
+      <c r="G81" s="66"/>
+      <c r="H81" s="66"/>
+    </row>
+    <row r="82" spans="2:8">
+      <c r="B82" s="66"/>
+      <c r="C82" s="66"/>
+      <c r="D82" s="66"/>
+      <c r="E82" s="66"/>
+      <c r="F82" s="66"/>
+      <c r="G82" s="66"/>
+      <c r="H82" s="66"/>
+    </row>
+    <row r="83" spans="2:8">
+      <c r="B83" s="66"/>
+      <c r="C83" s="66"/>
+      <c r="D83" s="66"/>
+      <c r="E83" s="66"/>
+      <c r="F83" s="66"/>
+      <c r="G83" s="66"/>
+      <c r="H83" s="66"/>
+    </row>
+    <row r="84" spans="2:8">
+      <c r="B84" s="66"/>
+      <c r="C84" s="66"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="66"/>
+      <c r="H84" s="66"/>
+    </row>
+    <row r="85" spans="2:8">
+      <c r="B85" s="66"/>
+      <c r="C85" s="66"/>
+      <c r="D85" s="66"/>
+      <c r="E85" s="66"/>
+      <c r="F85" s="66"/>
+      <c r="G85" s="66"/>
+      <c r="H85" s="66"/>
+    </row>
+    <row r="86" spans="2:8">
+      <c r="B86" s="66"/>
+      <c r="C86" s="66"/>
+      <c r="D86" s="66"/>
+      <c r="E86" s="66"/>
+      <c r="F86" s="66"/>
+      <c r="G86" s="66"/>
+      <c r="H86" s="66"/>
+    </row>
+    <row r="87" spans="2:8">
+      <c r="B87" s="66"/>
+      <c r="C87" s="66"/>
+      <c r="D87" s="66"/>
+      <c r="E87" s="66"/>
+      <c r="F87" s="66"/>
+      <c r="G87" s="66"/>
+      <c r="H87" s="66"/>
+    </row>
+    <row r="88" spans="2:8">
+      <c r="B88" s="66"/>
+      <c r="C88" s="66"/>
+      <c r="D88" s="66"/>
+      <c r="E88" s="66"/>
+      <c r="F88" s="66"/>
+      <c r="G88" s="66"/>
+      <c r="H88" s="66"/>
+    </row>
+    <row r="89" spans="2:8">
+      <c r="B89" s="66"/>
+      <c r="C89" s="66"/>
+      <c r="D89" s="66"/>
+      <c r="E89" s="66"/>
+      <c r="F89" s="66"/>
+      <c r="G89" s="66"/>
+      <c r="H89" s="66"/>
+    </row>
+    <row r="90" spans="2:8">
+      <c r="B90" s="66"/>
+      <c r="C90" s="66"/>
+      <c r="D90" s="66"/>
+      <c r="E90" s="66"/>
+      <c r="F90" s="66"/>
+      <c r="G90" s="66"/>
+      <c r="H90" s="66"/>
+    </row>
+    <row r="91" spans="2:8">
+      <c r="B91" s="66"/>
+      <c r="C91" s="66"/>
+      <c r="D91" s="66"/>
+      <c r="E91" s="66"/>
+      <c r="F91" s="66"/>
+      <c r="G91" s="66"/>
+      <c r="H91" s="66"/>
+    </row>
+    <row r="92" spans="2:8">
+      <c r="B92" s="66"/>
+      <c r="C92" s="66"/>
+      <c r="D92" s="66"/>
+      <c r="E92" s="66"/>
+      <c r="F92" s="66"/>
+      <c r="G92" s="66"/>
+      <c r="H92" s="66"/>
+    </row>
+    <row r="93" spans="2:8">
+      <c r="B93" s="66"/>
+      <c r="C93" s="66"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="66"/>
+      <c r="F93" s="66"/>
+      <c r="G93" s="66"/>
+      <c r="H93" s="66"/>
+    </row>
+    <row r="94" spans="2:8">
+      <c r="B94" s="66"/>
+      <c r="C94" s="66"/>
+      <c r="D94" s="66"/>
+      <c r="E94" s="66"/>
+      <c r="F94" s="66"/>
+      <c r="G94" s="66"/>
+      <c r="H94" s="66"/>
+    </row>
+    <row r="95" spans="2:8">
+      <c r="B95" s="66"/>
+      <c r="C95" s="66"/>
+      <c r="D95" s="66"/>
+      <c r="E95" s="66"/>
+      <c r="F95" s="66"/>
+      <c r="G95" s="66"/>
+      <c r="H95" s="66"/>
+    </row>
+    <row r="96" spans="2:8">
+      <c r="B96" s="66"/>
+      <c r="C96" s="66"/>
+      <c r="D96" s="66"/>
+      <c r="E96" s="66"/>
+      <c r="F96" s="66"/>
+      <c r="G96" s="66"/>
+      <c r="H96" s="66"/>
+    </row>
+    <row r="97" spans="2:8">
+      <c r="B97" s="66"/>
+      <c r="C97" s="66"/>
+      <c r="D97" s="66"/>
+      <c r="E97" s="66"/>
+      <c r="F97" s="66"/>
+      <c r="G97" s="66"/>
+      <c r="H97" s="66"/>
+    </row>
+    <row r="98" spans="2:8">
+      <c r="B98" s="66"/>
+      <c r="C98" s="66"/>
+      <c r="D98" s="66"/>
+      <c r="E98" s="66"/>
+      <c r="F98" s="66"/>
+      <c r="G98" s="66"/>
+      <c r="H98" s="66"/>
+    </row>
+    <row r="99" spans="2:8">
+      <c r="B99" s="66"/>
+      <c r="C99" s="66"/>
+      <c r="D99" s="66"/>
+      <c r="E99" s="66"/>
+      <c r="F99" s="66"/>
+      <c r="G99" s="66"/>
+      <c r="H99" s="66"/>
+    </row>
+    <row r="100" spans="2:8">
+      <c r="B100" s="66"/>
+      <c r="C100" s="66"/>
+      <c r="D100" s="66"/>
+      <c r="E100" s="66"/>
+      <c r="F100" s="66"/>
+      <c r="G100" s="66"/>
+      <c r="H100" s="66"/>
+    </row>
+    <row r="101" spans="2:8">
+      <c r="B101" s="66"/>
+      <c r="C101" s="66"/>
+      <c r="D101" s="66"/>
+      <c r="E101" s="66"/>
+      <c r="F101" s="66"/>
+      <c r="G101" s="66"/>
+      <c r="H101" s="66"/>
+    </row>
+    <row r="102" spans="2:8">
+      <c r="B102" s="66"/>
+      <c r="C102" s="66"/>
+      <c r="D102" s="66"/>
+      <c r="E102" s="66"/>
+      <c r="F102" s="66"/>
+      <c r="G102" s="66"/>
+      <c r="H102" s="66"/>
+    </row>
+    <row r="116" spans="2:4">
+      <c r="B116" t="s">
+        <v>236</v>
+      </c>
+      <c r="C116" t="s">
+        <v>237</v>
+      </c>
+      <c r="D116" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" ht="30" customHeight="1">
+      <c r="B117" s="66" t="s">
+        <v>214</v>
+      </c>
+      <c r="C117" s="66"/>
+      <c r="D117" s="66"/>
+    </row>
+    <row r="118" spans="2:4" ht="30" customHeight="1">
+      <c r="B118" s="92" t="s">
+        <v>213</v>
+      </c>
+      <c r="C118" s="92" t="s">
+        <v>215</v>
+      </c>
+      <c r="D118" s="92"/>
+    </row>
+    <row r="119" spans="2:4" ht="30" customHeight="1">
+      <c r="B119" s="92" t="s">
+        <v>239</v>
+      </c>
+      <c r="C119" s="92" t="s">
+        <v>240</v>
+      </c>
+      <c r="D119" s="92"/>
+    </row>
+    <row r="120" spans="2:4" ht="30" customHeight="1">
+      <c r="B120" s="92" t="s">
+        <v>216</v>
+      </c>
+      <c r="C120" s="92" t="s">
+        <v>229</v>
+      </c>
+      <c r="D120" s="92"/>
+    </row>
+    <row r="121" spans="2:4" ht="30" customHeight="1">
+      <c r="B121" s="92" t="s">
+        <v>217</v>
+      </c>
+      <c r="C121" s="92" t="s">
+        <v>230</v>
+      </c>
+      <c r="D121" s="92"/>
+    </row>
+    <row r="122" spans="2:4" ht="30" customHeight="1">
+      <c r="B122" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C122" s="92" t="s">
+        <v>219</v>
+      </c>
+      <c r="D122" s="92"/>
+    </row>
+    <row r="123" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B123" s="92"/>
+      <c r="C123" s="92"/>
+      <c r="D123" s="92"/>
+    </row>
+    <row r="124" spans="2:4" ht="30" customHeight="1">
+      <c r="B124" s="92" t="s">
         <v>220</v>
       </c>
-      <c r="E60" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8">
-      <c r="B61" t="s">
-        <v>205</v>
-      </c>
-      <c r="D61">
-        <v>1418</v>
-      </c>
-      <c r="E61" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="15">
-      <c r="B63" t="s">
-        <v>206</v>
-      </c>
-      <c r="D63" s="94">
-        <v>1035</v>
-      </c>
-      <c r="E63" t="s">
-        <v>201</v>
-      </c>
-      <c r="F63" t="s">
-        <v>209</v>
-      </c>
-      <c r="G63">
-        <v>1607</v>
-      </c>
-      <c r="H63" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" t="s">
-        <v>207</v>
-      </c>
-      <c r="D64">
-        <v>266</v>
-      </c>
-      <c r="E64" t="s">
-        <v>201</v>
-      </c>
-      <c r="F64" t="s">
-        <v>207</v>
-      </c>
-      <c r="G64">
-        <v>577</v>
-      </c>
-      <c r="H64" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="D65">
-        <v>138</v>
-      </c>
-      <c r="E65" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
-      <c r="D66">
-        <v>173</v>
-      </c>
-      <c r="E66" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" ht="15">
-      <c r="D67" s="94">
-        <f>D64+D65+D66</f>
-        <v>577</v>
-      </c>
-      <c r="E67" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" ht="15">
-      <c r="D69" s="94">
-        <f>D63+D67</f>
-        <v>1612</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B75" s="94" t="s">
+      <c r="C124" s="92" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="76" spans="2:8">
-      <c r="B76" s="71" t="s">
-        <v>199</v>
-      </c>
-      <c r="C76" s="72" t="s">
-        <v>210</v>
-      </c>
-      <c r="D76" s="72" t="s">
-        <v>211</v>
-      </c>
-      <c r="E76" s="72" t="s">
-        <v>203</v>
-      </c>
-      <c r="F76" s="72" t="s">
-        <v>212</v>
-      </c>
-      <c r="G76" s="72" t="s">
-        <v>213</v>
-      </c>
-      <c r="H76" s="73" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8">
-      <c r="B77" s="74">
-        <v>1</v>
-      </c>
-      <c r="C77" s="69">
-        <v>18</v>
-      </c>
-      <c r="D77" s="69">
-        <v>9.74</v>
-      </c>
-      <c r="E77" s="69">
-        <v>4</v>
-      </c>
-      <c r="F77" s="69"/>
-      <c r="G77" s="69"/>
-      <c r="H77" s="75">
-        <v>39.1</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8">
-      <c r="B78" s="74">
-        <v>2</v>
-      </c>
-      <c r="C78" s="69">
-        <v>18</v>
-      </c>
-      <c r="D78" s="69">
-        <v>3.27</v>
-      </c>
-      <c r="E78" s="69">
-        <v>4</v>
-      </c>
-      <c r="F78" s="69"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="75">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8">
-      <c r="B79" s="74">
-        <v>3</v>
-      </c>
-      <c r="C79" s="69">
-        <v>14</v>
-      </c>
-      <c r="D79" s="69">
-        <v>3.3</v>
-      </c>
-      <c r="E79" s="69">
-        <v>2</v>
-      </c>
-      <c r="F79" s="69"/>
-      <c r="G79" s="69">
-        <v>6.6</v>
-      </c>
-      <c r="H79" s="75"/>
-    </row>
-    <row r="80" spans="2:8">
-      <c r="B80" s="74">
-        <v>4</v>
-      </c>
-      <c r="C80" s="69">
-        <v>14</v>
-      </c>
-      <c r="D80" s="69">
-        <v>3.58</v>
-      </c>
-      <c r="E80" s="69">
-        <v>2</v>
-      </c>
-      <c r="F80" s="69"/>
-      <c r="G80" s="69">
-        <v>7.2</v>
-      </c>
-      <c r="H80" s="75"/>
-    </row>
-    <row r="81" spans="2:8">
-      <c r="B81" s="74">
-        <v>5</v>
-      </c>
-      <c r="C81" s="69">
-        <v>6</v>
-      </c>
-      <c r="D81" s="69">
-        <v>1.3</v>
-      </c>
-      <c r="E81" s="69">
-        <v>17</v>
-      </c>
-      <c r="F81" s="69">
-        <v>22.1</v>
-      </c>
-      <c r="G81" s="69"/>
-      <c r="H81" s="75"/>
-    </row>
-    <row r="82" spans="2:8">
-      <c r="B82" s="74">
-        <v>6</v>
-      </c>
-      <c r="C82" s="69">
-        <v>6</v>
-      </c>
-      <c r="D82" s="69">
-        <v>1.64</v>
-      </c>
-      <c r="E82" s="69">
-        <v>23</v>
-      </c>
-      <c r="F82" s="69">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="G82" s="69"/>
-      <c r="H82" s="75"/>
-    </row>
-    <row r="83" spans="2:8">
-      <c r="B83" s="74">
-        <v>7</v>
-      </c>
-      <c r="C83" s="69">
-        <v>18</v>
-      </c>
-      <c r="D83" s="69">
-        <v>7.2</v>
-      </c>
-      <c r="E83" s="69">
-        <v>4</v>
-      </c>
-      <c r="F83" s="69"/>
-      <c r="G83" s="69"/>
-      <c r="H83" s="75">
-        <v>28.8</v>
-      </c>
-    </row>
-    <row r="84" spans="2:8">
-      <c r="B84" s="74">
-        <v>8</v>
-      </c>
-      <c r="C84" s="69">
-        <v>14</v>
-      </c>
-      <c r="D84" s="69">
-        <v>6.52</v>
-      </c>
-      <c r="E84" s="69">
-        <v>2</v>
-      </c>
-      <c r="F84" s="69"/>
-      <c r="G84" s="69">
-        <v>13</v>
-      </c>
-      <c r="H84" s="75"/>
-    </row>
-    <row r="85" spans="2:8">
-      <c r="B85" s="74">
-        <v>9</v>
-      </c>
-      <c r="C85" s="69">
-        <v>6</v>
-      </c>
-      <c r="D85" s="69">
-        <v>1.64</v>
-      </c>
-      <c r="E85" s="69">
-        <v>35</v>
-      </c>
-      <c r="F85" s="69">
-        <v>57.4</v>
-      </c>
-      <c r="G85" s="69"/>
-      <c r="H85" s="75"/>
-    </row>
-    <row r="86" spans="2:8">
-      <c r="B86" s="74">
-        <v>10</v>
-      </c>
-      <c r="C86" s="69">
-        <v>14</v>
-      </c>
-      <c r="D86" s="69">
-        <v>5.67</v>
-      </c>
-      <c r="E86" s="69">
-        <v>2</v>
-      </c>
-      <c r="F86" s="69"/>
-      <c r="G86" s="69">
-        <v>11.3</v>
-      </c>
-      <c r="H86" s="75"/>
-    </row>
-    <row r="87" spans="2:8">
-      <c r="B87" s="74">
-        <v>11</v>
-      </c>
-      <c r="C87" s="69">
-        <v>14</v>
-      </c>
-      <c r="D87" s="69">
-        <v>4.63</v>
-      </c>
-      <c r="E87" s="69">
-        <v>4</v>
-      </c>
-      <c r="F87" s="69"/>
-      <c r="G87" s="69">
-        <v>18.5</v>
-      </c>
-      <c r="H87" s="75"/>
-    </row>
-    <row r="88" spans="2:8" ht="15" thickBot="1">
-      <c r="B88" s="76">
-        <v>12</v>
-      </c>
-      <c r="C88" s="77">
-        <v>6</v>
-      </c>
-      <c r="D88" s="77">
-        <v>1.64</v>
-      </c>
-      <c r="E88" s="77">
-        <v>29</v>
-      </c>
-      <c r="F88" s="77">
-        <v>47.6</v>
-      </c>
-      <c r="G88" s="77"/>
-      <c r="H88" s="78"/>
-    </row>
-    <row r="89" spans="2:8">
-      <c r="B89" s="70"/>
-      <c r="C89" s="70"/>
-      <c r="D89" s="70" t="s">
-        <v>215</v>
-      </c>
-      <c r="E89" s="70" t="s">
-        <v>216</v>
-      </c>
-      <c r="F89" s="70">
-        <v>164.8</v>
-      </c>
-      <c r="G89" s="70">
-        <v>56.7</v>
-      </c>
-      <c r="H89" s="70">
-        <v>80.8</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8">
-      <c r="B90" s="69"/>
-      <c r="C90" s="69"/>
-      <c r="D90" s="69" t="s">
-        <v>217</v>
-      </c>
-      <c r="E90" s="69" t="s">
-        <v>201</v>
-      </c>
-      <c r="F90" s="69">
-        <v>0.222</v>
-      </c>
-      <c r="G90" s="69">
-        <v>1.208</v>
-      </c>
-      <c r="H90" s="69">
-        <v>1.998</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8">
-      <c r="B91" s="69"/>
-      <c r="C91" s="69"/>
-      <c r="D91" s="69" t="s">
+      <c r="D124" s="92"/>
+    </row>
+    <row r="125" spans="2:4" ht="30" customHeight="1">
+      <c r="B125" s="92" t="s">
         <v>218</v>
       </c>
-      <c r="E91" s="69" t="s">
-        <v>201</v>
-      </c>
-      <c r="F91" s="69">
-        <v>36.6</v>
-      </c>
-      <c r="G91" s="69">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="H91" s="69">
-        <v>161.5</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" ht="15">
-      <c r="B92" s="69"/>
-      <c r="C92" s="69"/>
-      <c r="D92" s="95" t="s">
-        <v>219</v>
-      </c>
-      <c r="E92" s="95" t="s">
-        <v>220</v>
-      </c>
-      <c r="F92" s="69"/>
-      <c r="G92" s="69"/>
-      <c r="H92" s="69"/>
-    </row>
-    <row r="93" spans="2:8">
-      <c r="B93" s="69"/>
-      <c r="C93" s="69"/>
-      <c r="D93" s="69"/>
-      <c r="E93" s="69"/>
-      <c r="F93" s="69"/>
-      <c r="G93" s="69"/>
-      <c r="H93" s="69"/>
-    </row>
-    <row r="94" spans="2:8" ht="15">
-      <c r="B94" s="94" t="s">
+      <c r="C125" s="92" t="s">
         <v>222</v>
       </c>
-      <c r="C94" s="69"/>
-      <c r="D94" s="69"/>
-      <c r="E94" s="69"/>
-      <c r="F94" s="69"/>
-      <c r="G94" s="69"/>
-      <c r="H94" s="69"/>
-    </row>
-    <row r="95" spans="2:8">
-      <c r="B95" s="69"/>
-      <c r="C95" s="69"/>
-      <c r="D95" s="69"/>
-      <c r="E95" s="69"/>
-      <c r="F95" s="69"/>
-      <c r="G95" s="69"/>
-      <c r="H95" s="69"/>
-    </row>
-    <row r="96" spans="2:8">
-      <c r="B96" s="69"/>
-      <c r="C96" s="69"/>
-      <c r="D96" s="69"/>
-      <c r="E96" s="69"/>
-      <c r="F96" s="69"/>
-      <c r="G96" s="69"/>
-      <c r="H96" s="69"/>
-    </row>
-    <row r="97" spans="2:8">
-      <c r="B97" s="69"/>
-      <c r="C97" s="69"/>
-      <c r="D97" s="69"/>
-      <c r="E97" s="69"/>
-      <c r="F97" s="69"/>
-      <c r="G97" s="69"/>
-      <c r="H97" s="69"/>
-    </row>
-    <row r="98" spans="2:8">
-      <c r="B98" s="69"/>
-      <c r="C98" s="69"/>
-      <c r="D98" s="69"/>
-      <c r="E98" s="69"/>
-      <c r="F98" s="69"/>
-      <c r="G98" s="69"/>
-      <c r="H98" s="69"/>
-    </row>
-    <row r="99" spans="2:8">
-      <c r="B99" s="69"/>
-      <c r="C99" s="69"/>
-      <c r="D99" s="69"/>
-      <c r="E99" s="69"/>
-      <c r="F99" s="69"/>
-      <c r="G99" s="69"/>
-      <c r="H99" s="69"/>
-    </row>
-    <row r="100" spans="2:8">
-      <c r="B100" s="69"/>
-      <c r="C100" s="69"/>
-      <c r="D100" s="69"/>
-      <c r="E100" s="69"/>
-      <c r="F100" s="69"/>
-      <c r="G100" s="69"/>
-      <c r="H100" s="69"/>
-    </row>
-    <row r="101" spans="2:8">
-      <c r="B101" s="69"/>
-      <c r="C101" s="69"/>
-      <c r="D101" s="69"/>
-      <c r="E101" s="69"/>
-      <c r="F101" s="69"/>
-      <c r="G101" s="69"/>
-      <c r="H101" s="69"/>
-    </row>
-    <row r="102" spans="2:8">
-      <c r="B102" s="69"/>
-      <c r="C102" s="69"/>
-      <c r="D102" s="69"/>
-      <c r="E102" s="69"/>
-      <c r="F102" s="69"/>
-      <c r="G102" s="69"/>
-      <c r="H102" s="69"/>
-    </row>
-    <row r="103" spans="2:8">
-      <c r="B103" s="69"/>
-      <c r="C103" s="69"/>
-      <c r="D103" s="69"/>
-      <c r="E103" s="69"/>
-      <c r="F103" s="69"/>
-      <c r="G103" s="69"/>
-      <c r="H103" s="69"/>
-    </row>
-    <row r="104" spans="2:8">
-      <c r="B104" s="69"/>
-      <c r="C104" s="69"/>
-      <c r="D104" s="69"/>
-      <c r="E104" s="69"/>
-      <c r="F104" s="69"/>
-      <c r="G104" s="69"/>
-      <c r="H104" s="69"/>
-    </row>
-    <row r="105" spans="2:8">
-      <c r="B105" s="69"/>
-      <c r="C105" s="69"/>
-      <c r="D105" s="69"/>
-      <c r="E105" s="69"/>
-      <c r="F105" s="69"/>
-      <c r="G105" s="69"/>
-      <c r="H105" s="69"/>
-    </row>
-    <row r="106" spans="2:8">
-      <c r="B106" s="69"/>
-      <c r="C106" s="69"/>
-      <c r="D106" s="69"/>
-      <c r="E106" s="69"/>
-      <c r="F106" s="69"/>
-      <c r="G106" s="69"/>
-      <c r="H106" s="69"/>
-    </row>
-    <row r="107" spans="2:8">
-      <c r="B107" s="69"/>
-      <c r="C107" s="69"/>
-      <c r="D107" s="69"/>
-      <c r="E107" s="69"/>
-      <c r="F107" s="69"/>
-      <c r="G107" s="69"/>
-      <c r="H107" s="69"/>
-    </row>
-    <row r="108" spans="2:8">
-      <c r="B108" s="69"/>
-      <c r="C108" s="69"/>
-      <c r="D108" s="69"/>
-      <c r="E108" s="69"/>
-      <c r="F108" s="69"/>
-      <c r="G108" s="69"/>
-      <c r="H108" s="69"/>
-    </row>
-    <row r="109" spans="2:8">
-      <c r="B109" s="69"/>
-      <c r="C109" s="69"/>
-      <c r="D109" s="69"/>
-      <c r="E109" s="69"/>
-      <c r="F109" s="69"/>
-      <c r="G109" s="69"/>
-      <c r="H109" s="69"/>
-    </row>
-    <row r="110" spans="2:8">
-      <c r="B110" s="69"/>
-      <c r="C110" s="69"/>
-      <c r="D110" s="69"/>
-      <c r="E110" s="69"/>
-      <c r="F110" s="69"/>
-      <c r="G110" s="69"/>
-      <c r="H110" s="69"/>
-    </row>
-    <row r="111" spans="2:8">
-      <c r="B111" s="69"/>
-      <c r="C111" s="69"/>
-      <c r="D111" s="69"/>
-      <c r="E111" s="69"/>
-      <c r="F111" s="69"/>
-      <c r="G111" s="69"/>
-      <c r="H111" s="69"/>
-    </row>
-    <row r="112" spans="2:8">
-      <c r="B112" s="69"/>
-      <c r="C112" s="69"/>
-      <c r="D112" s="69"/>
-      <c r="E112" s="69"/>
-      <c r="F112" s="69"/>
-      <c r="G112" s="69"/>
-      <c r="H112" s="69"/>
-    </row>
-    <row r="113" spans="2:8">
-      <c r="B113" s="69"/>
-      <c r="C113" s="69"/>
-      <c r="D113" s="69"/>
-      <c r="E113" s="69"/>
-      <c r="F113" s="69"/>
-      <c r="G113" s="69"/>
-      <c r="H113" s="69"/>
-    </row>
-    <row r="114" spans="2:8">
-      <c r="B114" s="69"/>
-      <c r="C114" s="69"/>
-      <c r="D114" s="69"/>
-      <c r="E114" s="69"/>
-      <c r="F114" s="69"/>
-      <c r="G114" s="69"/>
-      <c r="H114" s="69"/>
-    </row>
-    <row r="115" spans="2:8">
-      <c r="B115" s="69"/>
-      <c r="C115" s="69"/>
-      <c r="D115" s="69"/>
-      <c r="E115" s="69"/>
-      <c r="F115" s="69"/>
-      <c r="G115" s="69"/>
-      <c r="H115" s="69"/>
-    </row>
-    <row r="116" spans="2:8">
-      <c r="B116" s="69"/>
-      <c r="C116" s="69"/>
-      <c r="D116" s="69"/>
-      <c r="E116" s="69"/>
-      <c r="F116" s="69"/>
-      <c r="G116" s="69"/>
-      <c r="H116" s="69"/>
-    </row>
-    <row r="117" spans="2:8">
-      <c r="B117" s="69"/>
-      <c r="C117" s="69"/>
-      <c r="D117" s="69"/>
-      <c r="E117" s="69"/>
-      <c r="F117" s="69"/>
-      <c r="G117" s="69"/>
-      <c r="H117" s="69"/>
-    </row>
-    <row r="118" spans="2:8">
-      <c r="B118" s="69"/>
-      <c r="C118" s="69"/>
-      <c r="D118" s="69"/>
-      <c r="E118" s="69"/>
-      <c r="F118" s="69"/>
-      <c r="G118" s="69"/>
-      <c r="H118" s="69"/>
-    </row>
-    <row r="119" spans="2:8">
-      <c r="B119" s="69"/>
-      <c r="C119" s="69"/>
-      <c r="D119" s="69"/>
-      <c r="E119" s="69"/>
-      <c r="F119" s="69"/>
-      <c r="G119" s="69"/>
-      <c r="H119" s="69"/>
-    </row>
-    <row r="120" spans="2:8">
-      <c r="B120" s="69"/>
-      <c r="C120" s="69"/>
-      <c r="D120" s="69"/>
-      <c r="E120" s="69"/>
-      <c r="F120" s="69"/>
-      <c r="G120" s="69"/>
-      <c r="H120" s="69"/>
-    </row>
-    <row r="121" spans="2:8">
-      <c r="B121" s="69"/>
-      <c r="C121" s="69"/>
-      <c r="D121" s="69"/>
-      <c r="E121" s="69"/>
-      <c r="F121" s="69"/>
-      <c r="G121" s="69"/>
-      <c r="H121" s="69"/>
-    </row>
-    <row r="135" spans="2:10">
-      <c r="B135" t="s">
-        <v>247</v>
-      </c>
-      <c r="C135" t="s">
-        <v>248</v>
-      </c>
-      <c r="D135" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="136" spans="2:10" ht="30" customHeight="1">
-      <c r="B136" s="69" t="s">
+      <c r="D125" s="92"/>
+    </row>
+    <row r="126" spans="2:4" ht="30" customHeight="1">
+      <c r="B126" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C126" s="92" t="s">
+        <v>228</v>
+      </c>
+      <c r="D126" s="92"/>
+    </row>
+    <row r="127" spans="2:4" ht="30" customHeight="1">
+      <c r="B127" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="C127" s="92" t="s">
+        <v>232</v>
+      </c>
+      <c r="D127" s="92"/>
+    </row>
+    <row r="128" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B128" s="92"/>
+      <c r="C128" s="92"/>
+      <c r="D128" s="92"/>
+    </row>
+    <row r="129" spans="2:4" ht="30" customHeight="1">
+      <c r="B129" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="C129" s="92" t="s">
+        <v>235</v>
+      </c>
+      <c r="D129" s="92"/>
+    </row>
+    <row r="130" spans="2:4" ht="30" customHeight="1">
+      <c r="B130" s="92" t="s">
         <v>224</v>
       </c>
-      <c r="C136" s="69"/>
-      <c r="D136" s="69"/>
-    </row>
-    <row r="137" spans="2:10" ht="30" customHeight="1">
-      <c r="B137" s="96" t="s">
-        <v>223</v>
-      </c>
-      <c r="C137" s="96" t="s">
+      <c r="C130" s="92" t="s">
         <v>225</v>
       </c>
-      <c r="D137" s="96"/>
-      <c r="J137" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="138" spans="2:10" ht="30" customHeight="1">
-      <c r="B138" s="96" t="s">
-        <v>250</v>
-      </c>
-      <c r="C138" s="96" t="s">
-        <v>251</v>
-      </c>
-      <c r="D138" s="96"/>
-    </row>
-    <row r="139" spans="2:10" ht="30" customHeight="1">
-      <c r="B139" s="96" t="s">
+      <c r="D130" s="92"/>
+    </row>
+    <row r="131" spans="2:4" ht="30" customHeight="1">
+      <c r="B131" s="92" t="s">
         <v>226</v>
       </c>
-      <c r="C139" s="96" t="s">
-        <v>239</v>
-      </c>
-      <c r="D139" s="96"/>
-    </row>
-    <row r="140" spans="2:10" ht="30" customHeight="1">
-      <c r="B140" s="96" t="s">
+      <c r="C131" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="C140" s="96" t="s">
-        <v>240</v>
-      </c>
-      <c r="D140" s="96"/>
-    </row>
-    <row r="141" spans="2:10" ht="30" customHeight="1">
-      <c r="B141" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="C141" s="96" t="s">
-        <v>229</v>
-      </c>
-      <c r="D141" s="96"/>
-    </row>
-    <row r="142" spans="2:10" ht="5.25" customHeight="1">
-      <c r="B142" s="96"/>
-      <c r="C142" s="96"/>
-      <c r="D142" s="96"/>
-    </row>
-    <row r="143" spans="2:10" ht="30" customHeight="1">
-      <c r="B143" s="96" t="s">
-        <v>230</v>
-      </c>
-      <c r="C143" s="96" t="s">
-        <v>231</v>
-      </c>
-      <c r="D143" s="96"/>
-    </row>
-    <row r="144" spans="2:10" ht="30" customHeight="1">
-      <c r="B144" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="C144" s="96" t="s">
-        <v>232</v>
-      </c>
-      <c r="D144" s="96"/>
-    </row>
-    <row r="145" spans="2:4" ht="30" customHeight="1">
-      <c r="B145" s="96" t="s">
-        <v>228</v>
-      </c>
-      <c r="C145" s="96" t="s">
-        <v>238</v>
-      </c>
-      <c r="D145" s="96"/>
-    </row>
-    <row r="146" spans="2:4" ht="30" customHeight="1">
-      <c r="B146" s="96" t="s">
-        <v>242</v>
-      </c>
-      <c r="C146" s="96" t="s">
-        <v>243</v>
-      </c>
-      <c r="D146" s="96"/>
-    </row>
-    <row r="147" spans="2:4" ht="5.25" customHeight="1">
-      <c r="B147" s="96"/>
-      <c r="C147" s="96"/>
-      <c r="D147" s="96"/>
-    </row>
-    <row r="148" spans="2:4" ht="30" customHeight="1">
-      <c r="B148" s="96" t="s">
+      <c r="D131" s="92"/>
+    </row>
+    <row r="132" spans="2:4" ht="4.5" customHeight="1">
+      <c r="B132" s="92"/>
+      <c r="C132" s="92"/>
+      <c r="D132" s="92"/>
+    </row>
+    <row r="133" spans="2:4" ht="30" customHeight="1">
+      <c r="B133" s="93" t="s">
         <v>233</v>
       </c>
-      <c r="C148" s="96" t="s">
-        <v>246</v>
-      </c>
-      <c r="D148" s="96"/>
-    </row>
-    <row r="149" spans="2:4" ht="30" customHeight="1">
-      <c r="B149" s="96" t="s">
+      <c r="C133" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="C149" s="96" t="s">
-        <v>235</v>
-      </c>
-      <c r="D149" s="96"/>
-    </row>
-    <row r="150" spans="2:4" ht="30" customHeight="1">
-      <c r="B150" s="96" t="s">
-        <v>236</v>
-      </c>
-      <c r="C150" s="96" t="s">
-        <v>237</v>
-      </c>
-      <c r="D150" s="96"/>
-    </row>
-    <row r="151" spans="2:4" ht="4.5" customHeight="1">
-      <c r="B151" s="96"/>
-      <c r="C151" s="96"/>
-      <c r="D151" s="96"/>
-    </row>
-    <row r="152" spans="2:4" ht="30" customHeight="1">
-      <c r="B152" s="97" t="s">
-        <v>244</v>
-      </c>
-      <c r="C152" s="97" t="s">
-        <v>245</v>
-      </c>
-      <c r="D152" s="97"/>
+      <c r="D133" s="93"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H23" r:id="rId1"/>
-    <hyperlink ref="D24" r:id="rId2"/>
-    <hyperlink ref="D25" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E12"/>
+  <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="52.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5">
-      <c r="B2" s="69"/>
-      <c r="C2" s="69" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="69" t="s">
+      <c r="D2" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="66" t="s">
         <v>275</v>
       </c>
-      <c r="E2" s="69" t="s">
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="66">
+        <v>1</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="99">
+        <v>41442</v>
+      </c>
+      <c r="E3" s="66"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="66">
+        <v>2</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>266</v>
+      </c>
+      <c r="E4" s="66"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="66">
+        <v>3</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="66">
+        <v>4</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="99">
+        <v>41426</v>
+      </c>
+      <c r="E6" s="66"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="66">
+        <v>5</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="99">
+        <v>41425</v>
+      </c>
+      <c r="E7" s="66"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="66">
+        <v>6</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" s="99">
+        <v>41427</v>
+      </c>
+      <c r="E8" s="66"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="66">
+        <v>7</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="99">
+        <v>41428</v>
+      </c>
+      <c r="E9" s="66"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="66">
+        <v>8</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="66">
+        <v>9</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="66">
+        <v>10</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="C14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+    </row>
+    <row r="16" spans="2:5" ht="28.5">
+      <c r="C16" s="108" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="108" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="42.75">
+      <c r="C17" s="108" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="108" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="57">
+      <c r="C18" s="108" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="108" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="28.5">
+      <c r="C19" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="108" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="69">
-        <v>1</v>
-      </c>
-      <c r="C3" s="69" t="s">
-        <v>274</v>
-      </c>
-      <c r="D3" s="103">
-        <v>41442</v>
-      </c>
-      <c r="E3" s="69"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="69">
-        <v>2</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>276</v>
-      </c>
-      <c r="D4" s="69" t="s">
-        <v>277</v>
-      </c>
-      <c r="E4" s="69"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="69">
-        <v>3</v>
-      </c>
-      <c r="C5" s="69" t="s">
-        <v>285</v>
-      </c>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="69">
-        <v>4</v>
-      </c>
-      <c r="C6" s="69" t="s">
-        <v>278</v>
-      </c>
-      <c r="D6" s="103">
-        <v>41426</v>
-      </c>
-      <c r="E6" s="69"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="69">
-        <v>5</v>
-      </c>
-      <c r="C7" s="69" t="s">
-        <v>279</v>
-      </c>
-      <c r="D7" s="103">
-        <v>41425</v>
-      </c>
-      <c r="E7" s="69"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="69">
-        <v>6</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>280</v>
-      </c>
-      <c r="D8" s="103">
-        <v>41427</v>
-      </c>
-      <c r="E8" s="69"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="69">
-        <v>7</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>281</v>
-      </c>
-      <c r="D9" s="103">
-        <v>41428</v>
-      </c>
-      <c r="E9" s="69"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="69">
-        <v>8</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>282</v>
-      </c>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="69">
-        <v>9</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>283</v>
-      </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="69">
-        <v>10</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>284</v>
-      </c>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
+    <row r="20" spans="3:4" ht="28.5">
+      <c r="C20" s="108"/>
+      <c r="D20" s="108" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" s="109"/>
+      <c r="D21" s="109" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="109" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="C23" s="110" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="109"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wybor stali itp, jakiś zapomniany komit sprzed miesiaca
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="307">
   <si>
     <t>Id</t>
   </si>
@@ -1006,9 +1006,6 @@
   </si>
   <si>
     <t>Sebastian Kita www.centrostal.com.pl</t>
-  </si>
-  <si>
-    <t>do uzgodnienia</t>
   </si>
   <si>
     <t>2390/1000</t>
@@ -3923,7 +3920,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740566"/>
+          <c:w val="0.71441426071740555"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4241,8 +4238,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288574"/>
-          <c:y val="0.29353966170895557"/>
+          <c:x val="0.86438523325288585"/>
+          <c:y val="0.29353966170895562"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -4252,7 +4249,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4503,7 +4500,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4705,7 +4702,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000003" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4858,7 +4855,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4874,10 +4871,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961883"/>
-          <c:y val="3.2882035578886061E-2"/>
+          <c:x val="0.1718156283096188"/>
+          <c:y val="3.2882035578886068E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420123"/>
+          <c:h val="0.63861876640420134"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5079,7 +5076,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9727,7 +9724,7 @@
   <dimension ref="A1:K134"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9956,10 +9953,13 @@
       <c r="E9" s="114">
         <v>2.23</v>
       </c>
-      <c r="F9" s="115" t="s">
-        <v>306</v>
-      </c>
-      <c r="G9" s="116"/>
+      <c r="F9" s="115">
+        <v>0</v>
+      </c>
+      <c r="G9" s="116">
+        <f>C9*F33+D9*G33+E9*H33+F9</f>
+        <v>3902.86</v>
+      </c>
       <c r="H9" s="96" t="s">
         <v>294</v>
       </c>
@@ -10028,7 +10028,7 @@
         <v>303</v>
       </c>
       <c r="C12" s="96">
-        <v>5.52</v>
+        <v>2.52</v>
       </c>
       <c r="D12" s="97">
         <v>2.39</v>
@@ -10039,7 +10039,10 @@
       <c r="F12" s="97">
         <v>0</v>
       </c>
-      <c r="G12" s="98"/>
+      <c r="G12" s="98">
+        <f>C12*F33+D12*G33+E12*H33+F12</f>
+        <v>3979.1099999999997</v>
+      </c>
       <c r="H12" s="96"/>
       <c r="I12" s="96"/>
     </row>
@@ -10550,7 +10553,7 @@
         <v>5.52</v>
       </c>
       <c r="J44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="45" spans="2:11" ht="15">

</xml_diff>

<commit_message>
nowa lista odbiorców zapytania o cene stali
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="315">
   <si>
     <t>Id</t>
   </si>
@@ -1009,6 +1009,30 @@
   </si>
   <si>
     <t>2390/1000</t>
+  </si>
+  <si>
+    <t>brutto</t>
+  </si>
+  <si>
+    <t>ah@komp-stal.pl</t>
+  </si>
+  <si>
+    <t>car-met.pl</t>
+  </si>
+  <si>
+    <t>biuro@stalkat.pl</t>
+  </si>
+  <si>
+    <t>Wyslane 2013-08-15</t>
+  </si>
+  <si>
+    <t>Centrozłom Wrocław</t>
+  </si>
+  <si>
+    <t>dcstal@dcstal.com.pl</t>
+  </si>
+  <si>
+    <t>centrostal@centrostal.com.pl</t>
   </si>
 </sst>
 </file>
@@ -1489,7 +1513,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1716,6 +1740,10 @@
     <xf numFmtId="3" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -3920,7 +3948,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740555"/>
+          <c:w val="0.71441426071740532"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4200,24 +4228,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62755584"/>
-        <c:axId val="62757120"/>
+        <c:axId val="52205440"/>
+        <c:axId val="52206976"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62755584"/>
+        <c:axId val="52205440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62757120"/>
+        <c:crossAx val="52206976"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62757120"/>
+        <c:axId val="52206976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -4227,7 +4255,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62755584"/>
+        <c:crossAx val="52205440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4238,8 +4266,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288585"/>
-          <c:y val="0.29353966170895562"/>
+          <c:x val="0.86438523325288619"/>
+          <c:y val="0.29353966170895573"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -4249,7 +4277,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4461,24 +4489,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62815232"/>
-        <c:axId val="62837504"/>
+        <c:axId val="70299008"/>
+        <c:axId val="70304896"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62815232"/>
+        <c:axId val="70299008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62837504"/>
+        <c:crossAx val="70304896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62837504"/>
+        <c:axId val="70304896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -4488,7 +4516,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62815232"/>
+        <c:crossAx val="70299008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4500,7 +4528,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4663,24 +4691,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63972864"/>
-        <c:axId val="63974400"/>
+        <c:axId val="71370624"/>
+        <c:axId val="71372160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63972864"/>
+        <c:axId val="71370624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63974400"/>
+        <c:crossAx val="71372160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63974400"/>
+        <c:axId val="71372160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -4690,7 +4718,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63972864"/>
+        <c:crossAx val="71370624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4702,7 +4730,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4817,11 +4845,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64055936"/>
-        <c:axId val="64057728"/>
+        <c:axId val="71384064"/>
+        <c:axId val="71443200"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64055936"/>
+        <c:axId val="71384064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4829,13 +4857,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64057728"/>
+        <c:crossAx val="71443200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64057728"/>
+        <c:axId val="71443200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4843,7 +4871,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64055936"/>
+        <c:crossAx val="71384064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4855,7 +4883,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4871,10 +4899,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1718156283096188"/>
-          <c:y val="3.2882035578886068E-2"/>
+          <c:x val="0.17181562830961875"/>
+          <c:y val="3.2882035578886089E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420134"/>
+          <c:h val="0.63861876640420157"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5037,11 +5065,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64140032"/>
-        <c:axId val="64141568"/>
+        <c:axId val="71521408"/>
+        <c:axId val="71522944"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64140032"/>
+        <c:axId val="71521408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5049,13 +5077,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64141568"/>
+        <c:crossAx val="71522944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64141568"/>
+        <c:axId val="71522944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5064,7 +5092,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64140032"/>
+        <c:crossAx val="71521408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5076,7 +5104,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5352,8 +5380,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B117:D134" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B117:D134"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B124:D141" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B124:D141"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Temat" dataDxfId="2"/>
     <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
@@ -9721,25 +9749,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K134"/>
+  <dimension ref="A1:L141"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="14.77734375" customWidth="1"/>
     <col min="4" max="4" width="17.88671875" customWidth="1"/>
     <col min="5" max="5" width="17.5546875" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19" customWidth="1"/>
+    <col min="9" max="9" width="10.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" s="94"/>
       <c r="B1" s="94"/>
       <c r="C1" s="94"/>
@@ -9751,8 +9779,9 @@
       <c r="I1" s="94"/>
       <c r="J1" s="94"/>
       <c r="K1" s="94"/>
-    </row>
-    <row r="2" spans="1:11" ht="21" customHeight="1">
+      <c r="L1" s="94"/>
+    </row>
+    <row r="2" spans="1:12" ht="21" customHeight="1">
       <c r="A2" s="94"/>
       <c r="B2" s="95" t="s">
         <v>241</v>
@@ -9772,16 +9801,17 @@
       <c r="G2" s="95" t="s">
         <v>257</v>
       </c>
-      <c r="H2" s="95" t="s">
+      <c r="H2" s="95"/>
+      <c r="I2" s="95" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="95" t="s">
+      <c r="J2" s="95" t="s">
         <v>276</v>
       </c>
-      <c r="J2" s="94"/>
       <c r="K2" s="94"/>
-    </row>
-    <row r="3" spans="1:11" ht="32.25">
+      <c r="L2" s="94"/>
+    </row>
+    <row r="3" spans="1:12" ht="32.25">
       <c r="A3" s="94"/>
       <c r="B3" s="104" t="s">
         <v>246</v>
@@ -9802,16 +9832,17 @@
         <f>F3+D3</f>
         <v>6239</v>
       </c>
-      <c r="H3" s="104" t="s">
+      <c r="H3" s="106"/>
+      <c r="I3" s="104" t="s">
         <v>177</v>
       </c>
-      <c r="I3" s="104">
+      <c r="J3" s="104">
         <v>600939523</v>
       </c>
-      <c r="J3" s="94"/>
       <c r="K3" s="94"/>
-    </row>
-    <row r="4" spans="1:11" ht="21.75">
+      <c r="L3" s="94"/>
+    </row>
+    <row r="4" spans="1:12" ht="21.75">
       <c r="A4" s="94"/>
       <c r="B4" s="96" t="s">
         <v>251</v>
@@ -9832,16 +9863,17 @@
         <f t="shared" ref="G4:G5" si="0">F4+D4</f>
         <v>16900</v>
       </c>
-      <c r="H4" s="96" t="s">
+      <c r="H4" s="98"/>
+      <c r="I4" s="96" t="s">
         <v>250</v>
       </c>
-      <c r="I4" s="96">
+      <c r="J4" s="96">
         <v>713169022</v>
       </c>
-      <c r="J4" s="94"/>
       <c r="K4" s="94"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="94"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="94"/>
       <c r="B5" s="96" t="s">
         <v>254</v>
@@ -9862,14 +9894,15 @@
         <f t="shared" si="0"/>
         <v>6510</v>
       </c>
-      <c r="H5" s="96"/>
-      <c r="I5" s="96">
+      <c r="H5" s="98"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96">
         <v>508870624</v>
       </c>
-      <c r="J5" s="94"/>
       <c r="K5" s="94"/>
-    </row>
-    <row r="6" spans="1:11" ht="32.25">
+      <c r="L5" s="94"/>
+    </row>
+    <row r="6" spans="1:12" ht="32.25">
       <c r="A6" s="94"/>
       <c r="B6" s="96" t="s">
         <v>258</v>
@@ -9889,16 +9922,17 @@
       <c r="G6" s="98">
         <v>6553</v>
       </c>
-      <c r="H6" s="96" t="s">
+      <c r="H6" s="98"/>
+      <c r="I6" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="I6" s="96" t="s">
+      <c r="J6" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="J6" s="94"/>
       <c r="K6" s="94"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="94"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="94"/>
       <c r="B7" s="94"/>
       <c r="C7" s="94"/>
@@ -9910,8 +9944,9 @@
       <c r="I7" s="94"/>
       <c r="J7" s="94"/>
       <c r="K7" s="94"/>
-    </row>
-    <row r="8" spans="1:11" ht="21.75">
+      <c r="L7" s="94"/>
+    </row>
+    <row r="8" spans="1:12" ht="21.75">
       <c r="A8" s="94"/>
       <c r="B8" s="95" t="s">
         <v>218</v>
@@ -9932,15 +9967,18 @@
         <v>304</v>
       </c>
       <c r="H8" s="95" t="s">
+        <v>307</v>
+      </c>
+      <c r="I8" s="95" t="s">
         <v>247</v>
       </c>
-      <c r="I8" s="95" t="s">
+      <c r="J8" s="95" t="s">
         <v>276</v>
       </c>
-      <c r="J8" s="94"/>
       <c r="K8" s="94"/>
-    </row>
-    <row r="9" spans="1:11" ht="21.75">
+      <c r="L8" s="94"/>
+    </row>
+    <row r="9" spans="1:12" ht="21.75">
       <c r="B9" s="114" t="s">
         <v>293</v>
       </c>
@@ -9957,18 +9995,22 @@
         <v>0</v>
       </c>
       <c r="G9" s="116">
-        <f>C9*F33+D9*G33+E9*H33+F9</f>
+        <f>C9*F40+D9*G40+E9*I40+F9</f>
         <v>3902.86</v>
       </c>
-      <c r="H9" s="96" t="s">
+      <c r="H9" s="116">
+        <f>G9*1.23</f>
+        <v>4800.5178000000005</v>
+      </c>
+      <c r="I9" s="96" t="s">
         <v>294</v>
       </c>
-      <c r="I9" s="96" t="s">
+      <c r="J9" s="96" t="s">
         <v>295</v>
       </c>
-      <c r="J9" s="96"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="K9" s="96"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="B10" s="96" t="s">
         <v>296</v>
       </c>
@@ -9985,18 +10027,22 @@
         <v>150</v>
       </c>
       <c r="G10" s="98">
-        <f>C10*F33+D10*G33+E10*H33+150</f>
+        <f>C10*F40+D10*G40+E10*I40+150</f>
         <v>4298.82</v>
       </c>
-      <c r="H10" s="96" t="s">
+      <c r="H10" s="116">
+        <f t="shared" ref="H10:H11" si="1">G10*1.23</f>
+        <v>5287.5485999999992</v>
+      </c>
+      <c r="I10" s="96" t="s">
         <v>297</v>
       </c>
-      <c r="I10" s="96">
+      <c r="J10" s="96">
         <v>607821822</v>
       </c>
-      <c r="J10" s="96"/>
-    </row>
-    <row r="11" spans="1:11" ht="32.25">
+      <c r="K10" s="96"/>
+    </row>
+    <row r="11" spans="1:12" ht="32.25">
       <c r="B11" s="96" t="s">
         <v>298</v>
       </c>
@@ -10013,596 +10059,586 @@
         <v>300</v>
       </c>
       <c r="G11" s="98">
-        <f>C11*F33+D11*G33+E11*H33+F11</f>
+        <f>C11*F40+D11*G40+E11*I40+F11</f>
         <v>4251.5</v>
       </c>
-      <c r="H11" s="96" t="s">
+      <c r="H11" s="116">
+        <f t="shared" si="1"/>
+        <v>5229.3450000000003</v>
+      </c>
+      <c r="I11" s="96" t="s">
         <v>305</v>
       </c>
-      <c r="I11" s="121">
+      <c r="J11" s="121">
         <v>692287354</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:12">
       <c r="B12" s="96" t="s">
         <v>303</v>
       </c>
       <c r="C12" s="96">
-        <v>2.52</v>
+        <v>2.5</v>
       </c>
       <c r="D12" s="97">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="E12" s="96">
         <v>2.39</v>
-      </c>
-      <c r="E12" s="96">
-        <v>2.2999999999999998</v>
       </c>
       <c r="F12" s="97">
         <v>0</v>
       </c>
       <c r="G12" s="98">
-        <f>C12*F33+D12*G33+E12*H33+F12</f>
-        <v>3979.1099999999997</v>
-      </c>
-      <c r="H12" s="96"/>
+        <f>C12*F40+D12*G40+E12*I40+F12</f>
+        <v>3982.58</v>
+      </c>
+      <c r="H12" s="116">
+        <f>G12*1.23*1.1</f>
+        <v>5388.4307400000007</v>
+      </c>
       <c r="I12" s="96"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="111"/>
+      <c r="J12" s="96"/>
+    </row>
+    <row r="13" spans="1:12" ht="21.75">
+      <c r="B13" s="123" t="s">
+        <v>311</v>
+      </c>
       <c r="C13" s="111"/>
       <c r="D13" s="112"/>
       <c r="E13" s="111"/>
       <c r="F13" s="112"/>
       <c r="G13" s="113"/>
-      <c r="H13" s="111"/>
+      <c r="H13" s="113"/>
       <c r="I13" s="111"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="B14" t="s">
+      <c r="J13" s="111"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="B14" s="96" t="s">
+        <v>308</v>
+      </c>
+      <c r="C14" s="111"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="111"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="111"/>
+      <c r="J14" s="111"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="B15" s="111" t="s">
+        <v>309</v>
+      </c>
+      <c r="C15" s="111"/>
+      <c r="D15" s="112"/>
+      <c r="E15" s="111"/>
+      <c r="F15" s="112"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="111"/>
+      <c r="J15" s="111"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" s="111" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="111"/>
+      <c r="D16" s="112"/>
+      <c r="E16" s="111"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="111"/>
+      <c r="J16" s="111"/>
+    </row>
+    <row r="17" spans="2:10">
+      <c r="B17" s="111" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="111"/>
+      <c r="D17" s="112"/>
+      <c r="E17" s="111"/>
+      <c r="F17" s="112"/>
+      <c r="G17" s="113"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="111"/>
+      <c r="J17" s="111"/>
+    </row>
+    <row r="18" spans="2:10">
+      <c r="B18" s="111" t="s">
+        <v>313</v>
+      </c>
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="111"/>
+      <c r="F18" s="112"/>
+      <c r="G18" s="113"/>
+      <c r="H18" s="113"/>
+      <c r="I18" s="111"/>
+      <c r="J18" s="111"/>
+    </row>
+    <row r="19" spans="2:10" ht="21.75">
+      <c r="B19" s="111" t="s">
+        <v>314</v>
+      </c>
+      <c r="C19" s="111"/>
+      <c r="D19" s="112"/>
+      <c r="E19" s="111"/>
+      <c r="F19" s="112"/>
+      <c r="G19" s="113"/>
+      <c r="H19" s="113"/>
+      <c r="I19" s="111"/>
+      <c r="J19" s="111"/>
+    </row>
+    <row r="20" spans="2:10">
+      <c r="B20" s="96" t="s">
+        <v>295</v>
+      </c>
+      <c r="C20" s="111"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="111"/>
+      <c r="F20" s="112"/>
+      <c r="G20" s="113"/>
+      <c r="H20" s="113"/>
+      <c r="I20" s="111"/>
+      <c r="J20" s="111"/>
+    </row>
+    <row r="21" spans="2:10">
+      <c r="B21" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15" thickBot="1"/>
-    <row r="16" spans="1:11">
-      <c r="B16" s="68" t="s">
+    <row r="22" spans="2:10" ht="15" thickBot="1"/>
+    <row r="23" spans="2:10">
+      <c r="B23" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C23" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="D16" s="69" t="s">
+      <c r="D23" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="E16" s="76" t="s">
+      <c r="E23" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="F16" s="68" t="s">
+      <c r="F23" s="68" t="s">
         <v>185</v>
       </c>
-      <c r="G16" s="69" t="s">
+      <c r="G23" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="H16" s="70" t="s">
+      <c r="H23" s="76"/>
+      <c r="I23" s="70" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="71">
+    <row r="24" spans="2:10">
+      <c r="B24" s="71">
         <v>1</v>
-      </c>
-      <c r="C17" s="66">
-        <v>8</v>
-      </c>
-      <c r="D17" s="66">
-        <v>9640</v>
-      </c>
-      <c r="E17" s="77">
-        <v>16</v>
-      </c>
-      <c r="F17" s="71">
-        <f>E17*D17/1000</f>
-        <v>154.24</v>
-      </c>
-      <c r="G17" s="66"/>
-      <c r="H17" s="72"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="71">
-        <v>2</v>
-      </c>
-      <c r="C18" s="66">
-        <v>8</v>
-      </c>
-      <c r="D18" s="66">
-        <v>6870</v>
-      </c>
-      <c r="E18" s="77">
-        <v>116</v>
-      </c>
-      <c r="F18" s="71">
-        <f t="shared" ref="F18:F29" si="1">E18*D18/1000</f>
-        <v>796.92</v>
-      </c>
-      <c r="G18" s="66"/>
-      <c r="H18" s="72"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="71">
-        <v>3</v>
-      </c>
-      <c r="C19" s="66">
-        <v>8</v>
-      </c>
-      <c r="D19" s="66">
-        <v>7970</v>
-      </c>
-      <c r="E19" s="77">
-        <v>28</v>
-      </c>
-      <c r="F19" s="71">
-        <f t="shared" si="1"/>
-        <v>223.16</v>
-      </c>
-      <c r="G19" s="66"/>
-      <c r="H19" s="72"/>
-    </row>
-    <row r="20" spans="2:8">
-      <c r="B20" s="71">
-        <v>4</v>
-      </c>
-      <c r="C20" s="66">
-        <v>8</v>
-      </c>
-      <c r="D20" s="66">
-        <v>7540</v>
-      </c>
-      <c r="E20" s="77">
-        <v>8</v>
-      </c>
-      <c r="F20" s="71">
-        <f t="shared" si="1"/>
-        <v>60.32</v>
-      </c>
-      <c r="G20" s="66"/>
-      <c r="H20" s="72"/>
-    </row>
-    <row r="21" spans="2:8">
-      <c r="B21" s="71">
-        <v>5</v>
-      </c>
-      <c r="C21" s="66">
-        <v>8</v>
-      </c>
-      <c r="D21" s="66">
-        <v>3180</v>
-      </c>
-      <c r="E21" s="77">
-        <v>10</v>
-      </c>
-      <c r="F21" s="71">
-        <f t="shared" si="1"/>
-        <v>31.8</v>
-      </c>
-      <c r="G21" s="66"/>
-      <c r="H21" s="72"/>
-    </row>
-    <row r="22" spans="2:8">
-      <c r="B22" s="71">
-        <v>6</v>
-      </c>
-      <c r="C22" s="66">
-        <v>8</v>
-      </c>
-      <c r="D22" s="66">
-        <v>9140</v>
-      </c>
-      <c r="E22" s="77">
-        <v>54</v>
-      </c>
-      <c r="F22" s="71">
-        <f t="shared" si="1"/>
-        <v>493.56</v>
-      </c>
-      <c r="G22" s="66"/>
-      <c r="H22" s="72"/>
-    </row>
-    <row r="23" spans="2:8">
-      <c r="B23" s="71">
-        <v>7</v>
-      </c>
-      <c r="C23" s="66">
-        <v>8</v>
-      </c>
-      <c r="D23" s="66">
-        <v>10040</v>
-      </c>
-      <c r="E23" s="77">
-        <v>36</v>
-      </c>
-      <c r="F23" s="71">
-        <f t="shared" si="1"/>
-        <v>361.44</v>
-      </c>
-      <c r="G23" s="66"/>
-      <c r="H23" s="72"/>
-    </row>
-    <row r="24" spans="2:8">
-      <c r="B24" s="71">
-        <v>8</v>
       </c>
       <c r="C24" s="66">
         <v>8</v>
       </c>
       <c r="D24" s="66">
-        <v>8340</v>
+        <v>9640</v>
       </c>
       <c r="E24" s="77">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F24" s="71">
-        <f t="shared" si="1"/>
-        <v>283.56</v>
+        <f>E24*D24/1000</f>
+        <v>154.24</v>
       </c>
       <c r="G24" s="66"/>
-      <c r="H24" s="72"/>
-    </row>
-    <row r="25" spans="2:8">
+      <c r="H24" s="77"/>
+      <c r="I24" s="72"/>
+    </row>
+    <row r="25" spans="2:10">
       <c r="B25" s="71">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C25" s="66">
         <v>8</v>
       </c>
       <c r="D25" s="66">
-        <v>2500</v>
+        <v>6870</v>
       </c>
       <c r="E25" s="77">
-        <v>83</v>
+        <v>116</v>
       </c>
       <c r="F25" s="71">
-        <f t="shared" si="1"/>
-        <v>207.5</v>
+        <f t="shared" ref="F25:F36" si="2">E25*D25/1000</f>
+        <v>796.92</v>
       </c>
       <c r="G25" s="66"/>
-      <c r="H25" s="72"/>
-    </row>
-    <row r="26" spans="2:8">
+      <c r="H25" s="77"/>
+      <c r="I25" s="72"/>
+    </row>
+    <row r="26" spans="2:10">
       <c r="B26" s="71">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C26" s="66">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D26" s="66">
-        <v>970</v>
+        <v>7970</v>
       </c>
       <c r="E26" s="77">
-        <v>38</v>
-      </c>
-      <c r="F26" s="71"/>
-      <c r="G26" s="66">
-        <f>E26*D26/1000</f>
-        <v>36.86</v>
-      </c>
-      <c r="H26" s="72"/>
-    </row>
-    <row r="27" spans="2:8">
+        <v>28</v>
+      </c>
+      <c r="F26" s="71">
+        <f t="shared" si="2"/>
+        <v>223.16</v>
+      </c>
+      <c r="G26" s="66"/>
+      <c r="H26" s="77"/>
+      <c r="I26" s="72"/>
+    </row>
+    <row r="27" spans="2:10">
       <c r="B27" s="71">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C27" s="66">
         <v>8</v>
       </c>
       <c r="D27" s="66">
-        <v>1780</v>
+        <v>7540</v>
       </c>
       <c r="E27" s="77">
-        <v>240</v>
+        <v>8</v>
       </c>
       <c r="F27" s="71">
-        <f t="shared" si="1"/>
-        <v>427.2</v>
+        <f t="shared" si="2"/>
+        <v>60.32</v>
       </c>
       <c r="G27" s="66"/>
-      <c r="H27" s="72"/>
-    </row>
-    <row r="28" spans="2:8">
+      <c r="H27" s="77"/>
+      <c r="I27" s="72"/>
+    </row>
+    <row r="28" spans="2:10">
       <c r="B28" s="71">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C28" s="66">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D28" s="66">
-        <v>78000</v>
+        <v>3180</v>
       </c>
       <c r="E28" s="77">
-        <v>4</v>
-      </c>
-      <c r="F28" s="71"/>
+        <v>10</v>
+      </c>
+      <c r="F28" s="71">
+        <f t="shared" si="2"/>
+        <v>31.8</v>
+      </c>
       <c r="G28" s="66"/>
-      <c r="H28" s="72">
-        <f>E28*D28/1000</f>
-        <v>312</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8">
+      <c r="H28" s="77"/>
+      <c r="I28" s="72"/>
+    </row>
+    <row r="29" spans="2:10">
       <c r="B29" s="71">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C29" s="66">
         <v>8</v>
       </c>
       <c r="D29" s="66">
+        <v>9140</v>
+      </c>
+      <c r="E29" s="77">
+        <v>54</v>
+      </c>
+      <c r="F29" s="71">
+        <f t="shared" si="2"/>
+        <v>493.56</v>
+      </c>
+      <c r="G29" s="66"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="72"/>
+    </row>
+    <row r="30" spans="2:10">
+      <c r="B30" s="71">
+        <v>7</v>
+      </c>
+      <c r="C30" s="66">
+        <v>8</v>
+      </c>
+      <c r="D30" s="66">
+        <v>10040</v>
+      </c>
+      <c r="E30" s="77">
+        <v>36</v>
+      </c>
+      <c r="F30" s="71">
+        <f t="shared" si="2"/>
+        <v>361.44</v>
+      </c>
+      <c r="G30" s="66"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="72"/>
+    </row>
+    <row r="31" spans="2:10">
+      <c r="B31" s="71">
+        <v>8</v>
+      </c>
+      <c r="C31" s="66">
+        <v>8</v>
+      </c>
+      <c r="D31" s="66">
+        <v>8340</v>
+      </c>
+      <c r="E31" s="77">
+        <v>34</v>
+      </c>
+      <c r="F31" s="71">
+        <f t="shared" si="2"/>
+        <v>283.56</v>
+      </c>
+      <c r="G31" s="66"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="72"/>
+    </row>
+    <row r="32" spans="2:10">
+      <c r="B32" s="71">
+        <v>9</v>
+      </c>
+      <c r="C32" s="66">
+        <v>8</v>
+      </c>
+      <c r="D32" s="66">
+        <v>2500</v>
+      </c>
+      <c r="E32" s="77">
+        <v>83</v>
+      </c>
+      <c r="F32" s="71">
+        <f t="shared" si="2"/>
+        <v>207.5</v>
+      </c>
+      <c r="G32" s="66"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="72"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" s="71">
+        <v>10</v>
+      </c>
+      <c r="C33" s="66">
+        <v>10</v>
+      </c>
+      <c r="D33" s="66">
+        <v>970</v>
+      </c>
+      <c r="E33" s="77">
+        <v>38</v>
+      </c>
+      <c r="F33" s="71"/>
+      <c r="G33" s="66">
+        <f>E33*D33/1000</f>
+        <v>36.86</v>
+      </c>
+      <c r="H33" s="77"/>
+      <c r="I33" s="72"/>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" s="71">
+        <v>11</v>
+      </c>
+      <c r="C34" s="66">
+        <v>8</v>
+      </c>
+      <c r="D34" s="66">
+        <v>1780</v>
+      </c>
+      <c r="E34" s="77">
+        <v>240</v>
+      </c>
+      <c r="F34" s="71">
+        <f t="shared" si="2"/>
+        <v>427.2</v>
+      </c>
+      <c r="G34" s="66"/>
+      <c r="H34" s="77"/>
+      <c r="I34" s="72"/>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="71">
+        <v>12</v>
+      </c>
+      <c r="C35" s="66">
+        <v>12</v>
+      </c>
+      <c r="D35" s="66">
+        <v>78000</v>
+      </c>
+      <c r="E35" s="77">
+        <v>4</v>
+      </c>
+      <c r="F35" s="71"/>
+      <c r="G35" s="66"/>
+      <c r="H35" s="77"/>
+      <c r="I35" s="72">
+        <f>E35*D35/1000</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" s="71">
+        <v>13</v>
+      </c>
+      <c r="C36" s="66">
+        <v>8</v>
+      </c>
+      <c r="D36" s="66">
         <v>880</v>
       </c>
-      <c r="E29" s="77">
+      <c r="E36" s="77">
         <v>220</v>
       </c>
-      <c r="F29" s="71">
-        <f t="shared" si="1"/>
+      <c r="F36" s="71">
+        <f t="shared" si="2"/>
         <v>193.6</v>
       </c>
-      <c r="G29" s="66"/>
-      <c r="H29" s="72"/>
-    </row>
-    <row r="30" spans="2:8" ht="15" thickBot="1">
-      <c r="B30" s="73">
+      <c r="G36" s="66"/>
+      <c r="H36" s="77"/>
+      <c r="I36" s="72"/>
+    </row>
+    <row r="37" spans="2:12" ht="15" thickBot="1">
+      <c r="B37" s="73">
         <v>14</v>
       </c>
-      <c r="C30" s="74">
+      <c r="C37" s="74">
         <v>12</v>
       </c>
-      <c r="D30" s="74">
+      <c r="D37" s="74">
         <v>4200</v>
       </c>
-      <c r="E30" s="78">
+      <c r="E37" s="78">
         <v>8</v>
       </c>
-      <c r="F30" s="73"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="75">
-        <f t="shared" ref="H30" si="2">E30*D30/1000</f>
+      <c r="F37" s="73"/>
+      <c r="G37" s="74"/>
+      <c r="H37" s="78"/>
+      <c r="I37" s="75">
+        <f t="shared" ref="I37" si="3">E37*D37/1000</f>
         <v>33.6</v>
       </c>
     </row>
-    <row r="31" spans="2:8">
-      <c r="B31" s="67" t="s">
+    <row r="38" spans="2:12">
+      <c r="B38" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="79"/>
-      <c r="F31" s="80">
-        <f>SUM(F17:F30)</f>
+      <c r="C38" s="67"/>
+      <c r="D38" s="67"/>
+      <c r="E38" s="79"/>
+      <c r="F38" s="80">
+        <f>SUM(F24:F37)</f>
         <v>3233.2999999999993</v>
       </c>
-      <c r="G31" s="67">
-        <f t="shared" ref="G31:H31" si="3">SUM(G17:G30)</f>
+      <c r="G38" s="67">
+        <f t="shared" ref="G38:I38" si="4">SUM(G24:G37)</f>
         <v>36.86</v>
       </c>
-      <c r="H31" s="81">
-        <f t="shared" si="3"/>
+      <c r="H38" s="79"/>
+      <c r="I38" s="81">
+        <f t="shared" si="4"/>
         <v>345.6</v>
       </c>
     </row>
-    <row r="32" spans="2:8">
-      <c r="B32" s="66" t="s">
+    <row r="39" spans="2:12">
+      <c r="B39" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="77"/>
-      <c r="F32" s="71">
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="77"/>
+      <c r="F39" s="71">
         <v>0.39500000000000002</v>
       </c>
-      <c r="G32" s="66">
+      <c r="G39" s="66">
         <v>0.61699999999999999</v>
       </c>
-      <c r="H32" s="72">
+      <c r="H39" s="77"/>
+      <c r="I39" s="72">
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="33" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B33" s="91" t="s">
+    <row r="40" spans="2:12" ht="15.75" thickBot="1">
+      <c r="B40" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="C33" s="91"/>
-      <c r="D33" s="91"/>
-      <c r="E33" s="117"/>
-      <c r="F33" s="118">
-        <f>ROUND(F31*F32,0)</f>
+      <c r="C40" s="91"/>
+      <c r="D40" s="91"/>
+      <c r="E40" s="117"/>
+      <c r="F40" s="118">
+        <f>ROUND(F38*F39,0)</f>
         <v>1277</v>
       </c>
-      <c r="G33" s="119">
-        <f t="shared" ref="G33:H33" si="4">ROUND(G31*G32,0)</f>
+      <c r="G40" s="119">
+        <f t="shared" ref="G40:I40" si="5">ROUND(G38*G39,0)</f>
         <v>23</v>
       </c>
-      <c r="H33" s="120">
-        <f t="shared" si="4"/>
+      <c r="H40" s="122"/>
+      <c r="I40" s="120">
+        <f t="shared" si="5"/>
         <v>307</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-    </row>
-    <row r="36" spans="2:11">
-      <c r="I36">
+    <row r="41" spans="2:12">
+      <c r="B41" s="66"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="67"/>
+      <c r="G41" s="67"/>
+      <c r="H41" s="67"/>
+      <c r="I41" s="67"/>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="J43">
         <v>1.23</v>
       </c>
-      <c r="J36">
+      <c r="K43">
         <v>2.74</v>
       </c>
     </row>
-    <row r="37" spans="2:11">
-      <c r="B37" t="s">
+    <row r="44" spans="2:12">
+      <c r="B44" t="s">
         <v>278</v>
       </c>
-      <c r="I37">
+      <c r="J44">
         <v>1</v>
       </c>
-      <c r="J37">
+      <c r="K44">
         <f>2.74/1.23</f>
         <v>2.2276422764227646</v>
       </c>
     </row>
-    <row r="38" spans="2:11">
-      <c r="J38">
+    <row r="45" spans="2:12">
+      <c r="K45">
         <v>2.48</v>
       </c>
-      <c r="K38">
+      <c r="L45">
         <f>2.48*1.23</f>
         <v>3.0503999999999998</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
-      <c r="I39">
+    <row r="46" spans="2:12">
+      <c r="J46">
         <v>5520</v>
       </c>
     </row>
-    <row r="40" spans="2:11" ht="57">
-      <c r="B40" s="92" t="s">
+    <row r="47" spans="2:12" ht="57">
+      <c r="B47" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="C40" s="66"/>
-      <c r="D40" s="66">
-        <v>0.68</v>
-      </c>
-      <c r="E40" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F40" s="66"/>
-      <c r="G40" s="66"/>
-      <c r="H40" s="66"/>
-      <c r="I40">
-        <v>1.23</v>
-      </c>
-      <c r="J40">
-        <f>5520*1.3</f>
-        <v>7176</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11">
-      <c r="B41" s="66" t="s">
-        <v>192</v>
-      </c>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66">
-        <v>242</v>
-      </c>
-      <c r="E41" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="F41" s="66"/>
-      <c r="G41" s="66"/>
-      <c r="H41" s="66"/>
-      <c r="I41">
-        <f>I40*I39</f>
-        <v>6789.5999999999995</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11">
-      <c r="B42" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C42" s="66"/>
-      <c r="D42" s="66">
-        <v>220</v>
-      </c>
-      <c r="E42" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F42" s="66"/>
-      <c r="G42" s="66"/>
-      <c r="H42" s="66"/>
-      <c r="I42">
-        <f>I41*1.3</f>
-        <v>8826.48</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11">
-      <c r="B43" s="66" t="s">
-        <v>195</v>
-      </c>
-      <c r="C43" s="66"/>
-      <c r="D43" s="66">
-        <v>1418</v>
-      </c>
-      <c r="E43" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F43" s="66"/>
-      <c r="G43" s="66"/>
-      <c r="H43" s="66"/>
-    </row>
-    <row r="44" spans="2:11">
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44">
-        <f>5520/1000</f>
-        <v>5.52</v>
-      </c>
-      <c r="J44" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" ht="15">
-      <c r="B45" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="C45" s="66"/>
-      <c r="D45" s="91">
-        <v>1035</v>
-      </c>
-      <c r="E45" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F45" s="66" t="s">
-        <v>199</v>
-      </c>
-      <c r="G45" s="66">
-        <v>1607</v>
-      </c>
-      <c r="H45" s="66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11">
-      <c r="B46" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="C46" s="66"/>
-      <c r="D46" s="66">
-        <v>266</v>
-      </c>
-      <c r="E46" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F46" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="G46" s="66">
-        <v>577</v>
-      </c>
-      <c r="H46" s="66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11">
-      <c r="B47" s="66"/>
       <c r="C47" s="66"/>
       <c r="D47" s="66">
-        <v>138</v>
+        <v>0.68</v>
       </c>
       <c r="E47" s="66" t="s">
         <v>191</v>
@@ -10610,447 +10646,542 @@
       <c r="F47" s="66"/>
       <c r="G47" s="66"/>
       <c r="H47" s="66"/>
-    </row>
-    <row r="48" spans="2:11">
-      <c r="B48" s="66"/>
+      <c r="I47" s="66"/>
+      <c r="J47">
+        <v>1.23</v>
+      </c>
+      <c r="K47">
+        <f>5520*1.3</f>
+        <v>7176</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="B48" s="66" t="s">
+        <v>192</v>
+      </c>
       <c r="C48" s="66"/>
       <c r="D48" s="66">
-        <v>173</v>
+        <v>242</v>
       </c>
       <c r="E48" s="66" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F48" s="66"/>
       <c r="G48" s="66"/>
       <c r="H48" s="66"/>
-    </row>
-    <row r="49" spans="2:8" ht="15">
-      <c r="B49" s="66"/>
+      <c r="I48" s="66"/>
+      <c r="J48">
+        <f>J47*J46</f>
+        <v>6789.5999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11">
+      <c r="B49" s="66" t="s">
+        <v>194</v>
+      </c>
       <c r="C49" s="66"/>
-      <c r="D49" s="91">
-        <f>D46+D47+D48</f>
-        <v>577</v>
+      <c r="D49" s="66">
+        <v>220</v>
       </c>
       <c r="E49" s="66" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="F49" s="66"/>
       <c r="G49" s="66"/>
       <c r="H49" s="66"/>
-    </row>
-    <row r="50" spans="2:8">
-      <c r="B50" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49">
+        <f>J48*1.3</f>
+        <v>8826.48</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11">
+      <c r="B50" s="66" t="s">
+        <v>195</v>
+      </c>
       <c r="C50" s="66"/>
-      <c r="D50" s="66"/>
-      <c r="E50" s="66"/>
+      <c r="D50" s="66">
+        <v>1418</v>
+      </c>
+      <c r="E50" s="66" t="s">
+        <v>191</v>
+      </c>
       <c r="F50" s="66"/>
       <c r="G50" s="66"/>
       <c r="H50" s="66"/>
-    </row>
-    <row r="51" spans="2:8" ht="15">
+      <c r="I50" s="66"/>
+    </row>
+    <row r="51" spans="2:11">
       <c r="B51" s="66"/>
       <c r="C51" s="66"/>
-      <c r="D51" s="91">
-        <f>D45+D49</f>
-        <v>1612</v>
-      </c>
+      <c r="D51" s="66"/>
       <c r="E51" s="66"/>
       <c r="F51" s="66"/>
       <c r="G51" s="66"/>
       <c r="H51" s="66"/>
-    </row>
-    <row r="57" spans="2:8" ht="15.75" thickBot="1">
-      <c r="B57" s="90" t="s">
+      <c r="I51" s="66"/>
+      <c r="J51">
+        <f>5520/1000</f>
+        <v>5.52</v>
+      </c>
+      <c r="K51" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" ht="15">
+      <c r="B52" s="66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C52" s="66"/>
+      <c r="D52" s="91">
+        <v>1035</v>
+      </c>
+      <c r="E52" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F52" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="G52" s="66">
+        <v>1607</v>
+      </c>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11">
+      <c r="B53" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66">
+        <v>266</v>
+      </c>
+      <c r="E53" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F53" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="G53" s="66">
+        <v>577</v>
+      </c>
+      <c r="H53" s="66"/>
+      <c r="I53" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11">
+      <c r="B54" s="66"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="66">
+        <v>138</v>
+      </c>
+      <c r="E54" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F54" s="66"/>
+      <c r="G54" s="66"/>
+      <c r="H54" s="66"/>
+      <c r="I54" s="66"/>
+    </row>
+    <row r="55" spans="2:11">
+      <c r="B55" s="66"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="66">
+        <v>173</v>
+      </c>
+      <c r="E55" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F55" s="66"/>
+      <c r="G55" s="66"/>
+      <c r="H55" s="66"/>
+      <c r="I55" s="66"/>
+    </row>
+    <row r="56" spans="2:11" ht="15">
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="91">
+        <f>D53+D54+D55</f>
+        <v>577</v>
+      </c>
+      <c r="E56" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="66"/>
+      <c r="I56" s="66"/>
+    </row>
+    <row r="57" spans="2:11">
+      <c r="B57" s="66"/>
+      <c r="C57" s="66"/>
+      <c r="D57" s="66"/>
+      <c r="E57" s="66"/>
+      <c r="F57" s="66"/>
+      <c r="G57" s="66"/>
+      <c r="H57" s="66"/>
+      <c r="I57" s="66"/>
+    </row>
+    <row r="58" spans="2:11" ht="15">
+      <c r="B58" s="66"/>
+      <c r="C58" s="66"/>
+      <c r="D58" s="91">
+        <f>D52+D56</f>
+        <v>1612</v>
+      </c>
+      <c r="E58" s="66"/>
+      <c r="F58" s="66"/>
+      <c r="G58" s="66"/>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66"/>
+    </row>
+    <row r="64" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B64" s="90" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="58" spans="2:8">
-      <c r="B58" s="68" t="s">
+    <row r="65" spans="2:9">
+      <c r="B65" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C58" s="69" t="s">
+      <c r="C65" s="69" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="69" t="s">
+      <c r="D65" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="E58" s="69" t="s">
+      <c r="E65" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="F58" s="69" t="s">
+      <c r="F65" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="G58" s="69" t="s">
+      <c r="G65" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="H58" s="70" t="s">
+      <c r="H65" s="76"/>
+      <c r="I65" s="70" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="59" spans="2:8">
-      <c r="B59" s="71">
+    <row r="66" spans="2:9">
+      <c r="B66" s="71">
         <v>1</v>
       </c>
-      <c r="C59" s="66">
+      <c r="C66" s="66">
         <v>18</v>
       </c>
-      <c r="D59" s="66">
+      <c r="D66" s="66">
         <v>9.74</v>
       </c>
-      <c r="E59" s="66">
+      <c r="E66" s="66">
         <v>4</v>
       </c>
-      <c r="F59" s="66"/>
-      <c r="G59" s="66"/>
-      <c r="H59" s="72">
+      <c r="F66" s="66"/>
+      <c r="G66" s="66"/>
+      <c r="H66" s="77"/>
+      <c r="I66" s="72">
         <v>39.1</v>
       </c>
     </row>
-    <row r="60" spans="2:8">
-      <c r="B60" s="71">
+    <row r="67" spans="2:9">
+      <c r="B67" s="71">
         <v>2</v>
       </c>
-      <c r="C60" s="66">
+      <c r="C67" s="66">
         <v>18</v>
       </c>
-      <c r="D60" s="66">
+      <c r="D67" s="66">
         <v>3.27</v>
       </c>
-      <c r="E60" s="66">
+      <c r="E67" s="66">
         <v>4</v>
       </c>
-      <c r="F60" s="66"/>
-      <c r="G60" s="66"/>
-      <c r="H60" s="72">
+      <c r="F67" s="66"/>
+      <c r="G67" s="66"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="72">
         <v>13.1</v>
       </c>
     </row>
-    <row r="61" spans="2:8">
-      <c r="B61" s="71">
+    <row r="68" spans="2:9">
+      <c r="B68" s="71">
         <v>3</v>
-      </c>
-      <c r="C61" s="66">
-        <v>14</v>
-      </c>
-      <c r="D61" s="66">
-        <v>3.3</v>
-      </c>
-      <c r="E61" s="66">
-        <v>2</v>
-      </c>
-      <c r="F61" s="66"/>
-      <c r="G61" s="66">
-        <v>6.6</v>
-      </c>
-      <c r="H61" s="72"/>
-    </row>
-    <row r="62" spans="2:8">
-      <c r="B62" s="71">
-        <v>4</v>
-      </c>
-      <c r="C62" s="66">
-        <v>14</v>
-      </c>
-      <c r="D62" s="66">
-        <v>3.58</v>
-      </c>
-      <c r="E62" s="66">
-        <v>2</v>
-      </c>
-      <c r="F62" s="66"/>
-      <c r="G62" s="66">
-        <v>7.2</v>
-      </c>
-      <c r="H62" s="72"/>
-    </row>
-    <row r="63" spans="2:8">
-      <c r="B63" s="71">
-        <v>5</v>
-      </c>
-      <c r="C63" s="66">
-        <v>6</v>
-      </c>
-      <c r="D63" s="66">
-        <v>1.3</v>
-      </c>
-      <c r="E63" s="66">
-        <v>17</v>
-      </c>
-      <c r="F63" s="66">
-        <v>22.1</v>
-      </c>
-      <c r="G63" s="66"/>
-      <c r="H63" s="72"/>
-    </row>
-    <row r="64" spans="2:8">
-      <c r="B64" s="71">
-        <v>6</v>
-      </c>
-      <c r="C64" s="66">
-        <v>6</v>
-      </c>
-      <c r="D64" s="66">
-        <v>1.64</v>
-      </c>
-      <c r="E64" s="66">
-        <v>23</v>
-      </c>
-      <c r="F64" s="66">
-        <v>37.700000000000003</v>
-      </c>
-      <c r="G64" s="66"/>
-      <c r="H64" s="72"/>
-    </row>
-    <row r="65" spans="2:8">
-      <c r="B65" s="71">
-        <v>7</v>
-      </c>
-      <c r="C65" s="66">
-        <v>18</v>
-      </c>
-      <c r="D65" s="66">
-        <v>7.2</v>
-      </c>
-      <c r="E65" s="66">
-        <v>4</v>
-      </c>
-      <c r="F65" s="66"/>
-      <c r="G65" s="66"/>
-      <c r="H65" s="72">
-        <v>28.8</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8">
-      <c r="B66" s="71">
-        <v>8</v>
-      </c>
-      <c r="C66" s="66">
-        <v>14</v>
-      </c>
-      <c r="D66" s="66">
-        <v>6.52</v>
-      </c>
-      <c r="E66" s="66">
-        <v>2</v>
-      </c>
-      <c r="F66" s="66"/>
-      <c r="G66" s="66">
-        <v>13</v>
-      </c>
-      <c r="H66" s="72"/>
-    </row>
-    <row r="67" spans="2:8">
-      <c r="B67" s="71">
-        <v>9</v>
-      </c>
-      <c r="C67" s="66">
-        <v>6</v>
-      </c>
-      <c r="D67" s="66">
-        <v>1.64</v>
-      </c>
-      <c r="E67" s="66">
-        <v>35</v>
-      </c>
-      <c r="F67" s="66">
-        <v>57.4</v>
-      </c>
-      <c r="G67" s="66"/>
-      <c r="H67" s="72"/>
-    </row>
-    <row r="68" spans="2:8">
-      <c r="B68" s="71">
-        <v>10</v>
       </c>
       <c r="C68" s="66">
         <v>14</v>
       </c>
       <c r="D68" s="66">
-        <v>5.67</v>
+        <v>3.3</v>
       </c>
       <c r="E68" s="66">
         <v>2</v>
       </c>
       <c r="F68" s="66"/>
       <c r="G68" s="66">
-        <v>11.3</v>
-      </c>
-      <c r="H68" s="72"/>
-    </row>
-    <row r="69" spans="2:8">
+        <v>6.6</v>
+      </c>
+      <c r="H68" s="77"/>
+      <c r="I68" s="72"/>
+    </row>
+    <row r="69" spans="2:9">
       <c r="B69" s="71">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C69" s="66">
         <v>14</v>
       </c>
       <c r="D69" s="66">
-        <v>4.63</v>
+        <v>3.58</v>
       </c>
       <c r="E69" s="66">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F69" s="66"/>
       <c r="G69" s="66">
+        <v>7.2</v>
+      </c>
+      <c r="H69" s="77"/>
+      <c r="I69" s="72"/>
+    </row>
+    <row r="70" spans="2:9">
+      <c r="B70" s="71">
+        <v>5</v>
+      </c>
+      <c r="C70" s="66">
+        <v>6</v>
+      </c>
+      <c r="D70" s="66">
+        <v>1.3</v>
+      </c>
+      <c r="E70" s="66">
+        <v>17</v>
+      </c>
+      <c r="F70" s="66">
+        <v>22.1</v>
+      </c>
+      <c r="G70" s="66"/>
+      <c r="H70" s="77"/>
+      <c r="I70" s="72"/>
+    </row>
+    <row r="71" spans="2:9">
+      <c r="B71" s="71">
+        <v>6</v>
+      </c>
+      <c r="C71" s="66">
+        <v>6</v>
+      </c>
+      <c r="D71" s="66">
+        <v>1.64</v>
+      </c>
+      <c r="E71" s="66">
+        <v>23</v>
+      </c>
+      <c r="F71" s="66">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G71" s="66"/>
+      <c r="H71" s="77"/>
+      <c r="I71" s="72"/>
+    </row>
+    <row r="72" spans="2:9">
+      <c r="B72" s="71">
+        <v>7</v>
+      </c>
+      <c r="C72" s="66">
+        <v>18</v>
+      </c>
+      <c r="D72" s="66">
+        <v>7.2</v>
+      </c>
+      <c r="E72" s="66">
+        <v>4</v>
+      </c>
+      <c r="F72" s="66"/>
+      <c r="G72" s="66"/>
+      <c r="H72" s="77"/>
+      <c r="I72" s="72">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="73" spans="2:9">
+      <c r="B73" s="71">
+        <v>8</v>
+      </c>
+      <c r="C73" s="66">
+        <v>14</v>
+      </c>
+      <c r="D73" s="66">
+        <v>6.52</v>
+      </c>
+      <c r="E73" s="66">
+        <v>2</v>
+      </c>
+      <c r="F73" s="66"/>
+      <c r="G73" s="66">
+        <v>13</v>
+      </c>
+      <c r="H73" s="77"/>
+      <c r="I73" s="72"/>
+    </row>
+    <row r="74" spans="2:9">
+      <c r="B74" s="71">
+        <v>9</v>
+      </c>
+      <c r="C74" s="66">
+        <v>6</v>
+      </c>
+      <c r="D74" s="66">
+        <v>1.64</v>
+      </c>
+      <c r="E74" s="66">
+        <v>35</v>
+      </c>
+      <c r="F74" s="66">
+        <v>57.4</v>
+      </c>
+      <c r="G74" s="66"/>
+      <c r="H74" s="77"/>
+      <c r="I74" s="72"/>
+    </row>
+    <row r="75" spans="2:9">
+      <c r="B75" s="71">
+        <v>10</v>
+      </c>
+      <c r="C75" s="66">
+        <v>14</v>
+      </c>
+      <c r="D75" s="66">
+        <v>5.67</v>
+      </c>
+      <c r="E75" s="66">
+        <v>2</v>
+      </c>
+      <c r="F75" s="66"/>
+      <c r="G75" s="66">
+        <v>11.3</v>
+      </c>
+      <c r="H75" s="77"/>
+      <c r="I75" s="72"/>
+    </row>
+    <row r="76" spans="2:9">
+      <c r="B76" s="71">
+        <v>11</v>
+      </c>
+      <c r="C76" s="66">
+        <v>14</v>
+      </c>
+      <c r="D76" s="66">
+        <v>4.63</v>
+      </c>
+      <c r="E76" s="66">
+        <v>4</v>
+      </c>
+      <c r="F76" s="66"/>
+      <c r="G76" s="66">
         <v>18.5</v>
       </c>
-      <c r="H69" s="72"/>
-    </row>
-    <row r="70" spans="2:8" ht="15" thickBot="1">
-      <c r="B70" s="73">
+      <c r="H76" s="77"/>
+      <c r="I76" s="72"/>
+    </row>
+    <row r="77" spans="2:9" ht="15" thickBot="1">
+      <c r="B77" s="73">
         <v>12</v>
       </c>
-      <c r="C70" s="74">
+      <c r="C77" s="74">
         <v>6</v>
       </c>
-      <c r="D70" s="74">
+      <c r="D77" s="74">
         <v>1.64</v>
       </c>
-      <c r="E70" s="74">
+      <c r="E77" s="74">
         <v>29</v>
       </c>
-      <c r="F70" s="74">
+      <c r="F77" s="74">
         <v>47.6</v>
       </c>
-      <c r="G70" s="74"/>
-      <c r="H70" s="75"/>
-    </row>
-    <row r="71" spans="2:8">
-      <c r="B71" s="67"/>
-      <c r="C71" s="67"/>
-      <c r="D71" s="67" t="s">
+      <c r="G77" s="74"/>
+      <c r="H77" s="78"/>
+      <c r="I77" s="75"/>
+    </row>
+    <row r="78" spans="2:9">
+      <c r="B78" s="67"/>
+      <c r="C78" s="67"/>
+      <c r="D78" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="E71" s="67" t="s">
+      <c r="E78" s="67" t="s">
         <v>206</v>
       </c>
-      <c r="F71" s="67">
+      <c r="F78" s="67">
         <v>164.8</v>
       </c>
-      <c r="G71" s="67">
+      <c r="G78" s="67">
         <v>56.7</v>
       </c>
-      <c r="H71" s="67">
+      <c r="H78" s="67"/>
+      <c r="I78" s="67">
         <v>80.8</v>
       </c>
     </row>
-    <row r="72" spans="2:8">
-      <c r="B72" s="66"/>
-      <c r="C72" s="66"/>
-      <c r="D72" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="E72" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F72" s="66">
-        <v>0.222</v>
-      </c>
-      <c r="G72" s="66">
-        <v>1.208</v>
-      </c>
-      <c r="H72" s="66">
-        <v>1.998</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8">
-      <c r="B73" s="66"/>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="E73" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F73" s="66">
-        <v>36.6</v>
-      </c>
-      <c r="G73" s="66">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="H73" s="66">
-        <v>161.5</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" ht="15">
-      <c r="B74" s="66"/>
-      <c r="C74" s="66"/>
-      <c r="D74" s="91" t="s">
-        <v>209</v>
-      </c>
-      <c r="E74" s="91" t="s">
-        <v>210</v>
-      </c>
-      <c r="F74" s="66"/>
-      <c r="G74" s="66"/>
-      <c r="H74" s="66"/>
-    </row>
-    <row r="75" spans="2:8">
-      <c r="B75" s="66"/>
-      <c r="C75" s="66"/>
-      <c r="D75" s="66"/>
-      <c r="E75" s="66"/>
-      <c r="F75" s="66"/>
-      <c r="G75" s="66"/>
-      <c r="H75" s="66"/>
-    </row>
-    <row r="76" spans="2:8" ht="15">
-      <c r="B76" s="90" t="s">
-        <v>212</v>
-      </c>
-      <c r="C76" s="66"/>
-      <c r="D76" s="66"/>
-      <c r="E76" s="66"/>
-      <c r="F76" s="66"/>
-      <c r="G76" s="66"/>
-      <c r="H76" s="66"/>
-    </row>
-    <row r="77" spans="2:8">
-      <c r="B77" s="66"/>
-      <c r="C77" s="66"/>
-      <c r="D77" s="66"/>
-      <c r="E77" s="66"/>
-      <c r="F77" s="66"/>
-      <c r="G77" s="66"/>
-      <c r="H77" s="66"/>
-    </row>
-    <row r="78" spans="2:8">
-      <c r="B78" s="66"/>
-      <c r="C78" s="66"/>
-      <c r="D78" s="66"/>
-      <c r="E78" s="66"/>
-      <c r="F78" s="66"/>
-      <c r="G78" s="66"/>
-      <c r="H78" s="66"/>
-    </row>
-    <row r="79" spans="2:8">
+    <row r="79" spans="2:9">
       <c r="B79" s="66"/>
       <c r="C79" s="66"/>
-      <c r="D79" s="66"/>
-      <c r="E79" s="66"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
+      <c r="D79" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="E79" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F79" s="66">
+        <v>0.222</v>
+      </c>
+      <c r="G79" s="66">
+        <v>1.208</v>
+      </c>
       <c r="H79" s="66"/>
-    </row>
-    <row r="80" spans="2:8">
+      <c r="I79" s="66">
+        <v>1.998</v>
+      </c>
+    </row>
+    <row r="80" spans="2:9">
       <c r="B80" s="66"/>
       <c r="C80" s="66"/>
-      <c r="D80" s="66"/>
-      <c r="E80" s="66"/>
-      <c r="F80" s="66"/>
-      <c r="G80" s="66"/>
+      <c r="D80" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E80" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F80" s="66">
+        <v>36.6</v>
+      </c>
+      <c r="G80" s="66">
+        <v>68.400000000000006</v>
+      </c>
       <c r="H80" s="66"/>
-    </row>
-    <row r="81" spans="2:8">
+      <c r="I80" s="66">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="15">
       <c r="B81" s="66"/>
       <c r="C81" s="66"/>
-      <c r="D81" s="66"/>
-      <c r="E81" s="66"/>
+      <c r="D81" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E81" s="91" t="s">
+        <v>210</v>
+      </c>
       <c r="F81" s="66"/>
       <c r="G81" s="66"/>
       <c r="H81" s="66"/>
-    </row>
-    <row r="82" spans="2:8">
+      <c r="I81" s="66"/>
+    </row>
+    <row r="82" spans="2:9">
       <c r="B82" s="66"/>
       <c r="C82" s="66"/>
       <c r="D82" s="66"/>
@@ -11058,17 +11189,21 @@
       <c r="F82" s="66"/>
       <c r="G82" s="66"/>
       <c r="H82" s="66"/>
-    </row>
-    <row r="83" spans="2:8">
-      <c r="B83" s="66"/>
+      <c r="I82" s="66"/>
+    </row>
+    <row r="83" spans="2:9" ht="15">
+      <c r="B83" s="90" t="s">
+        <v>212</v>
+      </c>
       <c r="C83" s="66"/>
       <c r="D83" s="66"/>
       <c r="E83" s="66"/>
       <c r="F83" s="66"/>
       <c r="G83" s="66"/>
       <c r="H83" s="66"/>
-    </row>
-    <row r="84" spans="2:8">
+      <c r="I83" s="66"/>
+    </row>
+    <row r="84" spans="2:9">
       <c r="B84" s="66"/>
       <c r="C84" s="66"/>
       <c r="D84" s="66"/>
@@ -11076,8 +11211,9 @@
       <c r="F84" s="66"/>
       <c r="G84" s="66"/>
       <c r="H84" s="66"/>
-    </row>
-    <row r="85" spans="2:8">
+      <c r="I84" s="66"/>
+    </row>
+    <row r="85" spans="2:9">
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
       <c r="D85" s="66"/>
@@ -11085,8 +11221,9 @@
       <c r="F85" s="66"/>
       <c r="G85" s="66"/>
       <c r="H85" s="66"/>
-    </row>
-    <row r="86" spans="2:8">
+      <c r="I85" s="66"/>
+    </row>
+    <row r="86" spans="2:9">
       <c r="B86" s="66"/>
       <c r="C86" s="66"/>
       <c r="D86" s="66"/>
@@ -11094,8 +11231,9 @@
       <c r="F86" s="66"/>
       <c r="G86" s="66"/>
       <c r="H86" s="66"/>
-    </row>
-    <row r="87" spans="2:8">
+      <c r="I86" s="66"/>
+    </row>
+    <row r="87" spans="2:9">
       <c r="B87" s="66"/>
       <c r="C87" s="66"/>
       <c r="D87" s="66"/>
@@ -11103,8 +11241,9 @@
       <c r="F87" s="66"/>
       <c r="G87" s="66"/>
       <c r="H87" s="66"/>
-    </row>
-    <row r="88" spans="2:8">
+      <c r="I87" s="66"/>
+    </row>
+    <row r="88" spans="2:9">
       <c r="B88" s="66"/>
       <c r="C88" s="66"/>
       <c r="D88" s="66"/>
@@ -11112,8 +11251,9 @@
       <c r="F88" s="66"/>
       <c r="G88" s="66"/>
       <c r="H88" s="66"/>
-    </row>
-    <row r="89" spans="2:8">
+      <c r="I88" s="66"/>
+    </row>
+    <row r="89" spans="2:9">
       <c r="B89" s="66"/>
       <c r="C89" s="66"/>
       <c r="D89" s="66"/>
@@ -11121,8 +11261,9 @@
       <c r="F89" s="66"/>
       <c r="G89" s="66"/>
       <c r="H89" s="66"/>
-    </row>
-    <row r="90" spans="2:8">
+      <c r="I89" s="66"/>
+    </row>
+    <row r="90" spans="2:9">
       <c r="B90" s="66"/>
       <c r="C90" s="66"/>
       <c r="D90" s="66"/>
@@ -11130,8 +11271,9 @@
       <c r="F90" s="66"/>
       <c r="G90" s="66"/>
       <c r="H90" s="66"/>
-    </row>
-    <row r="91" spans="2:8">
+      <c r="I90" s="66"/>
+    </row>
+    <row r="91" spans="2:9">
       <c r="B91" s="66"/>
       <c r="C91" s="66"/>
       <c r="D91" s="66"/>
@@ -11139,8 +11281,9 @@
       <c r="F91" s="66"/>
       <c r="G91" s="66"/>
       <c r="H91" s="66"/>
-    </row>
-    <row r="92" spans="2:8">
+      <c r="I91" s="66"/>
+    </row>
+    <row r="92" spans="2:9">
       <c r="B92" s="66"/>
       <c r="C92" s="66"/>
       <c r="D92" s="66"/>
@@ -11148,8 +11291,9 @@
       <c r="F92" s="66"/>
       <c r="G92" s="66"/>
       <c r="H92" s="66"/>
-    </row>
-    <row r="93" spans="2:8">
+      <c r="I92" s="66"/>
+    </row>
+    <row r="93" spans="2:9">
       <c r="B93" s="66"/>
       <c r="C93" s="66"/>
       <c r="D93" s="66"/>
@@ -11157,8 +11301,9 @@
       <c r="F93" s="66"/>
       <c r="G93" s="66"/>
       <c r="H93" s="66"/>
-    </row>
-    <row r="94" spans="2:8">
+      <c r="I93" s="66"/>
+    </row>
+    <row r="94" spans="2:9">
       <c r="B94" s="66"/>
       <c r="C94" s="66"/>
       <c r="D94" s="66"/>
@@ -11166,8 +11311,9 @@
       <c r="F94" s="66"/>
       <c r="G94" s="66"/>
       <c r="H94" s="66"/>
-    </row>
-    <row r="95" spans="2:8">
+      <c r="I94" s="66"/>
+    </row>
+    <row r="95" spans="2:9">
       <c r="B95" s="66"/>
       <c r="C95" s="66"/>
       <c r="D95" s="66"/>
@@ -11175,8 +11321,9 @@
       <c r="F95" s="66"/>
       <c r="G95" s="66"/>
       <c r="H95" s="66"/>
-    </row>
-    <row r="96" spans="2:8">
+      <c r="I95" s="66"/>
+    </row>
+    <row r="96" spans="2:9">
       <c r="B96" s="66"/>
       <c r="C96" s="66"/>
       <c r="D96" s="66"/>
@@ -11184,8 +11331,9 @@
       <c r="F96" s="66"/>
       <c r="G96" s="66"/>
       <c r="H96" s="66"/>
-    </row>
-    <row r="97" spans="2:8">
+      <c r="I96" s="66"/>
+    </row>
+    <row r="97" spans="2:9">
       <c r="B97" s="66"/>
       <c r="C97" s="66"/>
       <c r="D97" s="66"/>
@@ -11193,8 +11341,9 @@
       <c r="F97" s="66"/>
       <c r="G97" s="66"/>
       <c r="H97" s="66"/>
-    </row>
-    <row r="98" spans="2:8">
+      <c r="I97" s="66"/>
+    </row>
+    <row r="98" spans="2:9">
       <c r="B98" s="66"/>
       <c r="C98" s="66"/>
       <c r="D98" s="66"/>
@@ -11202,8 +11351,9 @@
       <c r="F98" s="66"/>
       <c r="G98" s="66"/>
       <c r="H98" s="66"/>
-    </row>
-    <row r="99" spans="2:8">
+      <c r="I98" s="66"/>
+    </row>
+    <row r="99" spans="2:9">
       <c r="B99" s="66"/>
       <c r="C99" s="66"/>
       <c r="D99" s="66"/>
@@ -11211,8 +11361,9 @@
       <c r="F99" s="66"/>
       <c r="G99" s="66"/>
       <c r="H99" s="66"/>
-    </row>
-    <row r="100" spans="2:8">
+      <c r="I99" s="66"/>
+    </row>
+    <row r="100" spans="2:9">
       <c r="B100" s="66"/>
       <c r="C100" s="66"/>
       <c r="D100" s="66"/>
@@ -11220,8 +11371,9 @@
       <c r="F100" s="66"/>
       <c r="G100" s="66"/>
       <c r="H100" s="66"/>
-    </row>
-    <row r="101" spans="2:8">
+      <c r="I100" s="66"/>
+    </row>
+    <row r="101" spans="2:9">
       <c r="B101" s="66"/>
       <c r="C101" s="66"/>
       <c r="D101" s="66"/>
@@ -11229,8 +11381,9 @@
       <c r="F101" s="66"/>
       <c r="G101" s="66"/>
       <c r="H101" s="66"/>
-    </row>
-    <row r="102" spans="2:8">
+      <c r="I101" s="66"/>
+    </row>
+    <row r="102" spans="2:9">
       <c r="B102" s="66"/>
       <c r="C102" s="66"/>
       <c r="D102" s="66"/>
@@ -11238,8 +11391,9 @@
       <c r="F102" s="66"/>
       <c r="G102" s="66"/>
       <c r="H102" s="66"/>
-    </row>
-    <row r="103" spans="2:8">
+      <c r="I102" s="66"/>
+    </row>
+    <row r="103" spans="2:9">
       <c r="B103" s="66"/>
       <c r="C103" s="66"/>
       <c r="D103" s="66"/>
@@ -11247,165 +11401,242 @@
       <c r="F103" s="66"/>
       <c r="G103" s="66"/>
       <c r="H103" s="66"/>
-    </row>
-    <row r="117" spans="2:4">
-      <c r="B117" t="s">
+      <c r="I103" s="66"/>
+    </row>
+    <row r="104" spans="2:9">
+      <c r="B104" s="66"/>
+      <c r="C104" s="66"/>
+      <c r="D104" s="66"/>
+      <c r="E104" s="66"/>
+      <c r="F104" s="66"/>
+      <c r="G104" s="66"/>
+      <c r="H104" s="66"/>
+      <c r="I104" s="66"/>
+    </row>
+    <row r="105" spans="2:9">
+      <c r="B105" s="66"/>
+      <c r="C105" s="66"/>
+      <c r="D105" s="66"/>
+      <c r="E105" s="66"/>
+      <c r="F105" s="66"/>
+      <c r="G105" s="66"/>
+      <c r="H105" s="66"/>
+      <c r="I105" s="66"/>
+    </row>
+    <row r="106" spans="2:9">
+      <c r="B106" s="66"/>
+      <c r="C106" s="66"/>
+      <c r="D106" s="66"/>
+      <c r="E106" s="66"/>
+      <c r="F106" s="66"/>
+      <c r="G106" s="66"/>
+      <c r="H106" s="66"/>
+      <c r="I106" s="66"/>
+    </row>
+    <row r="107" spans="2:9">
+      <c r="B107" s="66"/>
+      <c r="C107" s="66"/>
+      <c r="D107" s="66"/>
+      <c r="E107" s="66"/>
+      <c r="F107" s="66"/>
+      <c r="G107" s="66"/>
+      <c r="H107" s="66"/>
+      <c r="I107" s="66"/>
+    </row>
+    <row r="108" spans="2:9">
+      <c r="B108" s="66"/>
+      <c r="C108" s="66"/>
+      <c r="D108" s="66"/>
+      <c r="E108" s="66"/>
+      <c r="F108" s="66"/>
+      <c r="G108" s="66"/>
+      <c r="H108" s="66"/>
+      <c r="I108" s="66"/>
+    </row>
+    <row r="109" spans="2:9">
+      <c r="B109" s="66"/>
+      <c r="C109" s="66"/>
+      <c r="D109" s="66"/>
+      <c r="E109" s="66"/>
+      <c r="F109" s="66"/>
+      <c r="G109" s="66"/>
+      <c r="H109" s="66"/>
+      <c r="I109" s="66"/>
+    </row>
+    <row r="110" spans="2:9">
+      <c r="B110" s="66"/>
+      <c r="C110" s="66"/>
+      <c r="D110" s="66"/>
+      <c r="E110" s="66"/>
+      <c r="F110" s="66"/>
+      <c r="G110" s="66"/>
+      <c r="H110" s="66"/>
+      <c r="I110" s="66"/>
+    </row>
+    <row r="124" spans="2:4">
+      <c r="B124" t="s">
         <v>236</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C124" t="s">
         <v>237</v>
       </c>
-      <c r="D117" t="s">
+      <c r="D124" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="118" spans="2:4" ht="30" customHeight="1">
-      <c r="B118" s="66" t="s">
+    <row r="125" spans="2:4" ht="30" customHeight="1">
+      <c r="B125" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="C118" s="66"/>
-      <c r="D118" s="66"/>
-    </row>
-    <row r="119" spans="2:4" ht="30" customHeight="1">
-      <c r="B119" s="92" t="s">
-        <v>213</v>
-      </c>
-      <c r="C119" s="92" t="s">
-        <v>215</v>
-      </c>
-      <c r="D119" s="92"/>
-    </row>
-    <row r="120" spans="2:4" ht="30" customHeight="1">
-      <c r="B120" s="92" t="s">
-        <v>239</v>
-      </c>
-      <c r="C120" s="92" t="s">
-        <v>240</v>
-      </c>
-      <c r="D120" s="92"/>
-    </row>
-    <row r="121" spans="2:4" ht="30" customHeight="1">
-      <c r="B121" s="92" t="s">
-        <v>216</v>
-      </c>
-      <c r="C121" s="92" t="s">
-        <v>229</v>
-      </c>
-      <c r="D121" s="92"/>
-    </row>
-    <row r="122" spans="2:4" ht="30" customHeight="1">
-      <c r="B122" s="92" t="s">
-        <v>217</v>
-      </c>
-      <c r="C122" s="92" t="s">
-        <v>230</v>
-      </c>
-      <c r="D122" s="92"/>
-    </row>
-    <row r="123" spans="2:4" ht="30" customHeight="1">
-      <c r="B123" s="92" t="s">
-        <v>218</v>
-      </c>
-      <c r="C123" s="92" t="s">
-        <v>219</v>
-      </c>
-      <c r="D123" s="92"/>
-    </row>
-    <row r="124" spans="2:4" ht="5.25" customHeight="1">
-      <c r="B124" s="92"/>
-      <c r="C124" s="92"/>
-      <c r="D124" s="92"/>
-    </row>
-    <row r="125" spans="2:4" ht="30" customHeight="1">
-      <c r="B125" s="92" t="s">
-        <v>220</v>
-      </c>
-      <c r="C125" s="92" t="s">
-        <v>221</v>
-      </c>
-      <c r="D125" s="92"/>
+      <c r="C125" s="66"/>
+      <c r="D125" s="66"/>
     </row>
     <row r="126" spans="2:4" ht="30" customHeight="1">
       <c r="B126" s="92" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C126" s="92" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="D126" s="92"/>
     </row>
     <row r="127" spans="2:4" ht="30" customHeight="1">
       <c r="B127" s="92" t="s">
-        <v>218</v>
+        <v>239</v>
       </c>
       <c r="C127" s="92" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="D127" s="92"/>
     </row>
     <row r="128" spans="2:4" ht="30" customHeight="1">
       <c r="B128" s="92" t="s">
-        <v>231</v>
+        <v>216</v>
       </c>
       <c r="C128" s="92" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D128" s="92"/>
     </row>
-    <row r="129" spans="2:4" ht="5.25" customHeight="1">
-      <c r="B129" s="92"/>
-      <c r="C129" s="92"/>
+    <row r="129" spans="2:4" ht="30" customHeight="1">
+      <c r="B129" s="92" t="s">
+        <v>217</v>
+      </c>
+      <c r="C129" s="92" t="s">
+        <v>230</v>
+      </c>
       <c r="D129" s="92"/>
     </row>
     <row r="130" spans="2:4" ht="30" customHeight="1">
       <c r="B130" s="92" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="C130" s="92" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="D130" s="92"/>
     </row>
-    <row r="131" spans="2:4" ht="30" customHeight="1">
-      <c r="B131" s="92" t="s">
-        <v>224</v>
-      </c>
-      <c r="C131" s="92" t="s">
-        <v>225</v>
-      </c>
+    <row r="131" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B131" s="92"/>
+      <c r="C131" s="92"/>
       <c r="D131" s="92"/>
     </row>
     <row r="132" spans="2:4" ht="30" customHeight="1">
       <c r="B132" s="92" t="s">
+        <v>220</v>
+      </c>
+      <c r="C132" s="92" t="s">
+        <v>221</v>
+      </c>
+      <c r="D132" s="92"/>
+    </row>
+    <row r="133" spans="2:4" ht="30" customHeight="1">
+      <c r="B133" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C133" s="92" t="s">
+        <v>222</v>
+      </c>
+      <c r="D133" s="92"/>
+    </row>
+    <row r="134" spans="2:4" ht="30" customHeight="1">
+      <c r="B134" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C134" s="92" t="s">
+        <v>228</v>
+      </c>
+      <c r="D134" s="92"/>
+    </row>
+    <row r="135" spans="2:4" ht="30" customHeight="1">
+      <c r="B135" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="C135" s="92" t="s">
+        <v>232</v>
+      </c>
+      <c r="D135" s="92"/>
+    </row>
+    <row r="136" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B136" s="92"/>
+      <c r="C136" s="92"/>
+      <c r="D136" s="92"/>
+    </row>
+    <row r="137" spans="2:4" ht="30" customHeight="1">
+      <c r="B137" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="C137" s="92" t="s">
+        <v>235</v>
+      </c>
+      <c r="D137" s="92"/>
+    </row>
+    <row r="138" spans="2:4" ht="30" customHeight="1">
+      <c r="B138" s="92" t="s">
+        <v>224</v>
+      </c>
+      <c r="C138" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D138" s="92"/>
+    </row>
+    <row r="139" spans="2:4" ht="30" customHeight="1">
+      <c r="B139" s="92" t="s">
         <v>226</v>
       </c>
-      <c r="C132" s="92" t="s">
+      <c r="C139" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="D132" s="92"/>
-    </row>
-    <row r="133" spans="2:4" ht="4.5" customHeight="1">
-      <c r="B133" s="92"/>
-      <c r="C133" s="92"/>
-      <c r="D133" s="92"/>
-    </row>
-    <row r="134" spans="2:4" ht="30" customHeight="1">
-      <c r="B134" s="93" t="s">
+      <c r="D139" s="92"/>
+    </row>
+    <row r="140" spans="2:4" ht="4.5" customHeight="1">
+      <c r="B140" s="92"/>
+      <c r="C140" s="92"/>
+      <c r="D140" s="92"/>
+    </row>
+    <row r="141" spans="2:4" ht="30" customHeight="1">
+      <c r="B141" s="93" t="s">
         <v>233</v>
       </c>
-      <c r="C134" s="93" t="s">
+      <c r="C141" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="D134" s="93"/>
+      <c r="D141" s="93"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H10" r:id="rId1"/>
+    <hyperlink ref="I10" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B16" r:id="rId3"/>
+    <hyperlink ref="B18" r:id="rId4"/>
+    <hyperlink ref="B19" r:id="rId5"/>
+    <hyperlink ref="J9" r:id="rId6"/>
+    <hyperlink ref="B20" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
nowe zestawienie cen stali
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="322">
   <si>
     <t>Id</t>
   </si>
@@ -1023,9 +1023,6 @@
     <t>biuro@stalkat.pl</t>
   </si>
   <si>
-    <t>Wyslane 2013-08-15</t>
-  </si>
-  <si>
     <t>Centrozłom Wrocław</t>
   </si>
   <si>
@@ -1033,13 +1030,37 @@
   </si>
   <si>
     <t>centrostal@centrostal.com.pl</t>
+  </si>
+  <si>
+    <t>MANEX - z faktur</t>
+  </si>
+  <si>
+    <t>Zapytania wyslane 2013-08-15</t>
+  </si>
+  <si>
+    <t>10mm</t>
+  </si>
+  <si>
+    <t>12mm</t>
+  </si>
+  <si>
+    <t>16mm</t>
+  </si>
+  <si>
+    <t>na koszt kupującego</t>
+  </si>
+  <si>
+    <t>RAZEM</t>
+  </si>
+  <si>
+    <t>5990,72 + dostawa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,6 +1197,14 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1209,7 +1238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -1509,11 +1538,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1741,7 +1826,52 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3948,7 +4078,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740532"/>
+          <c:w val="0.71441426071740521"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4228,24 +4358,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="52205440"/>
-        <c:axId val="52206976"/>
+        <c:axId val="63148800"/>
+        <c:axId val="63150336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52205440"/>
+        <c:axId val="63148800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52206976"/>
+        <c:crossAx val="63150336"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52206976"/>
+        <c:axId val="63150336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -4255,7 +4385,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52205440"/>
+        <c:crossAx val="63148800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4266,8 +4396,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288619"/>
-          <c:y val="0.29353966170895573"/>
+          <c:x val="0.86438523325288641"/>
+          <c:y val="0.29353966170895585"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -4277,7 +4407,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4489,24 +4619,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="70299008"/>
-        <c:axId val="70304896"/>
+        <c:axId val="63208448"/>
+        <c:axId val="63230720"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="70299008"/>
+        <c:axId val="63208448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70304896"/>
+        <c:crossAx val="63230720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="70304896"/>
+        <c:axId val="63230720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -4516,7 +4646,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70299008"/>
+        <c:crossAx val="63208448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4528,7 +4658,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4691,24 +4821,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71370624"/>
-        <c:axId val="71372160"/>
+        <c:axId val="64431616"/>
+        <c:axId val="64433152"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="71370624"/>
+        <c:axId val="64431616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71372160"/>
+        <c:crossAx val="64433152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="71372160"/>
+        <c:axId val="64433152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -4718,7 +4848,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71370624"/>
+        <c:crossAx val="64431616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4730,7 +4860,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4845,11 +4975,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71384064"/>
-        <c:axId val="71443200"/>
+        <c:axId val="64383616"/>
+        <c:axId val="64385408"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="71384064"/>
+        <c:axId val="64383616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4857,13 +4987,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71443200"/>
+        <c:crossAx val="64385408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="71443200"/>
+        <c:axId val="64385408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4871,7 +5001,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71384064"/>
+        <c:crossAx val="64383616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4883,7 +5013,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4899,10 +5029,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961875"/>
-          <c:y val="3.2882035578886089E-2"/>
+          <c:x val="0.17181562830961872"/>
+          <c:y val="3.2882035578886096E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420157"/>
+          <c:h val="0.63861876640420179"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5065,11 +5195,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="71521408"/>
-        <c:axId val="71522944"/>
+        <c:axId val="64533248"/>
+        <c:axId val="64534784"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="71521408"/>
+        <c:axId val="64533248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5077,13 +5207,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71522944"/>
+        <c:crossAx val="64534784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="71522944"/>
+        <c:axId val="64534784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5092,7 +5222,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71521408"/>
+        <c:crossAx val="64533248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5104,7 +5234,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000211" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000211" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5380,8 +5510,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B124:D141" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B124:D141"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Temat" dataDxfId="2"/>
     <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
@@ -9749,10 +9879,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L141"/>
+  <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9995,7 +10125,7 @@
         <v>0</v>
       </c>
       <c r="G9" s="116">
-        <f>C9*F40+D9*G40+E9*I40+F9</f>
+        <f>C9*F45+D9*G45+E9*I45+F9</f>
         <v>3902.86</v>
       </c>
       <c r="H9" s="116">
@@ -10027,7 +10157,7 @@
         <v>150</v>
       </c>
       <c r="G10" s="98">
-        <f>C10*F40+D10*G40+E10*I40+150</f>
+        <f>C10*F45+D10*G45+E10*I45+150</f>
         <v>4298.82</v>
       </c>
       <c r="H10" s="116">
@@ -10059,7 +10189,7 @@
         <v>300</v>
       </c>
       <c r="G11" s="98">
-        <f>C11*F40+D11*G40+E11*I40+F11</f>
+        <f>C11*F45+D11*G45+E11*I45+F11</f>
         <v>4251.5</v>
       </c>
       <c r="H11" s="116">
@@ -10090,7 +10220,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="98">
-        <f>C12*F40+D12*G40+E12*I40+F12</f>
+        <f>C12*F45+D12*G45+E12*I45+F12</f>
         <v>3982.58</v>
       </c>
       <c r="H12" s="116">
@@ -10100,261 +10230,254 @@
       <c r="I12" s="96"/>
       <c r="J12" s="96"/>
     </row>
-    <row r="13" spans="1:12" ht="21.75">
-      <c r="B13" s="123" t="s">
-        <v>311</v>
-      </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="112"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="112"/>
+    <row r="13" spans="1:12" ht="15" thickBot="1">
+      <c r="B13" s="111"/>
+      <c r="C13" s="124"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="124"/>
+      <c r="F13" s="125"/>
       <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
+      <c r="H13" s="123"/>
       <c r="I13" s="111"/>
       <c r="J13" s="111"/>
     </row>
-    <row r="14" spans="1:12">
-      <c r="B14" s="96" t="s">
-        <v>308</v>
-      </c>
-      <c r="C14" s="111"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="111"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="113"/>
+    <row r="14" spans="1:12" ht="21.75">
+      <c r="B14" s="126" t="s">
+        <v>315</v>
+      </c>
+      <c r="C14" s="127" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" s="128" t="s">
+        <v>317</v>
+      </c>
+      <c r="E14" s="127" t="s">
+        <v>318</v>
+      </c>
+      <c r="F14" s="133" t="s">
+        <v>302</v>
+      </c>
+      <c r="G14" s="136" t="s">
+        <v>320</v>
+      </c>
       <c r="H14" s="113"/>
       <c r="I14" s="111"/>
       <c r="J14" s="111"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="B15" s="111" t="s">
-        <v>309</v>
-      </c>
-      <c r="C15" s="111"/>
-      <c r="D15" s="112"/>
-      <c r="E15" s="111"/>
-      <c r="F15" s="112"/>
-      <c r="G15" s="113"/>
+      <c r="B15" s="129" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="96"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="96"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="137"/>
       <c r="H15" s="113"/>
       <c r="I15" s="111"/>
       <c r="J15" s="111"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="B16" s="111" t="s">
-        <v>310</v>
-      </c>
-      <c r="C16" s="111"/>
-      <c r="D16" s="112"/>
-      <c r="E16" s="111"/>
-      <c r="F16" s="112"/>
-      <c r="G16" s="113"/>
+      <c r="B16" s="129" t="s">
+        <v>309</v>
+      </c>
+      <c r="C16" s="96"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="96"/>
+      <c r="F16" s="134"/>
+      <c r="G16" s="137"/>
       <c r="H16" s="113"/>
       <c r="I16" s="111"/>
       <c r="J16" s="111"/>
     </row>
-    <row r="17" spans="2:10">
-      <c r="B17" s="111" t="s">
-        <v>312</v>
-      </c>
-      <c r="C17" s="111"/>
-      <c r="D17" s="112"/>
-      <c r="E17" s="111"/>
-      <c r="F17" s="112"/>
-      <c r="G17" s="113"/>
+    <row r="17" spans="2:10" ht="21.75">
+      <c r="B17" s="129" t="s">
+        <v>310</v>
+      </c>
+      <c r="C17" s="96">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="D17" s="97">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="E17" s="96">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F17" s="134" t="s">
+        <v>319</v>
+      </c>
+      <c r="G17" s="137" t="s">
+        <v>321</v>
+      </c>
       <c r="H17" s="113"/>
       <c r="I17" s="111"/>
       <c r="J17" s="111"/>
     </row>
     <row r="18" spans="2:10">
-      <c r="B18" s="111" t="s">
-        <v>313</v>
-      </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="111"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="113"/>
+      <c r="B18" s="129" t="s">
+        <v>311</v>
+      </c>
+      <c r="C18" s="96"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="96"/>
+      <c r="F18" s="134"/>
+      <c r="G18" s="137"/>
       <c r="H18" s="113"/>
       <c r="I18" s="111"/>
       <c r="J18" s="111"/>
     </row>
-    <row r="19" spans="2:10" ht="21.75">
-      <c r="B19" s="111" t="s">
-        <v>314</v>
-      </c>
-      <c r="C19" s="111"/>
-      <c r="D19" s="112"/>
-      <c r="E19" s="111"/>
-      <c r="F19" s="112"/>
-      <c r="G19" s="113"/>
+    <row r="19" spans="2:10">
+      <c r="B19" s="129" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="96"/>
+      <c r="D19" s="97"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="137"/>
       <c r="H19" s="113"/>
       <c r="I19" s="111"/>
       <c r="J19" s="111"/>
     </row>
-    <row r="20" spans="2:10">
-      <c r="B20" s="96" t="s">
-        <v>295</v>
-      </c>
-      <c r="C20" s="111"/>
-      <c r="D20" s="112"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="112"/>
-      <c r="G20" s="113"/>
+    <row r="20" spans="2:10" ht="21.75">
+      <c r="B20" s="129" t="s">
+        <v>313</v>
+      </c>
+      <c r="C20" s="96"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="137"/>
       <c r="H20" s="113"/>
       <c r="I20" s="111"/>
       <c r="J20" s="111"/>
     </row>
     <row r="21" spans="2:10">
-      <c r="B21" t="s">
+      <c r="B21" s="129" t="s">
+        <v>295</v>
+      </c>
+      <c r="C21" s="96">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="D21" s="97">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="E21" s="96">
+        <v>2.23</v>
+      </c>
+      <c r="F21" s="134">
+        <v>200</v>
+      </c>
+      <c r="G21" s="137">
+        <f>5150.4+200</f>
+        <v>5350.4</v>
+      </c>
+      <c r="H21" s="113"/>
+      <c r="I21" s="111"/>
+      <c r="J21" s="111"/>
+    </row>
+    <row r="22" spans="2:10" ht="15" thickBot="1">
+      <c r="B22" s="132" t="s">
+        <v>314</v>
+      </c>
+      <c r="C22" s="130">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="D22" s="131">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E22" s="130">
+        <v>2.39</v>
+      </c>
+      <c r="F22" s="135">
+        <v>0</v>
+      </c>
+      <c r="G22" s="138">
+        <v>5878.78</v>
+      </c>
+      <c r="H22" s="113"/>
+      <c r="I22" s="111"/>
+      <c r="J22" s="111"/>
+    </row>
+    <row r="23" spans="2:10">
+      <c r="B23" s="111"/>
+      <c r="C23" s="111"/>
+      <c r="D23" s="112"/>
+      <c r="E23" s="111"/>
+      <c r="F23" s="112"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="111"/>
+      <c r="J23" s="111"/>
+    </row>
+    <row r="24" spans="2:10">
+      <c r="B24" s="111"/>
+      <c r="C24" s="111"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="111"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="113"/>
+      <c r="H24" s="113"/>
+      <c r="I24" s="111"/>
+      <c r="J24" s="111"/>
+    </row>
+    <row r="25" spans="2:10">
+      <c r="B25" s="111"/>
+      <c r="C25" s="111"/>
+      <c r="D25" s="112"/>
+      <c r="E25" s="111"/>
+      <c r="F25" s="112"/>
+      <c r="G25" s="113"/>
+      <c r="H25" s="113"/>
+      <c r="I25" s="111"/>
+      <c r="J25" s="111"/>
+    </row>
+    <row r="26" spans="2:10">
+      <c r="B26" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="22" spans="2:10" ht="15" thickBot="1"/>
-    <row r="23" spans="2:10">
-      <c r="B23" s="68" t="s">
+    <row r="27" spans="2:10" ht="15" thickBot="1"/>
+    <row r="28" spans="2:10">
+      <c r="B28" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C23" s="69" t="s">
+      <c r="C28" s="69" t="s">
         <v>180</v>
       </c>
-      <c r="D23" s="69" t="s">
+      <c r="D28" s="69" t="s">
         <v>181</v>
       </c>
-      <c r="E23" s="76" t="s">
+      <c r="E28" s="76" t="s">
         <v>182</v>
       </c>
-      <c r="F23" s="68" t="s">
+      <c r="F28" s="68" t="s">
         <v>185</v>
       </c>
-      <c r="G23" s="69" t="s">
+      <c r="G28" s="69" t="s">
         <v>184</v>
       </c>
-      <c r="H23" s="76"/>
-      <c r="I23" s="70" t="s">
+      <c r="H28" s="76"/>
+      <c r="I28" s="70" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="24" spans="2:10">
-      <c r="B24" s="71">
-        <v>1</v>
-      </c>
-      <c r="C24" s="66">
-        <v>8</v>
-      </c>
-      <c r="D24" s="66">
-        <v>9640</v>
-      </c>
-      <c r="E24" s="77">
-        <v>16</v>
-      </c>
-      <c r="F24" s="71">
-        <f>E24*D24/1000</f>
-        <v>154.24</v>
-      </c>
-      <c r="G24" s="66"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="72"/>
-    </row>
-    <row r="25" spans="2:10">
-      <c r="B25" s="71">
-        <v>2</v>
-      </c>
-      <c r="C25" s="66">
-        <v>8</v>
-      </c>
-      <c r="D25" s="66">
-        <v>6870</v>
-      </c>
-      <c r="E25" s="77">
-        <v>116</v>
-      </c>
-      <c r="F25" s="71">
-        <f t="shared" ref="F25:F36" si="2">E25*D25/1000</f>
-        <v>796.92</v>
-      </c>
-      <c r="G25" s="66"/>
-      <c r="H25" s="77"/>
-      <c r="I25" s="72"/>
-    </row>
-    <row r="26" spans="2:10">
-      <c r="B26" s="71">
-        <v>3</v>
-      </c>
-      <c r="C26" s="66">
-        <v>8</v>
-      </c>
-      <c r="D26" s="66">
-        <v>7970</v>
-      </c>
-      <c r="E26" s="77">
-        <v>28</v>
-      </c>
-      <c r="F26" s="71">
-        <f t="shared" si="2"/>
-        <v>223.16</v>
-      </c>
-      <c r="G26" s="66"/>
-      <c r="H26" s="77"/>
-      <c r="I26" s="72"/>
-    </row>
-    <row r="27" spans="2:10">
-      <c r="B27" s="71">
-        <v>4</v>
-      </c>
-      <c r="C27" s="66">
-        <v>8</v>
-      </c>
-      <c r="D27" s="66">
-        <v>7540</v>
-      </c>
-      <c r="E27" s="77">
-        <v>8</v>
-      </c>
-      <c r="F27" s="71">
-        <f t="shared" si="2"/>
-        <v>60.32</v>
-      </c>
-      <c r="G27" s="66"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="72"/>
-    </row>
-    <row r="28" spans="2:10">
-      <c r="B28" s="71">
-        <v>5</v>
-      </c>
-      <c r="C28" s="66">
-        <v>8</v>
-      </c>
-      <c r="D28" s="66">
-        <v>3180</v>
-      </c>
-      <c r="E28" s="77">
-        <v>10</v>
-      </c>
-      <c r="F28" s="71">
-        <f t="shared" si="2"/>
-        <v>31.8</v>
-      </c>
-      <c r="G28" s="66"/>
-      <c r="H28" s="77"/>
-      <c r="I28" s="72"/>
     </row>
     <row r="29" spans="2:10">
       <c r="B29" s="71">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C29" s="66">
         <v>8</v>
       </c>
       <c r="D29" s="66">
-        <v>9140</v>
+        <v>9640</v>
       </c>
       <c r="E29" s="77">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="F29" s="71">
-        <f t="shared" si="2"/>
-        <v>493.56</v>
+        <f>E29*D29/1000</f>
+        <v>154.24</v>
       </c>
       <c r="G29" s="66"/>
       <c r="H29" s="77"/>
@@ -10362,20 +10485,20 @@
     </row>
     <row r="30" spans="2:10">
       <c r="B30" s="71">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C30" s="66">
         <v>8</v>
       </c>
       <c r="D30" s="66">
-        <v>10040</v>
+        <v>6870</v>
       </c>
       <c r="E30" s="77">
-        <v>36</v>
+        <v>116</v>
       </c>
       <c r="F30" s="71">
-        <f t="shared" si="2"/>
-        <v>361.44</v>
+        <f t="shared" ref="F30:F41" si="2">E30*D30/1000</f>
+        <v>796.92</v>
       </c>
       <c r="G30" s="66"/>
       <c r="H30" s="77"/>
@@ -10383,20 +10506,20 @@
     </row>
     <row r="31" spans="2:10">
       <c r="B31" s="71">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C31" s="66">
         <v>8</v>
       </c>
       <c r="D31" s="66">
-        <v>8340</v>
+        <v>7970</v>
       </c>
       <c r="E31" s="77">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F31" s="71">
         <f t="shared" si="2"/>
-        <v>283.56</v>
+        <v>223.16</v>
       </c>
       <c r="G31" s="66"/>
       <c r="H31" s="77"/>
@@ -10404,379 +10527,389 @@
     </row>
     <row r="32" spans="2:10">
       <c r="B32" s="71">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C32" s="66">
         <v>8</v>
       </c>
       <c r="D32" s="66">
-        <v>2500</v>
+        <v>7540</v>
       </c>
       <c r="E32" s="77">
-        <v>83</v>
+        <v>8</v>
       </c>
       <c r="F32" s="71">
         <f t="shared" si="2"/>
-        <v>207.5</v>
+        <v>60.32</v>
       </c>
       <c r="G32" s="66"/>
       <c r="H32" s="77"/>
       <c r="I32" s="72"/>
     </row>
-    <row r="33" spans="2:12">
+    <row r="33" spans="2:11">
       <c r="B33" s="71">
+        <v>5</v>
+      </c>
+      <c r="C33" s="66">
+        <v>8</v>
+      </c>
+      <c r="D33" s="66">
+        <v>3180</v>
+      </c>
+      <c r="E33" s="77">
         <v>10</v>
       </c>
-      <c r="C33" s="66">
-        <v>10</v>
-      </c>
-      <c r="D33" s="66">
-        <v>970</v>
-      </c>
-      <c r="E33" s="77">
-        <v>38</v>
-      </c>
-      <c r="F33" s="71"/>
-      <c r="G33" s="66">
-        <f>E33*D33/1000</f>
-        <v>36.86</v>
-      </c>
+      <c r="F33" s="71">
+        <f t="shared" si="2"/>
+        <v>31.8</v>
+      </c>
+      <c r="G33" s="66"/>
       <c r="H33" s="77"/>
       <c r="I33" s="72"/>
     </row>
-    <row r="34" spans="2:12">
+    <row r="34" spans="2:11">
       <c r="B34" s="71">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C34" s="66">
         <v>8</v>
       </c>
       <c r="D34" s="66">
-        <v>1780</v>
+        <v>9140</v>
       </c>
       <c r="E34" s="77">
-        <v>240</v>
+        <v>54</v>
       </c>
       <c r="F34" s="71">
         <f t="shared" si="2"/>
-        <v>427.2</v>
+        <v>493.56</v>
       </c>
       <c r="G34" s="66"/>
       <c r="H34" s="77"/>
       <c r="I34" s="72"/>
     </row>
-    <row r="35" spans="2:12">
+    <row r="35" spans="2:11">
       <c r="B35" s="71">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C35" s="66">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D35" s="66">
-        <v>78000</v>
+        <v>10040</v>
       </c>
       <c r="E35" s="77">
-        <v>4</v>
-      </c>
-      <c r="F35" s="71"/>
+        <v>36</v>
+      </c>
+      <c r="F35" s="71">
+        <f t="shared" si="2"/>
+        <v>361.44</v>
+      </c>
       <c r="G35" s="66"/>
       <c r="H35" s="77"/>
-      <c r="I35" s="72">
-        <f>E35*D35/1000</f>
-        <v>312</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12">
+      <c r="I35" s="72"/>
+    </row>
+    <row r="36" spans="2:11">
       <c r="B36" s="71">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C36" s="66">
         <v>8</v>
       </c>
       <c r="D36" s="66">
-        <v>880</v>
+        <v>8340</v>
       </c>
       <c r="E36" s="77">
-        <v>220</v>
+        <v>34</v>
       </c>
       <c r="F36" s="71">
         <f t="shared" si="2"/>
-        <v>193.6</v>
+        <v>283.56</v>
       </c>
       <c r="G36" s="66"/>
       <c r="H36" s="77"/>
       <c r="I36" s="72"/>
     </row>
-    <row r="37" spans="2:12" ht="15" thickBot="1">
-      <c r="B37" s="73">
+    <row r="37" spans="2:11">
+      <c r="B37" s="71">
+        <v>9</v>
+      </c>
+      <c r="C37" s="66">
+        <v>8</v>
+      </c>
+      <c r="D37" s="66">
+        <v>2500</v>
+      </c>
+      <c r="E37" s="77">
+        <v>83</v>
+      </c>
+      <c r="F37" s="71">
+        <f t="shared" si="2"/>
+        <v>207.5</v>
+      </c>
+      <c r="G37" s="66"/>
+      <c r="H37" s="77"/>
+      <c r="I37" s="72"/>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="71">
+        <v>10</v>
+      </c>
+      <c r="C38" s="66">
+        <v>10</v>
+      </c>
+      <c r="D38" s="66">
+        <v>970</v>
+      </c>
+      <c r="E38" s="77">
+        <v>38</v>
+      </c>
+      <c r="F38" s="71"/>
+      <c r="G38" s="66">
+        <f>E38*D38/1000</f>
+        <v>36.86</v>
+      </c>
+      <c r="H38" s="77"/>
+      <c r="I38" s="72"/>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="71">
+        <v>11</v>
+      </c>
+      <c r="C39" s="66">
+        <v>8</v>
+      </c>
+      <c r="D39" s="66">
+        <v>1780</v>
+      </c>
+      <c r="E39" s="77">
+        <v>240</v>
+      </c>
+      <c r="F39" s="71">
+        <f t="shared" si="2"/>
+        <v>427.2</v>
+      </c>
+      <c r="G39" s="66"/>
+      <c r="H39" s="77"/>
+      <c r="I39" s="72"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="71">
+        <v>12</v>
+      </c>
+      <c r="C40" s="66">
+        <v>12</v>
+      </c>
+      <c r="D40" s="66">
+        <v>78000</v>
+      </c>
+      <c r="E40" s="77">
+        <v>4</v>
+      </c>
+      <c r="F40" s="71"/>
+      <c r="G40" s="66"/>
+      <c r="H40" s="77"/>
+      <c r="I40" s="72">
+        <f>E40*D40/1000</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="71">
+        <v>13</v>
+      </c>
+      <c r="C41" s="66">
+        <v>8</v>
+      </c>
+      <c r="D41" s="66">
+        <v>880</v>
+      </c>
+      <c r="E41" s="77">
+        <v>220</v>
+      </c>
+      <c r="F41" s="71">
+        <f t="shared" si="2"/>
+        <v>193.6</v>
+      </c>
+      <c r="G41" s="66"/>
+      <c r="H41" s="77"/>
+      <c r="I41" s="72"/>
+    </row>
+    <row r="42" spans="2:11" ht="15" thickBot="1">
+      <c r="B42" s="73">
         <v>14</v>
       </c>
-      <c r="C37" s="74">
+      <c r="C42" s="74">
         <v>12</v>
       </c>
-      <c r="D37" s="74">
+      <c r="D42" s="74">
         <v>4200</v>
       </c>
-      <c r="E37" s="78">
+      <c r="E42" s="78">
         <v>8</v>
       </c>
-      <c r="F37" s="73"/>
-      <c r="G37" s="74"/>
-      <c r="H37" s="78"/>
-      <c r="I37" s="75">
-        <f t="shared" ref="I37" si="3">E37*D37/1000</f>
+      <c r="F42" s="73"/>
+      <c r="G42" s="74"/>
+      <c r="H42" s="78"/>
+      <c r="I42" s="75">
+        <f t="shared" ref="I42" si="3">E42*D42/1000</f>
         <v>33.6</v>
       </c>
     </row>
-    <row r="38" spans="2:12">
-      <c r="B38" s="67" t="s">
+    <row r="43" spans="2:11">
+      <c r="B43" s="67" t="s">
         <v>187</v>
       </c>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="79"/>
-      <c r="F38" s="80">
-        <f>SUM(F24:F37)</f>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="79"/>
+      <c r="F43" s="80">
+        <f>SUM(F29:F42)</f>
         <v>3233.2999999999993</v>
       </c>
-      <c r="G38" s="67">
-        <f t="shared" ref="G38:I38" si="4">SUM(G24:G37)</f>
+      <c r="G43" s="67">
+        <f t="shared" ref="G43:I43" si="4">SUM(G29:G42)</f>
         <v>36.86</v>
       </c>
-      <c r="H38" s="79"/>
-      <c r="I38" s="81">
+      <c r="H43" s="79"/>
+      <c r="I43" s="81">
         <f t="shared" si="4"/>
         <v>345.6</v>
       </c>
     </row>
-    <row r="39" spans="2:12">
-      <c r="B39" s="66" t="s">
+    <row r="44" spans="2:11">
+      <c r="B44" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="C39" s="66"/>
-      <c r="D39" s="66"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="71">
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="77"/>
+      <c r="F44" s="71">
         <v>0.39500000000000002</v>
       </c>
-      <c r="G39" s="66">
+      <c r="G44" s="66">
         <v>0.61699999999999999</v>
       </c>
-      <c r="H39" s="77"/>
-      <c r="I39" s="72">
+      <c r="H44" s="77"/>
+      <c r="I44" s="72">
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="15.75" thickBot="1">
-      <c r="B40" s="91" t="s">
+    <row r="45" spans="2:11" ht="15.75" thickBot="1">
+      <c r="B45" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="C40" s="91"/>
-      <c r="D40" s="91"/>
-      <c r="E40" s="117"/>
-      <c r="F40" s="118">
-        <f>ROUND(F38*F39,0)</f>
+      <c r="C45" s="91"/>
+      <c r="D45" s="91"/>
+      <c r="E45" s="117"/>
+      <c r="F45" s="118">
+        <f>ROUND(F43*F44,0)</f>
         <v>1277</v>
       </c>
-      <c r="G40" s="119">
-        <f t="shared" ref="G40:I40" si="5">ROUND(G38*G39,0)</f>
+      <c r="G45" s="119">
+        <f t="shared" ref="G45:I45" si="5">ROUND(G43*G44,0)</f>
         <v>23</v>
       </c>
-      <c r="H40" s="122"/>
-      <c r="I40" s="120">
+      <c r="H45" s="122"/>
+      <c r="I45" s="120">
         <f t="shared" si="5"/>
         <v>307</v>
       </c>
     </row>
-    <row r="41" spans="2:12">
-      <c r="B41" s="66"/>
-      <c r="C41" s="66"/>
-      <c r="D41" s="66"/>
-      <c r="E41" s="66"/>
-      <c r="F41" s="67"/>
-      <c r="G41" s="67"/>
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-    </row>
-    <row r="43" spans="2:12">
-      <c r="J43">
+    <row r="46" spans="2:11">
+      <c r="B46" s="66"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="66"/>
+      <c r="E46" s="66"/>
+      <c r="F46" s="67"/>
+      <c r="G46" s="67"/>
+      <c r="H46" s="67"/>
+      <c r="I46" s="67"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="J48">
         <v>1.23</v>
       </c>
-      <c r="K43">
+      <c r="K48">
         <v>2.74</v>
       </c>
     </row>
-    <row r="44" spans="2:12">
-      <c r="B44" t="s">
+    <row r="49" spans="2:12">
+      <c r="B49" t="s">
         <v>278</v>
       </c>
-      <c r="J44">
+      <c r="J49">
         <v>1</v>
       </c>
-      <c r="K44">
+      <c r="K49">
         <f>2.74/1.23</f>
         <v>2.2276422764227646</v>
       </c>
     </row>
-    <row r="45" spans="2:12">
-      <c r="K45">
+    <row r="50" spans="2:12">
+      <c r="K50">
         <v>2.48</v>
       </c>
-      <c r="L45">
+      <c r="L50">
         <f>2.48*1.23</f>
         <v>3.0503999999999998</v>
       </c>
     </row>
-    <row r="46" spans="2:12">
-      <c r="J46">
+    <row r="51" spans="2:12">
+      <c r="J51">
         <v>5520</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="57">
-      <c r="B47" s="92" t="s">
+    <row r="52" spans="2:12" ht="57">
+      <c r="B52" s="92" t="s">
         <v>190</v>
       </c>
-      <c r="C47" s="66"/>
-      <c r="D47" s="66">
+      <c r="C52" s="66"/>
+      <c r="D52" s="66">
         <v>0.68</v>
       </c>
-      <c r="E47" s="66" t="s">
+      <c r="E52" s="66" t="s">
         <v>191</v>
       </c>
-      <c r="F47" s="66"/>
-      <c r="G47" s="66"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="66"/>
-      <c r="J47">
+      <c r="F52" s="66"/>
+      <c r="G52" s="66"/>
+      <c r="H52" s="66"/>
+      <c r="I52" s="66"/>
+      <c r="J52">
         <v>1.23</v>
       </c>
-      <c r="K47">
+      <c r="K52">
         <f>5520*1.3</f>
         <v>7176</v>
       </c>
     </row>
-    <row r="48" spans="2:12">
-      <c r="B48" s="66" t="s">
+    <row r="53" spans="2:12">
+      <c r="B53" s="66" t="s">
         <v>192</v>
-      </c>
-      <c r="C48" s="66"/>
-      <c r="D48" s="66">
-        <v>242</v>
-      </c>
-      <c r="E48" s="66" t="s">
-        <v>193</v>
-      </c>
-      <c r="F48" s="66"/>
-      <c r="G48" s="66"/>
-      <c r="H48" s="66"/>
-      <c r="I48" s="66"/>
-      <c r="J48">
-        <f>J47*J46</f>
-        <v>6789.5999999999995</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11">
-      <c r="B49" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="C49" s="66"/>
-      <c r="D49" s="66">
-        <v>220</v>
-      </c>
-      <c r="E49" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F49" s="66"/>
-      <c r="G49" s="66"/>
-      <c r="H49" s="66"/>
-      <c r="I49" s="66"/>
-      <c r="J49">
-        <f>J48*1.3</f>
-        <v>8826.48</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11">
-      <c r="B50" s="66" t="s">
-        <v>195</v>
-      </c>
-      <c r="C50" s="66"/>
-      <c r="D50" s="66">
-        <v>1418</v>
-      </c>
-      <c r="E50" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="66"/>
-    </row>
-    <row r="51" spans="2:11">
-      <c r="B51" s="66"/>
-      <c r="C51" s="66"/>
-      <c r="D51" s="66"/>
-      <c r="E51" s="66"/>
-      <c r="F51" s="66"/>
-      <c r="G51" s="66"/>
-      <c r="H51" s="66"/>
-      <c r="I51" s="66"/>
-      <c r="J51">
-        <f>5520/1000</f>
-        <v>5.52</v>
-      </c>
-      <c r="K51" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="52" spans="2:11" ht="15">
-      <c r="B52" s="66" t="s">
-        <v>196</v>
-      </c>
-      <c r="C52" s="66"/>
-      <c r="D52" s="91">
-        <v>1035</v>
-      </c>
-      <c r="E52" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F52" s="66" t="s">
-        <v>199</v>
-      </c>
-      <c r="G52" s="66">
-        <v>1607</v>
-      </c>
-      <c r="H52" s="66"/>
-      <c r="I52" s="66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="53" spans="2:11">
-      <c r="B53" s="66" t="s">
-        <v>197</v>
       </c>
       <c r="C53" s="66"/>
       <c r="D53" s="66">
-        <v>266</v>
+        <v>242</v>
       </c>
       <c r="E53" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F53" s="66" t="s">
-        <v>197</v>
-      </c>
-      <c r="G53" s="66">
-        <v>577</v>
-      </c>
+        <v>193</v>
+      </c>
+      <c r="F53" s="66"/>
+      <c r="G53" s="66"/>
       <c r="H53" s="66"/>
-      <c r="I53" s="66" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="54" spans="2:11">
-      <c r="B54" s="66"/>
+      <c r="I53" s="66"/>
+      <c r="J53">
+        <f>J52*J51</f>
+        <v>6789.5999999999995</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="66" t="s">
+        <v>194</v>
+      </c>
       <c r="C54" s="66"/>
       <c r="D54" s="66">
-        <v>138</v>
+        <v>220</v>
       </c>
       <c r="E54" s="66" t="s">
         <v>191</v>
@@ -10785,12 +10918,18 @@
       <c r="G54" s="66"/>
       <c r="H54" s="66"/>
       <c r="I54" s="66"/>
-    </row>
-    <row r="55" spans="2:11">
-      <c r="B55" s="66"/>
+      <c r="J54">
+        <f>J53*1.3</f>
+        <v>8826.48</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="B55" s="66" t="s">
+        <v>195</v>
+      </c>
       <c r="C55" s="66"/>
       <c r="D55" s="66">
-        <v>173</v>
+        <v>1418</v>
       </c>
       <c r="E55" s="66" t="s">
         <v>191</v>
@@ -10800,202 +10939,191 @@
       <c r="H55" s="66"/>
       <c r="I55" s="66"/>
     </row>
-    <row r="56" spans="2:11" ht="15">
+    <row r="56" spans="2:12">
       <c r="B56" s="66"/>
       <c r="C56" s="66"/>
-      <c r="D56" s="91">
-        <f>D53+D54+D55</f>
-        <v>577</v>
-      </c>
-      <c r="E56" s="66" t="s">
-        <v>198</v>
-      </c>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
       <c r="F56" s="66"/>
       <c r="G56" s="66"/>
       <c r="H56" s="66"/>
       <c r="I56" s="66"/>
-    </row>
-    <row r="57" spans="2:11">
-      <c r="B57" s="66"/>
+      <c r="J56">
+        <f>5520/1000</f>
+        <v>5.52</v>
+      </c>
+      <c r="K56" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" ht="15">
+      <c r="B57" s="66" t="s">
+        <v>196</v>
+      </c>
       <c r="C57" s="66"/>
-      <c r="D57" s="66"/>
-      <c r="E57" s="66"/>
-      <c r="F57" s="66"/>
-      <c r="G57" s="66"/>
+      <c r="D57" s="91">
+        <v>1035</v>
+      </c>
+      <c r="E57" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F57" s="66" t="s">
+        <v>199</v>
+      </c>
+      <c r="G57" s="66">
+        <v>1607</v>
+      </c>
       <c r="H57" s="66"/>
-      <c r="I57" s="66"/>
-    </row>
-    <row r="58" spans="2:11" ht="15">
-      <c r="B58" s="66"/>
+      <c r="I57" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="B58" s="66" t="s">
+        <v>197</v>
+      </c>
       <c r="C58" s="66"/>
-      <c r="D58" s="91">
-        <f>D52+D56</f>
+      <c r="D58" s="66">
+        <v>266</v>
+      </c>
+      <c r="E58" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F58" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="G58" s="66">
+        <v>577</v>
+      </c>
+      <c r="H58" s="66"/>
+      <c r="I58" s="66" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="B59" s="66"/>
+      <c r="C59" s="66"/>
+      <c r="D59" s="66">
+        <v>138</v>
+      </c>
+      <c r="E59" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F59" s="66"/>
+      <c r="G59" s="66"/>
+      <c r="H59" s="66"/>
+      <c r="I59" s="66"/>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="B60" s="66"/>
+      <c r="C60" s="66"/>
+      <c r="D60" s="66">
+        <v>173</v>
+      </c>
+      <c r="E60" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F60" s="66"/>
+      <c r="G60" s="66"/>
+      <c r="H60" s="66"/>
+      <c r="I60" s="66"/>
+    </row>
+    <row r="61" spans="2:12" ht="15">
+      <c r="B61" s="66"/>
+      <c r="C61" s="66"/>
+      <c r="D61" s="91">
+        <f>D58+D59+D60</f>
+        <v>577</v>
+      </c>
+      <c r="E61" s="66" t="s">
+        <v>198</v>
+      </c>
+      <c r="F61" s="66"/>
+      <c r="G61" s="66"/>
+      <c r="H61" s="66"/>
+      <c r="I61" s="66"/>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" s="66"/>
+      <c r="C62" s="66"/>
+      <c r="D62" s="66"/>
+      <c r="E62" s="66"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="66"/>
+      <c r="H62" s="66"/>
+      <c r="I62" s="66"/>
+    </row>
+    <row r="63" spans="2:12" ht="15">
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="91">
+        <f>D57+D61</f>
         <v>1612</v>
       </c>
-      <c r="E58" s="66"/>
-      <c r="F58" s="66"/>
-      <c r="G58" s="66"/>
-      <c r="H58" s="66"/>
-      <c r="I58" s="66"/>
-    </row>
-    <row r="64" spans="2:11" ht="15.75" thickBot="1">
-      <c r="B64" s="90" t="s">
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="66"/>
+    </row>
+    <row r="69" spans="2:9" ht="15.75" thickBot="1">
+      <c r="B69" s="90" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="65" spans="2:9">
-      <c r="B65" s="68" t="s">
+    <row r="70" spans="2:9">
+      <c r="B70" s="68" t="s">
         <v>189</v>
       </c>
-      <c r="C65" s="69" t="s">
+      <c r="C70" s="69" t="s">
         <v>200</v>
       </c>
-      <c r="D65" s="69" t="s">
+      <c r="D70" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="E65" s="69" t="s">
+      <c r="E70" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="F65" s="69" t="s">
+      <c r="F70" s="69" t="s">
         <v>202</v>
       </c>
-      <c r="G65" s="69" t="s">
+      <c r="G70" s="69" t="s">
         <v>203</v>
       </c>
-      <c r="H65" s="76"/>
-      <c r="I65" s="70" t="s">
+      <c r="H70" s="76"/>
+      <c r="I70" s="70" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="66" spans="2:9">
-      <c r="B66" s="71">
-        <v>1</v>
-      </c>
-      <c r="C66" s="66">
-        <v>18</v>
-      </c>
-      <c r="D66" s="66">
-        <v>9.74</v>
-      </c>
-      <c r="E66" s="66">
-        <v>4</v>
-      </c>
-      <c r="F66" s="66"/>
-      <c r="G66" s="66"/>
-      <c r="H66" s="77"/>
-      <c r="I66" s="72">
-        <v>39.1</v>
-      </c>
-    </row>
-    <row r="67" spans="2:9">
-      <c r="B67" s="71">
-        <v>2</v>
-      </c>
-      <c r="C67" s="66">
-        <v>18</v>
-      </c>
-      <c r="D67" s="66">
-        <v>3.27</v>
-      </c>
-      <c r="E67" s="66">
-        <v>4</v>
-      </c>
-      <c r="F67" s="66"/>
-      <c r="G67" s="66"/>
-      <c r="H67" s="77"/>
-      <c r="I67" s="72">
-        <v>13.1</v>
-      </c>
-    </row>
-    <row r="68" spans="2:9">
-      <c r="B68" s="71">
-        <v>3</v>
-      </c>
-      <c r="C68" s="66">
-        <v>14</v>
-      </c>
-      <c r="D68" s="66">
-        <v>3.3</v>
-      </c>
-      <c r="E68" s="66">
-        <v>2</v>
-      </c>
-      <c r="F68" s="66"/>
-      <c r="G68" s="66">
-        <v>6.6</v>
-      </c>
-      <c r="H68" s="77"/>
-      <c r="I68" s="72"/>
-    </row>
-    <row r="69" spans="2:9">
-      <c r="B69" s="71">
-        <v>4</v>
-      </c>
-      <c r="C69" s="66">
-        <v>14</v>
-      </c>
-      <c r="D69" s="66">
-        <v>3.58</v>
-      </c>
-      <c r="E69" s="66">
-        <v>2</v>
-      </c>
-      <c r="F69" s="66"/>
-      <c r="G69" s="66">
-        <v>7.2</v>
-      </c>
-      <c r="H69" s="77"/>
-      <c r="I69" s="72"/>
-    </row>
-    <row r="70" spans="2:9">
-      <c r="B70" s="71">
-        <v>5</v>
-      </c>
-      <c r="C70" s="66">
-        <v>6</v>
-      </c>
-      <c r="D70" s="66">
-        <v>1.3</v>
-      </c>
-      <c r="E70" s="66">
-        <v>17</v>
-      </c>
-      <c r="F70" s="66">
-        <v>22.1</v>
-      </c>
-      <c r="G70" s="66"/>
-      <c r="H70" s="77"/>
-      <c r="I70" s="72"/>
     </row>
     <row r="71" spans="2:9">
       <c r="B71" s="71">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C71" s="66">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D71" s="66">
-        <v>1.64</v>
+        <v>9.74</v>
       </c>
       <c r="E71" s="66">
-        <v>23</v>
-      </c>
-      <c r="F71" s="66">
-        <v>37.700000000000003</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="F71" s="66"/>
       <c r="G71" s="66"/>
       <c r="H71" s="77"/>
-      <c r="I71" s="72"/>
+      <c r="I71" s="72">
+        <v>39.1</v>
+      </c>
     </row>
     <row r="72" spans="2:9">
       <c r="B72" s="71">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C72" s="66">
         <v>18</v>
       </c>
       <c r="D72" s="66">
-        <v>7.2</v>
+        <v>3.27</v>
       </c>
       <c r="E72" s="66">
         <v>4</v>
@@ -11004,230 +11132,278 @@
       <c r="G72" s="66"/>
       <c r="H72" s="77"/>
       <c r="I72" s="72">
-        <v>28.8</v>
+        <v>13.1</v>
       </c>
     </row>
     <row r="73" spans="2:9">
       <c r="B73" s="71">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C73" s="66">
         <v>14</v>
       </c>
       <c r="D73" s="66">
-        <v>6.52</v>
+        <v>3.3</v>
       </c>
       <c r="E73" s="66">
         <v>2</v>
       </c>
       <c r="F73" s="66"/>
       <c r="G73" s="66">
-        <v>13</v>
+        <v>6.6</v>
       </c>
       <c r="H73" s="77"/>
       <c r="I73" s="72"/>
     </row>
     <row r="74" spans="2:9">
       <c r="B74" s="71">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C74" s="66">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D74" s="66">
-        <v>1.64</v>
+        <v>3.58</v>
       </c>
       <c r="E74" s="66">
-        <v>35</v>
-      </c>
-      <c r="F74" s="66">
-        <v>57.4</v>
-      </c>
-      <c r="G74" s="66"/>
+        <v>2</v>
+      </c>
+      <c r="F74" s="66"/>
+      <c r="G74" s="66">
+        <v>7.2</v>
+      </c>
       <c r="H74" s="77"/>
       <c r="I74" s="72"/>
     </row>
     <row r="75" spans="2:9">
       <c r="B75" s="71">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C75" s="66">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D75" s="66">
-        <v>5.67</v>
+        <v>1.3</v>
       </c>
       <c r="E75" s="66">
-        <v>2</v>
-      </c>
-      <c r="F75" s="66"/>
-      <c r="G75" s="66">
-        <v>11.3</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="F75" s="66">
+        <v>22.1</v>
+      </c>
+      <c r="G75" s="66"/>
       <c r="H75" s="77"/>
       <c r="I75" s="72"/>
     </row>
     <row r="76" spans="2:9">
       <c r="B76" s="71">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C76" s="66">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D76" s="66">
-        <v>4.63</v>
+        <v>1.64</v>
       </c>
       <c r="E76" s="66">
-        <v>4</v>
-      </c>
-      <c r="F76" s="66"/>
-      <c r="G76" s="66">
-        <v>18.5</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="F76" s="66">
+        <v>37.700000000000003</v>
+      </c>
+      <c r="G76" s="66"/>
       <c r="H76" s="77"/>
       <c r="I76" s="72"/>
     </row>
-    <row r="77" spans="2:9" ht="15" thickBot="1">
-      <c r="B77" s="73">
+    <row r="77" spans="2:9">
+      <c r="B77" s="71">
+        <v>7</v>
+      </c>
+      <c r="C77" s="66">
+        <v>18</v>
+      </c>
+      <c r="D77" s="66">
+        <v>7.2</v>
+      </c>
+      <c r="E77" s="66">
+        <v>4</v>
+      </c>
+      <c r="F77" s="66"/>
+      <c r="G77" s="66"/>
+      <c r="H77" s="77"/>
+      <c r="I77" s="72">
+        <v>28.8</v>
+      </c>
+    </row>
+    <row r="78" spans="2:9">
+      <c r="B78" s="71">
+        <v>8</v>
+      </c>
+      <c r="C78" s="66">
+        <v>14</v>
+      </c>
+      <c r="D78" s="66">
+        <v>6.52</v>
+      </c>
+      <c r="E78" s="66">
+        <v>2</v>
+      </c>
+      <c r="F78" s="66"/>
+      <c r="G78" s="66">
+        <v>13</v>
+      </c>
+      <c r="H78" s="77"/>
+      <c r="I78" s="72"/>
+    </row>
+    <row r="79" spans="2:9">
+      <c r="B79" s="71">
+        <v>9</v>
+      </c>
+      <c r="C79" s="66">
+        <v>6</v>
+      </c>
+      <c r="D79" s="66">
+        <v>1.64</v>
+      </c>
+      <c r="E79" s="66">
+        <v>35</v>
+      </c>
+      <c r="F79" s="66">
+        <v>57.4</v>
+      </c>
+      <c r="G79" s="66"/>
+      <c r="H79" s="77"/>
+      <c r="I79" s="72"/>
+    </row>
+    <row r="80" spans="2:9">
+      <c r="B80" s="71">
+        <v>10</v>
+      </c>
+      <c r="C80" s="66">
+        <v>14</v>
+      </c>
+      <c r="D80" s="66">
+        <v>5.67</v>
+      </c>
+      <c r="E80" s="66">
+        <v>2</v>
+      </c>
+      <c r="F80" s="66"/>
+      <c r="G80" s="66">
+        <v>11.3</v>
+      </c>
+      <c r="H80" s="77"/>
+      <c r="I80" s="72"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="71">
+        <v>11</v>
+      </c>
+      <c r="C81" s="66">
+        <v>14</v>
+      </c>
+      <c r="D81" s="66">
+        <v>4.63</v>
+      </c>
+      <c r="E81" s="66">
+        <v>4</v>
+      </c>
+      <c r="F81" s="66"/>
+      <c r="G81" s="66">
+        <v>18.5</v>
+      </c>
+      <c r="H81" s="77"/>
+      <c r="I81" s="72"/>
+    </row>
+    <row r="82" spans="2:9" ht="15" thickBot="1">
+      <c r="B82" s="73">
         <v>12</v>
       </c>
-      <c r="C77" s="74">
+      <c r="C82" s="74">
         <v>6</v>
       </c>
-      <c r="D77" s="74">
+      <c r="D82" s="74">
         <v>1.64</v>
       </c>
-      <c r="E77" s="74">
+      <c r="E82" s="74">
         <v>29</v>
       </c>
-      <c r="F77" s="74">
+      <c r="F82" s="74">
         <v>47.6</v>
       </c>
-      <c r="G77" s="74"/>
-      <c r="H77" s="78"/>
-      <c r="I77" s="75"/>
-    </row>
-    <row r="78" spans="2:9">
-      <c r="B78" s="67"/>
-      <c r="C78" s="67"/>
-      <c r="D78" s="67" t="s">
+      <c r="G82" s="74"/>
+      <c r="H82" s="78"/>
+      <c r="I82" s="75"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="67"/>
+      <c r="C83" s="67"/>
+      <c r="D83" s="67" t="s">
         <v>205</v>
       </c>
-      <c r="E78" s="67" t="s">
+      <c r="E83" s="67" t="s">
         <v>206</v>
       </c>
-      <c r="F78" s="67">
+      <c r="F83" s="67">
         <v>164.8</v>
       </c>
-      <c r="G78" s="67">
+      <c r="G83" s="67">
         <v>56.7</v>
       </c>
-      <c r="H78" s="67"/>
-      <c r="I78" s="67">
+      <c r="H83" s="67"/>
+      <c r="I83" s="67">
         <v>80.8</v>
       </c>
-    </row>
-    <row r="79" spans="2:9">
-      <c r="B79" s="66"/>
-      <c r="C79" s="66"/>
-      <c r="D79" s="66" t="s">
-        <v>207</v>
-      </c>
-      <c r="E79" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F79" s="66">
-        <v>0.222</v>
-      </c>
-      <c r="G79" s="66">
-        <v>1.208</v>
-      </c>
-      <c r="H79" s="66"/>
-      <c r="I79" s="66">
-        <v>1.998</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9">
-      <c r="B80" s="66"/>
-      <c r="C80" s="66"/>
-      <c r="D80" s="66" t="s">
-        <v>208</v>
-      </c>
-      <c r="E80" s="66" t="s">
-        <v>191</v>
-      </c>
-      <c r="F80" s="66">
-        <v>36.6</v>
-      </c>
-      <c r="G80" s="66">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="H80" s="66"/>
-      <c r="I80" s="66">
-        <v>161.5</v>
-      </c>
-    </row>
-    <row r="81" spans="2:9" ht="15">
-      <c r="B81" s="66"/>
-      <c r="C81" s="66"/>
-      <c r="D81" s="91" t="s">
-        <v>209</v>
-      </c>
-      <c r="E81" s="91" t="s">
-        <v>210</v>
-      </c>
-      <c r="F81" s="66"/>
-      <c r="G81" s="66"/>
-      <c r="H81" s="66"/>
-      <c r="I81" s="66"/>
-    </row>
-    <row r="82" spans="2:9">
-      <c r="B82" s="66"/>
-      <c r="C82" s="66"/>
-      <c r="D82" s="66"/>
-      <c r="E82" s="66"/>
-      <c r="F82" s="66"/>
-      <c r="G82" s="66"/>
-      <c r="H82" s="66"/>
-      <c r="I82" s="66"/>
-    </row>
-    <row r="83" spans="2:9" ht="15">
-      <c r="B83" s="90" t="s">
-        <v>212</v>
-      </c>
-      <c r="C83" s="66"/>
-      <c r="D83" s="66"/>
-      <c r="E83" s="66"/>
-      <c r="F83" s="66"/>
-      <c r="G83" s="66"/>
-      <c r="H83" s="66"/>
-      <c r="I83" s="66"/>
     </row>
     <row r="84" spans="2:9">
       <c r="B84" s="66"/>
       <c r="C84" s="66"/>
-      <c r="D84" s="66"/>
-      <c r="E84" s="66"/>
-      <c r="F84" s="66"/>
-      <c r="G84" s="66"/>
+      <c r="D84" s="66" t="s">
+        <v>207</v>
+      </c>
+      <c r="E84" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F84" s="66">
+        <v>0.222</v>
+      </c>
+      <c r="G84" s="66">
+        <v>1.208</v>
+      </c>
       <c r="H84" s="66"/>
-      <c r="I84" s="66"/>
+      <c r="I84" s="66">
+        <v>1.998</v>
+      </c>
     </row>
     <row r="85" spans="2:9">
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
-      <c r="D85" s="66"/>
-      <c r="E85" s="66"/>
-      <c r="F85" s="66"/>
-      <c r="G85" s="66"/>
+      <c r="D85" s="66" t="s">
+        <v>208</v>
+      </c>
+      <c r="E85" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="F85" s="66">
+        <v>36.6</v>
+      </c>
+      <c r="G85" s="66">
+        <v>68.400000000000006</v>
+      </c>
       <c r="H85" s="66"/>
-      <c r="I85" s="66"/>
-    </row>
-    <row r="86" spans="2:9">
+      <c r="I85" s="66">
+        <v>161.5</v>
+      </c>
+    </row>
+    <row r="86" spans="2:9" ht="15">
       <c r="B86" s="66"/>
       <c r="C86" s="66"/>
-      <c r="D86" s="66"/>
-      <c r="E86" s="66"/>
+      <c r="D86" s="91" t="s">
+        <v>209</v>
+      </c>
+      <c r="E86" s="91" t="s">
+        <v>210</v>
+      </c>
       <c r="F86" s="66"/>
       <c r="G86" s="66"/>
       <c r="H86" s="66"/>
@@ -11243,8 +11419,10 @@
       <c r="H87" s="66"/>
       <c r="I87" s="66"/>
     </row>
-    <row r="88" spans="2:9">
-      <c r="B88" s="66"/>
+    <row r="88" spans="2:9" ht="15">
+      <c r="B88" s="90" t="s">
+        <v>212</v>
+      </c>
       <c r="C88" s="66"/>
       <c r="D88" s="66"/>
       <c r="E88" s="66"/>
@@ -11473,107 +11651,116 @@
       <c r="H110" s="66"/>
       <c r="I110" s="66"/>
     </row>
-    <row r="124" spans="2:4">
-      <c r="B124" t="s">
+    <row r="111" spans="2:9">
+      <c r="B111" s="66"/>
+      <c r="C111" s="66"/>
+      <c r="D111" s="66"/>
+      <c r="E111" s="66"/>
+      <c r="F111" s="66"/>
+      <c r="G111" s="66"/>
+      <c r="H111" s="66"/>
+      <c r="I111" s="66"/>
+    </row>
+    <row r="112" spans="2:9">
+      <c r="B112" s="66"/>
+      <c r="C112" s="66"/>
+      <c r="D112" s="66"/>
+      <c r="E112" s="66"/>
+      <c r="F112" s="66"/>
+      <c r="G112" s="66"/>
+      <c r="H112" s="66"/>
+      <c r="I112" s="66"/>
+    </row>
+    <row r="113" spans="2:9">
+      <c r="B113" s="66"/>
+      <c r="C113" s="66"/>
+      <c r="D113" s="66"/>
+      <c r="E113" s="66"/>
+      <c r="F113" s="66"/>
+      <c r="G113" s="66"/>
+      <c r="H113" s="66"/>
+      <c r="I113" s="66"/>
+    </row>
+    <row r="114" spans="2:9">
+      <c r="B114" s="66"/>
+      <c r="C114" s="66"/>
+      <c r="D114" s="66"/>
+      <c r="E114" s="66"/>
+      <c r="F114" s="66"/>
+      <c r="G114" s="66"/>
+      <c r="H114" s="66"/>
+      <c r="I114" s="66"/>
+    </row>
+    <row r="115" spans="2:9">
+      <c r="B115" s="66"/>
+      <c r="C115" s="66"/>
+      <c r="D115" s="66"/>
+      <c r="E115" s="66"/>
+      <c r="F115" s="66"/>
+      <c r="G115" s="66"/>
+      <c r="H115" s="66"/>
+      <c r="I115" s="66"/>
+    </row>
+    <row r="129" spans="2:4">
+      <c r="B129" t="s">
         <v>236</v>
       </c>
-      <c r="C124" t="s">
+      <c r="C129" t="s">
         <v>237</v>
       </c>
-      <c r="D124" t="s">
+      <c r="D129" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="2:4" ht="30" customHeight="1">
-      <c r="B125" s="66" t="s">
+    <row r="130" spans="2:4" ht="30" customHeight="1">
+      <c r="B130" s="66" t="s">
         <v>214</v>
       </c>
-      <c r="C125" s="66"/>
-      <c r="D125" s="66"/>
-    </row>
-    <row r="126" spans="2:4" ht="30" customHeight="1">
-      <c r="B126" s="92" t="s">
+      <c r="C130" s="66"/>
+      <c r="D130" s="66"/>
+    </row>
+    <row r="131" spans="2:4" ht="30" customHeight="1">
+      <c r="B131" s="92" t="s">
         <v>213</v>
       </c>
-      <c r="C126" s="92" t="s">
+      <c r="C131" s="92" t="s">
         <v>215</v>
       </c>
-      <c r="D126" s="92"/>
-    </row>
-    <row r="127" spans="2:4" ht="30" customHeight="1">
-      <c r="B127" s="92" t="s">
-        <v>239</v>
-      </c>
-      <c r="C127" s="92" t="s">
-        <v>240</v>
-      </c>
-      <c r="D127" s="92"/>
-    </row>
-    <row r="128" spans="2:4" ht="30" customHeight="1">
-      <c r="B128" s="92" t="s">
-        <v>216</v>
-      </c>
-      <c r="C128" s="92" t="s">
-        <v>229</v>
-      </c>
-      <c r="D128" s="92"/>
-    </row>
-    <row r="129" spans="2:4" ht="30" customHeight="1">
-      <c r="B129" s="92" t="s">
-        <v>217</v>
-      </c>
-      <c r="C129" s="92" t="s">
-        <v>230</v>
-      </c>
-      <c r="D129" s="92"/>
-    </row>
-    <row r="130" spans="2:4" ht="30" customHeight="1">
-      <c r="B130" s="92" t="s">
-        <v>218</v>
-      </c>
-      <c r="C130" s="92" t="s">
-        <v>219</v>
-      </c>
-      <c r="D130" s="92"/>
-    </row>
-    <row r="131" spans="2:4" ht="5.25" customHeight="1">
-      <c r="B131" s="92"/>
-      <c r="C131" s="92"/>
       <c r="D131" s="92"/>
     </row>
     <row r="132" spans="2:4" ht="30" customHeight="1">
       <c r="B132" s="92" t="s">
-        <v>220</v>
+        <v>239</v>
       </c>
       <c r="C132" s="92" t="s">
-        <v>221</v>
+        <v>240</v>
       </c>
       <c r="D132" s="92"/>
     </row>
     <row r="133" spans="2:4" ht="30" customHeight="1">
       <c r="B133" s="92" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C133" s="92" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="D133" s="92"/>
     </row>
     <row r="134" spans="2:4" ht="30" customHeight="1">
       <c r="B134" s="92" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C134" s="92" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D134" s="92"/>
     </row>
     <row r="135" spans="2:4" ht="30" customHeight="1">
       <c r="B135" s="92" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="C135" s="92" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="D135" s="92"/>
     </row>
@@ -11584,54 +11771,95 @@
     </row>
     <row r="137" spans="2:4" ht="30" customHeight="1">
       <c r="B137" s="92" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C137" s="92" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="D137" s="92"/>
     </row>
     <row r="138" spans="2:4" ht="30" customHeight="1">
       <c r="B138" s="92" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C138" s="92" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D138" s="92"/>
     </row>
     <row r="139" spans="2:4" ht="30" customHeight="1">
       <c r="B139" s="92" t="s">
+        <v>218</v>
+      </c>
+      <c r="C139" s="92" t="s">
+        <v>228</v>
+      </c>
+      <c r="D139" s="92"/>
+    </row>
+    <row r="140" spans="2:4" ht="30" customHeight="1">
+      <c r="B140" s="92" t="s">
+        <v>231</v>
+      </c>
+      <c r="C140" s="92" t="s">
+        <v>232</v>
+      </c>
+      <c r="D140" s="92"/>
+    </row>
+    <row r="141" spans="2:4" ht="5.25" customHeight="1">
+      <c r="B141" s="92"/>
+      <c r="C141" s="92"/>
+      <c r="D141" s="92"/>
+    </row>
+    <row r="142" spans="2:4" ht="30" customHeight="1">
+      <c r="B142" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="C142" s="92" t="s">
+        <v>235</v>
+      </c>
+      <c r="D142" s="92"/>
+    </row>
+    <row r="143" spans="2:4" ht="30" customHeight="1">
+      <c r="B143" s="92" t="s">
+        <v>224</v>
+      </c>
+      <c r="C143" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="D143" s="92"/>
+    </row>
+    <row r="144" spans="2:4" ht="30" customHeight="1">
+      <c r="B144" s="92" t="s">
         <v>226</v>
       </c>
-      <c r="C139" s="92" t="s">
+      <c r="C144" s="92" t="s">
         <v>227</v>
       </c>
-      <c r="D139" s="92"/>
-    </row>
-    <row r="140" spans="2:4" ht="4.5" customHeight="1">
-      <c r="B140" s="92"/>
-      <c r="C140" s="92"/>
-      <c r="D140" s="92"/>
-    </row>
-    <row r="141" spans="2:4" ht="30" customHeight="1">
-      <c r="B141" s="93" t="s">
+      <c r="D144" s="92"/>
+    </row>
+    <row r="145" spans="2:4" ht="4.5" customHeight="1">
+      <c r="B145" s="92"/>
+      <c r="C145" s="92"/>
+      <c r="D145" s="92"/>
+    </row>
+    <row r="146" spans="2:4" ht="30" customHeight="1">
+      <c r="B146" s="93" t="s">
         <v>233</v>
       </c>
-      <c r="C141" s="93" t="s">
+      <c r="C146" s="93" t="s">
         <v>234</v>
       </c>
-      <c r="D141" s="93"/>
+      <c r="D146" s="93"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="I10" r:id="rId1"/>
-    <hyperlink ref="B14" r:id="rId2"/>
-    <hyperlink ref="B16" r:id="rId3"/>
-    <hyperlink ref="B18" r:id="rId4"/>
-    <hyperlink ref="B19" r:id="rId5"/>
+    <hyperlink ref="B15" r:id="rId2"/>
+    <hyperlink ref="B17" r:id="rId3"/>
+    <hyperlink ref="B19" r:id="rId4"/>
+    <hyperlink ref="B20" r:id="rId5"/>
     <hyperlink ref="J9" r:id="rId6"/>
-    <hyperlink ref="B20" r:id="rId7"/>
+    <hyperlink ref="B21" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId8"/>

</xml_diff>

<commit_message>
dodałam 'sprint' 6 jako listę spraw do załatwienia w najbliższym czasie
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -13,8 +13,9 @@
     <sheet name="03_Sprint" sheetId="4" r:id="rId4"/>
     <sheet name="04_Sprint" sheetId="5" r:id="rId5"/>
     <sheet name="05_Sprint" sheetId="6" r:id="rId6"/>
-    <sheet name="Piasek i stal" sheetId="7" r:id="rId7"/>
-    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId8"/>
+    <sheet name="06_Sprint" sheetId="9" r:id="rId7"/>
+    <sheet name="Piasek i stal" sheetId="7" r:id="rId8"/>
+    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -86,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="361">
   <si>
     <t>Id</t>
   </si>
@@ -1054,13 +1055,132 @@
   </si>
   <si>
     <t>5990,72 + dostawa</t>
+  </si>
+  <si>
+    <t>ceny netto</t>
+  </si>
+  <si>
+    <t>240 netto</t>
+  </si>
+  <si>
+    <t>SPRINT 06</t>
+  </si>
+  <si>
+    <t>SPOTKANIE Z GLAPĄ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wyliczyć dokładnie rozmiary i umiejscowienie w pionie otworów okiennych (i drzwi) </t>
+  </si>
+  <si>
+    <t>ustalić rozmiar bloczków</t>
+  </si>
+  <si>
+    <t>sprawdzić Glapie jak zmienić funkcjonalność lewego Alt</t>
+  </si>
+  <si>
+    <t>zabrać ze sobą projekt budowlany</t>
+  </si>
+  <si>
+    <t>KOZANOWSKA</t>
+  </si>
+  <si>
+    <t>opłacić składki ubezpieczenia na życie w ING</t>
+  </si>
+  <si>
+    <t>ŁADNA</t>
+  </si>
+  <si>
+    <t>sprawdzić, czy został opłacony podatek za grunt</t>
+  </si>
+  <si>
+    <t>KREDYT DB - URUCHOMIENIE</t>
+  </si>
+  <si>
+    <t>zakupić komplet potrzebnych euro na walutomacie</t>
+  </si>
+  <si>
+    <t>nadpłacić kredyt w mBanku</t>
+  </si>
+  <si>
+    <t>zawnioskować o wydanie opinii o kredycie</t>
+  </si>
+  <si>
+    <t>przygotować pisemna dyspozycję całkowitej spłaty</t>
+  </si>
+  <si>
+    <t>uzyskać podpis mBanku (Bogacka) na dyspozycji</t>
+  </si>
+  <si>
+    <t>złożyć dyspozycję wypłaty pierwszej transzy w DB</t>
+  </si>
+  <si>
+    <t>KREDYT DB - POSPRZEDAŻ</t>
+  </si>
+  <si>
+    <t>podpisać notarialnie Wniosek o wpis do hipoteki</t>
+  </si>
+  <si>
+    <t>złożyć w eurobanku zlecenie wypłaty wynagrodzenia na konto DB</t>
+  </si>
+  <si>
+    <t>pamiętać, że po otrzymaniu KK zrobić w ciągu miesiąca jedną operację</t>
+  </si>
+  <si>
+    <t>uzyskać dostęp do konta DB online</t>
+  </si>
+  <si>
+    <t>BUDOWA</t>
+  </si>
+  <si>
+    <t>wysłać zapytania ofertowe na bloczki silikatowe</t>
+  </si>
+  <si>
+    <t>wysłać zapytania ofertowe na strop Teriva</t>
+  </si>
+  <si>
+    <t>zrobić przelew wynagrodzenia dla Nowaka</t>
+  </si>
+  <si>
+    <t>przygotować gotówkę dla Nowaka za fakturę</t>
+  </si>
+  <si>
+    <t>opłacenie wiszącej faktury Manex (do 22.08)</t>
+  </si>
+  <si>
+    <t>przekazanie Manexowi telefonu do Słonki</t>
+  </si>
+  <si>
+    <t>dowiedzieć się co z fakturą za beton</t>
+  </si>
+  <si>
+    <t>INNE</t>
+  </si>
+  <si>
+    <t>kupić papier do drukarki</t>
+  </si>
+  <si>
+    <t>pamiętać o spłacie pożyczki od Borka</t>
+  </si>
+  <si>
+    <t>zaplanować spotkanie z Rekuparatorami (bądź oszacować, czy zrobimy instalację sami)</t>
+  </si>
+  <si>
+    <t>zrobić listę warunków posprzedażowych wraz z datami (żeby o niczym nie zapomnieć w trakcie 
+przynajmniej do terminu odbioru budynku)</t>
+  </si>
+  <si>
+    <t>zanieść Wnioski o wpis do hipoteki do odpowiednich sądów (pamiętać o uzupełnieniu daty, 
+zanieść 2egz niech od razu jeden podbiją)</t>
+  </si>
+  <si>
+    <t>Sprawy bieżące: kredyt DB, budowa, inne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="20">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1201,6 +1321,20 @@
       <b/>
       <sz val="8"/>
       <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="238"/>
@@ -1598,7 +1732,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1874,11 +2008,508 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="101">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -4078,7 +4709,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740521"/>
+          <c:w val="0.71441426071740499"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4358,24 +4989,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63148800"/>
-        <c:axId val="63150336"/>
+        <c:axId val="64688128"/>
+        <c:axId val="64689664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63148800"/>
+        <c:axId val="64688128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63150336"/>
+        <c:crossAx val="64689664"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63150336"/>
+        <c:axId val="64689664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -4385,7 +5016,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63148800"/>
+        <c:crossAx val="64688128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4396,8 +5027,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288641"/>
-          <c:y val="0.29353966170895585"/>
+          <c:x val="0.86438523325288674"/>
+          <c:y val="0.29353966170895596"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -4407,7 +5038,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4619,24 +5250,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63208448"/>
-        <c:axId val="63230720"/>
+        <c:axId val="65353984"/>
+        <c:axId val="65372160"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63208448"/>
+        <c:axId val="65353984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63230720"/>
+        <c:crossAx val="65372160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63230720"/>
+        <c:axId val="65372160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -4646,7 +5277,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63208448"/>
+        <c:crossAx val="65353984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4658,7 +5289,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000322" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4821,24 +5452,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64431616"/>
-        <c:axId val="64433152"/>
+        <c:axId val="77824768"/>
+        <c:axId val="77826304"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64431616"/>
+        <c:axId val="77824768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64433152"/>
+        <c:crossAx val="77826304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64433152"/>
+        <c:axId val="77826304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -4848,7 +5479,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64431616"/>
+        <c:crossAx val="77824768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4860,7 +5491,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4975,11 +5606,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64383616"/>
-        <c:axId val="64385408"/>
+        <c:axId val="77911936"/>
+        <c:axId val="77913472"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64383616"/>
+        <c:axId val="77911936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4987,13 +5618,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64385408"/>
+        <c:crossAx val="77913472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64385408"/>
+        <c:axId val="77913472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5001,7 +5632,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64383616"/>
+        <c:crossAx val="77911936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5013,7 +5644,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5029,10 +5660,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961872"/>
-          <c:y val="3.2882035578886096E-2"/>
+          <c:x val="0.17181562830961866"/>
+          <c:y val="3.2882035578886117E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420179"/>
+          <c:h val="0.63861876640420201"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5195,11 +5826,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64533248"/>
-        <c:axId val="64534784"/>
+        <c:axId val="77934592"/>
+        <c:axId val="77936128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64533248"/>
+        <c:axId val="77934592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5207,13 +5838,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64534784"/>
+        <c:crossAx val="77936128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64534784"/>
+        <c:axId val="77936128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5222,19 +5853,20 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64533248"/>
+        <c:crossAx val="77934592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5416,106 +6048,121 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="83" dataDxfId="81" headerRowBorderDxfId="82" tableBorderDxfId="80" totalsRowBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99" tableBorderDxfId="97" totalsRowBorderDxfId="96">
   <autoFilter ref="A1:F43"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="78"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="77"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="76"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="75"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="74"/>
-    <tableColumn id="6" name="Aby" dataDxfId="73"/>
+    <tableColumn id="1" name="Id" dataDxfId="95"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="94"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="93"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="92"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="91"/>
+    <tableColumn id="6" name="Aby" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
   <autoFilter ref="A4:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="70"/>
-    <tableColumn id="2" name="Status" dataDxfId="69"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="68"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="67"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="66"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="65"/>
+    <tableColumn id="1" name="Id" dataDxfId="87"/>
+    <tableColumn id="2" name="Status" dataDxfId="86"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="85"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="84"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="83"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="82"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="64" dataDxfId="63" tableBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="81" dataDxfId="80" tableBorderDxfId="79">
   <autoFilter ref="A4:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="2" name="Status" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="55" totalsRowDxfId="54">
+    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="2" name="Status" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="72" totalsRowDxfId="71">
       <totalsRowFormula>SUM([Rozmiar początkowy '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="69">
       <totalsRowFormula>SUM([Pozostało '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Zadanie" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="68" totalsRowDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
   <autoFilter ref="A6:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="44"/>
-    <tableColumn id="2" name="Status" dataDxfId="43"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="42"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="41"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="40"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="39"/>
+    <tableColumn id="1" name="Id" dataDxfId="61"/>
+    <tableColumn id="2" name="Status" dataDxfId="60"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="59"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="58"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="57"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
   <autoFilter ref="A5:F15"/>
   <tableColumns count="6">
+    <tableColumn id="1" name="Kolumna1" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="40" totalsRowDxfId="39"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+  <autoFilter ref="A5:F29"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="Kolumna1" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="2" name="Status" dataDxfId="31" totalsRowDxfId="30"/>
     <tableColumn id="3" name="Realizator" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
     <tableColumn id="6" name="Zadanie" dataDxfId="23" totalsRowDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="17">
-  <autoFilter ref="A5:F29"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela479" displayName="Tabela479" ref="A5:F41" totalsRowCount="1" headerRowDxfId="16" dataDxfId="6" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+  <autoFilter ref="A5:F40"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="16" totalsRowDxfId="15"/>
-    <tableColumn id="2" name="Status" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="12" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Status" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="10" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="7" totalsRowDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="21" tableBorderDxfId="20">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="2"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="0"/>
+    <tableColumn id="1" name="Temat" dataDxfId="19"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="18"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9136,8 +9783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H57"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B53" sqref="B53"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -9879,10 +10526,597 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="75.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="B3" s="64" t="s">
+        <v>360</v>
+      </c>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1"/>
+      <c r="B4" s="33"/>
+    </row>
+    <row r="5" spans="1:8" ht="38.25">
+      <c r="A5" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="E5" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="F5" s="41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="42">
+        <v>1</v>
+      </c>
+      <c r="B6" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="46"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="140" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="42">
+        <v>2</v>
+      </c>
+      <c r="B7" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="44" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="42">
+        <v>3</v>
+      </c>
+      <c r="B8" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="46"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="44" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="42">
+        <v>4</v>
+      </c>
+      <c r="B9" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="46"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="141" t="s">
+        <v>328</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="42">
+        <v>5</v>
+      </c>
+      <c r="B10" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="44"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="141" t="s">
+        <v>329</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="42">
+        <v>6</v>
+      </c>
+      <c r="B11" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="142" t="s">
+        <v>330</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="42">
+        <v>7</v>
+      </c>
+      <c r="B12" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C12" s="44"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="141" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="42">
+        <v>8</v>
+      </c>
+      <c r="B13" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="44"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="142" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="42">
+        <v>9</v>
+      </c>
+      <c r="B14" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="44"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="141" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="42">
+        <v>10</v>
+      </c>
+      <c r="B15" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="46"/>
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="142" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="42">
+        <v>11</v>
+      </c>
+      <c r="B16" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="46"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="141" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="42">
+        <v>12</v>
+      </c>
+      <c r="B17" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="46"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="141" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="42">
+        <v>13</v>
+      </c>
+      <c r="B18" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C18" s="46"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="141" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="42">
+        <v>14</v>
+      </c>
+      <c r="B19" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="46"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="141" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="42">
+        <v>15</v>
+      </c>
+      <c r="B20" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="46"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="141" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="42">
+        <v>16</v>
+      </c>
+      <c r="B21" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="46"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="141" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="42">
+        <v>17</v>
+      </c>
+      <c r="B22" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C22" s="46"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="142" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="42">
+        <v>18</v>
+      </c>
+      <c r="B23" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="46"/>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="141" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="25.5">
+      <c r="A24" s="42">
+        <v>19</v>
+      </c>
+      <c r="B24" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="46"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="143" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="42">
+        <v>20</v>
+      </c>
+      <c r="B25" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="46"/>
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="141" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="42">
+        <v>21</v>
+      </c>
+      <c r="B26" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="141" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="25.5">
+      <c r="A27" s="42">
+        <v>22</v>
+      </c>
+      <c r="B27" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="46"/>
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="143" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="42">
+        <v>23</v>
+      </c>
+      <c r="B28" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="46"/>
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="141" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="42">
+        <v>24</v>
+      </c>
+      <c r="B29" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="46"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="142" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="42">
+        <v>25</v>
+      </c>
+      <c r="B30" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="46"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="141" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="42">
+        <v>26</v>
+      </c>
+      <c r="B31" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="46"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="141" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="42">
+        <v>27</v>
+      </c>
+      <c r="B32" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C32" s="46"/>
+      <c r="D32" s="47"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="141" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="42">
+        <v>28</v>
+      </c>
+      <c r="B33" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="46"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="141" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="42">
+        <v>29</v>
+      </c>
+      <c r="B34" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="46"/>
+      <c r="D34" s="47"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="141" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="42">
+        <v>30</v>
+      </c>
+      <c r="B35" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="46"/>
+      <c r="D35" s="47"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="141" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="42">
+        <v>31</v>
+      </c>
+      <c r="B36" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C36" s="46"/>
+      <c r="D36" s="47"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="141" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" s="42">
+        <v>32</v>
+      </c>
+      <c r="B37" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="46"/>
+      <c r="D37" s="47"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="142" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="42">
+        <v>33</v>
+      </c>
+      <c r="B38" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C38" s="46"/>
+      <c r="D38" s="47"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="141" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="42">
+        <v>34</v>
+      </c>
+      <c r="B39" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="46"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="141" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="42">
+        <v>35</v>
+      </c>
+      <c r="B40" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="46"/>
+      <c r="D40" s="47"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="141" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="49"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="46"/>
+      <c r="D41" s="47">
+        <f>SUBTOTAL(109,[Rozmiar 
+początkowy '[h']])</f>
+        <v>0</v>
+      </c>
+      <c r="E41" s="46">
+        <f>SUBTOTAL(109,[Pozo-
+stało '[h']])</f>
+        <v>0</v>
+      </c>
+      <c r="F41" s="48"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B40">
+      <formula1>$H$9:$H$11</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10317,10 +11551,18 @@
       <c r="B18" s="129" t="s">
         <v>311</v>
       </c>
-      <c r="C18" s="96"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="96"/>
-      <c r="F18" s="134"/>
+      <c r="C18" s="96">
+        <v>2.15</v>
+      </c>
+      <c r="D18" s="97">
+        <v>2.15</v>
+      </c>
+      <c r="E18" s="96">
+        <v>2.16</v>
+      </c>
+      <c r="F18" s="134">
+        <v>200</v>
+      </c>
       <c r="G18" s="137"/>
       <c r="H18" s="113"/>
       <c r="I18" s="111"/>
@@ -10343,10 +11585,18 @@
       <c r="B20" s="129" t="s">
         <v>313</v>
       </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="96"/>
-      <c r="F20" s="134"/>
+      <c r="C20" s="96">
+        <v>2.1</v>
+      </c>
+      <c r="D20" s="97">
+        <v>2.1</v>
+      </c>
+      <c r="E20" s="96">
+        <v>2.1</v>
+      </c>
+      <c r="F20" s="134" t="s">
+        <v>323</v>
+      </c>
       <c r="G20" s="137"/>
       <c r="H20" s="113"/>
       <c r="I20" s="111"/>
@@ -10401,11 +11651,15 @@
     </row>
     <row r="23" spans="2:10">
       <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
+      <c r="C23" s="111" t="s">
+        <v>322</v>
+      </c>
       <c r="D23" s="112"/>
       <c r="E23" s="111"/>
       <c r="F23" s="112"/>
-      <c r="G23" s="113"/>
+      <c r="G23" s="113" t="s">
+        <v>307</v>
+      </c>
       <c r="H23" s="113"/>
       <c r="I23" s="111"/>
       <c r="J23" s="111"/>
@@ -11869,7 +13123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E23"/>
   <sheetViews>

</xml_diff>

<commit_message>
aktualizacja zadań ze sprintu 6
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -14,8 +14,9 @@
     <sheet name="04_Sprint" sheetId="5" r:id="rId5"/>
     <sheet name="05_Sprint" sheetId="6" r:id="rId6"/>
     <sheet name="06_Sprint" sheetId="9" r:id="rId7"/>
-    <sheet name="Piasek i stal" sheetId="7" r:id="rId8"/>
-    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId9"/>
+    <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId8"/>
+    <sheet name="Piasek i stal" sheetId="7" r:id="rId9"/>
+    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="388">
   <si>
     <t>Id</t>
   </si>
@@ -1135,9 +1136,6 @@
     <t>wysłać zapytania ofertowe na bloczki silikatowe</t>
   </si>
   <si>
-    <t>wysłać zapytania ofertowe na strop Teriva</t>
-  </si>
-  <si>
     <t>zrobić przelew wynagrodzenia dla Nowaka</t>
   </si>
   <si>
@@ -1174,13 +1172,97 @@
   </si>
   <si>
     <t>Sprawy bieżące: kredyt DB, budowa, inne</t>
+  </si>
+  <si>
+    <t>wypisać harmongram płatności dla Nowaka</t>
+  </si>
+  <si>
+    <t>rozliczyć się z pożyczki - Świdnica</t>
+  </si>
+  <si>
+    <t>rozliczyć się z pożyczki - Tynka</t>
+  </si>
+  <si>
+    <t>Firma</t>
+  </si>
+  <si>
+    <t>lukasz@cebj.pl</t>
+  </si>
+  <si>
+    <t>Cena bloczków 200m2</t>
+  </si>
+  <si>
+    <t>Cena kleju</t>
+  </si>
+  <si>
+    <t>Dostawa</t>
+  </si>
+  <si>
+    <t>Cena całość</t>
+  </si>
+  <si>
+    <t>http://www.cebj.pl</t>
+  </si>
+  <si>
+    <t>narysować komin w ścianie garażu</t>
+  </si>
+  <si>
+    <t>ArturPołetko</t>
+  </si>
+  <si>
+    <t>budomexolawa@wp.pl</t>
+  </si>
+  <si>
+    <t>Budomex - Allegro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rozliczyć się z rodzicami z pożyczki na garaż </t>
+  </si>
+  <si>
+    <t>Paleta</t>
+  </si>
+  <si>
+    <t>Cena bloczka</t>
+  </si>
+  <si>
+    <t>Ceny brutto</t>
+  </si>
+  <si>
+    <t>wysłać zapytania ofertowe na strop Teriva (zapytać Glape jak o to pytać)</t>
+  </si>
+  <si>
+    <t>http://www.mam-sklad.pl/</t>
+  </si>
+  <si>
+    <t>oferta na stronie</t>
+  </si>
+  <si>
+    <t>Klej25kg</t>
+  </si>
+  <si>
+    <t>MSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> biuro@gaja-msm.pl </t>
+  </si>
+  <si>
+    <t>biuro@magbez.pl</t>
+  </si>
+  <si>
+    <t>Magbez</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> biuro@budinpol.com.pl</t>
+  </si>
+  <si>
+    <t>Budinpol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1336,6 +1418,13 @@
       <b/>
       <sz val="10"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00B050"/>
+      <name val="Czcionka tekstu podstawowego"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
@@ -1732,7 +1821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2017,11 +2106,22 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="101">
+  <dxfs count="102">
     <dxf>
       <font>
         <b val="0"/>
@@ -2231,20 +2331,74 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2468,22 +2622,38 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="thin">
           <color theme="7" tint="0.39997558519241921"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
       </border>
     </dxf>
     <dxf>
@@ -2509,73 +2679,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -4709,7 +4812,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740499"/>
+          <c:w val="0.71441426071740488"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -4989,24 +5092,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64688128"/>
-        <c:axId val="64689664"/>
+        <c:axId val="63148800"/>
+        <c:axId val="63150336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="64688128"/>
+        <c:axId val="63148800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64689664"/>
+        <c:crossAx val="63150336"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64689664"/>
+        <c:axId val="63150336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -5016,7 +5119,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64688128"/>
+        <c:crossAx val="63148800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5027,8 +5130,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288674"/>
-          <c:y val="0.29353966170895596"/>
+          <c:x val="0.86438523325288685"/>
+          <c:y val="0.29353966170895601"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -5038,7 +5141,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000566" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000566" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5250,24 +5353,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65353984"/>
-        <c:axId val="65372160"/>
+        <c:axId val="63208448"/>
+        <c:axId val="63238912"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="65353984"/>
+        <c:axId val="63208448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65372160"/>
+        <c:crossAx val="63238912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="65372160"/>
+        <c:axId val="63238912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5277,7 +5380,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65353984"/>
+        <c:crossAx val="63208448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5289,7 +5392,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000355" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000355" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5452,24 +5555,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77824768"/>
-        <c:axId val="77826304"/>
+        <c:axId val="64370176"/>
+        <c:axId val="64371712"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77824768"/>
+        <c:axId val="64370176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77826304"/>
+        <c:crossAx val="64371712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77826304"/>
+        <c:axId val="64371712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -5479,7 +5582,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77824768"/>
+        <c:crossAx val="64370176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5491,7 +5594,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5606,11 +5709,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77911936"/>
-        <c:axId val="77913472"/>
+        <c:axId val="64457344"/>
+        <c:axId val="64459136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77911936"/>
+        <c:axId val="64457344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5618,13 +5721,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77913472"/>
+        <c:crossAx val="64459136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77913472"/>
+        <c:axId val="64459136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5632,7 +5735,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77911936"/>
+        <c:crossAx val="64457344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5644,7 +5747,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000233" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000233" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5660,10 +5763,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961866"/>
-          <c:y val="3.2882035578886117E-2"/>
+          <c:x val="0.17181562830961863"/>
+          <c:y val="3.288203557888613E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420201"/>
+          <c:h val="0.63861876640420212"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -5826,11 +5929,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77934592"/>
-        <c:axId val="77936128"/>
+        <c:axId val="64537344"/>
+        <c:axId val="64538880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="77934592"/>
+        <c:axId val="64537344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5838,13 +5941,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77936128"/>
+        <c:crossAx val="64538880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="77936128"/>
+        <c:axId val="64538880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -5853,20 +5956,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77934592"/>
+        <c:crossAx val="64537344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000244" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6048,121 +6150,145 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="100" dataDxfId="98" headerRowBorderDxfId="99" tableBorderDxfId="97" totalsRowBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="101" dataDxfId="99" headerRowBorderDxfId="100" tableBorderDxfId="98" totalsRowBorderDxfId="97">
   <autoFilter ref="A1:F43"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="95"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="94"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="93"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="92"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="91"/>
-    <tableColumn id="6" name="Aby" dataDxfId="90"/>
+    <tableColumn id="1" name="Id" dataDxfId="96"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="95"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="94"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="93"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="92"/>
+    <tableColumn id="6" name="Aby" dataDxfId="91"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="89" dataDxfId="88">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="90" dataDxfId="89">
   <autoFilter ref="A4:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="87"/>
-    <tableColumn id="2" name="Status" dataDxfId="86"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="85"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="84"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="83"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="82"/>
+    <tableColumn id="1" name="Id" dataDxfId="88"/>
+    <tableColumn id="2" name="Status" dataDxfId="87"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="86"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="85"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="84"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="83"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="81" dataDxfId="80" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81" tableBorderDxfId="80">
   <autoFilter ref="A4:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="2" name="Status" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="74" totalsRowDxfId="73"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="72" totalsRowDxfId="71">
+    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="2" name="Status" dataDxfId="77" totalsRowDxfId="76"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="75" totalsRowDxfId="74"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="73" totalsRowDxfId="72">
       <totalsRowFormula>SUM([Rozmiar początkowy '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="70" totalsRowDxfId="69">
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="70">
       <totalsRowFormula>SUM([Pozostało '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Zadanie" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="69" totalsRowDxfId="68"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="67" dataDxfId="65" headerRowBorderDxfId="66" tableBorderDxfId="64" totalsRowBorderDxfId="63">
   <autoFilter ref="A6:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="61"/>
-    <tableColumn id="2" name="Status" dataDxfId="60"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="59"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="58"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="57"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="56"/>
+    <tableColumn id="1" name="Id" dataDxfId="62"/>
+    <tableColumn id="2" name="Status" dataDxfId="61"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="60"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="59"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="58"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="55" dataDxfId="53" headerRowBorderDxfId="54" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A5:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="41" totalsRowDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="38" dataDxfId="36" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A5:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="2" name="Status" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="2" name="Status" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela479" displayName="Tabela479" ref="A5:F41" totalsRowCount="1" headerRowDxfId="16" dataDxfId="6" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
-  <autoFilter ref="A5:F40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela479" displayName="Tabela479" ref="A5:F47" totalsRowCount="1" headerRowDxfId="22" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+  <autoFilter ref="A5:F46"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="12" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Status" dataDxfId="11" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="10" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="9" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="7" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="17" totalsRowDxfId="5"/>
+    <tableColumn id="2" name="Status" dataDxfId="16" totalsRowDxfId="4"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="15" totalsRowDxfId="3"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="14" totalsRowDxfId="2"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="1"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="12" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="21" tableBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="B4:K19" totalsRowShown="0">
+  <autoFilter ref="B4:K19">
+    <filterColumn colId="2"/>
+    <filterColumn colId="3"/>
+    <filterColumn colId="5"/>
+    <filterColumn colId="7"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Firma"/>
+    <tableColumn id="2" name="Kontakt"/>
+    <tableColumn id="11" name="szt"/>
+    <tableColumn id="10" name="Cena bloczka" dataDxfId="6"/>
+    <tableColumn id="3" name="Cena bloczków 200m2"/>
+    <tableColumn id="12" name="Klej25kg"/>
+    <tableColumn id="4" name="Cena kleju"/>
+    <tableColumn id="9" name="Paleta"/>
+    <tableColumn id="5" name="Dostawa"/>
+    <tableColumn id="6" name="Cena całość"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="19"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="18"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="17"/>
+    <tableColumn id="1" name="Temat" dataDxfId="9"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="8"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7176,6 +7302,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:E23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
+    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" s="66"/>
+      <c r="C2" s="66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5">
+      <c r="B3" s="66">
+        <v>1</v>
+      </c>
+      <c r="C3" s="66" t="s">
+        <v>263</v>
+      </c>
+      <c r="D3" s="99">
+        <v>41442</v>
+      </c>
+      <c r="E3" s="66"/>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" s="66">
+        <v>2</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>265</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>266</v>
+      </c>
+      <c r="E4" s="66"/>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" s="66">
+        <v>3</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" s="66">
+        <v>4</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>267</v>
+      </c>
+      <c r="D6" s="99">
+        <v>41426</v>
+      </c>
+      <c r="E6" s="66"/>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" s="66">
+        <v>5</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>268</v>
+      </c>
+      <c r="D7" s="99">
+        <v>41425</v>
+      </c>
+      <c r="E7" s="66"/>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" s="66">
+        <v>6</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>269</v>
+      </c>
+      <c r="D8" s="99">
+        <v>41427</v>
+      </c>
+      <c r="E8" s="66"/>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" s="66">
+        <v>7</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>270</v>
+      </c>
+      <c r="D9" s="99">
+        <v>41428</v>
+      </c>
+      <c r="E9" s="66"/>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" s="66">
+        <v>8</v>
+      </c>
+      <c r="C10" s="66" t="s">
+        <v>271</v>
+      </c>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+    </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="66">
+        <v>9</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>272</v>
+      </c>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="66">
+        <v>10</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>273</v>
+      </c>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="C14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="C15" s="107"/>
+      <c r="D15" s="107"/>
+    </row>
+    <row r="16" spans="2:5" ht="28.5">
+      <c r="C16" s="108" t="s">
+        <v>279</v>
+      </c>
+      <c r="D16" s="108" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="28.5">
+      <c r="C17" s="108" t="s">
+        <v>280</v>
+      </c>
+      <c r="D17" s="108" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" ht="42.75">
+      <c r="C18" s="108" t="s">
+        <v>281</v>
+      </c>
+      <c r="D18" s="108" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" ht="28.5">
+      <c r="C19" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="D19" s="108" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" ht="28.5">
+      <c r="C20" s="108"/>
+      <c r="D20" s="108" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4">
+      <c r="C21" s="109"/>
+      <c r="D21" s="109" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4">
+      <c r="C22" s="110" t="s">
+        <v>288</v>
+      </c>
+      <c r="D22" s="109" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="C23" s="110" t="s">
+        <v>289</v>
+      </c>
+      <c r="D23" s="109"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I76"/>
@@ -10526,10 +10864,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -10537,6 +10875,7 @@
     <col min="4" max="4" width="9.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="75.109375" customWidth="1"/>
+    <col min="7" max="7" width="4.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -10551,7 +10890,7 @@
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="B3" s="64" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C3" s="65"/>
       <c r="D3" s="65"/>
@@ -10583,12 +10922,8 @@
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="42">
-        <v>1</v>
-      </c>
-      <c r="B6" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A6" s="42"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="46"/>
       <c r="D6" s="43"/>
       <c r="E6" s="43"/>
@@ -10648,11 +10983,11 @@
       <c r="B10" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="141" t="s">
-        <v>329</v>
+      <c r="C10" s="46"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="48" t="s">
+        <v>370</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>70</v>
@@ -10668,100 +11003,95 @@
       <c r="C11" s="44"/>
       <c r="D11" s="43"/>
       <c r="E11" s="43"/>
-      <c r="F11" s="142" t="s">
-        <v>330</v>
+      <c r="F11" s="141" t="s">
+        <v>329</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="42">
-        <v>7</v>
-      </c>
-      <c r="B12" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A12" s="42"/>
+      <c r="B12" s="139"/>
       <c r="C12" s="44"/>
       <c r="D12" s="43"/>
       <c r="E12" s="43"/>
-      <c r="F12" s="141" t="s">
+      <c r="F12" s="142" t="s">
+        <v>330</v>
+      </c>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="144">
+        <v>7</v>
+      </c>
+      <c r="B13" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="150" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="145"/>
+      <c r="E13" s="145"/>
+      <c r="F13" s="148" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="42">
-        <v>8</v>
-      </c>
-      <c r="B13" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="142" t="s">
-        <v>332</v>
-      </c>
-    </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="42">
-        <v>9</v>
-      </c>
-      <c r="B14" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A14" s="42"/>
+      <c r="B14" s="139"/>
       <c r="C14" s="44"/>
       <c r="D14" s="43"/>
       <c r="E14" s="43"/>
-      <c r="F14" s="141" t="s">
-        <v>333</v>
+      <c r="F14" s="142" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="42">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B15" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="142" t="s">
-        <v>334</v>
+      <c r="C15" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="141" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="42">
-        <v>11</v>
-      </c>
-      <c r="B16" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A16" s="42"/>
+      <c r="B16" s="139"/>
       <c r="C16" s="46"/>
       <c r="D16" s="47"/>
       <c r="E16" s="47"/>
-      <c r="F16" s="141" t="s">
+      <c r="F16" s="142" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="144">
+        <v>11</v>
+      </c>
+      <c r="B17" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="146" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="147"/>
+      <c r="E17" s="147"/>
+      <c r="F17" s="148" t="s">
         <v>335</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="42">
-        <v>12</v>
-      </c>
-      <c r="B17" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="47"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="141" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="42">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="139" t="s">
         <v>69</v>
@@ -10770,12 +11100,12 @@
       <c r="D18" s="47"/>
       <c r="E18" s="47"/>
       <c r="F18" s="141" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="42">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="139" t="s">
         <v>69</v>
@@ -10784,12 +11114,12 @@
       <c r="D19" s="47"/>
       <c r="E19" s="47"/>
       <c r="F19" s="141" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="42">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="139" t="s">
         <v>69</v>
@@ -10798,12 +11128,12 @@
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="141" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="42">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B21" s="139" t="s">
         <v>69</v>
@@ -10812,12 +11142,12 @@
       <c r="D21" s="47"/>
       <c r="E21" s="47"/>
       <c r="F21" s="141" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="42">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B22" s="139" t="s">
         <v>69</v>
@@ -10825,27 +11155,23 @@
       <c r="C22" s="46"/>
       <c r="D22" s="47"/>
       <c r="E22" s="47"/>
-      <c r="F22" s="142" t="s">
-        <v>341</v>
+      <c r="F22" s="141" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="42">
-        <v>18</v>
-      </c>
-      <c r="B23" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A23" s="42"/>
+      <c r="B23" s="139"/>
       <c r="C23" s="46"/>
       <c r="D23" s="47"/>
       <c r="E23" s="47"/>
-      <c r="F23" s="141" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="25.5">
+      <c r="F23" s="142" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="42">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B24" s="139" t="s">
         <v>69</v>
@@ -10853,13 +11179,13 @@
       <c r="C24" s="46"/>
       <c r="D24" s="47"/>
       <c r="E24" s="47"/>
-      <c r="F24" s="143" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="F24" s="141" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="25.5">
       <c r="A25" s="42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="139" t="s">
         <v>69</v>
@@ -10867,13 +11193,13 @@
       <c r="C25" s="46"/>
       <c r="D25" s="47"/>
       <c r="E25" s="47"/>
-      <c r="F25" s="141" t="s">
-        <v>343</v>
+      <c r="F25" s="143" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="42">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B26" s="139" t="s">
         <v>69</v>
@@ -10882,82 +11208,84 @@
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="141" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="25.5">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="42">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B27" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C27" s="46"/>
+      <c r="C27" s="46" t="s">
+        <v>72</v>
+      </c>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
-      <c r="F27" s="143" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="F27" s="141" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="25.5">
       <c r="A28" s="42">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B28" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="46"/>
+      <c r="C28" s="46" t="s">
+        <v>73</v>
+      </c>
       <c r="D28" s="47"/>
       <c r="E28" s="47"/>
-      <c r="F28" s="141" t="s">
-        <v>345</v>
+      <c r="F28" s="143" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="42">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B29" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="C29" s="46"/>
+      <c r="C29" s="46" t="s">
+        <v>77</v>
+      </c>
       <c r="D29" s="47"/>
       <c r="E29" s="47"/>
-      <c r="F29" s="142" t="s">
-        <v>346</v>
+      <c r="F29" s="141" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="42">
-        <v>25</v>
-      </c>
-      <c r="B30" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A30" s="42"/>
+      <c r="B30" s="139"/>
       <c r="C30" s="46"/>
       <c r="D30" s="47"/>
       <c r="E30" s="47"/>
-      <c r="F30" s="141" t="s">
+      <c r="F30" s="142" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="144">
+        <v>25</v>
+      </c>
+      <c r="B31" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="146"/>
+      <c r="D31" s="147"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="148" t="s">
         <v>347</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="42">
-        <v>26</v>
-      </c>
-      <c r="B31" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="141" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="42">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="139" t="s">
         <v>69</v>
@@ -10966,40 +11294,44 @@
       <c r="D32" s="47"/>
       <c r="E32" s="47"/>
       <c r="F32" s="141" t="s">
-        <v>349</v>
+        <v>378</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="42">
+      <c r="A33" s="144">
+        <v>27</v>
+      </c>
+      <c r="B33" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="147"/>
+      <c r="E33" s="147"/>
+      <c r="F33" s="148" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="144">
         <v>28</v>
       </c>
-      <c r="B33" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="46"/>
-      <c r="D33" s="47"/>
-      <c r="E33" s="47"/>
-      <c r="F33" s="141" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="42">
-        <v>29</v>
-      </c>
-      <c r="B34" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C34" s="46"/>
-      <c r="D34" s="47"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="141" t="s">
-        <v>351</v>
+      <c r="B34" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="147"/>
+      <c r="E34" s="147"/>
+      <c r="F34" s="149" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="42">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B35" s="139" t="s">
         <v>69</v>
@@ -11008,68 +11340,70 @@
       <c r="D35" s="47"/>
       <c r="E35" s="47"/>
       <c r="F35" s="141" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="42">
-        <v>31</v>
-      </c>
-      <c r="B36" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="46"/>
-      <c r="D36" s="47"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="141" t="s">
-        <v>353</v>
+      <c r="A36" s="144">
+        <v>30</v>
+      </c>
+      <c r="B36" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D36" s="147"/>
+      <c r="E36" s="147"/>
+      <c r="F36" s="148" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="42">
-        <v>32</v>
-      </c>
-      <c r="B37" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" s="46"/>
+        <v>31</v>
+      </c>
+      <c r="B37" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" s="146" t="s">
+        <v>73</v>
+      </c>
       <c r="D37" s="47"/>
       <c r="E37" s="47"/>
-      <c r="F37" s="142" t="s">
-        <v>354</v>
+      <c r="F37" s="148" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="42">
-        <v>33</v>
-      </c>
-      <c r="B38" s="139" t="s">
-        <v>69</v>
-      </c>
-      <c r="C38" s="46"/>
+        <v>32</v>
+      </c>
+      <c r="B38" s="145" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="146" t="s">
+        <v>73</v>
+      </c>
       <c r="D38" s="47"/>
       <c r="E38" s="47"/>
-      <c r="F38" s="141" t="s">
-        <v>355</v>
+      <c r="F38" s="148" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="42">
-        <v>34</v>
-      </c>
-      <c r="B39" s="139" t="s">
-        <v>69</v>
-      </c>
+      <c r="A39" s="42"/>
+      <c r="B39" s="139"/>
       <c r="C39" s="46"/>
       <c r="D39" s="47"/>
       <c r="E39" s="47"/>
-      <c r="F39" s="141" t="s">
-        <v>356</v>
+      <c r="F39" s="142" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="42">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="139" t="s">
         <v>69</v>
@@ -11078,29 +11412,109 @@
       <c r="D40" s="47"/>
       <c r="E40" s="47"/>
       <c r="F40" s="141" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="49"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="42">
+        <v>35</v>
+      </c>
+      <c r="B41" s="139" t="s">
+        <v>69</v>
+      </c>
       <c r="C41" s="46"/>
-      <c r="D41" s="47">
+      <c r="D41" s="47"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="141" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="42">
+        <v>36</v>
+      </c>
+      <c r="B42" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="46"/>
+      <c r="D42" s="47"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="141" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="100">
+        <v>37</v>
+      </c>
+      <c r="B43" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="102"/>
+      <c r="D43" s="101"/>
+      <c r="E43" s="101"/>
+      <c r="F43" s="103" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="100">
+        <v>38</v>
+      </c>
+      <c r="B44" s="139" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="102"/>
+      <c r="D44" s="101"/>
+      <c r="E44" s="101"/>
+      <c r="F44" s="103" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="144">
+        <v>39</v>
+      </c>
+      <c r="B45" s="147" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="147"/>
+      <c r="E45" s="147"/>
+      <c r="F45" s="149" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="100"/>
+      <c r="B46" s="101"/>
+      <c r="C46" s="102"/>
+      <c r="D46" s="101"/>
+      <c r="E46" s="101"/>
+      <c r="F46" s="103"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="49"/>
+      <c r="B47" s="47"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="47">
         <f>SUBTOTAL(109,[Rozmiar 
 początkowy '[h']])</f>
         <v>0</v>
       </c>
-      <c r="E41" s="46">
+      <c r="E47" s="46">
         <f>SUBTOTAL(109,[Pozo-
 stało '[h']])</f>
         <v>0</v>
       </c>
-      <c r="F41" s="48"/>
+      <c r="F47" s="48"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B40">
-      <formula1>$H$9:$H$11</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B46">
+      <formula1>$H$9:$H$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11112,6 +11526,172 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:11">
+      <c r="B2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11">
+      <c r="B4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4" t="s">
+        <v>276</v>
+      </c>
+      <c r="D4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" t="s">
+        <v>376</v>
+      </c>
+      <c r="F4" t="s">
+        <v>365</v>
+      </c>
+      <c r="G4" t="s">
+        <v>381</v>
+      </c>
+      <c r="H4" t="s">
+        <v>366</v>
+      </c>
+      <c r="I4" t="s">
+        <v>375</v>
+      </c>
+      <c r="J4" t="s">
+        <v>367</v>
+      </c>
+      <c r="K4" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11">
+      <c r="B5" t="s">
+        <v>369</v>
+      </c>
+      <c r="C5" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C6" t="s">
+        <v>371</v>
+      </c>
+      <c r="D6">
+        <v>3600</v>
+      </c>
+      <c r="E6">
+        <v>3.1</v>
+      </c>
+      <c r="F6">
+        <v>11160</v>
+      </c>
+      <c r="G6">
+        <v>16.809999999999999</v>
+      </c>
+      <c r="H6">
+        <v>1850</v>
+      </c>
+      <c r="I6">
+        <v>2030</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>15040</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" t="s">
+        <v>372</v>
+      </c>
+      <c r="D7">
+        <v>3600</v>
+      </c>
+      <c r="E7">
+        <v>3.05</v>
+      </c>
+      <c r="F7">
+        <v>10980</v>
+      </c>
+      <c r="G7">
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>575.64</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" t="s">
+        <v>385</v>
+      </c>
+      <c r="C10" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
+        <v>387</v>
+      </c>
+      <c r="C11" t="s">
+        <v>386</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L146"/>
   <sheetViews>
@@ -13121,216 +13701,4 @@
     <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:E23"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="3" max="3" width="34.44140625" customWidth="1"/>
-    <col min="4" max="4" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5">
-      <c r="B2" s="66"/>
-      <c r="C2" s="66" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="66" t="s">
-        <v>264</v>
-      </c>
-      <c r="E2" s="66" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5">
-      <c r="B3" s="66">
-        <v>1</v>
-      </c>
-      <c r="C3" s="66" t="s">
-        <v>263</v>
-      </c>
-      <c r="D3" s="99">
-        <v>41442</v>
-      </c>
-      <c r="E3" s="66"/>
-    </row>
-    <row r="4" spans="2:5">
-      <c r="B4" s="66">
-        <v>2</v>
-      </c>
-      <c r="C4" s="66" t="s">
-        <v>265</v>
-      </c>
-      <c r="D4" s="66" t="s">
-        <v>266</v>
-      </c>
-      <c r="E4" s="66"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="66">
-        <v>3</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>274</v>
-      </c>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-    </row>
-    <row r="6" spans="2:5">
-      <c r="B6" s="66">
-        <v>4</v>
-      </c>
-      <c r="C6" s="66" t="s">
-        <v>267</v>
-      </c>
-      <c r="D6" s="99">
-        <v>41426</v>
-      </c>
-      <c r="E6" s="66"/>
-    </row>
-    <row r="7" spans="2:5">
-      <c r="B7" s="66">
-        <v>5</v>
-      </c>
-      <c r="C7" s="66" t="s">
-        <v>268</v>
-      </c>
-      <c r="D7" s="99">
-        <v>41425</v>
-      </c>
-      <c r="E7" s="66"/>
-    </row>
-    <row r="8" spans="2:5">
-      <c r="B8" s="66">
-        <v>6</v>
-      </c>
-      <c r="C8" s="66" t="s">
-        <v>269</v>
-      </c>
-      <c r="D8" s="99">
-        <v>41427</v>
-      </c>
-      <c r="E8" s="66"/>
-    </row>
-    <row r="9" spans="2:5">
-      <c r="B9" s="66">
-        <v>7</v>
-      </c>
-      <c r="C9" s="66" t="s">
-        <v>270</v>
-      </c>
-      <c r="D9" s="99">
-        <v>41428</v>
-      </c>
-      <c r="E9" s="66"/>
-    </row>
-    <row r="10" spans="2:5">
-      <c r="B10" s="66">
-        <v>8</v>
-      </c>
-      <c r="C10" s="66" t="s">
-        <v>271</v>
-      </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-    </row>
-    <row r="11" spans="2:5">
-      <c r="B11" s="66">
-        <v>9</v>
-      </c>
-      <c r="C11" s="66" t="s">
-        <v>272</v>
-      </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="66"/>
-    </row>
-    <row r="12" spans="2:5">
-      <c r="B12" s="66">
-        <v>10</v>
-      </c>
-      <c r="C12" s="66" t="s">
-        <v>273</v>
-      </c>
-      <c r="D12" s="66"/>
-      <c r="E12" s="66"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="C14" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5">
-      <c r="C15" s="107"/>
-      <c r="D15" s="107"/>
-    </row>
-    <row r="16" spans="2:5" ht="28.5">
-      <c r="C16" s="108" t="s">
-        <v>279</v>
-      </c>
-      <c r="D16" s="108" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" ht="28.5">
-      <c r="C17" s="108" t="s">
-        <v>280</v>
-      </c>
-      <c r="D17" s="108" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="3:4" ht="42.75">
-      <c r="C18" s="108" t="s">
-        <v>281</v>
-      </c>
-      <c r="D18" s="108" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="19" spans="3:4" ht="28.5">
-      <c r="C19" s="108" t="s">
-        <v>282</v>
-      </c>
-      <c r="D19" s="108" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="3:4" ht="28.5">
-      <c r="C20" s="108"/>
-      <c r="D20" s="108" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="21" spans="3:4">
-      <c r="C21" s="109"/>
-      <c r="D21" s="109" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="22" spans="3:4">
-      <c r="C22" s="110" t="s">
-        <v>288</v>
-      </c>
-      <c r="D22" s="109" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="23" spans="3:4">
-      <c r="C23" s="110" t="s">
-        <v>289</v>
-      </c>
-      <c r="D23" s="109"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
krótki plan na kolejny tydzień: dach
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="3" activeTab="7"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="3" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -15,12 +15,13 @@
     <sheet name="05_Sprint" sheetId="6" r:id="rId6"/>
     <sheet name="06_Sprint" sheetId="9" r:id="rId7"/>
     <sheet name="07_Sprint" sheetId="13" r:id="rId8"/>
-    <sheet name="Dachówki" sheetId="14" r:id="rId9"/>
-    <sheet name="Strop" sheetId="11" r:id="rId10"/>
-    <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId11"/>
-    <sheet name="Piasek i stal" sheetId="7" r:id="rId12"/>
-    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId13"/>
-    <sheet name="Nadproża" sheetId="12" r:id="rId14"/>
+    <sheet name="08_Sprint" sheetId="15" r:id="rId9"/>
+    <sheet name="Dachówki" sheetId="14" r:id="rId10"/>
+    <sheet name="Strop" sheetId="11" r:id="rId11"/>
+    <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId12"/>
+    <sheet name="Piasek i stal" sheetId="7" r:id="rId13"/>
+    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId14"/>
+    <sheet name="Nadproża" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -92,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="487">
   <si>
     <t>Id</t>
   </si>
@@ -1401,13 +1402,171 @@
   </si>
   <si>
     <t>Okna: Spotkanie z extherm</t>
+  </si>
+  <si>
+    <t>Do stanu surowego zamkniętego potrzebujemy:</t>
+  </si>
+  <si>
+    <t>pełnej wyceny dachówek wraz z całym osprzętem dachowym od Manexu</t>
+  </si>
+  <si>
+    <t>obejrzeć wystawę okien połaciowych i zorientować się w ich cechac i określić jakie cechy okna są nam potrzebne</t>
+  </si>
+  <si>
+    <t>otrzymać wycenę okien z Manexu</t>
+  </si>
+  <si>
+    <t>otrzymać wycene okien od Agnieszki</t>
+  </si>
+  <si>
+    <t>wycen dachówek od dwóch firm z Bielan</t>
+  </si>
+  <si>
+    <t>Do zamontowania bramy garażowej potrzebujemy:</t>
+  </si>
+  <si>
+    <t>zebrać wyceny bram</t>
+  </si>
+  <si>
+    <t>wybrać bramę</t>
+  </si>
+  <si>
+    <t>zdecydować o tym co będzie na podłodze w garażu (żeby znać wysokość otworu do garażu)</t>
+  </si>
+  <si>
+    <t>zamówić bramę (oczekiwanie 4-5 tygodni)</t>
+  </si>
+  <si>
+    <t>Do zamontowanie okien potrzebujemy:</t>
+  </si>
+  <si>
+    <t>wykleić otwory okienne styropianem</t>
+  </si>
+  <si>
+    <t>zamówić okna</t>
+  </si>
+  <si>
+    <t>zamówić okna w extherm (oczekiwanie 4-5 tygodni)</t>
+  </si>
+  <si>
+    <t>ostatecznie upewnić się co do koloru okien oraz co do typu drzwi tarasowych (na razie mocca+klasyczne z ruchomym słupkiem)</t>
+  </si>
+  <si>
+    <t>Do zamontowania drzwi ogrodowych potrzebujemy:</t>
+  </si>
+  <si>
+    <t>wybrać drzwi ostateczne</t>
+  </si>
+  <si>
+    <t>zamówić drzwi, zorganizować ich montaż</t>
+  </si>
+  <si>
+    <t>Do zamontowania drzwi wejściowych potrzebujemy:</t>
+  </si>
+  <si>
+    <t>zakupić tymczasowe drzwi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zorganizować montaż drzwi wraz z dopasowaniem do otworu </t>
+  </si>
+  <si>
+    <t>Potrzebujemy dachówek</t>
+  </si>
+  <si>
+    <t>Do zakończenia robót przez Nowaka:</t>
+  </si>
+  <si>
+    <t>Aby mieć dachówki potrzebujemy:</t>
+  </si>
+  <si>
+    <t>Potrzebujemy okien połaciowych</t>
+  </si>
+  <si>
+    <t>Aby mieć okna musimy:</t>
+  </si>
+  <si>
+    <t>Potrzebujemy ścianek działowych</t>
+  </si>
+  <si>
+    <t>Aby mieć ścianki musimy:</t>
+  </si>
+  <si>
+    <t>zlecić wykonanie ścianek</t>
+  </si>
+  <si>
+    <t>wykonać projekt ścianek (nanieść na istniejący projekt korekty)</t>
+  </si>
+  <si>
+    <t>Zamontować bramę garażową</t>
+  </si>
+  <si>
+    <t>Zamontować okna</t>
+  </si>
+  <si>
+    <t>Zamontować drzwi ogrodowe</t>
+  </si>
+  <si>
+    <t>Zamontować drzwi wejściowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - proprosić jeszcze raz mailowo w sobotę
+- poprosić jeszcze raz telefonicznie w poniedziałek</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - ponaglić telefonicznie w sobotę</t>
+  </si>
+  <si>
+    <t>Prace jakie można robić zimą</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Fakro i Velux są w ExtraDach na Międzyleskiej (kier Brochów)
+ - Velux, Fakro, Roto w Budus na Brucknera</t>
+  </si>
+  <si>
+    <t>wycena ma być na poniedziałek</t>
+  </si>
+  <si>
+    <t>ponaglić telefonicznie w poniedziałek</t>
+  </si>
+  <si>
+    <t>potrzebna wizyta na Ładnej z kartonami i miarką</t>
+  </si>
+  <si>
+    <t>Zakupy materiałów budowalnych, za które można uzyskać zwrot VATu</t>
+  </si>
+  <si>
+    <t>Instalacja elektryczna</t>
+  </si>
+  <si>
+    <t>Instalacja gazowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instalacja wodno-kanalizacyjna </t>
+  </si>
+  <si>
+    <t>Telefon Glapa: Zdobyć wiedzę na temat montażu drzwi wejściowych przed zrobieniem wylewki i połozeniem kafelków.</t>
+  </si>
+  <si>
+    <t>SBB-Bielany ma przysłać wycenę dachu - jeśli nie przyjdzie do 12:00 zadzwonić</t>
+  </si>
+  <si>
+    <t>Wysłanie prośby o wycenę dachu (z oknami, rynnami, stopniami, ławami - całego dachu zgodnie z projektem) do trzech hurtowni</t>
+  </si>
+  <si>
+    <t>Zadzwonić do Agnieszki czy ma wycenę okien</t>
+  </si>
+  <si>
+    <t>Poprosić ponownie Manex o wycene dachu (po otrzymaniu wyceny-zestawienia elementów od SBB Bielany)</t>
+  </si>
+  <si>
+    <t>Telefon do Nowaka czy ma pomysł na zamówienie więźby dachowej</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="23">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1575,8 +1734,21 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1607,8 +1779,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -2012,11 +2190,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="7" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2337,11 +2595,62 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="112">
+  <dxfs count="119">
     <dxf>
       <font>
         <b val="0"/>
@@ -2359,20 +2668,27 @@
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2387,7 +2703,7 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color rgb="FF00B050"/>
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
@@ -2397,7 +2713,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2408,6 +2724,8 @@
           <color indexed="64"/>
         </top>
         <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2422,18 +2740,18 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color rgb="FF00B050"/>
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -2443,7 +2761,11 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -2458,19 +2780,19 @@
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
-        <color auto="1"/>
+        <color rgb="FF00B050"/>
         <name val="Tahoma"/>
         <scheme val="none"/>
       </font>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
-          <color indexed="64"/>
+          <color theme="4"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
@@ -2478,76 +2800,32 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="7" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -2920,7 +3198,39 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2992,6 +3302,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -3038,9 +3349,184 @@
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -5277,7 +5763,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740377"/>
+          <c:w val="0.71441426071740355"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -5557,24 +6043,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63031936"/>
-        <c:axId val="63050112"/>
+        <c:axId val="62647680"/>
+        <c:axId val="63317120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63031936"/>
+        <c:axId val="62647680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63050112"/>
+        <c:crossAx val="63317120"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63050112"/>
+        <c:axId val="63317120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -5584,7 +6070,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63031936"/>
+        <c:crossAx val="62647680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5595,8 +6081,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288863"/>
-          <c:y val="0.29353966170895662"/>
+          <c:x val="0.86438523325288885"/>
+          <c:y val="0.29353966170895673"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -5606,7 +6092,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000677" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000677" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5818,24 +6304,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63145088"/>
-        <c:axId val="63146624"/>
+        <c:axId val="63608704"/>
+        <c:axId val="63610240"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63145088"/>
+        <c:axId val="63608704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63146624"/>
+        <c:crossAx val="63610240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63146624"/>
+        <c:axId val="63610240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -5845,7 +6331,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63145088"/>
+        <c:crossAx val="63608704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5857,7 +6343,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000466" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000466" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6020,24 +6506,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63991168"/>
-        <c:axId val="64001152"/>
+        <c:axId val="63680896"/>
+        <c:axId val="63682432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63991168"/>
+        <c:axId val="63680896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64001152"/>
+        <c:crossAx val="63682432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64001152"/>
+        <c:axId val="63682432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -6047,7 +6533,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63991168"/>
+        <c:crossAx val="63680896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6059,7 +6545,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6174,11 +6660,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64357120"/>
-        <c:axId val="64358656"/>
+        <c:axId val="64046592"/>
+        <c:axId val="64048128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64357120"/>
+        <c:axId val="64046592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6186,13 +6672,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64358656"/>
+        <c:crossAx val="64048128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64358656"/>
+        <c:axId val="64048128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6200,7 +6686,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64357120"/>
+        <c:crossAx val="64046592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6212,7 +6698,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000344" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000344" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6228,10 +6714,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961833"/>
-          <c:y val="3.2882035578886221E-2"/>
+          <c:x val="0.17181562830961827"/>
+          <c:y val="3.2882035578886241E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420334"/>
+          <c:h val="0.63861876640420356"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6394,11 +6880,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64424576"/>
-        <c:axId val="64446848"/>
+        <c:axId val="64097664"/>
+        <c:axId val="64128128"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64424576"/>
+        <c:axId val="64097664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6406,13 +6892,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64446848"/>
+        <c:crossAx val="64128128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64446848"/>
+        <c:axId val="64128128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6421,7 +6907,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64424576"/>
+        <c:crossAx val="64097664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6433,7 +6919,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6615,21 +7101,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="111" dataDxfId="109" headerRowBorderDxfId="110" tableBorderDxfId="108" totalsRowBorderDxfId="107">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="118" dataDxfId="116" headerRowBorderDxfId="117" tableBorderDxfId="115" totalsRowBorderDxfId="114">
   <autoFilter ref="A1:F43"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="106"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="105"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="104"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="103"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="102"/>
-    <tableColumn id="6" name="Aby" dataDxfId="101"/>
+    <tableColumn id="1" name="Id" dataDxfId="113"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="112"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="111"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="110"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="109"/>
+    <tableColumn id="6" name="Aby" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela911" displayName="Tabela911" ref="B6:K21" totalsRowShown="0">
+  <autoFilter ref="B6:K21"/>
+  <tableColumns count="10">
+    <tableColumn id="1" name="Firma"/>
+    <tableColumn id="2" name="Kontakt"/>
+    <tableColumn id="11" name="Kolumna1"/>
+    <tableColumn id="10" name="Kolumna2" dataDxfId="13"/>
+    <tableColumn id="3" name="Kolumna3"/>
+    <tableColumn id="12" name="Kolumna4"/>
+    <tableColumn id="4" name="Kolumna5"/>
+    <tableColumn id="9" name="Kolumna6"/>
+    <tableColumn id="5" name="Kolumna7"/>
+    <tableColumn id="6" name="Kolumna8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="B4:K19" totalsRowShown="0">
   <autoFilter ref="B4:K19">
     <filterColumn colId="2"/>
@@ -6641,7 +7146,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="szt"/>
-    <tableColumn id="10" name="Cena bloczka" dataDxfId="11"/>
+    <tableColumn id="10" name="Cena bloczka" dataDxfId="12"/>
     <tableColumn id="3" name="Cena bloczków 200m2"/>
     <tableColumn id="12" name="Klej25kg"/>
     <tableColumn id="4" name="Cena kleju"/>
@@ -6653,121 +7158,121 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="10" tableBorderDxfId="9">
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="8"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="7"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="6"/>
+    <tableColumn id="1" name="Temat" dataDxfId="9"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="8"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A4:F20" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A4:F20"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="98"/>
-    <tableColumn id="2" name="Status" dataDxfId="97"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="96"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="95"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="94"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="93"/>
+    <tableColumn id="1" name="Id" dataDxfId="105"/>
+    <tableColumn id="2" name="Status" dataDxfId="104"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="103"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="102"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="101"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="92" dataDxfId="91" tableBorderDxfId="90">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3" displayName="Tabela3" ref="A4:F24" totalsRowCount="1" headerRowDxfId="99" dataDxfId="98" tableBorderDxfId="97">
   <autoFilter ref="A4:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="2" name="Status" dataDxfId="87" totalsRowDxfId="86"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
+    <tableColumn id="1" name="Id" totalsRowLabel="suma" dataDxfId="96" totalsRowDxfId="95"/>
+    <tableColumn id="2" name="Status" dataDxfId="94" totalsRowDxfId="93"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="92" totalsRowDxfId="91"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="custom" dataDxfId="90" totalsRowDxfId="89">
       <totalsRowFormula>SUM([Rozmiar początkowy '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="81" totalsRowDxfId="80">
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="87">
       <totalsRowFormula>SUM([Pozostało '[h']])</totalsRowFormula>
     </tableColumn>
-    <tableColumn id="6" name="Zadanie" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="86" totalsRowDxfId="85"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="77" dataDxfId="75" headerRowBorderDxfId="76" tableBorderDxfId="74" totalsRowBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tabela5" displayName="Tabela5" ref="A6:F29" totalsRowShown="0" headerRowDxfId="84" dataDxfId="82" headerRowBorderDxfId="83" tableBorderDxfId="81" totalsRowBorderDxfId="80">
   <autoFilter ref="A6:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="72"/>
-    <tableColumn id="2" name="Status" dataDxfId="71"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="70"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="69"/>
-    <tableColumn id="5" name="Pozostało [h]" dataDxfId="68"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="67"/>
+    <tableColumn id="1" name="Id" dataDxfId="79"/>
+    <tableColumn id="2" name="Status" dataDxfId="78"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="77"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" dataDxfId="76"/>
+    <tableColumn id="5" name="Pozostało [h]" dataDxfId="75"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="A5:F16" totalsRowCount="1" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70" totalsRowBorderDxfId="69">
   <autoFilter ref="A5:F15"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="57" totalsRowDxfId="56"/>
-    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="68" totalsRowDxfId="67"/>
+    <tableColumn id="2" name="Sprzedać mieszkanie." dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="4" name="Rozmiar początkowy [h]" totalsRowFunction="sum" dataDxfId="62" totalsRowDxfId="61"/>
+    <tableColumn id="5" name="Pozostało [h]" totalsRowFunction="sum" dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="58" totalsRowDxfId="57"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46" totalsRowBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tabela47" displayName="Tabela47" ref="A5:F30" totalsRowCount="1" headerRowDxfId="56" dataDxfId="54" headerRowBorderDxfId="55" tableBorderDxfId="53" totalsRowBorderDxfId="52">
   <autoFilter ref="A5:F29"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="2" name="Status" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="38" totalsRowDxfId="37"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="51" totalsRowDxfId="50"/>
+    <tableColumn id="2" name="Status" dataDxfId="49" totalsRowDxfId="48"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="47" totalsRowDxfId="46"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="45" totalsRowDxfId="44"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="41" totalsRowDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela479" displayName="Tabela479" ref="A5:F49" totalsRowCount="1" headerRowDxfId="32" dataDxfId="30" headerRowBorderDxfId="31" tableBorderDxfId="29" totalsRowBorderDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tabela479" displayName="Tabela479" ref="A5:F49" totalsRowCount="1" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36" totalsRowBorderDxfId="35">
   <autoFilter ref="A5:F48"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Kolumna1" dataDxfId="27" totalsRowDxfId="5"/>
-    <tableColumn id="2" name="Status" dataDxfId="26" totalsRowDxfId="4"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="25" totalsRowDxfId="3"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="24" totalsRowDxfId="2"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="23" totalsRowDxfId="1"/>
-    <tableColumn id="6" name="Zadanie" dataDxfId="22" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Kolumna1" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="2" name="Status" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" totalsRowFunction="sum" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" totalsRowFunction="sum" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="6" name="Zadanie" dataDxfId="24" totalsRowDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A5:F23" totalsRowShown="0" dataDxfId="20" headerRowBorderDxfId="21" tableBorderDxfId="19" totalsRowBorderDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tabela11" displayName="Tabela11" ref="A5:F23" totalsRowShown="0" dataDxfId="21" headerRowBorderDxfId="22" tableBorderDxfId="20" totalsRowBorderDxfId="19">
   <autoFilter ref="A5:F23"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Lp" dataDxfId="17"/>
-    <tableColumn id="2" name="Status" dataDxfId="16"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="15"/>
-    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" dataDxfId="14"/>
-    <tableColumn id="5" name="Pozo-&#10;stało [h]" dataDxfId="13"/>
+    <tableColumn id="1" name="Lp" dataDxfId="18"/>
+    <tableColumn id="2" name="Status" dataDxfId="17"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="16"/>
+    <tableColumn id="4" name="Rozmiar &#10;początkowy [h]" dataDxfId="15"/>
+    <tableColumn id="5" name="Pozo-&#10;stało [h]" dataDxfId="14"/>
     <tableColumn id="6" name="Zadanie"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6775,21 +7280,15 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Tabela911" displayName="Tabela911" ref="B6:K21" totalsRowShown="0">
-  <autoFilter ref="B6:K21"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="Firma"/>
-    <tableColumn id="2" name="Kontakt"/>
-    <tableColumn id="11" name="Kolumna1"/>
-    <tableColumn id="10" name="Kolumna2" dataDxfId="12"/>
-    <tableColumn id="3" name="Kolumna3"/>
-    <tableColumn id="12" name="Kolumna4"/>
-    <tableColumn id="4" name="Kolumna5"/>
-    <tableColumn id="9" name="Kolumna6"/>
-    <tableColumn id="5" name="Kolumna7"/>
-    <tableColumn id="6" name="Kolumna8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabela12" displayName="Tabela12" ref="A3:D10" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+  <autoFilter ref="A3:D10"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Lp" dataDxfId="3"/>
+    <tableColumn id="2" name="Status" dataDxfId="2"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="1"/>
+    <tableColumn id="4" name="Zadanie" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -7803,6 +8302,20 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B4:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7899,7 +8412,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K25"/>
   <sheetViews>
@@ -8101,7 +8614,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L146"/>
   <sheetViews>
@@ -10138,7 +10651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E23"/>
   <sheetViews>
@@ -10350,7 +10863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E16"/>
   <sheetViews>
@@ -14702,8 +15215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -14938,14 +15451,366 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A3:E56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="50.77734375" customWidth="1"/>
+    <col min="6" max="6" width="63.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5">
+      <c r="A3" s="179" t="s">
+        <v>423</v>
+      </c>
+      <c r="B3" s="180" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="181" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="182" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="163"/>
+    </row>
+    <row r="4" spans="1:5" ht="25.5">
+      <c r="A4" s="172"/>
+      <c r="B4" s="173"/>
+      <c r="C4" s="174" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="177" t="s">
+        <v>481</v>
+      </c>
+      <c r="E4" s="163"/>
+    </row>
+    <row r="5" spans="1:5" ht="26.25" customHeight="1">
+      <c r="A5" s="175" t="s">
+        <v>429</v>
+      </c>
+      <c r="B5" s="145"/>
+      <c r="C5" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="178" t="s">
+        <v>483</v>
+      </c>
+      <c r="E5" s="163"/>
+    </row>
+    <row r="6" spans="1:5" ht="24.75" customHeight="1">
+      <c r="A6" s="172"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="174" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="177" t="s">
+        <v>484</v>
+      </c>
+      <c r="E6" s="163"/>
+    </row>
+    <row r="7" spans="1:5" ht="24.75" customHeight="1">
+      <c r="A7" s="175"/>
+      <c r="B7" s="145"/>
+      <c r="C7" s="146" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="178" t="s">
+        <v>486</v>
+      </c>
+      <c r="E7" s="163"/>
+    </row>
+    <row r="8" spans="1:5" ht="25.5">
+      <c r="A8" s="172" t="s">
+        <v>430</v>
+      </c>
+      <c r="B8" s="173"/>
+      <c r="C8" s="174" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="177" t="s">
+        <v>482</v>
+      </c>
+      <c r="E8" s="163"/>
+    </row>
+    <row r="9" spans="1:5" ht="29.25" customHeight="1">
+      <c r="A9" s="175"/>
+      <c r="B9" s="145"/>
+      <c r="C9" s="146" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="178" t="s">
+        <v>485</v>
+      </c>
+      <c r="E9" s="163"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="175"/>
+      <c r="B10" s="145"/>
+      <c r="C10" s="176"/>
+      <c r="D10" s="178"/>
+      <c r="E10" s="163"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" s="163"/>
+      <c r="E11" s="163"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="D12" s="163"/>
+      <c r="E12" s="163"/>
+    </row>
+    <row r="22" spans="1:3" ht="15">
+      <c r="A22" s="162" t="s">
+        <v>458</v>
+      </c>
+      <c r="B22" s="163"/>
+      <c r="C22" s="163"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="163" t="s">
+        <v>457</v>
+      </c>
+      <c r="B23" s="163"/>
+      <c r="C23" s="163"/>
+    </row>
+    <row r="24" spans="1:3" ht="38.25" outlineLevel="1">
+      <c r="A24" s="166" t="s">
+        <v>459</v>
+      </c>
+      <c r="B24" s="167" t="s">
+        <v>436</v>
+      </c>
+      <c r="C24" s="168" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" outlineLevel="1">
+      <c r="A25" s="166"/>
+      <c r="B25" s="167" t="s">
+        <v>440</v>
+      </c>
+      <c r="C25" s="168" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="163" t="s">
+        <v>460</v>
+      </c>
+      <c r="B26" s="165"/>
+      <c r="C26" s="163"/>
+    </row>
+    <row r="27" spans="1:3" ht="38.25" outlineLevel="1">
+      <c r="A27" s="169" t="s">
+        <v>461</v>
+      </c>
+      <c r="B27" s="170" t="s">
+        <v>437</v>
+      </c>
+      <c r="C27" s="171" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" outlineLevel="1">
+      <c r="A28" s="169"/>
+      <c r="B28" s="170" t="s">
+        <v>438</v>
+      </c>
+      <c r="C28" s="171" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" outlineLevel="1">
+      <c r="A29" s="169"/>
+      <c r="B29" s="170" t="s">
+        <v>439</v>
+      </c>
+      <c r="C29" s="171" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" outlineLevel="1">
+      <c r="A30" s="169"/>
+      <c r="B30" s="170" t="s">
+        <v>448</v>
+      </c>
+      <c r="C30" s="171"/>
+    </row>
+    <row r="31" spans="1:3" collapsed="1">
+      <c r="A31" s="163" t="s">
+        <v>462</v>
+      </c>
+      <c r="B31" s="163"/>
+      <c r="C31" s="163"/>
+    </row>
+    <row r="32" spans="1:3" ht="25.5" hidden="1" outlineLevel="1">
+      <c r="A32" s="169" t="s">
+        <v>463</v>
+      </c>
+      <c r="B32" s="170" t="s">
+        <v>465</v>
+      </c>
+      <c r="C32" s="171" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="A33" s="170"/>
+      <c r="B33" s="170" t="s">
+        <v>464</v>
+      </c>
+      <c r="C33" s="163"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="163"/>
+      <c r="B34" s="163"/>
+      <c r="C34" s="163"/>
+    </row>
+    <row r="35" spans="1:3" ht="15">
+      <c r="A35" s="162" t="s">
+        <v>435</v>
+      </c>
+      <c r="B35" s="164"/>
+      <c r="C35" s="163"/>
+    </row>
+    <row r="36" spans="1:3" collapsed="1">
+      <c r="A36" t="s">
+        <v>466</v>
+      </c>
+      <c r="B36" s="163"/>
+      <c r="C36" s="163"/>
+    </row>
+    <row r="37" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="A37" t="s">
+        <v>441</v>
+      </c>
+      <c r="B37" t="s">
+        <v>442</v>
+      </c>
+      <c r="C37" s="163"/>
+    </row>
+    <row r="38" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B38" t="s">
+        <v>443</v>
+      </c>
+      <c r="C38" s="163"/>
+    </row>
+    <row r="39" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B39" t="s">
+        <v>444</v>
+      </c>
+      <c r="C39" s="163"/>
+    </row>
+    <row r="40" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B40" t="s">
+        <v>445</v>
+      </c>
+      <c r="C40" s="163"/>
+    </row>
+    <row r="41" spans="1:3" collapsed="1">
+      <c r="A41" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="A42" t="s">
+        <v>446</v>
+      </c>
+      <c r="B42" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B43" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B44" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="15" customHeight="1" collapsed="1">
+      <c r="A45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="A46" t="s">
+        <v>451</v>
+      </c>
+      <c r="B46" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" hidden="1" outlineLevel="1">
+      <c r="B47" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" collapsed="1">
+      <c r="A48" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="A49" t="s">
+        <v>454</v>
+      </c>
+      <c r="B49" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" outlineLevel="1">
+      <c r="B50" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15">
+      <c r="A52" s="162" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>480</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B10">
+      <formula1>$H$9:$H$14</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
wyslanie zapytan o dach
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="3" activeTab="8"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="492">
   <si>
     <t>Id</t>
   </si>
@@ -1560,6 +1560,21 @@
   </si>
   <si>
     <t>Telefon do Nowaka czy ma pomysł na zamówienie więźby dachowej</t>
+  </si>
+  <si>
+    <t>http://polskiecentrumdachowe.pl/kontakt/</t>
+  </si>
+  <si>
+    <t>Wysłane do:</t>
+  </si>
+  <si>
+    <t>http://www.extradach.com/kontakt</t>
+  </si>
+  <si>
+    <t>http://www.mbs.wroc.pl/dachy_i_akcesoria</t>
+  </si>
+  <si>
+    <t>http://www.mp24.com.pl/kontakt.php</t>
   </si>
 </sst>
 </file>
@@ -2274,7 +2289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2646,11 +2661,85 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="119">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2816,90 +2905,17 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color theme="7" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -5763,7 +5779,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740355"/>
+          <c:w val="0.71441426071740344"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -6043,24 +6059,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62647680"/>
-        <c:axId val="63317120"/>
+        <c:axId val="62635392"/>
+        <c:axId val="62727296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62647680"/>
+        <c:axId val="62635392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63317120"/>
+        <c:crossAx val="62727296"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63317120"/>
+        <c:axId val="62727296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -6070,7 +6086,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62647680"/>
+        <c:crossAx val="62635392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6081,8 +6097,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288885"/>
-          <c:y val="0.29353966170895673"/>
+          <c:x val="0.86438523325288896"/>
+          <c:y val="0.29353966170895684"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -6092,7 +6108,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000711" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000711" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6304,24 +6320,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63608704"/>
-        <c:axId val="63610240"/>
+        <c:axId val="63543168"/>
+        <c:axId val="63544704"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63608704"/>
+        <c:axId val="63543168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63610240"/>
+        <c:crossAx val="63544704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63610240"/>
+        <c:axId val="63544704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -6331,7 +6347,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63608704"/>
+        <c:crossAx val="63543168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6343,7 +6359,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6506,24 +6522,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63680896"/>
-        <c:axId val="63682432"/>
+        <c:axId val="63619456"/>
+        <c:axId val="63620992"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63680896"/>
+        <c:axId val="63619456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63682432"/>
+        <c:crossAx val="63620992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63682432"/>
+        <c:axId val="63620992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -6533,7 +6549,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63680896"/>
+        <c:crossAx val="63619456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6545,7 +6561,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6660,11 +6676,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64046592"/>
-        <c:axId val="64048128"/>
+        <c:axId val="63976960"/>
+        <c:axId val="63978496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64046592"/>
+        <c:axId val="63976960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6672,13 +6688,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64048128"/>
+        <c:crossAx val="63978496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64048128"/>
+        <c:axId val="63978496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6686,7 +6702,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64046592"/>
+        <c:crossAx val="63976960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6698,7 +6714,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6714,10 +6730,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961827"/>
-          <c:y val="3.2882035578886241E-2"/>
+          <c:x val="0.17181562830961825"/>
+          <c:y val="3.2882035578886248E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420356"/>
+          <c:h val="0.63861876640420379"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -6880,11 +6896,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64097664"/>
-        <c:axId val="64128128"/>
+        <c:axId val="64032128"/>
+        <c:axId val="64062592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64097664"/>
+        <c:axId val="64032128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6892,13 +6908,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64128128"/>
+        <c:crossAx val="64062592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64128128"/>
+        <c:axId val="64062592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -6907,7 +6923,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64097664"/>
+        <c:crossAx val="64032128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6919,7 +6935,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000004" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7122,7 +7138,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="Kolumna1"/>
-    <tableColumn id="10" name="Kolumna2" dataDxfId="13"/>
+    <tableColumn id="10" name="Kolumna2" dataDxfId="6"/>
     <tableColumn id="3" name="Kolumna3"/>
     <tableColumn id="12" name="Kolumna4"/>
     <tableColumn id="4" name="Kolumna5"/>
@@ -7146,7 +7162,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="szt"/>
-    <tableColumn id="10" name="Cena bloczka" dataDxfId="12"/>
+    <tableColumn id="10" name="Cena bloczka" dataDxfId="5"/>
     <tableColumn id="3" name="Cena bloczków 200m2"/>
     <tableColumn id="12" name="Klej25kg"/>
     <tableColumn id="4" name="Cena kleju"/>
@@ -7159,12 +7175,12 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="9"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="8"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="7"/>
+    <tableColumn id="1" name="Temat" dataDxfId="2"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7280,13 +7296,13 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabela12" displayName="Tabela12" ref="A3:D10" totalsRowShown="0" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Tabela12" displayName="Tabela12" ref="A3:D10" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A3:D10"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Lp" dataDxfId="3"/>
-    <tableColumn id="2" name="Status" dataDxfId="2"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="1"/>
-    <tableColumn id="4" name="Zadanie" dataDxfId="0"/>
+    <tableColumn id="1" name="Lp" dataDxfId="10"/>
+    <tableColumn id="2" name="Status" dataDxfId="9"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="8"/>
+    <tableColumn id="4" name="Zadanie" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8302,14 +8318,56 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3">
+      <c r="B3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>487</v>
+      </c>
+      <c r="C4" s="183">
+        <v>41533</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="B5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C5" s="183">
+        <v>41533</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>490</v>
+      </c>
+      <c r="C6" s="183">
+        <v>41533</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -15456,7 +15514,7 @@
   </sheetPr>
   <dimension ref="A3:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -15569,21 +15627,21 @@
       <c r="D12" s="163"/>
       <c r="E12" s="163"/>
     </row>
-    <row r="22" spans="1:3" ht="15">
+    <row r="22" spans="1:3" ht="75">
       <c r="A22" s="162" t="s">
         <v>458</v>
       </c>
       <c r="B22" s="163"/>
       <c r="C22" s="163"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" ht="57">
       <c r="A23" s="163" t="s">
         <v>457</v>
       </c>
       <c r="B23" s="163"/>
       <c r="C23" s="163"/>
     </row>
-    <row r="24" spans="1:3" ht="38.25" outlineLevel="1">
+    <row r="24" spans="1:3" ht="63.75" outlineLevel="1">
       <c r="A24" s="166" t="s">
         <v>459</v>
       </c>
@@ -15594,7 +15652,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="25" spans="1:3" outlineLevel="1">
+    <row r="25" spans="1:3" ht="25.5" outlineLevel="1">
       <c r="A25" s="166"/>
       <c r="B25" s="167" t="s">
         <v>440</v>
@@ -15603,14 +15661,14 @@
         <v>471</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" ht="71.25">
       <c r="A26" s="163" t="s">
         <v>460</v>
       </c>
       <c r="B26" s="165"/>
       <c r="C26" s="163"/>
     </row>
-    <row r="27" spans="1:3" ht="38.25" outlineLevel="1">
+    <row r="27" spans="1:3" ht="76.5" outlineLevel="1">
       <c r="A27" s="169" t="s">
         <v>461</v>
       </c>
@@ -15621,7 +15679,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="28" spans="1:3" outlineLevel="1">
+    <row r="28" spans="1:3" ht="25.5" outlineLevel="1">
       <c r="A28" s="169"/>
       <c r="B28" s="170" t="s">
         <v>438</v>
@@ -15630,7 +15688,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="29" spans="1:3" outlineLevel="1">
+    <row r="29" spans="1:3" ht="25.5" outlineLevel="1">
       <c r="A29" s="169"/>
       <c r="B29" s="170" t="s">
         <v>439</v>
@@ -15646,14 +15704,14 @@
       </c>
       <c r="C30" s="171"/>
     </row>
-    <row r="31" spans="1:3" collapsed="1">
+    <row r="31" spans="1:3" ht="71.25" collapsed="1">
       <c r="A31" s="163" t="s">
         <v>462</v>
       </c>
       <c r="B31" s="163"/>
       <c r="C31" s="163"/>
     </row>
-    <row r="32" spans="1:3" ht="25.5" hidden="1" outlineLevel="1">
+    <row r="32" spans="1:3" ht="38.25" hidden="1" outlineLevel="1">
       <c r="A32" s="169" t="s">
         <v>463</v>
       </c>
@@ -15676,7 +15734,7 @@
       <c r="B34" s="163"/>
       <c r="C34" s="163"/>
     </row>
-    <row r="35" spans="1:3" ht="15">
+    <row r="35" spans="1:3" ht="105">
       <c r="A35" s="162" t="s">
         <v>435</v>
       </c>
@@ -15776,7 +15834,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15">
+    <row r="52" spans="1:2" ht="75">
       <c r="A52" s="162" t="s">
         <v>472</v>
       </c>

</xml_diff>

<commit_message>
uzgodniony dach, okna i brama garażowa
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -17,7 +17,7 @@
     <sheet name="07_Sprint" sheetId="13" r:id="rId8"/>
     <sheet name="08_Sprint" sheetId="15" r:id="rId9"/>
     <sheet name="Brama garazowa" sheetId="16" r:id="rId10"/>
-    <sheet name="Dachówki" sheetId="14" r:id="rId11"/>
+    <sheet name="Dachówki i okna" sheetId="14" r:id="rId11"/>
     <sheet name="Strop" sheetId="11" r:id="rId12"/>
     <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId13"/>
     <sheet name="Piasek i stal" sheetId="7" r:id="rId14"/>
@@ -94,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="611">
   <si>
     <t>Id</t>
   </si>
@@ -1563,21 +1563,6 @@
     <t>Telefon do Nowaka czy ma pomysł na zamówienie więźby dachowej</t>
   </si>
   <si>
-    <t>http://polskiecentrumdachowe.pl/kontakt/</t>
-  </si>
-  <si>
-    <t>Wysłane do:</t>
-  </si>
-  <si>
-    <t>http://www.extradach.com/kontakt</t>
-  </si>
-  <si>
-    <t>http://www.mbs.wroc.pl/dachy_i_akcesoria</t>
-  </si>
-  <si>
-    <t>http://www.mp24.com.pl/kontakt.php</t>
-  </si>
-  <si>
     <t>Producent</t>
   </si>
   <si>
@@ -1702,13 +1687,263 @@
   </si>
   <si>
     <t>Uwagi</t>
+  </si>
+  <si>
+    <t>ProMatic</t>
+  </si>
+  <si>
+    <t>Dzik</t>
+  </si>
+  <si>
+    <t>Normstahl</t>
+  </si>
+  <si>
+    <t>PremiumCenter</t>
+  </si>
+  <si>
+    <t>Satin</t>
+  </si>
+  <si>
+    <t>bez</t>
+  </si>
+  <si>
+    <t>Magic600</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velux  </t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Modeł łazienkowy</t>
+  </si>
+  <si>
+    <t>GGU 0065 M06</t>
+  </si>
+  <si>
+    <t>GGL 3065 M06</t>
+  </si>
+  <si>
+    <t>Kołnierz</t>
+  </si>
+  <si>
+    <t>EDW 1000 M06</t>
+  </si>
+  <si>
+    <t>Cena brutto</t>
+  </si>
+  <si>
+    <t>ExtraDach</t>
+  </si>
+  <si>
+    <t>Fakro</t>
+  </si>
+  <si>
+    <t>PTP-V U5 06</t>
+  </si>
+  <si>
+    <t>EZV-P 06</t>
+  </si>
+  <si>
+    <t>GGL 3066 MK06</t>
+  </si>
+  <si>
+    <t>GGU 3066 MK06</t>
+  </si>
+  <si>
+    <t>EDW 0000+EKW 1021</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Wywiewnik</t>
+  </si>
+  <si>
+    <t>obowiązkowy</t>
+  </si>
+  <si>
+    <t>opcjonalny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U = 1,0 </t>
+  </si>
+  <si>
+    <t>U = 0,97</t>
+  </si>
+  <si>
+    <t>U = 1,1</t>
+  </si>
+  <si>
+    <t>Velux</t>
+  </si>
+  <si>
+    <t>1,07W</t>
+  </si>
+  <si>
+    <t>ahl</t>
+  </si>
+  <si>
+    <t>Rabaty</t>
+  </si>
+  <si>
+    <t>FTP-V U5 06</t>
+  </si>
+  <si>
+    <t>FTT/U U6 06</t>
+  </si>
+  <si>
+    <t>PTP-V U5</t>
+  </si>
+  <si>
+    <t>EHV-AT
+THERMO 06</t>
+  </si>
+  <si>
+    <t>Cena po rabacie</t>
+  </si>
+  <si>
+    <t>U = 0,71</t>
+  </si>
+  <si>
+    <t>Creaton</t>
+  </si>
+  <si>
+    <t>Harmonie Neu szara angoba, w kolorze lupka angoba</t>
+  </si>
+  <si>
+    <t>Dachówka podstawowa</t>
+  </si>
+  <si>
+    <t>1960szt</t>
+  </si>
+  <si>
+    <t>Cena</t>
+  </si>
+  <si>
+    <t>Dachówka wentylacyjna</t>
+  </si>
+  <si>
+    <t>8szt</t>
+  </si>
+  <si>
+    <t>Dachówki boczne</t>
+  </si>
+  <si>
+    <t>90szt</t>
+  </si>
+  <si>
+    <t>23szt</t>
+  </si>
+  <si>
+    <t>Gąsior z klamrą</t>
+  </si>
+  <si>
+    <t>Zaślepka pocz</t>
+  </si>
+  <si>
+    <t>2szt</t>
+  </si>
+  <si>
+    <t>Kominek wentylacyjny</t>
+  </si>
+  <si>
+    <t>1szt</t>
+  </si>
+  <si>
+    <t>SBB Bielany</t>
+  </si>
+  <si>
+    <t>Wentylacja kal i grzbietu Roll T</t>
+  </si>
+  <si>
+    <t>Grzebień do dachu okapu – wróblownica IVT</t>
+  </si>
+  <si>
+    <t>Folia dach. IVT Aqua Control XL 165 gram</t>
+  </si>
+  <si>
+    <t>Pas nadrynnowy  aluminium IVT</t>
+  </si>
+  <si>
+    <t>taśma do komina ołow Pbflex</t>
+  </si>
+  <si>
+    <t>listwa do komina 2m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mocowanie łaty kalenicowej </t>
+  </si>
+  <si>
+    <t>ława komin. malowana 80cm Tritt IVT kpl.</t>
+  </si>
+  <si>
+    <t>spinka do dachówki</t>
+  </si>
+  <si>
+    <t>wylaz dachowy versa 47x57</t>
+  </si>
+  <si>
+    <t>Dodatki razem</t>
+  </si>
+  <si>
+    <t>Pokrycie razem</t>
+  </si>
+  <si>
+    <t>Gerda</t>
+  </si>
+  <si>
+    <t>UHTRobotnicza</t>
+  </si>
+  <si>
+    <t>Clasic</t>
+  </si>
+  <si>
+    <t>Krem</t>
+  </si>
+  <si>
+    <t>76szt</t>
+  </si>
+  <si>
+    <t>28szt</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>HDS</t>
+  </si>
+  <si>
+    <t>Semko</t>
+  </si>
+  <si>
+    <t>Stanhdard</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>T-Sky</t>
+  </si>
+  <si>
+    <t>U = 0,8</t>
+  </si>
+  <si>
+    <t>Rynny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="25">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="#,##0\ &quot;zł&quot;;[Red]\-#,##0\ &quot;zł&quot;"/>
+  </numFmts>
+  <fonts count="35">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1889,8 +2124,78 @@
       <name val="Czcionka tekstu podstawowego"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial CE"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial CE"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial CE"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1927,8 +2232,20 @@
         <bgColor theme="4" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -2426,10 +2743,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -2439,10 +2756,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="medium">
         <color indexed="64"/>
-      </right>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -2451,11 +2768,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2827,16 +3190,55 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -5954,7 +6356,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740333"/>
+          <c:w val="0.71441426071740288"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -6234,24 +6636,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="61455744"/>
-        <c:axId val="61482112"/>
+        <c:axId val="71827456"/>
+        <c:axId val="74806016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="61455744"/>
+        <c:axId val="71827456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61482112"/>
+        <c:crossAx val="74806016"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61482112"/>
+        <c:axId val="74806016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -6261,7 +6663,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61455744"/>
+        <c:crossAx val="71827456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6272,8 +6674,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325288918"/>
-          <c:y val="0.2935396617089569"/>
+          <c:x val="0.86438523325288985"/>
+          <c:y val="0.29353966170895712"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -6283,7 +6685,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000722" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000722" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000766" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000766" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6495,24 +6897,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62363520"/>
-        <c:axId val="62365056"/>
+        <c:axId val="62977920"/>
+        <c:axId val="62979456"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62363520"/>
+        <c:axId val="62977920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62365056"/>
+        <c:crossAx val="62979456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62365056"/>
+        <c:axId val="62979456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -6522,7 +6924,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62363520"/>
+        <c:crossAx val="62977920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6534,7 +6936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6697,24 +7099,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62435712"/>
-        <c:axId val="62437248"/>
+        <c:axId val="63164800"/>
+        <c:axId val="63166336"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62435712"/>
+        <c:axId val="63164800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62437248"/>
+        <c:crossAx val="63166336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62437248"/>
+        <c:axId val="63166336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -6724,7 +7126,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62435712"/>
+        <c:crossAx val="63164800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6736,7 +7138,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6851,11 +7253,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62862848"/>
-        <c:axId val="62864384"/>
+        <c:axId val="63956480"/>
+        <c:axId val="63958016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62862848"/>
+        <c:axId val="63956480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6863,13 +7265,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62864384"/>
+        <c:crossAx val="63958016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62864384"/>
+        <c:axId val="63958016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6877,7 +7279,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62862848"/>
+        <c:crossAx val="63956480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6889,7 +7291,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6905,10 +7307,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961822"/>
-          <c:y val="3.2882035578886255E-2"/>
+          <c:x val="0.17181562830961811"/>
+          <c:y val="3.2882035578886283E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.6386187664042039"/>
+          <c:h val="0.63861876640420434"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -7071,11 +7473,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62913920"/>
-        <c:axId val="62948480"/>
+        <c:axId val="64011648"/>
+        <c:axId val="64021632"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62913920"/>
+        <c:axId val="64011648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7083,13 +7485,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62948480"/>
+        <c:crossAx val="64021632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62948480"/>
+        <c:axId val="64021632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -7098,7 +7500,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62913920"/>
+        <c:crossAx val="64011648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7110,7 +7512,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000411" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000411" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000455" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000455" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8493,401 +8895,1237 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:H18"/>
+  <dimension ref="A3:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+    <col min="4" max="6" width="14.5546875" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="13.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15" thickBot="1"/>
-    <row r="4" spans="2:8">
-      <c r="B4" s="185" t="s">
+    <row r="3" spans="1:4" ht="15" thickBot="1"/>
+    <row r="4" spans="1:4">
+      <c r="A4" s="184" t="s">
+        <v>487</v>
+      </c>
+      <c r="B4" s="183" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" s="225" t="s">
+        <v>489</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="185" t="s">
+        <v>488</v>
+      </c>
+      <c r="B5" s="183" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" s="225" t="s">
+        <v>504</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="185" t="s">
+        <v>491</v>
+      </c>
+      <c r="B6" s="183" t="s">
         <v>492</v>
       </c>
-      <c r="C4" s="184" t="s">
+      <c r="C6" s="225" t="s">
+        <v>510</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="185" t="s">
+        <v>493</v>
+      </c>
+      <c r="B7" s="183" t="s">
         <v>494</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="C7" s="225" t="s">
         <v>494</v>
       </c>
-      <c r="E4" s="66" t="s">
-        <v>494</v>
-      </c>
-      <c r="F4" s="66" t="s">
-        <v>521</v>
-      </c>
-      <c r="G4" s="66" t="s">
-        <v>521</v>
-      </c>
-      <c r="H4" s="66" t="s">
+      <c r="D7" s="66" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="185" t="s">
+        <v>507</v>
+      </c>
+      <c r="B8" s="183" t="s">
+        <v>508</v>
+      </c>
+      <c r="C8" s="225" t="s">
+        <v>508</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="185" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="183" t="s">
+        <v>495</v>
+      </c>
+      <c r="C9" s="225" t="s">
+        <v>495</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="185" t="s">
+        <v>497</v>
+      </c>
+      <c r="B10" s="183" t="s">
+        <v>498</v>
+      </c>
+      <c r="C10" s="225" t="s">
+        <v>505</v>
+      </c>
+      <c r="D10" s="66" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
-      <c r="B5" s="186" t="s">
-        <v>493</v>
-      </c>
-      <c r="C5" s="184" t="s">
-        <v>495</v>
-      </c>
-      <c r="D5" s="66" t="s">
+    <row r="11" spans="1:4">
+      <c r="A11" s="185" t="s">
         <v>509</v>
       </c>
-      <c r="E5" s="66" t="s">
-        <v>509</v>
-      </c>
-      <c r="F5" s="66" t="s">
-        <v>516</v>
-      </c>
-      <c r="G5" s="66" t="s">
-        <v>527</v>
-      </c>
-      <c r="H5" s="66" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8">
-      <c r="B6" s="186" t="s">
+      <c r="B11" s="183" t="s">
+        <v>499</v>
+      </c>
+      <c r="C11" s="225">
+        <v>206</v>
+      </c>
+      <c r="D11" s="66" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="185" t="s">
+        <v>500</v>
+      </c>
+      <c r="B12" s="183" t="s">
         <v>496</v>
       </c>
-      <c r="C6" s="184" t="s">
-        <v>497</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>515</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>515</v>
-      </c>
-      <c r="F6" s="66" t="s">
+      <c r="C12" s="225">
+        <v>150</v>
+      </c>
+      <c r="D12" s="66">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="185" t="s">
+        <v>501</v>
+      </c>
+      <c r="B13" s="183">
+        <v>75</v>
+      </c>
+      <c r="C13" s="225" t="s">
+        <v>506</v>
+      </c>
+      <c r="D13" s="66">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="185" t="s">
+        <v>502</v>
+      </c>
+      <c r="B14" s="183">
+        <v>750</v>
+      </c>
+      <c r="C14" s="225">
+        <v>500</v>
+      </c>
+      <c r="D14" s="66">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="185" t="s">
         <v>517</v>
       </c>
-      <c r="G6" s="66" t="s">
-        <v>517</v>
-      </c>
-      <c r="H6" s="66"/>
-    </row>
-    <row r="7" spans="2:8">
-      <c r="B7" s="186" t="s">
-        <v>498</v>
-      </c>
-      <c r="C7" s="184" t="s">
-        <v>499</v>
-      </c>
-      <c r="D7" s="66" t="s">
-        <v>499</v>
-      </c>
-      <c r="E7" s="66" t="s">
-        <v>499</v>
-      </c>
-      <c r="F7" s="66" t="s">
-        <v>524</v>
-      </c>
-      <c r="G7" s="66" t="s">
-        <v>524</v>
-      </c>
-      <c r="H7" s="66" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8">
-      <c r="B8" s="186" t="s">
-        <v>512</v>
-      </c>
-      <c r="C8" s="184" t="s">
-        <v>513</v>
-      </c>
-      <c r="D8" s="66" t="s">
-        <v>513</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>513</v>
-      </c>
-      <c r="F8" s="66" t="s">
-        <v>525</v>
-      </c>
-      <c r="G8" s="66" t="s">
-        <v>513</v>
-      </c>
-      <c r="H8" s="66" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8">
-      <c r="B9" s="186" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="184" t="s">
-        <v>500</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>500</v>
-      </c>
-      <c r="E9" s="66" t="s">
+      <c r="B15" s="183"/>
+      <c r="C15" s="225"/>
+      <c r="D15" s="66" t="s">
         <v>518</v>
       </c>
-      <c r="F9" s="66" t="s">
-        <v>518</v>
-      </c>
-      <c r="G9" s="66" t="s">
-        <v>518</v>
-      </c>
-      <c r="H9" s="66" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8">
-      <c r="B10" s="186" t="s">
-        <v>502</v>
-      </c>
-      <c r="C10" s="184" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="15" thickBot="1">
+      <c r="A16" s="186"/>
+      <c r="B16" s="187"/>
+      <c r="C16" s="227"/>
+      <c r="D16" s="188"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="189" t="s">
         <v>503</v>
       </c>
-      <c r="D10" s="66" t="s">
-        <v>510</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>510</v>
-      </c>
-      <c r="F10" s="66" t="s">
-        <v>520</v>
-      </c>
-      <c r="G10" s="66" t="s">
-        <v>528</v>
-      </c>
-      <c r="H10" s="66" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8">
-      <c r="B11" s="186" t="s">
-        <v>514</v>
-      </c>
-      <c r="C11" s="184" t="s">
-        <v>504</v>
-      </c>
-      <c r="D11" s="66">
-        <v>206</v>
-      </c>
-      <c r="E11" s="66">
-        <v>206</v>
-      </c>
-      <c r="F11" s="66" t="s">
-        <v>511</v>
-      </c>
-      <c r="G11" s="66" t="s">
-        <v>519</v>
-      </c>
-      <c r="H11" s="66" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8">
-      <c r="B12" s="186" t="s">
-        <v>505</v>
-      </c>
-      <c r="C12" s="184" t="s">
-        <v>501</v>
-      </c>
-      <c r="D12" s="66">
-        <v>150</v>
-      </c>
-      <c r="E12" s="66">
-        <v>150</v>
-      </c>
-      <c r="F12" s="66">
-        <v>126</v>
-      </c>
-      <c r="G12" s="66">
-        <v>124</v>
-      </c>
-      <c r="H12" s="66" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8">
-      <c r="B13" s="186" t="s">
-        <v>506</v>
-      </c>
-      <c r="C13" s="184">
-        <v>75</v>
-      </c>
-      <c r="D13" s="66" t="s">
-        <v>511</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>511</v>
-      </c>
-      <c r="F13" s="66">
-        <v>119</v>
-      </c>
-      <c r="G13" s="66">
-        <v>89</v>
-      </c>
-      <c r="H13" s="66" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8">
-      <c r="B14" s="186" t="s">
-        <v>507</v>
-      </c>
-      <c r="C14" s="184">
-        <v>750</v>
-      </c>
-      <c r="D14" s="66">
-        <v>500</v>
-      </c>
-      <c r="E14" s="66">
-        <v>500</v>
-      </c>
-      <c r="F14" s="66" t="s">
-        <v>511</v>
-      </c>
-      <c r="G14" s="66">
-        <v>700</v>
-      </c>
-      <c r="H14" s="66">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8">
-      <c r="B15" s="186" t="s">
-        <v>522</v>
-      </c>
-      <c r="C15" s="184"/>
-      <c r="D15" s="66"/>
-      <c r="E15" s="66"/>
-      <c r="F15" s="66" t="s">
-        <v>523</v>
-      </c>
-      <c r="G15" s="66" t="s">
-        <v>523</v>
-      </c>
-      <c r="H15" s="66"/>
-    </row>
-    <row r="16" spans="2:8" ht="15" thickBot="1">
-      <c r="B16" s="188"/>
-      <c r="C16" s="189"/>
-      <c r="D16" s="190"/>
-      <c r="E16" s="190"/>
-      <c r="F16" s="190"/>
-      <c r="G16" s="190"/>
-      <c r="H16" s="190"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="185" t="s">
-        <v>508</v>
-      </c>
-      <c r="C17" s="191">
+      <c r="B17" s="68">
         <v>5142</v>
       </c>
-      <c r="D17" s="69">
+      <c r="C17" s="228">
         <f>4059+150+206</f>
         <v>4415</v>
       </c>
-      <c r="E17" s="69">
+      <c r="D17" s="69">
+        <v>4737</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" thickBot="1">
+      <c r="A18" s="190" t="s">
+        <v>528</v>
+      </c>
+      <c r="B18" s="73" t="s">
+        <v>521</v>
+      </c>
+      <c r="C18" s="229"/>
+      <c r="D18" s="74" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15" thickBot="1"/>
+    <row r="21" spans="1:8">
+      <c r="A21" s="184" t="s">
+        <v>487</v>
+      </c>
+      <c r="B21" s="225" t="s">
+        <v>489</v>
+      </c>
+      <c r="C21" s="191" t="s">
+        <v>516</v>
+      </c>
+      <c r="D21" s="191" t="s">
+        <v>516</v>
+      </c>
+      <c r="E21" s="192" t="s">
+        <v>524</v>
+      </c>
+      <c r="F21" s="192" t="s">
+        <v>531</v>
+      </c>
+      <c r="G21" s="191" t="s">
+        <v>597</v>
+      </c>
+      <c r="H21" s="191" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="185" t="s">
+        <v>488</v>
+      </c>
+      <c r="B22" s="225" t="s">
+        <v>504</v>
+      </c>
+      <c r="C22" s="191" t="s">
+        <v>511</v>
+      </c>
+      <c r="D22" s="191" t="s">
+        <v>522</v>
+      </c>
+      <c r="E22" s="192" t="s">
+        <v>522</v>
+      </c>
+      <c r="F22" s="192" t="s">
+        <v>532</v>
+      </c>
+      <c r="G22" s="191" t="s">
+        <v>598</v>
+      </c>
+      <c r="H22" s="191" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="185" t="s">
+        <v>491</v>
+      </c>
+      <c r="B23" s="225" t="s">
+        <v>510</v>
+      </c>
+      <c r="C23" s="191" t="s">
+        <v>512</v>
+      </c>
+      <c r="D23" s="191" t="s">
+        <v>512</v>
+      </c>
+      <c r="E23" s="192"/>
+      <c r="F23" s="192" t="s">
+        <v>533</v>
+      </c>
+      <c r="G23" s="191" t="s">
+        <v>599</v>
+      </c>
+      <c r="H23" s="191" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="185" t="s">
+        <v>493</v>
+      </c>
+      <c r="B24" s="225" t="s">
+        <v>494</v>
+      </c>
+      <c r="C24" s="191" t="s">
+        <v>519</v>
+      </c>
+      <c r="D24" s="191" t="s">
+        <v>519</v>
+      </c>
+      <c r="E24" s="192" t="s">
+        <v>525</v>
+      </c>
+      <c r="F24" s="214" t="s">
+        <v>561</v>
+      </c>
+      <c r="G24" s="191" t="s">
+        <v>600</v>
+      </c>
+      <c r="H24" s="191" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="185" t="s">
+        <v>507</v>
+      </c>
+      <c r="B25" s="225" t="s">
+        <v>508</v>
+      </c>
+      <c r="C25" s="191" t="s">
+        <v>520</v>
+      </c>
+      <c r="D25" s="191" t="s">
+        <v>508</v>
+      </c>
+      <c r="E25" s="192" t="s">
+        <v>508</v>
+      </c>
+      <c r="F25" s="192" t="s">
+        <v>534</v>
+      </c>
+      <c r="G25" s="191" t="s">
+        <v>508</v>
+      </c>
+      <c r="H25" s="191" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15">
+      <c r="A26" s="185" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="226" t="s">
+        <v>513</v>
+      </c>
+      <c r="C26" s="193" t="s">
+        <v>513</v>
+      </c>
+      <c r="D26" s="193" t="s">
+        <v>513</v>
+      </c>
+      <c r="E26" s="194" t="s">
+        <v>513</v>
+      </c>
+      <c r="F26" s="194" t="s">
+        <v>513</v>
+      </c>
+      <c r="G26" s="193" t="s">
+        <v>513</v>
+      </c>
+      <c r="H26" s="191" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="185" t="s">
+        <v>497</v>
+      </c>
+      <c r="B27" s="225" t="s">
+        <v>505</v>
+      </c>
+      <c r="C27" s="191" t="s">
+        <v>515</v>
+      </c>
+      <c r="D27" s="191" t="s">
+        <v>523</v>
+      </c>
+      <c r="E27" s="192" t="s">
+        <v>526</v>
+      </c>
+      <c r="F27" s="192" t="s">
+        <v>535</v>
+      </c>
+      <c r="G27" s="191" t="s">
+        <v>510</v>
+      </c>
+      <c r="H27" s="191" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="185" t="s">
+        <v>509</v>
+      </c>
+      <c r="B28" s="225">
+        <v>206</v>
+      </c>
+      <c r="C28" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="D28" s="191" t="s">
+        <v>514</v>
+      </c>
+      <c r="E28" s="192" t="s">
+        <v>514</v>
+      </c>
+      <c r="F28" s="192">
+        <v>250</v>
+      </c>
+      <c r="G28" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="H28" s="191">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="185" t="s">
+        <v>500</v>
+      </c>
+      <c r="B29" s="225">
+        <v>150</v>
+      </c>
+      <c r="C29" s="191">
+        <v>126</v>
+      </c>
+      <c r="D29" s="191">
+        <v>124</v>
+      </c>
+      <c r="E29" s="192" t="s">
+        <v>514</v>
+      </c>
+      <c r="F29" s="192" t="s">
+        <v>506</v>
+      </c>
+      <c r="G29" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="H29" s="191">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="185" t="s">
+        <v>501</v>
+      </c>
+      <c r="B30" s="225" t="s">
+        <v>506</v>
+      </c>
+      <c r="C30" s="191">
+        <v>119</v>
+      </c>
+      <c r="D30" s="191">
+        <v>89</v>
+      </c>
+      <c r="E30" s="192" t="s">
+        <v>506</v>
+      </c>
+      <c r="F30" s="192" t="s">
+        <v>506</v>
+      </c>
+      <c r="G30" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="H30" s="191">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="185" t="s">
+        <v>502</v>
+      </c>
+      <c r="B31" s="225">
+        <v>500</v>
+      </c>
+      <c r="C31" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="D31" s="191">
+        <v>700</v>
+      </c>
+      <c r="E31" s="192">
+        <v>700</v>
+      </c>
+      <c r="F31" s="192" t="s">
+        <v>506</v>
+      </c>
+      <c r="G31" s="191" t="s">
+        <v>506</v>
+      </c>
+      <c r="H31" s="191">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="185" t="s">
+        <v>517</v>
+      </c>
+      <c r="B32" s="225" t="s">
+        <v>560</v>
+      </c>
+      <c r="C32" s="191" t="s">
+        <v>518</v>
+      </c>
+      <c r="D32" s="191" t="s">
+        <v>518</v>
+      </c>
+      <c r="E32" s="192"/>
+      <c r="F32" s="192"/>
+      <c r="G32" s="191"/>
+      <c r="H32" s="191"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" thickBot="1">
+      <c r="A33" s="186"/>
+      <c r="B33" s="227"/>
+      <c r="C33" s="195"/>
+      <c r="D33" s="195"/>
+      <c r="E33" s="196"/>
+      <c r="F33" s="196"/>
+      <c r="G33" s="195"/>
+      <c r="H33" s="191"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="189" t="s">
+        <v>503</v>
+      </c>
+      <c r="B34" s="223">
         <f>5016+150+206</f>
         <v>5372</v>
       </c>
-      <c r="F17" s="69">
+      <c r="C34" s="197">
         <f>6500+126+119</f>
         <v>6745</v>
       </c>
-      <c r="G17" s="69">
+      <c r="D34" s="197">
         <f>6599+124</f>
         <v>6723</v>
       </c>
-      <c r="H17" s="70">
+      <c r="E34" s="197">
         <f>5314</f>
         <v>5314</v>
       </c>
-    </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1">
-      <c r="B18" s="187" t="s">
-        <v>533</v>
-      </c>
-      <c r="C18" s="192" t="s">
-        <v>526</v>
-      </c>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74" t="s">
-        <v>526</v>
-      </c>
-      <c r="H18" s="75" t="s">
-        <v>532</v>
-      </c>
+      <c r="F34" s="215">
+        <f>5439+360</f>
+        <v>5799</v>
+      </c>
+      <c r="G34" s="197">
+        <v>6232</v>
+      </c>
+      <c r="H34" s="191">
+        <v>5292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15" thickBot="1">
+      <c r="A35" s="190" t="s">
+        <v>528</v>
+      </c>
+      <c r="B35" s="224"/>
+      <c r="C35" s="198"/>
+      <c r="D35" s="198" t="s">
+        <v>521</v>
+      </c>
+      <c r="E35" s="198" t="s">
+        <v>527</v>
+      </c>
+      <c r="F35" s="216"/>
+      <c r="G35" s="198"/>
+      <c r="H35" s="191"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:C7"/>
+  <dimension ref="A2:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="37.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="16.21875" customWidth="1"/>
+    <col min="6" max="7" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3">
-      <c r="B3" t="s">
+    <row r="2" spans="1:7">
+      <c r="A2" s="66" t="s">
+        <v>487</v>
+      </c>
+      <c r="B2" s="66" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="217" t="s">
+        <v>537</v>
+      </c>
+      <c r="D2" s="66" t="s">
+        <v>559</v>
+      </c>
+      <c r="E2" s="66" t="s">
+        <v>546</v>
+      </c>
+      <c r="F2" s="66" t="s">
+        <v>546</v>
+      </c>
+      <c r="G2" s="219" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="66" t="s">
         <v>488</v>
       </c>
-      <c r="C3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" t="s">
+      <c r="B3" s="66" t="s">
+        <v>545</v>
+      </c>
+      <c r="C3" s="217" t="s">
+        <v>399</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>490</v>
+      </c>
+      <c r="E3" s="66" t="s">
+        <v>545</v>
+      </c>
+      <c r="F3" s="66" t="s">
+        <v>545</v>
+      </c>
+      <c r="G3" s="219" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="66" t="s">
+        <v>538</v>
+      </c>
+      <c r="B4" s="66" t="s">
+        <v>541</v>
+      </c>
+      <c r="C4" s="217" t="s">
+        <v>549</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>541</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>563</v>
+      </c>
+      <c r="F4" s="66" t="s">
+        <v>564</v>
+      </c>
+      <c r="G4" s="219" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="66" t="s">
+        <v>552</v>
+      </c>
+      <c r="B5" s="66" t="s">
+        <v>556</v>
+      </c>
+      <c r="C5" s="217" t="s">
+        <v>556</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>556</v>
+      </c>
+      <c r="E5" s="66" t="s">
+        <v>557</v>
+      </c>
+      <c r="F5" s="66" t="s">
+        <v>609</v>
+      </c>
+      <c r="G5" s="219" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="66" t="s">
+        <v>539</v>
+      </c>
+      <c r="B6" s="66" t="s">
+        <v>540</v>
+      </c>
+      <c r="C6" s="217" t="s">
+        <v>550</v>
+      </c>
+      <c r="D6" s="66" t="s">
+        <v>540</v>
+      </c>
+      <c r="E6" s="66" t="s">
+        <v>547</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>565</v>
+      </c>
+      <c r="G6" s="219" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="66" t="s">
+        <v>552</v>
+      </c>
+      <c r="B7" s="66" t="s">
+        <v>556</v>
+      </c>
+      <c r="C7" s="217" t="s">
+        <v>556</v>
+      </c>
+      <c r="D7" s="66" t="s">
+        <v>556</v>
+      </c>
+      <c r="E7" s="66" t="s">
+        <v>558</v>
+      </c>
+      <c r="F7" s="66" t="s">
+        <v>558</v>
+      </c>
+      <c r="G7" s="219" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="66" t="s">
+        <v>553</v>
+      </c>
+      <c r="B8" s="66" t="s">
+        <v>554</v>
+      </c>
+      <c r="C8" s="217" t="s">
+        <v>554</v>
+      </c>
+      <c r="D8" s="66" t="s">
+        <v>554</v>
+      </c>
+      <c r="E8" s="66" t="s">
+        <v>555</v>
+      </c>
+      <c r="F8" s="66" t="s">
+        <v>510</v>
+      </c>
+      <c r="G8" s="219" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="28.5">
+      <c r="A9" s="66" t="s">
+        <v>542</v>
+      </c>
+      <c r="B9" s="92" t="s">
+        <v>543</v>
+      </c>
+      <c r="C9" s="217" t="s">
+        <v>551</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>510</v>
+      </c>
+      <c r="E9" s="66" t="s">
+        <v>548</v>
+      </c>
+      <c r="F9" s="66" t="s">
+        <v>548</v>
+      </c>
+      <c r="G9" s="220" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15">
+      <c r="A10" s="66" t="s">
+        <v>544</v>
+      </c>
+      <c r="B10" s="91">
+        <v>11332</v>
+      </c>
+      <c r="C10" s="218">
+        <v>12914</v>
+      </c>
+      <c r="D10" s="91">
+        <f>5*1874+2000</f>
+        <v>11370</v>
+      </c>
+      <c r="E10" s="91">
+        <v>9727</v>
+      </c>
+      <c r="F10" s="200">
+        <f>13327-387</f>
+        <v>12940</v>
+      </c>
+      <c r="G10" s="221">
+        <v>13327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="199" t="s">
+        <v>562</v>
+      </c>
+      <c r="B11" s="66">
+        <v>-400</v>
+      </c>
+      <c r="C11" s="217">
+        <v>-600</v>
+      </c>
+      <c r="D11" s="66">
+        <v>-400</v>
+      </c>
+      <c r="E11" s="66">
+        <v>0</v>
+      </c>
+      <c r="F11" s="66">
+        <v>-2500</v>
+      </c>
+      <c r="G11" s="219">
+        <v>-2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="199" t="s">
+        <v>567</v>
+      </c>
+      <c r="B12" s="66">
+        <f>B10+B11</f>
+        <v>10932</v>
+      </c>
+      <c r="C12" s="217">
+        <f t="shared" ref="C12:D12" si="0">C10+C11</f>
+        <v>12314</v>
+      </c>
+      <c r="D12" s="66">
+        <f t="shared" si="0"/>
+        <v>10970</v>
+      </c>
+      <c r="E12" s="66">
+        <f>E10+E11</f>
+        <v>9727</v>
+      </c>
+      <c r="F12" s="66">
+        <f>F10+F11</f>
+        <v>10440</v>
+      </c>
+      <c r="G12" s="219">
+        <f>G10+G11</f>
+        <v>10827</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1"/>
+    <row r="16" spans="1:7">
+      <c r="A16" s="77" t="s">
+        <v>488</v>
+      </c>
+      <c r="B16" s="68" t="s">
+        <v>584</v>
+      </c>
+      <c r="C16" s="70"/>
+      <c r="D16" s="70" t="s">
+        <v>573</v>
+      </c>
+      <c r="E16" s="68" t="s">
+        <v>545</v>
+      </c>
+      <c r="F16" s="70"/>
+      <c r="G16" s="70"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="77" t="s">
         <v>487</v>
       </c>
-      <c r="C4" s="183">
-        <v>41533</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" t="s">
-        <v>489</v>
-      </c>
-      <c r="C5" s="183">
-        <v>41533</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" t="s">
-        <v>490</v>
-      </c>
-      <c r="C6" s="183">
-        <v>41533</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" t="s">
-        <v>491</v>
+      <c r="B17" s="207" t="s">
+        <v>569</v>
+      </c>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72" t="s">
+        <v>536</v>
+      </c>
+      <c r="E17" s="207" t="s">
+        <v>569</v>
+      </c>
+      <c r="F17" s="72"/>
+      <c r="G17" s="72"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="77" t="s">
+        <v>538</v>
+      </c>
+      <c r="B18" s="71" t="s">
+        <v>570</v>
+      </c>
+      <c r="C18" s="72"/>
+      <c r="D18" s="72" t="s">
+        <v>536</v>
+      </c>
+      <c r="E18" s="71" t="s">
+        <v>570</v>
+      </c>
+      <c r="F18" s="72"/>
+      <c r="G18" s="72"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="77" t="s">
+        <v>571</v>
+      </c>
+      <c r="B19" s="71" t="s">
+        <v>572</v>
+      </c>
+      <c r="C19" s="72">
+        <f>D19/1960</f>
+        <v>2.8240816326530611</v>
+      </c>
+      <c r="D19" s="72">
+        <v>5535.2</v>
+      </c>
+      <c r="E19" s="71" t="s">
+        <v>572</v>
+      </c>
+      <c r="F19" s="213">
+        <f>G19/1960</f>
+        <v>2.9699999999999998</v>
+      </c>
+      <c r="G19" s="213">
+        <v>5821.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="203" t="s">
+        <v>574</v>
+      </c>
+      <c r="B20" s="71" t="s">
+        <v>575</v>
+      </c>
+      <c r="C20" s="72">
+        <f>D20/8</f>
+        <v>29.7925</v>
+      </c>
+      <c r="D20" s="72">
+        <v>238.34</v>
+      </c>
+      <c r="E20" s="71" t="s">
+        <v>575</v>
+      </c>
+      <c r="F20" s="72">
+        <f>G20/8</f>
+        <v>28.44</v>
+      </c>
+      <c r="G20" s="72">
+        <v>227.52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="204" t="s">
+        <v>576</v>
+      </c>
+      <c r="B21" s="71" t="s">
+        <v>577</v>
+      </c>
+      <c r="C21" s="72">
+        <f>D21/90</f>
+        <v>23.461111111111112</v>
+      </c>
+      <c r="D21" s="72">
+        <f>1055.75*2</f>
+        <v>2111.5</v>
+      </c>
+      <c r="E21" s="71" t="s">
+        <v>601</v>
+      </c>
+      <c r="F21" s="72">
+        <f>G21/76</f>
+        <v>22.400000000000002</v>
+      </c>
+      <c r="G21" s="72">
+        <f>851.2+851.2</f>
+        <v>1702.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="205" t="s">
+        <v>579</v>
+      </c>
+      <c r="B22" s="71" t="s">
+        <v>578</v>
+      </c>
+      <c r="C22" s="72">
+        <f>D22/23</f>
+        <v>25.634347826086959</v>
+      </c>
+      <c r="D22" s="72">
+        <v>589.59</v>
+      </c>
+      <c r="E22" s="71" t="s">
+        <v>602</v>
+      </c>
+      <c r="F22" s="72">
+        <f>G22/28</f>
+        <v>24.09</v>
+      </c>
+      <c r="G22" s="72">
+        <f>25.76+648.76</f>
+        <v>674.52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="205" t="s">
+        <v>580</v>
+      </c>
+      <c r="B23" s="71" t="s">
+        <v>581</v>
+      </c>
+      <c r="C23" s="72">
+        <f>D23/2</f>
+        <v>38.075000000000003</v>
+      </c>
+      <c r="D23" s="72">
+        <v>76.150000000000006</v>
+      </c>
+      <c r="E23" s="71" t="s">
+        <v>581</v>
+      </c>
+      <c r="F23" s="72">
+        <f>G23/2</f>
+        <v>36.340000000000003</v>
+      </c>
+      <c r="G23" s="72">
+        <v>72.680000000000007</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="205" t="s">
+        <v>582</v>
+      </c>
+      <c r="B24" s="71" t="s">
+        <v>583</v>
+      </c>
+      <c r="C24" s="72">
+        <f>D24</f>
+        <v>460.22</v>
+      </c>
+      <c r="D24" s="72">
+        <v>460.22</v>
+      </c>
+      <c r="E24" s="71" t="s">
+        <v>581</v>
+      </c>
+      <c r="F24" s="72">
+        <f>G24/2</f>
+        <v>450.22</v>
+      </c>
+      <c r="G24" s="72">
+        <v>900.44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="210" t="s">
+        <v>603</v>
+      </c>
+      <c r="B25" s="71"/>
+      <c r="C25" s="72"/>
+      <c r="D25" s="72" t="s">
+        <v>510</v>
+      </c>
+      <c r="E25" s="71" t="s">
+        <v>604</v>
+      </c>
+      <c r="F25" s="72"/>
+      <c r="G25" s="72">
+        <v>307.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15">
+      <c r="A26" s="211" t="s">
+        <v>596</v>
+      </c>
+      <c r="B26" s="71"/>
+      <c r="C26" s="212"/>
+      <c r="D26" s="212">
+        <v>9011.99</v>
+      </c>
+      <c r="E26" s="71"/>
+      <c r="F26" s="212"/>
+      <c r="G26" s="212">
+        <v>9706</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="201" t="s">
+        <v>587</v>
+      </c>
+      <c r="B27" s="71"/>
+      <c r="C27" s="72"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="72">
+        <f>G26-F24-G25</f>
+        <v>8948.2800000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="201" t="s">
+        <v>585</v>
+      </c>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="72"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="201" t="s">
+        <v>586</v>
+      </c>
+      <c r="B29" s="71"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="72"/>
+      <c r="E29" s="71"/>
+      <c r="F29" s="72"/>
+      <c r="G29" s="72"/>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" s="201" t="s">
+        <v>588</v>
+      </c>
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="71"/>
+      <c r="F30" s="72"/>
+      <c r="G30" s="72"/>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="202" t="s">
+        <v>589</v>
+      </c>
+      <c r="B31" s="71"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="72"/>
+      <c r="E31" s="71"/>
+      <c r="F31" s="72"/>
+      <c r="G31" s="72"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="202" t="s">
+        <v>590</v>
+      </c>
+      <c r="B32" s="71"/>
+      <c r="C32" s="72"/>
+      <c r="D32" s="72"/>
+      <c r="E32" s="71"/>
+      <c r="F32" s="72"/>
+      <c r="G32" s="72"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="202" t="s">
+        <v>591</v>
+      </c>
+      <c r="B33" s="71"/>
+      <c r="C33" s="72"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="71"/>
+      <c r="F33" s="72"/>
+      <c r="G33" s="72"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="202" t="s">
+        <v>592</v>
+      </c>
+      <c r="B34" s="71"/>
+      <c r="C34" s="72"/>
+      <c r="D34" s="72"/>
+      <c r="E34" s="71"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="72"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="202" t="s">
+        <v>593</v>
+      </c>
+      <c r="B35" s="71"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="72"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="202" t="s">
+        <v>594</v>
+      </c>
+      <c r="B36" s="208"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="71"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="72"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A37" s="206" t="s">
+        <v>595</v>
+      </c>
+      <c r="B37" s="209"/>
+      <c r="C37" s="120"/>
+      <c r="D37" s="120">
+        <v>2029</v>
+      </c>
+      <c r="E37" s="73"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="222" t="s">
+        <v>610</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update wyceny okien i dachu, s10
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ProductBacklog" sheetId="1" r:id="rId1"/>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1159" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="722">
   <si>
     <t>Id</t>
   </si>
@@ -1935,9 +1935,6 @@
     <t>U = 0,8</t>
   </si>
   <si>
-    <t>Rynny</t>
-  </si>
-  <si>
     <t>Rzeczy do zrobienia przed zimą:</t>
   </si>
   <si>
@@ -2160,16 +2157,134 @@
   </si>
   <si>
     <t>Dorotka</t>
+  </si>
+  <si>
+    <t>Wspornik N. ławy kominiarskiej</t>
+  </si>
+  <si>
+    <t>Mocownik N. ławy kominiarskiej</t>
+  </si>
+  <si>
+    <t>ŁAWA N. KOMINIARSKA</t>
+  </si>
+  <si>
+    <t>FOLIA MEMBRANA VENTMAX
+125g</t>
+  </si>
+  <si>
+    <t>TAŚMA KALENICOWA Vent-Roll</t>
+  </si>
+  <si>
+    <t>Wspornik łaty kalenicowej typ GW</t>
+  </si>
+  <si>
+    <t>Spinka do dachówki ceramicznej</t>
+  </si>
+  <si>
+    <t>BRAAS Taśma WAKAFLEX</t>
+  </si>
+  <si>
+    <t>Blacha płaska grafit 7024</t>
+  </si>
+  <si>
+    <t>SOUDAL USZCZELNIACZ
+DEKARSKI SPECJALISTY</t>
+  </si>
+  <si>
+    <t>Grzebień okapowy płaski</t>
+  </si>
+  <si>
+    <t>Blacha płaska grafit</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 127/3 rynna</t>
+  </si>
+  <si>
+    <t>OCYNK 127 uchwyt rynny</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 127 denko rynny</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 127 lej spustowy</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 100/2 rura</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 100 mufa</t>
+  </si>
+  <si>
+    <t>TYTAN CYNK 100 kolano</t>
+  </si>
+  <si>
+    <t>OCYNK 100 uchwyt rury</t>
+  </si>
+  <si>
+    <t>OB. ŚRUBA DO OBEJMY 20CM</t>
+  </si>
+  <si>
+    <t>STOPIEŃ N. KOMINARSKI
+GRAFIT</t>
+  </si>
+  <si>
+    <t>RYNNY</t>
+  </si>
+  <si>
+    <t>Rynna 127 3m</t>
+  </si>
+  <si>
+    <t>Sztucer</t>
+  </si>
+  <si>
+    <t>Denko</t>
+  </si>
+  <si>
+    <t>Rynhak</t>
+  </si>
+  <si>
+    <t>Rura spustowa</t>
+  </si>
+  <si>
+    <t>Mufa</t>
+  </si>
+  <si>
+    <t>Klej</t>
+  </si>
+  <si>
+    <t>Kolanko</t>
+  </si>
+  <si>
+    <t>Obejma</t>
+  </si>
+  <si>
+    <t>Sztyft 30cm</t>
+  </si>
+  <si>
+    <t>Materiał</t>
+  </si>
+  <si>
+    <t>cana brutto/szt</t>
+  </si>
+  <si>
+    <t>DODATKI DACHOWE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DACHÓWKI  </t>
+  </si>
+  <si>
+    <t>OKNA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;zł&quot;;[Red]\-#,##0\ &quot;zł&quot;"/>
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2358,19 +2473,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial CE"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial CE"/>
-      <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0" tint="-0.34998626667073579"/>
       <name val="Czcionka tekstu podstawowego"/>
@@ -2420,8 +2522,37 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial CE"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3" tint="-0.499984740745262"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <charset val="238"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2470,8 +2601,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="44">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -2995,30 +3132,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -3040,11 +3153,83 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="234">
+  <cellXfs count="260">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3434,37 +3619,27 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="30" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3475,31 +3650,125 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="133">
     <dxf>
-      <border outline="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3658,77 +3927,25 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color theme="7" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -6946,7 +7163,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740244"/>
+          <c:w val="0.71441426071740233"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -7226,24 +7443,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62787968"/>
-        <c:axId val="62789504"/>
+        <c:axId val="62784256"/>
+        <c:axId val="62785792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62787968"/>
+        <c:axId val="62784256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62789504"/>
+        <c:crossAx val="62785792"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="62789504"/>
+        <c:axId val="62785792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -7253,7 +7470,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62787968"/>
+        <c:crossAx val="62784256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7264,8 +7481,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325289063"/>
-          <c:y val="0.2935396617089574"/>
+          <c:x val="0.86438523325289074"/>
+          <c:y val="0.29353966170895746"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -7275,7 +7492,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000081" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000081" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000822" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000822" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7487,24 +7704,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62831232"/>
-        <c:axId val="62833024"/>
+        <c:axId val="62835712"/>
+        <c:axId val="62837504"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62831232"/>
+        <c:axId val="62835712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62833024"/>
+        <c:crossAx val="62837504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62833024"/>
+        <c:axId val="62837504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -7514,7 +7731,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62831232"/>
+        <c:crossAx val="62835712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7526,7 +7743,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000006" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000006" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000611" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000611" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7689,24 +7906,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63898752"/>
-        <c:axId val="63900288"/>
+        <c:axId val="63632896"/>
+        <c:axId val="63634432"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63898752"/>
+        <c:axId val="63632896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63900288"/>
+        <c:crossAx val="63634432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63900288"/>
+        <c:axId val="63634432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -7716,7 +7933,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63898752"/>
+        <c:crossAx val="63632896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7728,7 +7945,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000622" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000622" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000633" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000633" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7843,11 +8060,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63998208"/>
-        <c:axId val="64004096"/>
+        <c:axId val="63990400"/>
+        <c:axId val="64004480"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63998208"/>
+        <c:axId val="63990400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7855,13 +8072,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64004096"/>
+        <c:crossAx val="64004480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64004096"/>
+        <c:axId val="64004480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7869,7 +8086,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63998208"/>
+        <c:crossAx val="63990400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7881,7 +8098,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000477" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000477" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000488" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000488" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7897,10 +8114,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.171815628309618"/>
-          <c:y val="3.2882035578886311E-2"/>
+          <c:x val="0.17181562830961797"/>
+          <c:y val="3.2882035578886318E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.6386187664042049"/>
+          <c:h val="0.63861876640420501"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -8063,11 +8280,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64074112"/>
-        <c:axId val="64075648"/>
+        <c:axId val="64070400"/>
+        <c:axId val="64071936"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64074112"/>
+        <c:axId val="64070400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8075,13 +8292,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64075648"/>
+        <c:crossAx val="64071936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64075648"/>
+        <c:axId val="64071936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -8090,7 +8307,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64074112"/>
+        <c:crossAx val="64070400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8102,7 +8319,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000005" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000005" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000511" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000511" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8312,13 +8529,13 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabela121415" displayName="Tabela121415" ref="A2:D28" totalsRowShown="0" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Tabela121415" displayName="Tabela121415" ref="A2:D28" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A2:D28"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Lp" dataDxfId="6"/>
-    <tableColumn id="2" name="Status" dataDxfId="5"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="4"/>
-    <tableColumn id="4" name="Zadanie" dataDxfId="3"/>
+    <tableColumn id="1" name="Lp" dataDxfId="10"/>
+    <tableColumn id="2" name="Status" dataDxfId="9"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="8"/>
+    <tableColumn id="4" name="Zadanie" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8331,7 +8548,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="Kolumna1"/>
-    <tableColumn id="10" name="Kolumna2" dataDxfId="13"/>
+    <tableColumn id="10" name="Kolumna2" dataDxfId="6"/>
     <tableColumn id="3" name="Kolumna3"/>
     <tableColumn id="12" name="Kolumna4"/>
     <tableColumn id="4" name="Kolumna5"/>
@@ -8355,7 +8572,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="szt"/>
-    <tableColumn id="10" name="Cena bloczka" dataDxfId="12"/>
+    <tableColumn id="10" name="Cena bloczka" dataDxfId="5"/>
     <tableColumn id="3" name="Cena bloczków 200m2"/>
     <tableColumn id="12" name="Klej25kg"/>
     <tableColumn id="4" name="Cena kleju"/>
@@ -8368,12 +8585,12 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="9"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="8"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="7"/>
+    <tableColumn id="1" name="Temat" dataDxfId="2"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9548,85 +9765,85 @@
         <v>6</v>
       </c>
       <c r="D3" s="177" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="175"/>
       <c r="B4" s="145"/>
       <c r="C4" s="146" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D4" s="178" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="222"/>
+      <c r="B5" s="223"/>
+      <c r="C5" s="146" t="s">
+        <v>639</v>
+      </c>
+      <c r="D5" s="177" t="s">
         <v>635</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="230"/>
-      <c r="B5" s="231"/>
-      <c r="C5" s="146" t="s">
-        <v>640</v>
-      </c>
-      <c r="D5" s="177" t="s">
-        <v>636</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" ht="38.25">
-      <c r="A6" s="230"/>
-      <c r="B6" s="231"/>
+      <c r="A6" s="222"/>
+      <c r="B6" s="223"/>
       <c r="C6" s="146" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="177" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="222"/>
+      <c r="B7" s="223"/>
+      <c r="C7" s="146" t="s">
+        <v>639</v>
+      </c>
+      <c r="D7" s="177" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="230"/>
-      <c r="B7" s="231"/>
-      <c r="C7" s="146" t="s">
-        <v>640</v>
-      </c>
-      <c r="D7" s="177" t="s">
-        <v>639</v>
-      </c>
-    </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="230"/>
-      <c r="B8" s="231"/>
+      <c r="A8" s="222"/>
+      <c r="B8" s="223"/>
       <c r="C8" s="146"/>
       <c r="D8" s="177"/>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="172" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B9" s="173"/>
       <c r="C9" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="177" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="175"/>
       <c r="B10" s="145"/>
       <c r="C10" s="146" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D10" s="178" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="172" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B11" s="173"/>
       <c r="C11" s="174"/>
       <c r="D11" s="177" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -9643,21 +9860,21 @@
     </row>
     <row r="19" spans="1:5" ht="15">
       <c r="A19" s="91" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B19" s="66"/>
       <c r="C19" s="66" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="D19" s="66" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="E19" s="66" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="232"/>
+      <c r="A20" s="224"/>
       <c r="B20" s="92"/>
       <c r="C20" s="92"/>
       <c r="D20" s="92"/>
@@ -9666,10 +9883,10 @@
     <row r="21" spans="1:5" ht="28.5">
       <c r="A21" s="92"/>
       <c r="B21" s="92" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C21" s="92" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D21" s="92"/>
       <c r="E21" s="92">
@@ -9679,7 +9896,7 @@
     <row r="22" spans="1:5">
       <c r="A22" s="92"/>
       <c r="B22" s="92" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C22" s="92"/>
       <c r="D22" s="92"/>
@@ -9690,10 +9907,10 @@
     <row r="23" spans="1:5" ht="42.75">
       <c r="A23" s="92"/>
       <c r="B23" s="92" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C23" s="92" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D23" s="92"/>
       <c r="E23" s="92">
@@ -9703,10 +9920,10 @@
     <row r="24" spans="1:5" ht="57">
       <c r="A24" s="92"/>
       <c r="B24" s="92" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C24" s="92" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D24" s="92"/>
       <c r="E24" s="92">
@@ -9716,7 +9933,7 @@
     <row r="25" spans="1:5">
       <c r="A25" s="92"/>
       <c r="B25" s="92" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C25" s="92"/>
       <c r="D25" s="92"/>
@@ -9725,13 +9942,13 @@
     <row r="26" spans="1:5" ht="28.5">
       <c r="A26" s="92"/>
       <c r="B26" s="92" t="s">
+        <v>650</v>
+      </c>
+      <c r="C26" s="92" t="s">
+        <v>656</v>
+      </c>
+      <c r="D26" s="92" t="s">
         <v>651</v>
-      </c>
-      <c r="C26" s="92" t="s">
-        <v>657</v>
-      </c>
-      <c r="D26" s="92" t="s">
-        <v>652</v>
       </c>
       <c r="E26" s="92">
         <f>200*50</f>
@@ -9741,10 +9958,10 @@
     <row r="27" spans="1:5" ht="28.5">
       <c r="A27" s="92"/>
       <c r="B27" s="92" t="s">
-        <v>613</v>
-      </c>
-      <c r="C27" s="233" t="s">
-        <v>659</v>
+        <v>612</v>
+      </c>
+      <c r="C27" s="225" t="s">
+        <v>658</v>
       </c>
       <c r="D27" s="92"/>
       <c r="E27" s="92"/>
@@ -9752,13 +9969,13 @@
     <row r="28" spans="1:5" ht="28.5">
       <c r="A28" s="92"/>
       <c r="B28" s="92" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C28" s="92" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D28" s="92" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="E28" s="92">
         <v>5000</v>
@@ -9767,11 +9984,11 @@
     <row r="29" spans="1:5">
       <c r="A29" s="92"/>
       <c r="B29" s="92" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C29" s="92"/>
       <c r="D29" s="92" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E29" s="92">
         <v>0</v>
@@ -9783,10 +10000,10 @@
         <v>479</v>
       </c>
       <c r="C30" s="92" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D30" s="92" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E30" s="92">
         <v>2200</v>
@@ -9795,13 +10012,13 @@
     <row r="31" spans="1:5" ht="42.75">
       <c r="A31" s="92"/>
       <c r="B31" s="92" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C31" s="92" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D31" s="92" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E31" s="92">
         <v>9400</v>
@@ -9813,10 +10030,10 @@
         <v>478</v>
       </c>
       <c r="C32" s="92" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D32" s="92" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="E32" s="92">
         <v>15700</v>
@@ -9825,13 +10042,13 @@
     <row r="33" spans="1:5" ht="57">
       <c r="A33" s="92"/>
       <c r="B33" s="92" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C33" s="92" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D33" s="92" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E33" s="92">
         <f>35*180</f>
@@ -9841,10 +10058,10 @@
     <row r="34" spans="1:5" ht="57">
       <c r="A34" s="92"/>
       <c r="B34" s="92" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C34" s="92" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D34" s="92"/>
       <c r="E34" s="92"/>
@@ -9852,10 +10069,10 @@
     <row r="35" spans="1:5" ht="28.5">
       <c r="A35" s="92"/>
       <c r="B35" s="92" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C35" s="92" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D35" s="92"/>
       <c r="E35" s="92"/>
@@ -9863,10 +10080,10 @@
     <row r="36" spans="1:5" ht="99.75">
       <c r="A36" s="92"/>
       <c r="B36" s="92" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C36" s="92" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D36" s="92"/>
       <c r="E36" s="92"/>
@@ -9874,10 +10091,10 @@
     <row r="37" spans="1:5">
       <c r="A37" s="92"/>
       <c r="B37" s="92" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C37" s="92" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="D37" s="92"/>
       <c r="E37" s="92">
@@ -9887,7 +10104,7 @@
     <row r="38" spans="1:5">
       <c r="A38" s="92"/>
       <c r="B38" s="92" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C38" s="92" t="s">
         <v>496</v>
@@ -9898,7 +10115,7 @@
       </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="B39" s="233" t="s">
+      <c r="B39" s="225" t="s">
         <v>320</v>
       </c>
       <c r="E39">
@@ -9908,37 +10125,37 @@
     </row>
     <row r="41" spans="1:5" ht="15">
       <c r="A41" s="90" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -9992,17 +10209,17 @@
         <v>73</v>
       </c>
       <c r="D3" s="177" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="175"/>
       <c r="B4" s="145"/>
       <c r="C4" s="46" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D4" s="178" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -10015,20 +10232,20 @@
       <c r="A6" s="175"/>
       <c r="B6" s="145"/>
       <c r="C6" s="46" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D6" s="178" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="172"/>
       <c r="B7" s="173"/>
       <c r="C7" s="174" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D7" s="177" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -10041,20 +10258,20 @@
       <c r="A9" s="172"/>
       <c r="B9" s="173"/>
       <c r="C9" s="174" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D9" s="177" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="175"/>
       <c r="B10" s="145"/>
       <c r="C10" s="46" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D10" s="178" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -10067,10 +10284,10 @@
       <c r="A12" s="175"/>
       <c r="B12" s="145"/>
       <c r="C12" s="46" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D12" s="178" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -10083,20 +10300,20 @@
       <c r="A14" s="175"/>
       <c r="B14" s="145"/>
       <c r="C14" s="46" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D14" s="178" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="172"/>
       <c r="B15" s="173"/>
       <c r="C15" s="174" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D15" s="177" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -10112,7 +10329,7 @@
         <v>73</v>
       </c>
       <c r="D17" s="177" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -10122,7 +10339,7 @@
         <v>73</v>
       </c>
       <c r="D18" s="178" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -10132,7 +10349,7 @@
         <v>73</v>
       </c>
       <c r="D19" s="177" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -10142,7 +10359,7 @@
         <v>73</v>
       </c>
       <c r="D20" s="178" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -10152,7 +10369,7 @@
         <v>73</v>
       </c>
       <c r="D21" s="177" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -10162,7 +10379,7 @@
         <v>73</v>
       </c>
       <c r="D22" s="178" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -10242,7 +10459,7 @@
       <c r="B4" s="183" t="s">
         <v>489</v>
       </c>
-      <c r="C4" s="225" t="s">
+      <c r="C4" s="217" t="s">
         <v>489</v>
       </c>
       <c r="D4" s="66" t="s">
@@ -10256,7 +10473,7 @@
       <c r="B5" s="183" t="s">
         <v>490</v>
       </c>
-      <c r="C5" s="225" t="s">
+      <c r="C5" s="217" t="s">
         <v>504</v>
       </c>
       <c r="D5" s="66" t="s">
@@ -10270,7 +10487,7 @@
       <c r="B6" s="183" t="s">
         <v>492</v>
       </c>
-      <c r="C6" s="225" t="s">
+      <c r="C6" s="217" t="s">
         <v>510</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -10284,7 +10501,7 @@
       <c r="B7" s="183" t="s">
         <v>494</v>
       </c>
-      <c r="C7" s="225" t="s">
+      <c r="C7" s="217" t="s">
         <v>494</v>
       </c>
       <c r="D7" s="66" t="s">
@@ -10298,7 +10515,7 @@
       <c r="B8" s="183" t="s">
         <v>508</v>
       </c>
-      <c r="C8" s="225" t="s">
+      <c r="C8" s="217" t="s">
         <v>508</v>
       </c>
       <c r="D8" s="66" t="s">
@@ -10312,7 +10529,7 @@
       <c r="B9" s="183" t="s">
         <v>495</v>
       </c>
-      <c r="C9" s="225" t="s">
+      <c r="C9" s="217" t="s">
         <v>495</v>
       </c>
       <c r="D9" s="66" t="s">
@@ -10326,7 +10543,7 @@
       <c r="B10" s="183" t="s">
         <v>498</v>
       </c>
-      <c r="C10" s="225" t="s">
+      <c r="C10" s="217" t="s">
         <v>505</v>
       </c>
       <c r="D10" s="66" t="s">
@@ -10340,7 +10557,7 @@
       <c r="B11" s="183" t="s">
         <v>499</v>
       </c>
-      <c r="C11" s="225">
+      <c r="C11" s="217">
         <v>206</v>
       </c>
       <c r="D11" s="66" t="s">
@@ -10354,7 +10571,7 @@
       <c r="B12" s="183" t="s">
         <v>496</v>
       </c>
-      <c r="C12" s="225">
+      <c r="C12" s="217">
         <v>150</v>
       </c>
       <c r="D12" s="66">
@@ -10368,7 +10585,7 @@
       <c r="B13" s="183">
         <v>75</v>
       </c>
-      <c r="C13" s="225" t="s">
+      <c r="C13" s="217" t="s">
         <v>506</v>
       </c>
       <c r="D13" s="66">
@@ -10382,7 +10599,7 @@
       <c r="B14" s="183">
         <v>750</v>
       </c>
-      <c r="C14" s="225">
+      <c r="C14" s="217">
         <v>500</v>
       </c>
       <c r="D14" s="66">
@@ -10394,7 +10611,7 @@
         <v>517</v>
       </c>
       <c r="B15" s="183"/>
-      <c r="C15" s="225"/>
+      <c r="C15" s="217"/>
       <c r="D15" s="66" t="s">
         <v>518</v>
       </c>
@@ -10402,7 +10619,7 @@
     <row r="16" spans="1:4" ht="15" thickBot="1">
       <c r="A16" s="186"/>
       <c r="B16" s="187"/>
-      <c r="C16" s="227"/>
+      <c r="C16" s="219"/>
       <c r="D16" s="188"/>
     </row>
     <row r="17" spans="1:8">
@@ -10412,7 +10629,7 @@
       <c r="B17" s="68">
         <v>5142</v>
       </c>
-      <c r="C17" s="228">
+      <c r="C17" s="220">
         <f>4059+150+206</f>
         <v>4415</v>
       </c>
@@ -10427,7 +10644,7 @@
       <c r="B18" s="73" t="s">
         <v>521</v>
       </c>
-      <c r="C18" s="229"/>
+      <c r="C18" s="221"/>
       <c r="D18" s="74" t="s">
         <v>521</v>
       </c>
@@ -10437,7 +10654,7 @@
       <c r="A21" s="184" t="s">
         <v>487</v>
       </c>
-      <c r="B21" s="225" t="s">
+      <c r="B21" s="217" t="s">
         <v>489</v>
       </c>
       <c r="C21" s="191" t="s">
@@ -10463,7 +10680,7 @@
       <c r="A22" s="185" t="s">
         <v>488</v>
       </c>
-      <c r="B22" s="225" t="s">
+      <c r="B22" s="217" t="s">
         <v>504</v>
       </c>
       <c r="C22" s="191" t="s">
@@ -10489,7 +10706,7 @@
       <c r="A23" s="185" t="s">
         <v>491</v>
       </c>
-      <c r="B23" s="225" t="s">
+      <c r="B23" s="217" t="s">
         <v>510</v>
       </c>
       <c r="C23" s="191" t="s">
@@ -10513,7 +10730,7 @@
       <c r="A24" s="185" t="s">
         <v>493</v>
       </c>
-      <c r="B24" s="225" t="s">
+      <c r="B24" s="217" t="s">
         <v>494</v>
       </c>
       <c r="C24" s="191" t="s">
@@ -10525,7 +10742,7 @@
       <c r="E24" s="192" t="s">
         <v>525</v>
       </c>
-      <c r="F24" s="214" t="s">
+      <c r="F24" s="210" t="s">
         <v>561</v>
       </c>
       <c r="G24" s="191" t="s">
@@ -10539,7 +10756,7 @@
       <c r="A25" s="185" t="s">
         <v>507</v>
       </c>
-      <c r="B25" s="225" t="s">
+      <c r="B25" s="217" t="s">
         <v>508</v>
       </c>
       <c r="C25" s="191" t="s">
@@ -10565,7 +10782,7 @@
       <c r="A26" s="185" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="226" t="s">
+      <c r="B26" s="218" t="s">
         <v>513</v>
       </c>
       <c r="C26" s="193" t="s">
@@ -10591,7 +10808,7 @@
       <c r="A27" s="185" t="s">
         <v>497</v>
       </c>
-      <c r="B27" s="225" t="s">
+      <c r="B27" s="217" t="s">
         <v>505</v>
       </c>
       <c r="C27" s="191" t="s">
@@ -10617,7 +10834,7 @@
       <c r="A28" s="185" t="s">
         <v>509</v>
       </c>
-      <c r="B28" s="225">
+      <c r="B28" s="217">
         <v>206</v>
       </c>
       <c r="C28" s="191" t="s">
@@ -10643,7 +10860,7 @@
       <c r="A29" s="185" t="s">
         <v>500</v>
       </c>
-      <c r="B29" s="225">
+      <c r="B29" s="217">
         <v>150</v>
       </c>
       <c r="C29" s="191">
@@ -10669,7 +10886,7 @@
       <c r="A30" s="185" t="s">
         <v>501</v>
       </c>
-      <c r="B30" s="225" t="s">
+      <c r="B30" s="217" t="s">
         <v>506</v>
       </c>
       <c r="C30" s="191">
@@ -10695,7 +10912,7 @@
       <c r="A31" s="185" t="s">
         <v>502</v>
       </c>
-      <c r="B31" s="225">
+      <c r="B31" s="217">
         <v>500</v>
       </c>
       <c r="C31" s="191" t="s">
@@ -10721,7 +10938,7 @@
       <c r="A32" s="185" t="s">
         <v>517</v>
       </c>
-      <c r="B32" s="225" t="s">
+      <c r="B32" s="217" t="s">
         <v>560</v>
       </c>
       <c r="C32" s="191" t="s">
@@ -10737,7 +10954,7 @@
     </row>
     <row r="33" spans="1:8" ht="15" thickBot="1">
       <c r="A33" s="186"/>
-      <c r="B33" s="227"/>
+      <c r="B33" s="219"/>
       <c r="C33" s="195"/>
       <c r="D33" s="195"/>
       <c r="E33" s="196"/>
@@ -10749,7 +10966,7 @@
       <c r="A34" s="189" t="s">
         <v>503</v>
       </c>
-      <c r="B34" s="223">
+      <c r="B34" s="215">
         <f>5016+150+206</f>
         <v>5372</v>
       </c>
@@ -10765,7 +10982,7 @@
         <f>5314</f>
         <v>5314</v>
       </c>
-      <c r="F34" s="215">
+      <c r="F34" s="211">
         <f>5439+360</f>
         <v>5799</v>
       </c>
@@ -10780,7 +10997,7 @@
       <c r="A35" s="190" t="s">
         <v>528</v>
       </c>
-      <c r="B35" s="224"/>
+      <c r="B35" s="216"/>
       <c r="C35" s="198"/>
       <c r="D35" s="198" t="s">
         <v>521</v>
@@ -10788,7 +11005,7 @@
       <c r="E35" s="198" t="s">
         <v>527</v>
       </c>
-      <c r="F35" s="216"/>
+      <c r="F35" s="212"/>
       <c r="G35" s="198"/>
       <c r="H35" s="191"/>
     </row>
@@ -10800,30 +11017,37 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G38"/>
+  <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.21875" customWidth="1"/>
-    <col min="6" max="7" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
+    <col min="2" max="2" width="16.21875" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="1" spans="1:8" ht="15">
+      <c r="A1" s="256" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="66" t="s">
         <v>487</v>
       </c>
       <c r="B2" s="66" t="s">
         <v>537</v>
       </c>
-      <c r="C2" s="217" t="s">
+      <c r="C2" s="213" t="s">
         <v>537</v>
       </c>
       <c r="D2" s="66" t="s">
@@ -10835,18 +11059,21 @@
       <c r="F2" s="66" t="s">
         <v>546</v>
       </c>
-      <c r="G2" s="219" t="s">
+      <c r="G2" s="226" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" s="229" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="66" t="s">
         <v>488</v>
       </c>
       <c r="B3" s="66" t="s">
         <v>545</v>
       </c>
-      <c r="C3" s="217" t="s">
+      <c r="C3" s="213" t="s">
         <v>399</v>
       </c>
       <c r="D3" s="66" t="s">
@@ -10858,18 +11085,21 @@
       <c r="F3" s="66" t="s">
         <v>545</v>
       </c>
-      <c r="G3" s="219" t="s">
+      <c r="G3" s="226" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3" s="229" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="66" t="s">
         <v>538</v>
       </c>
       <c r="B4" s="66" t="s">
         <v>541</v>
       </c>
-      <c r="C4" s="217" t="s">
+      <c r="C4" s="213" t="s">
         <v>549</v>
       </c>
       <c r="D4" s="66" t="s">
@@ -10881,18 +11111,21 @@
       <c r="F4" s="66" t="s">
         <v>564</v>
       </c>
-      <c r="G4" s="219" t="s">
+      <c r="G4" s="226" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4" s="229" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="66" t="s">
         <v>552</v>
       </c>
       <c r="B5" s="66" t="s">
         <v>556</v>
       </c>
-      <c r="C5" s="217" t="s">
+      <c r="C5" s="213" t="s">
         <v>556</v>
       </c>
       <c r="D5" s="66" t="s">
@@ -10904,18 +11137,21 @@
       <c r="F5" s="66" t="s">
         <v>609</v>
       </c>
-      <c r="G5" s="219" t="s">
+      <c r="G5" s="226" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="H5" s="229" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="66" t="s">
         <v>539</v>
       </c>
       <c r="B6" s="66" t="s">
         <v>540</v>
       </c>
-      <c r="C6" s="217" t="s">
+      <c r="C6" s="213" t="s">
         <v>550</v>
       </c>
       <c r="D6" s="66" t="s">
@@ -10927,18 +11163,21 @@
       <c r="F6" s="66" t="s">
         <v>565</v>
       </c>
-      <c r="G6" s="219" t="s">
+      <c r="G6" s="226" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="H6" s="229" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="66" t="s">
         <v>552</v>
       </c>
       <c r="B7" s="66" t="s">
         <v>556</v>
       </c>
-      <c r="C7" s="217" t="s">
+      <c r="C7" s="213" t="s">
         <v>556</v>
       </c>
       <c r="D7" s="66" t="s">
@@ -10950,18 +11189,21 @@
       <c r="F7" s="66" t="s">
         <v>558</v>
       </c>
-      <c r="G7" s="219" t="s">
+      <c r="G7" s="226" t="s">
         <v>558</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="H7" s="229" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="66" t="s">
         <v>553</v>
       </c>
       <c r="B8" s="66" t="s">
         <v>554</v>
       </c>
-      <c r="C8" s="217" t="s">
+      <c r="C8" s="213" t="s">
         <v>554</v>
       </c>
       <c r="D8" s="66" t="s">
@@ -10973,18 +11215,21 @@
       <c r="F8" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="226" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.5">
+      <c r="H8" s="229" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="28.5">
       <c r="A9" s="66" t="s">
         <v>542</v>
       </c>
       <c r="B9" s="92" t="s">
         <v>543</v>
       </c>
-      <c r="C9" s="217" t="s">
+      <c r="C9" s="213" t="s">
         <v>551</v>
       </c>
       <c r="D9" s="66" t="s">
@@ -10996,18 +11241,21 @@
       <c r="F9" s="66" t="s">
         <v>548</v>
       </c>
-      <c r="G9" s="220" t="s">
+      <c r="G9" s="227" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15">
+      <c r="H9" s="230" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="66" t="s">
         <v>544</v>
       </c>
       <c r="B10" s="91">
         <v>11332</v>
       </c>
-      <c r="C10" s="218">
+      <c r="C10" s="214">
         <v>12914</v>
       </c>
       <c r="D10" s="91">
@@ -11021,18 +11269,21 @@
         <f>13327-387</f>
         <v>12940</v>
       </c>
-      <c r="G10" s="221">
+      <c r="G10" s="228">
         <v>13327</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="H10" s="231">
+        <v>12076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" s="199" t="s">
         <v>562</v>
       </c>
       <c r="B11" s="66">
         <v>-400</v>
       </c>
-      <c r="C11" s="217">
+      <c r="C11" s="213">
         <v>-600</v>
       </c>
       <c r="D11" s="66">
@@ -11044,11 +11295,14 @@
       <c r="F11" s="66">
         <v>-2500</v>
       </c>
-      <c r="G11" s="219">
+      <c r="G11" s="226">
         <v>-2500</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="H11" s="229">
+        <v>-2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="199" t="s">
         <v>567</v>
       </c>
@@ -11056,7 +11310,7 @@
         <f>B10+B11</f>
         <v>10932</v>
       </c>
-      <c r="C12" s="217">
+      <c r="C12" s="213">
         <f t="shared" ref="C12:D12" si="0">C10+C11</f>
         <v>12314</v>
       </c>
@@ -11072,13 +11326,21 @@
         <f>F10+F11</f>
         <v>10440</v>
       </c>
-      <c r="G12" s="219">
+      <c r="G12" s="226">
         <f>G10+G11</f>
         <v>10827</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1"/>
-    <row r="16" spans="1:7">
+      <c r="H12" s="258">
+        <f>H10+H11</f>
+        <v>9576</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A15" s="256" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16" s="77" t="s">
         <v>488</v>
       </c>
@@ -11095,24 +11357,24 @@
       <c r="F16" s="70"/>
       <c r="G16" s="70"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:8">
       <c r="A17" s="77" t="s">
         <v>487</v>
       </c>
-      <c r="B17" s="207" t="s">
+      <c r="B17" s="204" t="s">
         <v>569</v>
       </c>
       <c r="C17" s="72"/>
       <c r="D17" s="72" t="s">
         <v>536</v>
       </c>
-      <c r="E17" s="207" t="s">
+      <c r="E17" s="204" t="s">
         <v>569</v>
       </c>
       <c r="F17" s="72"/>
       <c r="G17" s="72"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:8">
       <c r="A18" s="77" t="s">
         <v>538</v>
       </c>
@@ -11129,7 +11391,7 @@
       <c r="F18" s="72"/>
       <c r="G18" s="72"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:8">
       <c r="A19" s="77" t="s">
         <v>571</v>
       </c>
@@ -11137,8 +11399,8 @@
         <v>572</v>
       </c>
       <c r="C19" s="72">
-        <f>D19/1960</f>
-        <v>2.8240816326530611</v>
+        <f>ROUND(D19/1960,2)</f>
+        <v>2.82</v>
       </c>
       <c r="D19" s="72">
         <v>5535.2</v>
@@ -11146,24 +11408,27 @@
       <c r="E19" s="71" t="s">
         <v>572</v>
       </c>
-      <c r="F19" s="213">
+      <c r="F19" s="209">
         <f>G19/1960</f>
         <v>2.9699999999999998</v>
       </c>
-      <c r="G19" s="213">
+      <c r="G19" s="209">
         <v>5821.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="203" t="s">
+      <c r="H19" s="259">
+        <f>G19-D19</f>
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="201" t="s">
         <v>574</v>
       </c>
       <c r="B20" s="71" t="s">
         <v>575</v>
       </c>
       <c r="C20" s="72">
-        <f>D20/8</f>
-        <v>29.7925</v>
+        <v>29.8</v>
       </c>
       <c r="D20" s="72">
         <v>238.34</v>
@@ -11179,16 +11444,15 @@
         <v>227.52</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="204" t="s">
+    <row r="21" spans="1:8">
+      <c r="A21" s="202" t="s">
         <v>576</v>
       </c>
       <c r="B21" s="71" t="s">
         <v>577</v>
       </c>
       <c r="C21" s="72">
-        <f>D21/90</f>
-        <v>23.461111111111112</v>
+        <v>23.46</v>
       </c>
       <c r="D21" s="72">
         <f>1055.75*2</f>
@@ -11206,16 +11470,15 @@
         <v>1702.4</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="205" t="s">
+    <row r="22" spans="1:8">
+      <c r="A22" s="203" t="s">
         <v>579</v>
       </c>
       <c r="B22" s="71" t="s">
         <v>578</v>
       </c>
       <c r="C22" s="72">
-        <f>D22/23</f>
-        <v>25.634347826086959</v>
+        <v>25.63</v>
       </c>
       <c r="D22" s="72">
         <v>589.59</v>
@@ -11232,16 +11495,15 @@
         <v>674.52</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="205" t="s">
+    <row r="23" spans="1:8">
+      <c r="A23" s="203" t="s">
         <v>580</v>
       </c>
       <c r="B23" s="71" t="s">
         <v>581</v>
       </c>
       <c r="C23" s="72">
-        <f>D23/2</f>
-        <v>38.075000000000003</v>
+        <v>38.08</v>
       </c>
       <c r="D23" s="72">
         <v>76.150000000000006</v>
@@ -11257,8 +11519,8 @@
         <v>72.680000000000007</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="205" t="s">
+    <row r="24" spans="1:8">
+      <c r="A24" s="203" t="s">
         <v>582</v>
       </c>
       <c r="B24" s="71" t="s">
@@ -11282,8 +11544,8 @@
         <v>900.44</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="210" t="s">
+    <row r="25" spans="1:8">
+      <c r="A25" s="206" t="s">
         <v>603</v>
       </c>
       <c r="B25" s="71"/>
@@ -11299,150 +11561,560 @@
         <v>307.5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15">
-      <c r="A26" s="211" t="s">
+    <row r="26" spans="1:8" ht="15">
+      <c r="A26" s="207" t="s">
         <v>596</v>
       </c>
       <c r="B26" s="71"/>
-      <c r="C26" s="212"/>
-      <c r="D26" s="212">
+      <c r="C26" s="208"/>
+      <c r="D26" s="208">
         <v>9011.99</v>
       </c>
       <c r="E26" s="71"/>
-      <c r="F26" s="212"/>
-      <c r="G26" s="212">
+      <c r="F26" s="208"/>
+      <c r="G26" s="208">
         <v>9706</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="201" t="s">
+    <row r="27" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A27" s="239"/>
+      <c r="B27" s="205"/>
+      <c r="C27" s="232"/>
+      <c r="D27" s="232"/>
+      <c r="E27" s="205"/>
+      <c r="F27" s="232"/>
+      <c r="G27" s="232">
+        <f>G26-F24</f>
+        <v>9255.7800000000007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" s="257" t="s">
+        <v>719</v>
+      </c>
+      <c r="B28" s="246"/>
+      <c r="C28" s="247"/>
+      <c r="D28" s="247"/>
+      <c r="E28" s="246"/>
+      <c r="F28" s="247"/>
+      <c r="G28" s="247"/>
+    </row>
+    <row r="29" spans="1:8" ht="25.5">
+      <c r="A29" s="248" t="s">
         <v>587</v>
       </c>
-      <c r="B27" s="71"/>
-      <c r="C27" s="72"/>
-      <c r="D27" s="72"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="72">
-        <f>G26-F24-G25</f>
-        <v>8948.2800000000007</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="201" t="s">
+      <c r="B29" s="240"/>
+      <c r="C29" s="241"/>
+      <c r="D29" s="241"/>
+      <c r="E29" s="242" t="s">
+        <v>687</v>
+      </c>
+      <c r="F29" s="241"/>
+      <c r="G29" s="241"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" s="248" t="s">
         <v>585</v>
       </c>
-      <c r="B28" s="71"/>
-      <c r="C28" s="72"/>
-      <c r="D28" s="72"/>
-      <c r="E28" s="71"/>
-      <c r="F28" s="72"/>
-      <c r="G28" s="72"/>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="201" t="s">
+      <c r="B30" s="240"/>
+      <c r="C30" s="241"/>
+      <c r="D30" s="241"/>
+      <c r="E30" s="240"/>
+      <c r="F30" s="241"/>
+      <c r="G30" s="241"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" s="248" t="s">
         <v>586</v>
       </c>
-      <c r="B29" s="71"/>
-      <c r="C29" s="72"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="71"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="72"/>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="201" t="s">
+      <c r="B31" s="240"/>
+      <c r="C31" s="241"/>
+      <c r="D31" s="241"/>
+      <c r="E31" s="240" t="s">
+        <v>694</v>
+      </c>
+      <c r="F31" s="241"/>
+      <c r="G31" s="241"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="248" t="s">
         <v>588</v>
       </c>
-      <c r="B30" s="71"/>
-      <c r="C30" s="72"/>
-      <c r="D30" s="72"/>
-      <c r="E30" s="71"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="72"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="202" t="s">
+      <c r="B32" s="240"/>
+      <c r="C32" s="241"/>
+      <c r="D32" s="241"/>
+      <c r="E32" s="240"/>
+      <c r="F32" s="241"/>
+      <c r="G32" s="241"/>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="249" t="s">
         <v>589</v>
       </c>
-      <c r="B31" s="71"/>
-      <c r="C31" s="72"/>
-      <c r="D31" s="72"/>
-      <c r="E31" s="71"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="72"/>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="202" t="s">
+      <c r="B33" s="240"/>
+      <c r="C33" s="241"/>
+      <c r="D33" s="241"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="241"/>
+      <c r="G33" s="241"/>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="249" t="s">
         <v>590</v>
       </c>
-      <c r="B32" s="71"/>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
-      <c r="E32" s="71"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="72"/>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="202" t="s">
+      <c r="B34" s="240"/>
+      <c r="C34" s="241"/>
+      <c r="D34" s="241"/>
+      <c r="E34" s="240"/>
+      <c r="F34" s="241"/>
+      <c r="G34" s="241"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="249" t="s">
         <v>591</v>
       </c>
-      <c r="B33" s="71"/>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
-      <c r="E33" s="71"/>
-      <c r="F33" s="72"/>
-      <c r="G33" s="72"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="202" t="s">
+      <c r="B35" s="240"/>
+      <c r="C35" s="241"/>
+      <c r="D35" s="241"/>
+      <c r="E35" s="240"/>
+      <c r="F35" s="241"/>
+      <c r="G35" s="241"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="249" t="s">
         <v>592</v>
       </c>
-      <c r="B34" s="71"/>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="72"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="202" t="s">
+      <c r="B36" s="240"/>
+      <c r="C36" s="241"/>
+      <c r="D36" s="241"/>
+      <c r="E36" s="240" t="s">
+        <v>686</v>
+      </c>
+      <c r="F36" s="241"/>
+      <c r="G36" s="241"/>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="249" t="s">
         <v>593</v>
       </c>
-      <c r="B35" s="71"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="72"/>
-      <c r="G35" s="72"/>
-    </row>
-    <row r="36" spans="1:7">
-      <c r="A36" s="202" t="s">
+      <c r="B37" s="240"/>
+      <c r="C37" s="241"/>
+      <c r="D37" s="241"/>
+      <c r="E37" s="243" t="s">
+        <v>690</v>
+      </c>
+      <c r="F37" s="241"/>
+      <c r="G37" s="241"/>
+    </row>
+    <row r="38" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A38" s="249" t="s">
         <v>594</v>
       </c>
-      <c r="B36" s="208"/>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
-      <c r="E36" s="71"/>
-      <c r="F36" s="72"/>
-      <c r="G36" s="72"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A37" s="206" t="s">
+      <c r="B38" s="243"/>
+      <c r="C38" s="241"/>
+      <c r="D38" s="241"/>
+      <c r="E38" s="240"/>
+      <c r="F38" s="241"/>
+      <c r="G38" s="241"/>
+    </row>
+    <row r="39" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A39" s="250"/>
+      <c r="B39" s="243"/>
+      <c r="C39" s="244"/>
+      <c r="D39" s="244"/>
+      <c r="E39" s="245" t="s">
+        <v>705</v>
+      </c>
+      <c r="F39" s="244"/>
+      <c r="G39" s="244"/>
+    </row>
+    <row r="40" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A40" s="250"/>
+      <c r="B40" s="243"/>
+      <c r="C40" s="244"/>
+      <c r="D40" s="244"/>
+      <c r="E40" s="243" t="s">
+        <v>695</v>
+      </c>
+      <c r="F40" s="244"/>
+      <c r="G40" s="244"/>
+    </row>
+    <row r="41" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A41" s="250"/>
+      <c r="B41" s="243"/>
+      <c r="C41" s="244"/>
+      <c r="D41" s="244"/>
+      <c r="E41" s="245" t="s">
+        <v>693</v>
+      </c>
+      <c r="F41" s="244"/>
+      <c r="G41" s="244"/>
+    </row>
+    <row r="42" spans="1:7" ht="11.25" customHeight="1">
+      <c r="A42" s="250"/>
+      <c r="B42" s="243"/>
+      <c r="C42" s="244"/>
+      <c r="D42" s="244"/>
+      <c r="E42" s="243" t="s">
+        <v>692</v>
+      </c>
+      <c r="F42" s="244"/>
+      <c r="G42" s="244"/>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" s="250"/>
+      <c r="B43" s="243"/>
+      <c r="C43" s="244"/>
+      <c r="D43" s="244"/>
+      <c r="E43" s="243" t="s">
+        <v>689</v>
+      </c>
+      <c r="F43" s="244"/>
+      <c r="G43" s="244"/>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" s="250"/>
+      <c r="B44" s="243"/>
+      <c r="C44" s="244"/>
+      <c r="D44" s="244"/>
+      <c r="E44" s="243" t="s">
+        <v>688</v>
+      </c>
+      <c r="F44" s="244"/>
+      <c r="G44" s="244"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="250"/>
+      <c r="B45" s="243"/>
+      <c r="C45" s="244"/>
+      <c r="D45" s="244"/>
+      <c r="E45" s="243" t="s">
+        <v>685</v>
+      </c>
+      <c r="F45" s="244"/>
+      <c r="G45" s="244"/>
+    </row>
+    <row r="46" spans="1:7">
+      <c r="A46" s="250"/>
+      <c r="B46" s="243"/>
+      <c r="C46" s="244"/>
+      <c r="D46" s="244"/>
+      <c r="F46" s="244"/>
+      <c r="G46" s="244"/>
+    </row>
+    <row r="47" spans="1:7">
+      <c r="A47" s="250"/>
+      <c r="B47" s="243"/>
+      <c r="C47" s="244"/>
+      <c r="D47" s="244"/>
+      <c r="E47" s="243" t="s">
+        <v>691</v>
+      </c>
+      <c r="F47" s="244"/>
+      <c r="G47" s="244"/>
+    </row>
+    <row r="48" spans="1:7">
+      <c r="A48" s="250"/>
+      <c r="B48" s="243"/>
+      <c r="C48" s="244"/>
+      <c r="D48" s="244"/>
+      <c r="E48" s="243" t="s">
+        <v>684</v>
+      </c>
+      <c r="F48" s="244"/>
+      <c r="G48" s="244"/>
+    </row>
+    <row r="49" spans="1:7" ht="15" thickBot="1">
+      <c r="A49" s="251" t="s">
         <v>595</v>
       </c>
-      <c r="B37" s="209"/>
-      <c r="C37" s="120"/>
-      <c r="D37" s="120">
+      <c r="B49" s="252"/>
+      <c r="C49" s="253"/>
+      <c r="D49" s="253">
         <v>2029</v>
       </c>
-      <c r="E37" s="73"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-    </row>
-    <row r="38" spans="1:7">
-      <c r="A38" s="222" t="s">
-        <v>610</v>
+      <c r="E49" s="254"/>
+      <c r="F49" s="255"/>
+      <c r="G49" s="253">
+        <v>2793</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="234" t="s">
+        <v>706</v>
+      </c>
+      <c r="B50" s="69"/>
+      <c r="C50" s="69"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="235"/>
+      <c r="F50" s="69"/>
+      <c r="G50" s="70"/>
+    </row>
+    <row r="51" spans="1:7" ht="15">
+      <c r="A51" s="237" t="s">
+        <v>717</v>
+      </c>
+      <c r="B51" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" s="91" t="s">
+        <v>718</v>
+      </c>
+      <c r="D51" s="72"/>
+      <c r="E51" s="238" t="s">
+        <v>717</v>
+      </c>
+      <c r="F51" s="91" t="s">
+        <v>193</v>
+      </c>
+      <c r="G51" s="208" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="71" t="s">
+        <v>707</v>
+      </c>
+      <c r="B52" s="66">
+        <v>7</v>
+      </c>
+      <c r="C52" s="66">
+        <v>123.66</v>
+      </c>
+      <c r="D52" s="72"/>
+      <c r="E52" s="183" t="s">
+        <v>696</v>
+      </c>
+      <c r="F52" s="66">
+        <v>3</v>
+      </c>
+      <c r="G52" s="233">
+        <v>85.61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="71" t="s">
+        <v>710</v>
+      </c>
+      <c r="B53" s="66">
+        <v>42</v>
+      </c>
+      <c r="C53" s="66">
+        <v>8.16</v>
+      </c>
+      <c r="D53" s="72"/>
+      <c r="E53" s="183" t="s">
+        <v>697</v>
+      </c>
+      <c r="F53" s="66">
+        <v>34</v>
+      </c>
+      <c r="G53" s="72">
+        <v>6.64</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="71" t="s">
+        <v>709</v>
+      </c>
+      <c r="B54" s="66">
+        <v>6</v>
+      </c>
+      <c r="C54" s="66">
+        <v>3.47</v>
+      </c>
+      <c r="D54" s="72"/>
+      <c r="E54" s="183" t="s">
+        <v>698</v>
+      </c>
+      <c r="F54" s="66">
+        <v>6</v>
+      </c>
+      <c r="G54" s="72">
+        <v>3.15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="71" t="s">
+        <v>711</v>
+      </c>
+      <c r="B55" s="66">
+        <v>5</v>
+      </c>
+      <c r="C55" s="66">
+        <v>133.66</v>
+      </c>
+      <c r="D55" s="72"/>
+      <c r="E55" s="183" t="s">
+        <v>699</v>
+      </c>
+      <c r="F55" s="66">
+        <v>3</v>
+      </c>
+      <c r="G55" s="72">
+        <v>39.36</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="71"/>
+      <c r="B56" s="66"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="72"/>
+      <c r="E56" s="183" t="s">
+        <v>700</v>
+      </c>
+      <c r="F56" s="66">
+        <v>6</v>
+      </c>
+      <c r="G56" s="72">
+        <v>59.04</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="71" t="s">
+        <v>712</v>
+      </c>
+      <c r="B57" s="66">
+        <v>4</v>
+      </c>
+      <c r="C57" s="66">
+        <v>20.58</v>
+      </c>
+      <c r="D57" s="72"/>
+      <c r="E57" s="183" t="s">
+        <v>701</v>
+      </c>
+      <c r="F57" s="66">
+        <v>3</v>
+      </c>
+      <c r="G57" s="72">
+        <v>8.36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="71" t="s">
+        <v>714</v>
+      </c>
+      <c r="B58" s="66">
+        <v>8</v>
+      </c>
+      <c r="C58" s="66">
+        <v>20.420000000000002</v>
+      </c>
+      <c r="D58" s="72"/>
+      <c r="E58" s="183" t="s">
+        <v>702</v>
+      </c>
+      <c r="F58" s="66">
+        <v>6</v>
+      </c>
+      <c r="G58" s="72">
+        <v>22.63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="71" t="s">
+        <v>716</v>
+      </c>
+      <c r="B59" s="66">
+        <v>12</v>
+      </c>
+      <c r="C59" s="66">
+        <v>9.19</v>
+      </c>
+      <c r="D59" s="72"/>
+      <c r="E59" s="183" t="s">
+        <v>703</v>
+      </c>
+      <c r="F59" s="66">
+        <v>12</v>
+      </c>
+      <c r="G59" s="72">
+        <v>6.89</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="71" t="s">
+        <v>715</v>
+      </c>
+      <c r="B60" s="66">
+        <v>12</v>
+      </c>
+      <c r="C60" s="66">
+        <v>13.3</v>
+      </c>
+      <c r="D60" s="72"/>
+      <c r="E60" s="183" t="s">
+        <v>704</v>
+      </c>
+      <c r="F60" s="66">
+        <v>12</v>
+      </c>
+      <c r="G60" s="72">
+        <v>1.78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15">
+      <c r="A61" s="71" t="s">
+        <v>708</v>
+      </c>
+      <c r="B61" s="66">
+        <v>4</v>
+      </c>
+      <c r="C61" s="66">
+        <v>44.03</v>
+      </c>
+      <c r="D61" s="72"/>
+      <c r="E61" s="183"/>
+      <c r="F61" s="66"/>
+      <c r="G61" s="208">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="71" t="s">
+        <v>713</v>
+      </c>
+      <c r="B62" s="66">
+        <v>1</v>
+      </c>
+      <c r="C62" s="66">
+        <v>42.12</v>
+      </c>
+      <c r="D62" s="72"/>
+      <c r="E62" s="183"/>
+      <c r="F62" s="66"/>
+      <c r="G62" s="72"/>
+    </row>
+    <row r="63" spans="1:7">
+      <c r="D63" s="72"/>
+      <c r="E63" s="183"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="72"/>
+    </row>
+    <row r="64" spans="1:7" ht="15">
+      <c r="A64" s="71"/>
+      <c r="B64" s="66"/>
+      <c r="C64" s="91">
+        <v>2631</v>
+      </c>
+      <c r="D64" s="72"/>
+      <c r="E64" s="183"/>
+      <c r="F64" s="66"/>
+      <c r="G64" s="72"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" thickBot="1">
+      <c r="A65" s="73"/>
+      <c r="B65" s="74"/>
+      <c r="C65" s="74"/>
+      <c r="D65" s="75"/>
+      <c r="E65" s="236"/>
+      <c r="F65" s="74"/>
+      <c r="G65" s="75"/>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="C67">
+        <v>23000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update s13, update zestawienia palet
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -21,15 +21,16 @@
     <sheet name="11_Sprint" sheetId="19" r:id="rId12"/>
     <sheet name="12_Sprint" sheetId="20" r:id="rId13"/>
     <sheet name="13_Sprint" sheetId="23" r:id="rId14"/>
-    <sheet name="Zwrot VAT" sheetId="22" r:id="rId15"/>
-    <sheet name="Palety" sheetId="21" r:id="rId16"/>
-    <sheet name="Brama garazowa" sheetId="16" r:id="rId17"/>
-    <sheet name="Dachówki i okna" sheetId="14" r:id="rId18"/>
-    <sheet name="Strop" sheetId="11" r:id="rId19"/>
-    <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId20"/>
-    <sheet name="Piasek i stal" sheetId="7" r:id="rId21"/>
-    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId22"/>
-    <sheet name="Nadproża" sheetId="12" r:id="rId23"/>
+    <sheet name="Drenaż ceny" sheetId="24" r:id="rId15"/>
+    <sheet name="Zwrot VAT" sheetId="22" r:id="rId16"/>
+    <sheet name="Palety" sheetId="21" r:id="rId17"/>
+    <sheet name="Brama garazowa" sheetId="16" r:id="rId18"/>
+    <sheet name="Dachówki i okna" sheetId="14" r:id="rId19"/>
+    <sheet name="Strop" sheetId="11" r:id="rId20"/>
+    <sheet name="Bloczki silikatowe" sheetId="10" r:id="rId21"/>
+    <sheet name="Piasek i stal" sheetId="7" r:id="rId22"/>
+    <sheet name="Warunki uruchomienia" sheetId="8" r:id="rId23"/>
+    <sheet name="Nadproża" sheetId="12" r:id="rId24"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'11_Sprint'!$F$3:$F$5</definedName>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1493" uniqueCount="848">
   <si>
     <t>Id</t>
   </si>
@@ -2534,6 +2535,132 @@
   </si>
   <si>
     <t>Zakres</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>http://forum.muratordom.pl/showthread.php?159421-drenaz-opaskowy-150zl-mb-material</t>
+  </si>
+  <si>
+    <t>Rok</t>
+  </si>
+  <si>
+    <t>150zł/mb</t>
+  </si>
+  <si>
+    <t>drenaż, kanalizacja deszczowa, styropian</t>
+  </si>
+  <si>
+    <t>Gdzie</t>
+  </si>
+  <si>
+    <t>Śląsk</t>
+  </si>
+  <si>
+    <t>120zł/mb</t>
+  </si>
+  <si>
+    <t>Warszawa</t>
+  </si>
+  <si>
+    <t>95zł/mb</t>
+  </si>
+  <si>
+    <t>70zł/mb</t>
+  </si>
+  <si>
+    <t>33-116/mb</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>chyba TAK</t>
+  </si>
+  <si>
+    <t>http://oferia.pl/zlecenie/item525576-wykonanie-drenazu-opaskowego-ok-60mb-grunt-gliniasty-bud-bez-piwnic</t>
+  </si>
+  <si>
+    <t>drenaż razem ze studzienkami</t>
+  </si>
+  <si>
+    <t>85zł/mb</t>
+  </si>
+  <si>
+    <t>100zł/mb</t>
+  </si>
+  <si>
+    <t>92zł/mb</t>
+  </si>
+  <si>
+    <t>133zł/mb</t>
+  </si>
+  <si>
+    <t>116zł.mb</t>
+  </si>
+  <si>
+    <t>Zlecę wykonanie drenażu opaskowego ok.60mb</t>
+  </si>
+  <si>
+    <t>http://www.szukajfachowca.pl/zlecenia/budowlane/inne/drenaz-opaskowy-4795-3</t>
+  </si>
+  <si>
+    <t>Zlecę wykonanie kompletnego drenażu opaskowego - ok. 50 mb - wraz z wykonaniem studni chłonnej.</t>
+  </si>
+  <si>
+    <t>90zł/mb</t>
+  </si>
+  <si>
+    <t>Jastrzębie</t>
+  </si>
+  <si>
+    <t>130zł/mb</t>
+  </si>
+  <si>
+    <t>Panowie cena 130zł za drenaż opaskowy ( z całym materiałem czyli żwir, rura drenarska, geowłóknina, 1 studzienka rewizyjna, i 1 zbiorcza, koparka ) to nie jest za dużo tak żeby nie przestraszyć inwestora.</t>
+  </si>
+  <si>
+    <t>http://www.kopaczka.pl/viewtopic.php?f=6&amp;t=9406&amp;start=380</t>
+  </si>
+  <si>
+    <t>http://polskabudowlana.pl/ogloszenie_1822_drenaz_opaskowy_domu_oraz_osuszanie_dzialki_i_terenow.html</t>
+  </si>
+  <si>
+    <t>Pomorskie</t>
+  </si>
+  <si>
+    <t>75zł/mb</t>
+  </si>
+  <si>
+    <t>25zł/mb</t>
+  </si>
+  <si>
+    <t>Legnica</t>
+  </si>
+  <si>
+    <t>http://www.forum-brukarskie.pl/topics95/1745.htm</t>
+  </si>
+  <si>
+    <t>35zł/mb</t>
+  </si>
+  <si>
+    <t>odwodnienie (?)</t>
+  </si>
+  <si>
+    <t>położenie rury</t>
+  </si>
+  <si>
+    <t>6922/10/2013</t>
+  </si>
+  <si>
+    <t>betard</t>
+  </si>
+  <si>
+    <t>Sprawdzić termin i szczegóły realizacji producenta bramy</t>
+  </si>
+  <si>
+    <t>Umówić na pomiar bramy</t>
   </si>
 </sst>
 </file>
@@ -2544,7 +2671,7 @@
     <numFmt numFmtId="6" formatCode="#,##0\ &quot;zł&quot;;[Red]\-#,##0\ &quot;zł&quot;"/>
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;zł&quot;;[Red]\-#,##0.00\ &quot;zł&quot;"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="39">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2814,6 +2941,14 @@
     <font>
       <sz val="10"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Czcionka tekstu podstawowego"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="10">
@@ -3490,10 +3625,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="276">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3988,38 +4127,60 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="157">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -4032,33 +4193,19 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <bottom style="thin">
-          <color theme="7" tint="0.39997558519241921"/>
+          <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -4094,6 +4241,43 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -4206,27 +4390,14 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+      <border outline="0">
         <top style="thin">
           <color indexed="64"/>
         </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -4239,44 +4410,14 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
-          <color indexed="64"/>
+          <color theme="7" tint="0.39997558519241921"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -8060,7 +8201,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071740166"/>
+          <c:w val="0.71441426071740144"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -8340,24 +8481,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63068032"/>
-        <c:axId val="63069568"/>
+        <c:axId val="65600128"/>
+        <c:axId val="69210496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63068032"/>
+        <c:axId val="65600128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63069568"/>
+        <c:crossAx val="69210496"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63069568"/>
+        <c:axId val="69210496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -8367,7 +8508,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63068032"/>
+        <c:crossAx val="65600128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8378,8 +8519,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325289174"/>
-          <c:y val="0.29353966170895784"/>
+          <c:x val="0.86438523325289196"/>
+          <c:y val="0.29353966170895796"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -8389,7 +8530,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000888" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000888" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000091" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000091" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8601,24 +8742,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62906752"/>
-        <c:axId val="62908288"/>
+        <c:axId val="69235840"/>
+        <c:axId val="69237376"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="62906752"/>
+        <c:axId val="69235840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62908288"/>
+        <c:crossAx val="69237376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="62908288"/>
+        <c:axId val="69237376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -8628,7 +8769,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62906752"/>
+        <c:crossAx val="69235840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8640,7 +8781,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000677" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000677" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8803,24 +8944,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64031360"/>
-        <c:axId val="64057728"/>
+        <c:axId val="69336448"/>
+        <c:axId val="69543040"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64031360"/>
+        <c:axId val="69336448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64057728"/>
+        <c:crossAx val="69543040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64057728"/>
+        <c:axId val="69543040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -8830,7 +8971,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64031360"/>
+        <c:crossAx val="69336448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8842,7 +8983,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000699" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000699" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000722" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000722" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8957,11 +9098,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64118784"/>
-        <c:axId val="64120320"/>
+        <c:axId val="69620480"/>
+        <c:axId val="69622016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64118784"/>
+        <c:axId val="69620480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8969,13 +9110,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64120320"/>
+        <c:crossAx val="69622016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64120320"/>
+        <c:axId val="69622016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8983,7 +9124,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64118784"/>
+        <c:crossAx val="69620480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8995,7 +9136,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000555" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000555" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9011,10 +9152,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961777"/>
-          <c:y val="3.2882035578886373E-2"/>
+          <c:x val="0.17181562830961772"/>
+          <c:y val="3.2882035578886401E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640420578"/>
+          <c:h val="0.63861876640420601"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -9177,11 +9318,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64206720"/>
-        <c:axId val="64208256"/>
+        <c:axId val="69683840"/>
+        <c:axId val="69702016"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64206720"/>
+        <c:axId val="69683840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9189,13 +9330,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64208256"/>
+        <c:crossAx val="69702016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64208256"/>
+        <c:axId val="69702016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -9204,7 +9345,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64206720"/>
+        <c:crossAx val="69683840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9216,7 +9357,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000577" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000577" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000006" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000006" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -9467,16 +9608,16 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabela151718" displayName="Tabela151718" ref="B4:F27" totalsRowShown="0" headerRowBorderDxfId="2" tableBorderDxfId="3" totalsRowBorderDxfId="1">
-  <autoFilter ref="B4:F27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="17" name="Tabela151718" displayName="Tabela151718" ref="B4:F29" totalsRowShown="0" headerRowBorderDxfId="14" tableBorderDxfId="13" totalsRowBorderDxfId="12">
+  <autoFilter ref="B4:F29">
     <filterColumn colId="3"/>
   </autoFilter>
   <tableColumns count="5">
-    <tableColumn id="1" name="Lp" dataDxfId="7"/>
-    <tableColumn id="2" name="Status" dataDxfId="6"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="5"/>
-    <tableColumn id="5" name="Zakres" dataDxfId="0"/>
-    <tableColumn id="4" name="Zadanie" dataDxfId="4"/>
+    <tableColumn id="1" name="Lp" dataDxfId="11"/>
+    <tableColumn id="2" name="Status" dataDxfId="10"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="9"/>
+    <tableColumn id="5" name="Zakres" dataDxfId="8"/>
+    <tableColumn id="4" name="Zadanie" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9489,7 +9630,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="Kolumna1"/>
-    <tableColumn id="10" name="Kolumna2" dataDxfId="14"/>
+    <tableColumn id="10" name="Kolumna2" dataDxfId="6"/>
     <tableColumn id="3" name="Kolumna3"/>
     <tableColumn id="12" name="Kolumna4"/>
     <tableColumn id="4" name="Kolumna5"/>
@@ -9513,7 +9654,7 @@
     <tableColumn id="1" name="Firma"/>
     <tableColumn id="2" name="Kontakt"/>
     <tableColumn id="11" name="szt"/>
-    <tableColumn id="10" name="Cena bloczka" dataDxfId="13"/>
+    <tableColumn id="10" name="Cena bloczka" dataDxfId="5"/>
     <tableColumn id="3" name="Cena bloczków 200m2"/>
     <tableColumn id="12" name="Klej25kg"/>
     <tableColumn id="4" name="Cena kleju"/>
@@ -9526,12 +9667,12 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="B129:D146" totalsRowShown="0" dataDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="B129:D146"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Temat" dataDxfId="10"/>
-    <tableColumn id="2" name="Pytanie" dataDxfId="9"/>
-    <tableColumn id="3" name="Ustalenie" dataDxfId="8"/>
+    <tableColumn id="1" name="Temat" dataDxfId="2"/>
+    <tableColumn id="2" name="Pytanie" dataDxfId="1"/>
+    <tableColumn id="3" name="Ustalenie" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium19" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11792,10 +11933,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:F27"/>
+  <dimension ref="B4:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -11830,8 +11971,12 @@
     </row>
     <row r="6" spans="2:6">
       <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="44"/>
+      <c r="C6" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="E6" s="45"/>
       <c r="F6" s="160" t="s">
         <v>743</v>
@@ -11884,7 +12029,9 @@
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="C12" s="42" t="s">
+        <v>71</v>
+      </c>
       <c r="D12" s="44"/>
       <c r="E12" s="44"/>
       <c r="F12" s="160" t="s">
@@ -11893,8 +12040,12 @@
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="44"/>
+      <c r="C13" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="44" t="s">
+        <v>73</v>
+      </c>
       <c r="E13" s="44"/>
       <c r="F13" s="160" t="s">
         <v>797</v>
@@ -11909,8 +12060,12 @@
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="E15" s="44" t="s">
         <v>619</v>
       </c>
@@ -11929,8 +12084,12 @@
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="268"/>
-      <c r="C17" s="268"/>
-      <c r="D17" s="269"/>
+      <c r="C17" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>72</v>
+      </c>
       <c r="E17" s="269"/>
       <c r="F17" s="270" t="s">
         <v>793</v>
@@ -11945,8 +12104,12 @@
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="44" t="s">
+        <v>73</v>
+      </c>
       <c r="E19" s="44" t="s">
         <v>790</v>
       </c>
@@ -11972,8 +12135,12 @@
     </row>
     <row r="22" spans="2:6">
       <c r="B22" s="268"/>
-      <c r="C22" s="268"/>
-      <c r="D22" s="269"/>
+      <c r="C22" s="268" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="269" t="s">
+        <v>72</v>
+      </c>
       <c r="E22" s="269" t="s">
         <v>233</v>
       </c>
@@ -11983,8 +12150,12 @@
     </row>
     <row r="23" spans="2:6">
       <c r="B23" s="268"/>
-      <c r="C23" s="268"/>
-      <c r="D23" s="269"/>
+      <c r="C23" s="268" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="269" t="s">
+        <v>73</v>
+      </c>
       <c r="E23" s="269"/>
       <c r="F23" s="270" t="s">
         <v>799</v>
@@ -12001,28 +12172,50 @@
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="268"/>
-      <c r="C25" s="268"/>
-      <c r="D25" s="269"/>
+      <c r="C25" s="268" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="269" t="s">
+        <v>73</v>
+      </c>
       <c r="E25" s="275"/>
-      <c r="F25" s="270"/>
+      <c r="F25" s="270" t="s">
+        <v>846</v>
+      </c>
     </row>
     <row r="26" spans="2:6">
-      <c r="B26" s="49"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46" t="s">
+      <c r="B26" s="268"/>
+      <c r="C26" s="268"/>
+      <c r="D26" s="269"/>
+      <c r="E26" s="275"/>
+      <c r="F26" s="270" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6">
+      <c r="B27" s="268"/>
+      <c r="C27" s="268"/>
+      <c r="D27" s="269"/>
+      <c r="E27" s="275"/>
+      <c r="F27" s="270"/>
+    </row>
+    <row r="28" spans="2:6">
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46" t="s">
         <v>803</v>
       </c>
-      <c r="F26" s="262" t="s">
+      <c r="F28" s="262" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
-      <c r="B27" s="271"/>
-      <c r="C27" s="271"/>
-      <c r="D27" s="272"/>
-      <c r="E27" s="272"/>
-      <c r="F27" s="273"/>
+    <row r="29" spans="2:6">
+      <c r="B29" s="271"/>
+      <c r="C29" s="271"/>
+      <c r="D29" s="272"/>
+      <c r="E29" s="272"/>
+      <c r="F29" s="273"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12033,6 +12226,483 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A3:F25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>573</v>
+      </c>
+      <c r="B3" t="s">
+        <v>805</v>
+      </c>
+      <c r="C3" t="s">
+        <v>717</v>
+      </c>
+      <c r="D3" t="s">
+        <v>811</v>
+      </c>
+      <c r="E3" t="s">
+        <v>808</v>
+      </c>
+      <c r="F3" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>809</v>
+      </c>
+      <c r="B4" t="s">
+        <v>810</v>
+      </c>
+      <c r="C4" t="s">
+        <v>514</v>
+      </c>
+      <c r="D4" t="s">
+        <v>818</v>
+      </c>
+      <c r="E4">
+        <v>2010</v>
+      </c>
+      <c r="F4" s="276" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>809</v>
+      </c>
+      <c r="C5" t="s">
+        <v>506</v>
+      </c>
+      <c r="D5" t="s">
+        <v>818</v>
+      </c>
+      <c r="E5">
+        <v>2010</v>
+      </c>
+      <c r="F5" s="276" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>813</v>
+      </c>
+      <c r="C6" t="s">
+        <v>514</v>
+      </c>
+      <c r="D6" t="s">
+        <v>812</v>
+      </c>
+      <c r="E6">
+        <v>2010</v>
+      </c>
+      <c r="F6" s="276" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>815</v>
+      </c>
+      <c r="C7" t="s">
+        <v>514</v>
+      </c>
+      <c r="D7" t="s">
+        <v>814</v>
+      </c>
+      <c r="E7">
+        <v>2010</v>
+      </c>
+      <c r="F7" s="276" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>816</v>
+      </c>
+      <c r="C8" t="s">
+        <v>514</v>
+      </c>
+      <c r="D8" t="s">
+        <v>818</v>
+      </c>
+      <c r="E8">
+        <v>2010</v>
+      </c>
+      <c r="F8" s="276" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>817</v>
+      </c>
+      <c r="B9" t="s">
+        <v>827</v>
+      </c>
+      <c r="C9" t="s">
+        <v>818</v>
+      </c>
+      <c r="D9" t="s">
+        <v>812</v>
+      </c>
+      <c r="E9">
+        <v>2013</v>
+      </c>
+      <c r="F9" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>822</v>
+      </c>
+      <c r="B10" t="s">
+        <v>821</v>
+      </c>
+      <c r="C10" t="s">
+        <v>819</v>
+      </c>
+      <c r="D10" t="s">
+        <v>812</v>
+      </c>
+      <c r="E10">
+        <v>2013</v>
+      </c>
+      <c r="F10" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>823</v>
+      </c>
+      <c r="B11" t="s">
+        <v>827</v>
+      </c>
+      <c r="C11" t="s">
+        <v>818</v>
+      </c>
+      <c r="D11" t="s">
+        <v>812</v>
+      </c>
+      <c r="E11">
+        <v>2013</v>
+      </c>
+      <c r="F11" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>823</v>
+      </c>
+      <c r="B12" t="s">
+        <v>827</v>
+      </c>
+      <c r="C12" t="s">
+        <v>514</v>
+      </c>
+      <c r="D12" t="s">
+        <v>812</v>
+      </c>
+      <c r="E12">
+        <v>2013</v>
+      </c>
+      <c r="F12" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>824</v>
+      </c>
+      <c r="B13" t="s">
+        <v>827</v>
+      </c>
+      <c r="C13" t="s">
+        <v>506</v>
+      </c>
+      <c r="D13" t="s">
+        <v>812</v>
+      </c>
+      <c r="E13">
+        <v>2013</v>
+      </c>
+      <c r="F13" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>825</v>
+      </c>
+      <c r="B14" t="s">
+        <v>827</v>
+      </c>
+      <c r="C14" t="s">
+        <v>819</v>
+      </c>
+      <c r="D14" t="s">
+        <v>812</v>
+      </c>
+      <c r="E14">
+        <v>2013</v>
+      </c>
+      <c r="F14" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>826</v>
+      </c>
+      <c r="B15" t="s">
+        <v>827</v>
+      </c>
+      <c r="C15" t="s">
+        <v>818</v>
+      </c>
+      <c r="D15" t="s">
+        <v>812</v>
+      </c>
+      <c r="E15">
+        <v>2013</v>
+      </c>
+      <c r="F15" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>823</v>
+      </c>
+      <c r="B16" t="s">
+        <v>827</v>
+      </c>
+      <c r="C16" t="s">
+        <v>818</v>
+      </c>
+      <c r="D16" t="s">
+        <v>812</v>
+      </c>
+      <c r="E16">
+        <v>2013</v>
+      </c>
+      <c r="F16" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>825</v>
+      </c>
+      <c r="B17" t="s">
+        <v>827</v>
+      </c>
+      <c r="C17" t="s">
+        <v>818</v>
+      </c>
+      <c r="D17" t="s">
+        <v>812</v>
+      </c>
+      <c r="E17">
+        <v>2013</v>
+      </c>
+      <c r="F17" s="276" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>823</v>
+      </c>
+      <c r="B18" t="s">
+        <v>829</v>
+      </c>
+      <c r="C18" t="s">
+        <v>818</v>
+      </c>
+      <c r="D18" t="s">
+        <v>814</v>
+      </c>
+      <c r="E18">
+        <v>2009</v>
+      </c>
+      <c r="F18" s="276" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>823</v>
+      </c>
+      <c r="B19" t="s">
+        <v>829</v>
+      </c>
+      <c r="C19" t="s">
+        <v>818</v>
+      </c>
+      <c r="D19" t="s">
+        <v>814</v>
+      </c>
+      <c r="E19">
+        <v>2009</v>
+      </c>
+      <c r="F19" s="276" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>830</v>
+      </c>
+      <c r="B20" t="s">
+        <v>829</v>
+      </c>
+      <c r="C20" t="s">
+        <v>818</v>
+      </c>
+      <c r="D20" t="s">
+        <v>814</v>
+      </c>
+      <c r="E20">
+        <v>2009</v>
+      </c>
+      <c r="F20" s="276" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>832</v>
+      </c>
+      <c r="B21" t="s">
+        <v>833</v>
+      </c>
+      <c r="C21" t="s">
+        <v>506</v>
+      </c>
+      <c r="D21" t="s">
+        <v>831</v>
+      </c>
+      <c r="E21">
+        <v>2011</v>
+      </c>
+      <c r="F21" s="276" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>837</v>
+      </c>
+      <c r="C22" t="s">
+        <v>818</v>
+      </c>
+      <c r="D22" t="s">
+        <v>836</v>
+      </c>
+      <c r="E22">
+        <v>2011</v>
+      </c>
+      <c r="F22" s="276" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C23" t="s">
+        <v>514</v>
+      </c>
+      <c r="D23" t="s">
+        <v>839</v>
+      </c>
+      <c r="E23">
+        <v>2012</v>
+      </c>
+      <c r="F23" s="276" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>841</v>
+      </c>
+      <c r="B24" t="s">
+        <v>842</v>
+      </c>
+      <c r="C24" t="s">
+        <v>506</v>
+      </c>
+      <c r="E24">
+        <v>2012</v>
+      </c>
+      <c r="F24" s="276" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>838</v>
+      </c>
+      <c r="B25" t="s">
+        <v>843</v>
+      </c>
+      <c r="E25">
+        <v>2012</v>
+      </c>
+      <c r="F25" s="276" t="s">
+        <v>840</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F4" r:id="rId1"/>
+    <hyperlink ref="F5" r:id="rId2"/>
+    <hyperlink ref="F6" r:id="rId3"/>
+    <hyperlink ref="F7" r:id="rId4"/>
+    <hyperlink ref="F8" r:id="rId5"/>
+    <hyperlink ref="F9" r:id="rId6"/>
+    <hyperlink ref="F10" r:id="rId7"/>
+    <hyperlink ref="F11" r:id="rId8"/>
+    <hyperlink ref="F12" r:id="rId9"/>
+    <hyperlink ref="F13" r:id="rId10"/>
+    <hyperlink ref="F14" r:id="rId11"/>
+    <hyperlink ref="F15" r:id="rId12"/>
+    <hyperlink ref="F16" r:id="rId13"/>
+    <hyperlink ref="F17" r:id="rId14"/>
+    <hyperlink ref="F18" r:id="rId15"/>
+    <hyperlink ref="F19" r:id="rId16"/>
+    <hyperlink ref="F20" r:id="rId17"/>
+    <hyperlink ref="F21" r:id="rId18"/>
+    <hyperlink ref="F22" r:id="rId19"/>
+    <hyperlink ref="F23" r:id="rId20"/>
+    <hyperlink ref="F24" r:id="rId21"/>
+    <hyperlink ref="F25" r:id="rId22"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:G20"/>
   <sheetViews>
@@ -12152,12 +12822,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:H16"/>
+  <dimension ref="B5:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B15" sqref="B15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -12233,7 +12903,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="66">
-        <f t="shared" ref="H7:H14" si="0">G7-E7</f>
+        <f t="shared" ref="H7:H16" si="0">G7-E7</f>
         <v>0</v>
       </c>
     </row>
@@ -12398,35 +13068,79 @@
       </c>
     </row>
     <row r="15" spans="2:8">
-      <c r="E15" t="s">
+      <c r="B15" s="99">
+        <v>41570</v>
+      </c>
+      <c r="C15" s="199" t="s">
+        <v>844</v>
+      </c>
+      <c r="D15" s="199" t="s">
+        <v>753</v>
+      </c>
+      <c r="E15" s="199">
+        <v>18</v>
+      </c>
+      <c r="F15" s="199">
+        <v>487.08</v>
+      </c>
+      <c r="G15" s="66"/>
+      <c r="H15" s="199">
+        <f t="shared" si="0"/>
+        <v>-18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8">
+      <c r="B16" s="99">
+        <v>41570</v>
+      </c>
+      <c r="C16" s="199" t="s">
+        <v>844</v>
+      </c>
+      <c r="D16" s="199" t="s">
+        <v>845</v>
+      </c>
+      <c r="E16" s="199">
+        <v>1</v>
+      </c>
+      <c r="F16" s="199">
+        <v>34.44</v>
+      </c>
+      <c r="G16" s="66"/>
+      <c r="H16" s="199">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8">
+      <c r="E17" t="s">
         <v>765</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G17" t="s">
         <v>766</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H17" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
-      <c r="D16" t="s">
+    <row r="18" spans="4:8">
+      <c r="D18" t="s">
         <v>76</v>
       </c>
-      <c r="E16" s="66">
-        <f>SUM(E6:E14)</f>
-        <v>88</v>
-      </c>
-      <c r="F16" s="66">
-        <f>SUM(F6:F14)</f>
-        <v>2680.17</v>
-      </c>
-      <c r="G16" s="66">
-        <f t="shared" ref="G16:H16" si="1">SUM(G6:G14)</f>
+      <c r="E18" s="66">
+        <f t="shared" ref="E18:G18" si="1">SUM(E6:E16)</f>
+        <v>107</v>
+      </c>
+      <c r="F18" s="66">
+        <f t="shared" si="1"/>
+        <v>3201.69</v>
+      </c>
+      <c r="G18" s="66">
+        <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="H16" s="66">
-        <f t="shared" si="1"/>
-        <v>-51</v>
+      <c r="H18" s="66">
+        <f>SUM(H6:H16)</f>
+        <v>-70</v>
       </c>
     </row>
   </sheetData>
@@ -12434,7 +13148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:H35"/>
   <sheetViews>
@@ -13017,7 +13731,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H67"/>
   <sheetViews>
@@ -14122,104 +14836,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B4:K11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="2:11">
-      <c r="B4" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11">
-      <c r="B6" t="s">
-        <v>363</v>
-      </c>
-      <c r="C6" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" t="s">
-        <v>145</v>
-      </c>
-      <c r="E6" t="s">
-        <v>389</v>
-      </c>
-      <c r="F6" t="s">
-        <v>390</v>
-      </c>
-      <c r="G6" t="s">
-        <v>391</v>
-      </c>
-      <c r="H6" t="s">
-        <v>392</v>
-      </c>
-      <c r="I6" t="s">
-        <v>393</v>
-      </c>
-      <c r="J6" t="s">
-        <v>394</v>
-      </c>
-      <c r="K6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11">
-      <c r="B7" t="s">
-        <v>397</v>
-      </c>
-      <c r="C7" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11">
-      <c r="B8" t="s">
-        <v>399</v>
-      </c>
-      <c r="C8" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11">
-      <c r="B9" t="s">
-        <v>400</v>
-      </c>
-      <c r="C9" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11">
-      <c r="B10" t="s">
-        <v>382</v>
-      </c>
-      <c r="C10" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11">
-      <c r="B11" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" t="s">
-        <v>403</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
 
@@ -14912,6 +15528,104 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B4:K11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="25.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:11">
+      <c r="B4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11">
+      <c r="B6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" t="s">
+        <v>389</v>
+      </c>
+      <c r="F6" t="s">
+        <v>390</v>
+      </c>
+      <c r="G6" t="s">
+        <v>391</v>
+      </c>
+      <c r="H6" t="s">
+        <v>392</v>
+      </c>
+      <c r="I6" t="s">
+        <v>393</v>
+      </c>
+      <c r="J6" t="s">
+        <v>394</v>
+      </c>
+      <c r="K6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11">
+      <c r="B7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C7" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11">
+      <c r="B8" t="s">
+        <v>399</v>
+      </c>
+      <c r="C8" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11">
+      <c r="B9" t="s">
+        <v>400</v>
+      </c>
+      <c r="C9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11">
+      <c r="B10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C10" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11">
+      <c r="B11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C11" t="s">
+        <v>403</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15112,7 +15826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L146"/>
   <sheetViews>
@@ -17149,7 +17863,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:E23"/>
   <sheetViews>
@@ -17361,7 +18075,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:E16"/>
   <sheetViews>

</xml_diff>

<commit_message>
pierwsze wersje backloga 2014
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1743" uniqueCount="789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1784" uniqueCount="825">
   <si>
     <t>Id</t>
   </si>
@@ -2486,6 +2486,114 @@
   </si>
   <si>
     <t>Mieć gdzie prać, suszyć i prasować.</t>
+  </si>
+  <si>
+    <t>Przyłącze gazowe+instalacja gazowa.</t>
+  </si>
+  <si>
+    <t>Zakupić kocioł gazowy.</t>
+  </si>
+  <si>
+    <t>pom gosp</t>
+  </si>
+  <si>
+    <t>garaz</t>
+  </si>
+  <si>
+    <t>pom ogrod</t>
+  </si>
+  <si>
+    <t>wiatrolap</t>
+  </si>
+  <si>
+    <t>przedpokoj</t>
+  </si>
+  <si>
+    <t>salon</t>
+  </si>
+  <si>
+    <t>jadalnia</t>
+  </si>
+  <si>
+    <t>kuchnia</t>
+  </si>
+  <si>
+    <t>spizarnia</t>
+  </si>
+  <si>
+    <t>gabinet</t>
+  </si>
+  <si>
+    <t>lazienka</t>
+  </si>
+  <si>
+    <t>korytarz</t>
+  </si>
+  <si>
+    <t>sypialnie</t>
+  </si>
+  <si>
+    <t>garderoba</t>
+  </si>
+  <si>
+    <t>poddasze</t>
+  </si>
+  <si>
+    <t>kocioł gazowy, rozdzielnia, pralka, suszarka, zelazko, radio, kafelki, zlew</t>
+  </si>
+  <si>
+    <t>kafle, gniazdo siłowe, szafki na narzędzia, wieszaki na rowery</t>
+  </si>
+  <si>
+    <t>kafle, regał</t>
+  </si>
+  <si>
+    <t>szafa, kafle, wieszaki</t>
+  </si>
+  <si>
+    <t>szafy, kalfe(gdzie się kończą?), drzwi</t>
+  </si>
+  <si>
+    <t>tynki wewnętrzne, malowanie, listwy podłogowe, ustawienie mebli do podłogówki</t>
+  </si>
+  <si>
+    <t>gniazdka, kominek, obudowa kominka, dystrybucja powietrza z kominka</t>
+  </si>
+  <si>
+    <t>sprzęta agd, meble, oświetlenie, kafle, centralny odkurzacz(?)</t>
+  </si>
+  <si>
+    <t>kafelki, półki, lampka</t>
+  </si>
+  <si>
+    <t>deski podłogowe</t>
+  </si>
+  <si>
+    <t>kafle, sprzęt</t>
+  </si>
+  <si>
+    <t>kafle</t>
+  </si>
+  <si>
+    <t>kafle, sprzęt, piony wod-kan</t>
+  </si>
+  <si>
+    <t>Systemy szaf w przedpokoju, sypialni, garderobie</t>
+  </si>
+  <si>
+    <t>Żeby móc wygodnie przechowywać fatałaszki</t>
+  </si>
+  <si>
+    <t>Wykończyć poddasze</t>
+  </si>
+  <si>
+    <t>Żeby móc się tam bawić</t>
+  </si>
+  <si>
+    <t>Drewnianą podłogę w gabinecie</t>
+  </si>
+  <si>
+    <t>Żeby spełnić marzenie Słonka</t>
   </si>
 </sst>
 </file>
@@ -4059,6 +4167,14 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4068,20 +4184,144 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="211">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4120,6 +4360,86 @@
         </bottom>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -4154,218 +4474,6 @@
         </right>
         <top/>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -9594,7 +9702,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.13448840769903794"/>
           <c:y val="8.3692403032954207E-2"/>
-          <c:w val="0.71441426071739744"/>
+          <c:w val="0.71441426071739733"/>
           <c:h val="0.49521580635753881"/>
         </c:manualLayout>
       </c:layout>
@@ -9874,24 +9982,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63255296"/>
-        <c:axId val="63256832"/>
+        <c:axId val="63251584"/>
+        <c:axId val="63253120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="63255296"/>
+        <c:axId val="63251584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63256832"/>
+        <c:crossAx val="63253120"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63256832"/>
+        <c:axId val="63253120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="81"/>
@@ -9901,7 +10009,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63255296"/>
+        <c:crossAx val="63251584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9912,8 +10020,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.86438523325289796"/>
-          <c:y val="0.29353966170896018"/>
+          <c:x val="0.86438523325289818"/>
+          <c:y val="0.29353966170896023"/>
           <c:w val="0.11894812645906698"/>
           <c:h val="0.22334823203957854"/>
         </c:manualLayout>
@@ -9923,7 +10031,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.7500000000000131" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000131" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001321" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001321" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10135,24 +10243,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="63208448"/>
-        <c:axId val="63214336"/>
+        <c:axId val="63204736"/>
+        <c:axId val="63218816"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="63208448"/>
+        <c:axId val="63204736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63214336"/>
+        <c:crossAx val="63218816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="63214336"/>
+        <c:axId val="63218816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="60"/>
@@ -10162,7 +10270,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63208448"/>
+        <c:crossAx val="63204736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10174,7 +10282,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001099" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001099" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10337,24 +10445,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64148992"/>
-        <c:axId val="64150528"/>
+        <c:axId val="64153472"/>
+        <c:axId val="64155008"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64148992"/>
+        <c:axId val="64153472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64150528"/>
+        <c:crossAx val="64155008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64150528"/>
+        <c:axId val="64155008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="85"/>
@@ -10364,7 +10472,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64148992"/>
+        <c:crossAx val="64153472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10376,7 +10484,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000001121" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001121" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000001132" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000001132" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10491,11 +10599,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64477824"/>
-        <c:axId val="64491904"/>
+        <c:axId val="64482304"/>
+        <c:axId val="64561920"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64477824"/>
+        <c:axId val="64482304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10503,13 +10611,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64491904"/>
+        <c:crossAx val="64561920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64491904"/>
+        <c:axId val="64561920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10517,7 +10625,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64477824"/>
+        <c:crossAx val="64482304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10529,7 +10637,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000977" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000977" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000988" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000988" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -10545,10 +10653,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.17181562830961666"/>
-          <c:y val="3.2882035578886692E-2"/>
+          <c:x val="0.17181562830961664"/>
+          <c:y val="3.2882035578886699E-2"/>
           <c:w val="0.65643820838184763"/>
-          <c:h val="0.63861876640421045"/>
+          <c:h val="0.63861876640421056"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -10711,11 +10819,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="64574208"/>
-        <c:axId val="64575744"/>
+        <c:axId val="64513152"/>
+        <c:axId val="64514688"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="64574208"/>
+        <c:axId val="64513152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10723,13 +10831,13 @@
         <c:numFmt formatCode="yyyy/mm/dd" sourceLinked="1"/>
         <c:majorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64575744"/>
+        <c:crossAx val="64514688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="64575744"/>
+        <c:axId val="64514688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -10738,7 +10846,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64574208"/>
+        <c:crossAx val="64513152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10750,7 +10858,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000999" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000999" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.7500000000000101" l="0.70000000000000062" r="0.70000000000000062" t="0.7500000000000101" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -11108,15 +11216,15 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tabela20" displayName="Tabela20" ref="A1:F24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="2" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="20" name="Tabela20" displayName="Tabela20" ref="A1:F24" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A1:F24"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Id" dataDxfId="7"/>
-    <tableColumn id="2" name="Priorytet" dataDxfId="0"/>
-    <tableColumn id="3" name="Rozmiar" dataDxfId="6"/>
-    <tableColumn id="4" name="Nr Sprintu" dataDxfId="5"/>
-    <tableColumn id="5" name="Chcę" dataDxfId="4"/>
-    <tableColumn id="6" name="Aby" dataDxfId="3"/>
+    <tableColumn id="1" name="Id" dataDxfId="5"/>
+    <tableColumn id="2" name="Priorytet" dataDxfId="4"/>
+    <tableColumn id="3" name="Rozmiar" dataDxfId="3"/>
+    <tableColumn id="4" name="Nr Sprintu" dataDxfId="2"/>
+    <tableColumn id="5" name="Chcę" dataDxfId="1"/>
+    <tableColumn id="6" name="Aby" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -17099,9 +17207,9 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -17116,22 +17224,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="300" t="s">
+      <c r="A1" s="297" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="301" t="s">
+      <c r="B1" s="298" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="301" t="s">
+      <c r="C1" s="298" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="301" t="s">
+      <c r="D1" s="298" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="302" t="s">
+      <c r="E1" s="299" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="303" t="s">
+      <c r="F1" s="300" t="s">
         <v>4</v>
       </c>
     </row>
@@ -17423,31 +17531,49 @@
       <c r="A20" s="50">
         <v>18</v>
       </c>
-      <c r="B20" s="54"/>
+      <c r="B20" s="54" t="s">
+        <v>7</v>
+      </c>
       <c r="C20" s="54"/>
       <c r="D20" s="54"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="56"/>
+      <c r="E20" s="55" t="s">
+        <v>819</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>820</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="50">
         <v>19</v>
       </c>
-      <c r="B21" s="54"/>
+      <c r="B21" s="54" t="s">
+        <v>7</v>
+      </c>
       <c r="C21" s="54"/>
       <c r="D21" s="54"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
+      <c r="E21" s="55" t="s">
+        <v>821</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>822</v>
+      </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="50">
         <v>20</v>
       </c>
-      <c r="B22" s="54"/>
+      <c r="B22" s="54" t="s">
+        <v>7</v>
+      </c>
       <c r="C22" s="54"/>
       <c r="D22" s="54"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="56"/>
+      <c r="E22" s="55" t="s">
+        <v>823</v>
+      </c>
+      <c r="F22" s="56" t="s">
+        <v>824</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="50">
@@ -17468,6 +17594,138 @@
       <c r="D24" s="54"/>
       <c r="E24" s="55"/>
       <c r="F24" s="56"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="E26" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="E27" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="D28" t="s">
+        <v>791</v>
+      </c>
+      <c r="E28" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="D29" t="s">
+        <v>792</v>
+      </c>
+      <c r="E29" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="D30" t="s">
+        <v>793</v>
+      </c>
+      <c r="E30" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="D31" t="s">
+        <v>794</v>
+      </c>
+      <c r="E31" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="D32" t="s">
+        <v>795</v>
+      </c>
+      <c r="E32" t="s">
+        <v>810</v>
+      </c>
+      <c r="F32" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5">
+      <c r="D33" t="s">
+        <v>796</v>
+      </c>
+      <c r="E33" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5">
+      <c r="D34" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5">
+      <c r="D35" t="s">
+        <v>798</v>
+      </c>
+      <c r="E35" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5">
+      <c r="D36" t="s">
+        <v>799</v>
+      </c>
+      <c r="E36" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="37" spans="4:5">
+      <c r="D37" t="s">
+        <v>800</v>
+      </c>
+      <c r="E37" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="38" spans="4:5">
+      <c r="D38" t="s">
+        <v>801</v>
+      </c>
+      <c r="E38" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="39" spans="4:5">
+      <c r="D39" t="s">
+        <v>802</v>
+      </c>
+      <c r="E39" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="40" spans="4:5">
+      <c r="D40" t="s">
+        <v>803</v>
+      </c>
+      <c r="E40" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="41" spans="4:5">
+      <c r="D41" t="s">
+        <v>801</v>
+      </c>
+      <c r="E41" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="42" spans="4:5">
+      <c r="D42" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="43" spans="4:5">
+      <c r="D43" t="s">
+        <v>805</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21234,53 +21492,53 @@
   <sheetData>
     <row r="1" spans="1:62" ht="15" thickBot="1">
       <c r="A1" s="192"/>
-      <c r="B1" s="297" t="s">
+      <c r="B1" s="301" t="s">
         <v>534</v>
       </c>
-      <c r="C1" s="298"/>
-      <c r="D1" s="298"/>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
-      <c r="H1" s="298"/>
-      <c r="I1" s="298"/>
-      <c r="J1" s="298"/>
-      <c r="K1" s="298"/>
-      <c r="L1" s="298"/>
-      <c r="M1" s="298"/>
-      <c r="N1" s="298"/>
-      <c r="O1" s="298"/>
-      <c r="P1" s="298"/>
-      <c r="Q1" s="298"/>
-      <c r="R1" s="298"/>
-      <c r="S1" s="298"/>
-      <c r="T1" s="298"/>
-      <c r="U1" s="298"/>
-      <c r="V1" s="298"/>
-      <c r="W1" s="298"/>
-      <c r="X1" s="298"/>
-      <c r="Y1" s="298"/>
-      <c r="Z1" s="298"/>
-      <c r="AA1" s="298"/>
-      <c r="AB1" s="298"/>
-      <c r="AC1" s="298"/>
-      <c r="AD1" s="298"/>
-      <c r="AE1" s="299"/>
-      <c r="AF1" s="298" t="s">
+      <c r="C1" s="302"/>
+      <c r="D1" s="302"/>
+      <c r="E1" s="302"/>
+      <c r="F1" s="302"/>
+      <c r="G1" s="302"/>
+      <c r="H1" s="302"/>
+      <c r="I1" s="302"/>
+      <c r="J1" s="302"/>
+      <c r="K1" s="302"/>
+      <c r="L1" s="302"/>
+      <c r="M1" s="302"/>
+      <c r="N1" s="302"/>
+      <c r="O1" s="302"/>
+      <c r="P1" s="302"/>
+      <c r="Q1" s="302"/>
+      <c r="R1" s="302"/>
+      <c r="S1" s="302"/>
+      <c r="T1" s="302"/>
+      <c r="U1" s="302"/>
+      <c r="V1" s="302"/>
+      <c r="W1" s="302"/>
+      <c r="X1" s="302"/>
+      <c r="Y1" s="302"/>
+      <c r="Z1" s="302"/>
+      <c r="AA1" s="302"/>
+      <c r="AB1" s="302"/>
+      <c r="AC1" s="302"/>
+      <c r="AD1" s="302"/>
+      <c r="AE1" s="303"/>
+      <c r="AF1" s="302" t="s">
         <v>535</v>
       </c>
-      <c r="AG1" s="298"/>
-      <c r="AH1" s="298"/>
-      <c r="AI1" s="298"/>
-      <c r="AJ1" s="298"/>
-      <c r="AK1" s="298"/>
-      <c r="AL1" s="298"/>
-      <c r="AM1" s="298"/>
-      <c r="AN1" s="298"/>
-      <c r="AO1" s="298"/>
-      <c r="AP1" s="298"/>
-      <c r="AQ1" s="298"/>
-      <c r="AR1" s="299"/>
+      <c r="AG1" s="302"/>
+      <c r="AH1" s="302"/>
+      <c r="AI1" s="302"/>
+      <c r="AJ1" s="302"/>
+      <c r="AK1" s="302"/>
+      <c r="AL1" s="302"/>
+      <c r="AM1" s="302"/>
+      <c r="AN1" s="302"/>
+      <c r="AO1" s="302"/>
+      <c r="AP1" s="302"/>
+      <c r="AQ1" s="302"/>
+      <c r="AR1" s="303"/>
       <c r="AS1" s="204"/>
       <c r="AT1" s="204"/>
       <c r="AU1" s="204"/>

</xml_diff>

<commit_message>
Cel sprintu i data
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="180">
   <si>
     <t>Id</t>
   </si>
@@ -557,6 +557,12 @@
   </si>
   <si>
     <t>Umówić się na montaż doprowadzenia powietrza do kominka na środę</t>
+  </si>
+  <si>
+    <t>17-23.III.2014</t>
+  </si>
+  <si>
+    <t>Instalacja wod-kan</t>
   </si>
 </sst>
 </file>
@@ -2276,7 +2282,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="I4:J8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <location ref="I5:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
     <pivotField showAll="0"/>
@@ -2366,8 +2372,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="B2:G29" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
-  <autoFilter ref="B2:G29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela24" displayName="Tabela24" ref="B3:G30" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="B3:G30"/>
   <tableColumns count="6">
     <tableColumn id="1" name="SP" dataDxfId="9"/>
     <tableColumn id="2" name="Status" dataDxfId="8"/>
@@ -4543,10 +4549,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:J29"/>
+  <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4560,45 +4566,37 @@
     <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
-      <c r="B2" s="49" t="s">
+    <row r="1" spans="2:10">
+      <c r="B1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="52" t="s">
+      <c r="E3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="53" t="s">
+      <c r="F3" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G3" s="53" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="3" spans="2:10">
-      <c r="B3" s="55">
-        <v>3</v>
-      </c>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="55" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="55" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="56"/>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="55" t="s">
@@ -4608,72 +4606,66 @@
         <v>80</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G4" s="56"/>
-      <c r="I4" s="58" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="55">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C5" s="55"/>
       <c r="D5" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" s="56"/>
+      <c r="I5" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" s="55">
+        <v>5</v>
+      </c>
+      <c r="C6" s="55"/>
+      <c r="D6" s="55" t="s">
         <v>168</v>
       </c>
-      <c r="E5" s="55" t="s">
+      <c r="E6" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F6" s="55" t="s">
         <v>160</v>
       </c>
-      <c r="G5" s="56"/>
-      <c r="I5" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="60">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="12" customHeight="1">
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
       <c r="G6" s="56"/>
       <c r="I6" s="59" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="J6" s="60">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="55">
-        <v>5</v>
-      </c>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="12" customHeight="1">
+      <c r="B7" s="55"/>
       <c r="C7" s="55"/>
-      <c r="D7" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F7" s="55" t="s">
-        <v>170</v>
-      </c>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55"/>
       <c r="G7" s="56"/>
       <c r="I7" s="59" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
       <c r="J7" s="60">
-        <v>10</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:10">
@@ -4688,14 +4680,14 @@
         <v>135</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G8" s="56"/>
       <c r="I8" s="59" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="J8" s="60">
-        <v>73</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:10">
@@ -4710,32 +4702,38 @@
         <v>135</v>
       </c>
       <c r="F9" s="55" t="s">
+        <v>171</v>
+      </c>
+      <c r="G9" s="56"/>
+      <c r="I9" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J9" s="60">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" s="55">
+        <v>5</v>
+      </c>
+      <c r="C10" s="55"/>
+      <c r="D10" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10" s="55" t="s">
         <v>172</v>
       </c>
-      <c r="G9" s="56"/>
-    </row>
-    <row r="10" spans="2:10" ht="4.5" customHeight="1">
-      <c r="B10" s="55"/>
-      <c r="C10" s="55"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
       <c r="G10" s="56"/>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="55">
-        <v>5</v>
-      </c>
+    <row r="11" spans="2:10" ht="4.5" customHeight="1">
+      <c r="B11" s="55"/>
       <c r="C11" s="55"/>
-      <c r="D11" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" s="55" t="s">
-        <v>138</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>139</v>
-      </c>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="56"/>
     </row>
     <row r="12" spans="2:10">
@@ -4744,7 +4742,7 @@
       </c>
       <c r="C12" s="55"/>
       <c r="D12" s="55" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="E12" s="55" t="s">
         <v>138</v>
@@ -4760,19 +4758,19 @@
       </c>
       <c r="C13" s="55"/>
       <c r="D13" s="55" t="s">
-        <v>79</v>
+        <v>13</v>
       </c>
       <c r="E13" s="55" t="s">
         <v>138</v>
       </c>
       <c r="F13" s="55" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="G13" s="56"/>
     </row>
     <row r="14" spans="2:10">
       <c r="B14" s="55">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C14" s="55"/>
       <c r="D14" s="55" t="s">
@@ -4782,13 +4780,13 @@
         <v>138</v>
       </c>
       <c r="F14" s="55" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G14" s="56"/>
     </row>
     <row r="15" spans="2:10">
       <c r="B15" s="55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15" s="55"/>
       <c r="D15" s="55" t="s">
@@ -4798,47 +4796,47 @@
         <v>138</v>
       </c>
       <c r="F15" s="55" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="56"/>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="B16" s="55">
+        <v>2</v>
+      </c>
+      <c r="C16" s="55"/>
+      <c r="D16" s="55" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" s="55" t="s">
         <v>167</v>
       </c>
-      <c r="G15" s="56"/>
-    </row>
-    <row r="16" spans="2:10" ht="3.75" customHeight="1">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
       <c r="G16" s="56"/>
     </row>
-    <row r="17" spans="2:7">
-      <c r="B17" s="55">
-        <v>5</v>
-      </c>
+    <row r="17" spans="2:7" ht="3.75" customHeight="1">
+      <c r="B17" s="55"/>
       <c r="C17" s="55"/>
-      <c r="D17" s="55" t="s">
-        <v>168</v>
-      </c>
-      <c r="E17" s="55" t="s">
-        <v>165</v>
-      </c>
-      <c r="F17" s="55" t="s">
-        <v>173</v>
-      </c>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
       <c r="G17" s="56"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="55"/>
       <c r="D18" s="55" t="s">
-        <v>13</v>
+        <v>168</v>
       </c>
       <c r="E18" s="55" t="s">
-        <v>106</v>
+        <v>165</v>
       </c>
       <c r="F18" s="55" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="G18" s="56"/>
     </row>
@@ -4851,40 +4849,40 @@
         <v>13</v>
       </c>
       <c r="E19" s="55" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="56"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="55">
+        <v>2</v>
+      </c>
+      <c r="C20" s="55"/>
+      <c r="D20" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="F19" s="55" t="s">
+      <c r="F20" s="55" t="s">
         <v>166</v>
       </c>
-      <c r="G19" s="56"/>
-    </row>
-    <row r="20" spans="2:7" ht="3.75" customHeight="1">
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
       <c r="G20" s="56"/>
     </row>
-    <row r="21" spans="2:7">
-      <c r="B21" s="55">
-        <v>5</v>
-      </c>
+    <row r="21" spans="2:7" ht="3.75" customHeight="1">
+      <c r="B21" s="55"/>
       <c r="C21" s="55"/>
-      <c r="D21" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="55" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="55" t="s">
-        <v>161</v>
-      </c>
+      <c r="D21" s="55"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="55"/>
       <c r="G21" s="56"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C22" s="55"/>
       <c r="D22" s="55" t="s">
@@ -4894,13 +4892,13 @@
         <v>17</v>
       </c>
       <c r="F22" s="55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G22" s="56"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="55">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" s="55"/>
       <c r="D23" s="55" t="s">
@@ -4910,32 +4908,32 @@
         <v>17</v>
       </c>
       <c r="F23" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="G23" s="56"/>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="55">
+        <v>3</v>
+      </c>
+      <c r="C24" s="55"/>
+      <c r="D24" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="55" t="s">
         <v>163</v>
       </c>
-      <c r="G23" s="56"/>
-    </row>
-    <row r="24" spans="2:7" ht="3.75" customHeight="1">
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
       <c r="G24" s="56"/>
     </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="55">
-        <v>3</v>
-      </c>
+    <row r="25" spans="2:7" ht="3.75" customHeight="1">
+      <c r="B25" s="55"/>
       <c r="C25" s="55"/>
-      <c r="D25" s="55" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="57" t="s">
-        <v>21</v>
-      </c>
+      <c r="D25" s="55"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
       <c r="G25" s="56"/>
     </row>
     <row r="26" spans="2:7">
@@ -4950,7 +4948,7 @@
         <v>19</v>
       </c>
       <c r="F26" s="57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G26" s="56"/>
     </row>
@@ -4966,16 +4964,24 @@
         <v>19</v>
       </c>
       <c r="F27" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="56"/>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="55">
+        <v>3</v>
+      </c>
+      <c r="C28" s="55"/>
+      <c r="D28" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="57" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="56"/>
-    </row>
-    <row r="28" spans="2:7">
-      <c r="B28" s="55"/>
-      <c r="C28" s="55"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="55"/>
-      <c r="F28" s="56"/>
       <c r="G28" s="56"/>
     </row>
     <row r="29" spans="2:7">
@@ -4983,8 +4989,16 @@
       <c r="C29" s="55"/>
       <c r="D29" s="55"/>
       <c r="E29" s="55"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="54"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="55"/>
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="54"/>
+      <c r="G30" s="54"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update backlog (kontola db)
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="180">
   <si>
     <t>Id</t>
   </si>
@@ -4551,8 +4551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -4774,7 +4774,9 @@
       <c r="B14" s="55">
         <v>5</v>
       </c>
-      <c r="C14" s="55"/>
+      <c r="C14" s="55" t="s">
+        <v>132</v>
+      </c>
       <c r="D14" s="55" t="s">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
szacowania i przydział i6
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" activeTab="7"/>
@@ -16,15 +16,16 @@
     <sheet name="05_Sprint" sheetId="42" r:id="rId7"/>
     <sheet name="06_Sprint" sheetId="43" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId9"/>
+    <pivotCache cacheId="9" r:id="rId9"/>
+    <pivotCache cacheId="12" r:id="rId10"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="197">
   <si>
     <t>Id</t>
   </si>
@@ -609,13 +610,19 @@
   </si>
   <si>
     <t xml:space="preserve">Poprawki: wyrównanie schodów i drzwi garażowych. </t>
+  </si>
+  <si>
+    <t>Poprawki: umycie dachu i rynien</t>
+  </si>
+  <si>
+    <t>(puste)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,6 +680,11 @@
       <sz val="11"/>
       <color theme="0"/>
       <name val="Czcionka tekstu podstawowego"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1024,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1149,45 +1161,15 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="59">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="0"/>
-        <name val="Tahoma"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1388,23 +1370,54 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="0"/>
+        <name val="Tahoma"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color theme="0"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -2463,16 +2476,21 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kotek" refreshedDate="41714.556780208331" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="27">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kotek" refreshedDate="41730.736791782409" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="27">
   <cacheSource type="worksheet">
     <worksheetSource name="Tabela24[[#Wszystko];[SP]:[Realizator]]"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="SP" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="5"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="5" count="4">
+        <n v="3"/>
+        <n v="2"/>
+        <n v="5"/>
+        <m/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Status" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Realizator" numFmtId="0">
       <sharedItems containsBlank="1" count="5">
@@ -2487,10 +2505,174 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Kotek" refreshedDate="41730.738203819441" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="24">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Tabela4[[SP]:[Realizator]]"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="SP" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="5"/>
+    </cacheField>
+    <cacheField name="Status" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+    <cacheField name="Realizator" numFmtId="0">
+      <sharedItems containsBlank="1" count="4">
+        <s v="Słonek"/>
+        <m/>
+        <s v="Słonka"/>
+        <s v="Słonki"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="27">
   <r>
-    <n v="3"/>
+    <x v="0"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="done"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <s v="done"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="done"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="done"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="24">
+  <r>
+    <n v="5"/>
     <m/>
     <x v="0"/>
   </r>
@@ -2500,24 +2682,44 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="5"/>
+    <n v="3"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
     <m/>
     <x v="1"/>
   </r>
   <r>
+    <n v="3"/>
     <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <m/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
     <m/>
     <x v="2"/>
   </r>
   <r>
-    <n v="5"/>
+    <n v="3"/>
     <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="5"/>
@@ -2527,7 +2729,42 @@
   <r>
     <m/>
     <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <n v="5"/>
+    <m/>
     <x v="2"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <n v="3"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <n v="2"/>
+    <m/>
+    <x v="0"/>
   </r>
   <r>
     <n v="5"/>
@@ -2540,9 +2777,9 @@
     <x v="3"/>
   </r>
   <r>
-    <n v="5"/>
+    <n v="3"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <n v="3"/>
@@ -2550,85 +2787,15 @@
     <x v="0"/>
   </r>
   <r>
-    <n v="2"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
     <m/>
     <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <m/>
     <x v="1"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="5"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="2"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <n v="3"/>
-    <m/>
-    <x v="3"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="2"/>
-  </r>
-  <r>
-    <m/>
-    <m/>
-    <x v="2"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I5:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField dataField="1" showAll="0"/>
@@ -2650,6 +2817,52 @@
   <rowItems count="4">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Suma z SP" fld="0" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela przestawna3" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Wartości" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I5:J10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
     </i>
     <i>
       <x v="2"/>
@@ -2734,15 +2947,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B2:G25" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <autoFilter ref="B2:G25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tabela4" displayName="Tabela4" ref="B2:G26" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="B2:G26"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="SP" dataDxfId="7"/>
-    <tableColumn id="2" name="Status" dataDxfId="6"/>
-    <tableColumn id="3" name="Realizator" dataDxfId="5"/>
-    <tableColumn id="4" name="Zakres" dataDxfId="4"/>
-    <tableColumn id="5" name="Zadanie" dataDxfId="3"/>
-    <tableColumn id="6" name="Uwagi" dataDxfId="2"/>
+    <tableColumn id="1" name="SP" dataDxfId="5"/>
+    <tableColumn id="2" name="Status" dataDxfId="4"/>
+    <tableColumn id="3" name="Realizator" dataDxfId="3"/>
+    <tableColumn id="4" name="Zakres" dataDxfId="2"/>
+    <tableColumn id="5" name="Zadanie" dataDxfId="1"/>
+    <tableColumn id="6" name="Uwagi" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3041,12 +3254,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="6.875" customWidth="1"/>
-    <col min="3" max="3" width="5.25" customWidth="1"/>
-    <col min="4" max="4" width="6.125" customWidth="1"/>
-    <col min="5" max="5" width="43.625" customWidth="1"/>
-    <col min="6" max="6" width="52.75" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" customWidth="1"/>
+    <col min="5" max="5" width="43.6640625" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3069,7 +3282,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -3444,9 +3657,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1">
@@ -3725,8 +3938,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6">
@@ -3918,8 +4131,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7">
@@ -4234,9 +4447,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7">
@@ -4651,8 +4864,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4914,18 +5127,18 @@
   <dimension ref="B1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:F13"/>
+      <selection activeCell="I5" sqref="I5:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="9.125" customWidth="1"/>
-    <col min="6" max="6" width="44.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -5394,21 +5607,26 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:G25"/>
+  <dimension ref="B2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
-    <col min="6" max="6" width="32.125" customWidth="1"/>
-    <col min="7" max="7" width="27.75" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" thickBot="1">
+    <row r="2" spans="2:10" ht="15" thickBot="1">
       <c r="B2" s="61" t="s">
         <v>23</v>
       </c>
@@ -5428,7 +5646,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="3" spans="2:7">
+    <row r="3" spans="2:10">
       <c r="B3" s="65">
         <v>5</v>
       </c>
@@ -5444,7 +5662,7 @@
       </c>
       <c r="G3" s="56"/>
     </row>
-    <row r="4" spans="2:7">
+    <row r="4" spans="2:10">
       <c r="B4" s="65">
         <v>2</v>
       </c>
@@ -5460,7 +5678,7 @@
       </c>
       <c r="G4" s="56"/>
     </row>
-    <row r="5" spans="2:7">
+    <row r="5" spans="2:10">
       <c r="B5" s="65">
         <v>3</v>
       </c>
@@ -5475,16 +5693,28 @@
         <v>163</v>
       </c>
       <c r="G5" s="56"/>
-    </row>
-    <row r="6" spans="2:7">
+      <c r="I5" s="58" t="s">
+        <v>174</v>
+      </c>
+      <c r="J5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
       <c r="B6" s="65"/>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
       <c r="F6" s="55"/>
       <c r="G6" s="56"/>
-    </row>
-    <row r="7" spans="2:7">
+      <c r="I6" s="59" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="60">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
       <c r="B7" s="65">
         <v>3</v>
       </c>
@@ -5499,8 +5729,14 @@
         <v>21</v>
       </c>
       <c r="G7" s="56"/>
-    </row>
-    <row r="8" spans="2:7">
+      <c r="I7" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="J7" s="60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
       <c r="B8" s="65">
         <v>3</v>
       </c>
@@ -5515,8 +5751,14 @@
         <v>22</v>
       </c>
       <c r="G8" s="56"/>
-    </row>
-    <row r="9" spans="2:7">
+      <c r="I8" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="J8" s="60">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
       <c r="B9" s="65">
         <v>3</v>
       </c>
@@ -5531,17 +5773,27 @@
         <v>164</v>
       </c>
       <c r="G9" s="56"/>
-    </row>
-    <row r="10" spans="2:7">
+      <c r="I9" s="59" t="s">
+        <v>196</v>
+      </c>
+      <c r="J9" s="60"/>
+    </row>
+    <row r="10" spans="2:10">
       <c r="B10" s="65"/>
       <c r="C10" s="55"/>
       <c r="D10" s="55"/>
       <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="F10" s="57"/>
       <c r="G10" s="56"/>
-    </row>
-    <row r="11" spans="2:7">
-      <c r="B11" s="55">
+      <c r="I10" s="59" t="s">
+        <v>175</v>
+      </c>
+      <c r="J10" s="60">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" s="65">
         <v>2</v>
       </c>
       <c r="C11" s="55"/>
@@ -5551,13 +5803,13 @@
       <c r="E11" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="55" t="s">
+      <c r="F11" s="57" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="68"/>
-    </row>
-    <row r="12" spans="2:7">
-      <c r="B12" s="55">
+      <c r="G11" s="56"/>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="B12" s="65">
         <v>3</v>
       </c>
       <c r="C12" s="55"/>
@@ -5567,13 +5819,13 @@
       <c r="E12" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="F12" s="55" t="s">
+      <c r="F12" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="G12" s="69"/>
-    </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="55">
+      <c r="G12" s="56"/>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="B13" s="65">
         <v>5</v>
       </c>
       <c r="C13" s="55"/>
@@ -5583,172 +5835,208 @@
       <c r="E13" s="55" t="s">
         <v>138</v>
       </c>
-      <c r="F13" s="55" t="s">
+      <c r="F13" s="57" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="69"/>
-    </row>
-    <row r="14" spans="2:7">
+      <c r="G13" s="56"/>
+    </row>
+    <row r="14" spans="2:10">
       <c r="B14" s="65"/>
       <c r="C14" s="55"/>
       <c r="D14" s="55"/>
       <c r="E14" s="55"/>
-      <c r="F14" s="54"/>
-      <c r="G14" s="69"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="66">
+      <c r="F14" s="57"/>
+      <c r="G14" s="56"/>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="B15" s="65">
         <v>2</v>
       </c>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67" t="s">
+      <c r="C15" s="55"/>
+      <c r="D15" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="57" t="s">
         <v>192</v>
       </c>
-      <c r="G15" s="70"/>
-    </row>
-    <row r="16" spans="2:7">
+      <c r="G15" s="56"/>
+    </row>
+    <row r="16" spans="2:10">
       <c r="B16" s="65">
         <v>3</v>
       </c>
       <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="67" t="s">
+      <c r="D16" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="E16" s="55" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="57" t="s">
         <v>180</v>
       </c>
-      <c r="G16" s="69"/>
+      <c r="G16" s="56"/>
     </row>
     <row r="17" spans="2:7">
       <c r="B17" s="65">
         <v>5</v>
       </c>
       <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
+      <c r="D17" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="E17" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="F17" s="54" t="s">
+      <c r="F17" s="57" t="s">
         <v>181</v>
       </c>
-      <c r="G17" s="69"/>
+      <c r="G17" s="56"/>
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="65">
         <v>2</v>
       </c>
       <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
+      <c r="D18" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="E18" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="57" t="s">
         <v>182</v>
       </c>
-      <c r="G18" s="69"/>
+      <c r="G18" s="56"/>
     </row>
     <row r="19" spans="2:7">
       <c r="B19" s="65">
         <v>2</v>
       </c>
       <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
+      <c r="D19" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="E19" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="F19" s="54" t="s">
+      <c r="F19" s="57" t="s">
         <v>184</v>
       </c>
-      <c r="G19" s="69"/>
+      <c r="G19" s="56"/>
     </row>
     <row r="20" spans="2:7">
       <c r="B20" s="65">
         <v>3</v>
       </c>
       <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
+      <c r="D20" s="55" t="s">
+        <v>79</v>
+      </c>
       <c r="E20" s="55" t="s">
         <v>183</v>
       </c>
-      <c r="F20" s="54" t="s">
+      <c r="F20" s="57" t="s">
         <v>193</v>
       </c>
-      <c r="G20" s="69"/>
+      <c r="G20" s="56"/>
     </row>
     <row r="21" spans="2:7">
       <c r="B21" s="65">
         <v>2</v>
       </c>
       <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
+      <c r="D21" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="E21" s="55" t="s">
         <v>185</v>
       </c>
-      <c r="F21" s="54" t="s">
+      <c r="F21" s="57" t="s">
         <v>186</v>
       </c>
-      <c r="G21" s="69"/>
+      <c r="G21" s="56"/>
     </row>
     <row r="22" spans="2:7">
       <c r="B22" s="65">
         <v>5</v>
       </c>
       <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
+      <c r="D22" s="55" t="s">
+        <v>13</v>
+      </c>
       <c r="E22" s="55" t="s">
         <v>185</v>
       </c>
-      <c r="F22" s="54" t="s">
+      <c r="F22" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="G22" s="69"/>
+      <c r="G22" s="56"/>
     </row>
     <row r="23" spans="2:7">
       <c r="B23" s="65">
         <v>5</v>
       </c>
       <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
+      <c r="D23" s="55" t="s">
+        <v>168</v>
+      </c>
       <c r="E23" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="F23" s="54" t="s">
+      <c r="F23" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="G23" s="69"/>
+      <c r="G23" s="56"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="65">
+      <c r="B24" s="70">
         <v>3</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="55" t="s">
+        <v>168</v>
+      </c>
       <c r="E24" s="55" t="s">
+        <v>189</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="G24" s="68"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="65">
+        <v>3</v>
+      </c>
+      <c r="C25" s="55"/>
+      <c r="D25" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="55" t="s">
         <v>190</v>
       </c>
-      <c r="F24" s="54" t="s">
+      <c r="F25" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="G24" s="69"/>
-    </row>
-    <row r="25" spans="2:7">
-      <c r="B25" s="66"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="70"/>
+      <c r="G25" s="56"/>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="66"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
przegląd przed montażem kuchni i drzwi
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" activeTab="11"/>
@@ -21,7 +21,7 @@
     <sheet name="10_Sprint" sheetId="48" r:id="rId12"/>
     <sheet name="Arkusz1" sheetId="47" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId14"/>
     <pivotCache cacheId="1" r:id="rId15"/>
@@ -620,7 +620,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="441">
   <si>
     <t>Id</t>
   </si>
@@ -1745,9 +1745,6 @@
   </si>
   <si>
     <t>Łazienki</t>
-  </si>
-  <si>
-    <t>Dopilnować: montażu drzwi prysznicowych na dole</t>
   </si>
   <si>
     <t>Dopilnować: wykończenia wanny</t>
@@ -2665,14 +2662,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -6665,7 +6662,11 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tabela7" displayName="Tabela7" ref="A3:F75" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A3:F75">
-    <filterColumn colId="4"/>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5"/>
   </autoFilter>
   <sortState ref="A4:I73">
@@ -6976,12 +6977,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="6.875" customWidth="1"/>
-    <col min="3" max="3" width="5.25" customWidth="1"/>
-    <col min="4" max="4" width="10.375" customWidth="1"/>
-    <col min="5" max="5" width="43.625" customWidth="1"/>
-    <col min="6" max="6" width="52.75" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="43.6640625" customWidth="1"/>
+    <col min="6" max="6" width="52.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7004,7 +7005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5">
+    <row r="2" spans="1:6">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -7387,9 +7388,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="10.125" customWidth="1"/>
-    <col min="5" max="5" width="11.125" customWidth="1"/>
-    <col min="6" max="6" width="91.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="6" max="6" width="91.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -8119,10 +8120,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="10.875" customWidth="1"/>
-    <col min="5" max="5" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.5" customWidth="1"/>
-    <col min="7" max="7" width="22.25" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -8904,7 +8905,7 @@
       </c>
       <c r="G68" s="87"/>
     </row>
-    <row r="69" spans="2:7" ht="25.5">
+    <row r="69" spans="2:7">
       <c r="B69" s="88"/>
       <c r="C69" s="83"/>
       <c r="D69" s="83" t="s">
@@ -9228,30 +9229,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:R145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="8.125" style="106" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.875" style="106" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" style="106" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.5" style="106" customWidth="1"/>
-    <col min="5" max="5" width="10.125" style="106" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" style="106" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5" style="106" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" style="106" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.44140625" style="106" customWidth="1"/>
+    <col min="5" max="5" width="10.109375" style="106" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.44140625" style="106" customWidth="1"/>
     <col min="8" max="8" width="22" style="106" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.125" style="106" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.875" style="106" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="106" customWidth="1"/>
-    <col min="12" max="12" width="5.5" style="106" customWidth="1"/>
-    <col min="13" max="13" width="6.75" style="106" customWidth="1"/>
-    <col min="14" max="14" width="6.25" style="106" customWidth="1"/>
-    <col min="15" max="15" width="16.625" style="106" customWidth="1"/>
-    <col min="16" max="16" width="12.5" style="106" customWidth="1"/>
-    <col min="17" max="17" width="7.125" style="106" customWidth="1"/>
-    <col min="18" max="18" width="14.125" style="106" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="106" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" style="106" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.44140625" style="106" customWidth="1"/>
+    <col min="12" max="12" width="5.44140625" style="106" customWidth="1"/>
+    <col min="13" max="13" width="6.77734375" style="106" customWidth="1"/>
+    <col min="14" max="14" width="6.21875" style="106" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" style="106" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" style="106" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="106" customWidth="1"/>
+    <col min="18" max="18" width="14.109375" style="106" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="9" style="106"/>
   </cols>
   <sheetData>
@@ -9275,37 +9276,37 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" hidden="1">
       <c r="A4" s="81"/>
       <c r="B4" s="81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C4" s="83" t="s">
         <v>355</v>
       </c>
-      <c r="D4" s="117" t="s">
-        <v>440</v>
+      <c r="D4" s="115" t="s">
+        <v>439</v>
       </c>
       <c r="E4" s="83">
-        <v>1</v>
-      </c>
-      <c r="F4" s="116"/>
-    </row>
-    <row r="5" spans="1:10">
+        <v>2</v>
+      </c>
+      <c r="F4" s="114"/>
+    </row>
+    <row r="5" spans="1:10" hidden="1">
       <c r="A5" s="81"/>
       <c r="B5" s="81" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C5" s="83" t="s">
         <v>355</v>
       </c>
-      <c r="D5" s="117" t="s">
-        <v>441</v>
+      <c r="D5" s="115" t="s">
+        <v>440</v>
       </c>
       <c r="E5" s="83">
-        <v>1</v>
-      </c>
-      <c r="F5" s="116"/>
+        <v>2</v>
+      </c>
+      <c r="F5" s="114"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="83" t="s">
@@ -9328,7 +9329,7 @@
         <v>173</v>
       </c>
       <c r="I6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J6"/>
     </row>
@@ -9400,14 +9401,14 @@
       </c>
       <c r="F9" s="107"/>
       <c r="H9" s="113" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I9" s="60">
         <v>1</v>
       </c>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" hidden="1">
       <c r="A10" s="83"/>
       <c r="B10" s="83" t="s">
         <v>78</v>
@@ -9419,7 +9420,7 @@
         <v>362</v>
       </c>
       <c r="E10" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="107"/>
       <c r="H10" s="113" t="s">
@@ -9430,7 +9431,7 @@
       </c>
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" hidden="1">
       <c r="A11" s="83"/>
       <c r="B11" s="83" t="s">
         <v>78</v>
@@ -9442,7 +9443,7 @@
         <v>363</v>
       </c>
       <c r="E11" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="107"/>
       <c r="H11" s="113" t="s">
@@ -9453,10 +9454,10 @@
       </c>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" hidden="1">
       <c r="A12" s="83"/>
       <c r="B12" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C12" s="83" t="s">
         <v>355</v>
@@ -9465,7 +9466,7 @@
         <v>364</v>
       </c>
       <c r="E12" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" s="28"/>
       <c r="H12" s="113" t="s">
@@ -9476,10 +9477,10 @@
       </c>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" hidden="1">
       <c r="A13" s="101"/>
       <c r="B13" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C13" s="83" t="s">
         <v>355</v>
@@ -9488,34 +9489,34 @@
         <v>365</v>
       </c>
       <c r="E13" s="101">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F13" s="108"/>
       <c r="H13" s="113" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I13" s="60">
         <v>2</v>
       </c>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" hidden="1">
       <c r="A14" s="83"/>
       <c r="B14" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C14" s="83" t="s">
         <v>366</v>
       </c>
       <c r="D14" s="108" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="E14" s="83">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F14" s="108"/>
       <c r="H14" s="113" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I14" s="60">
         <v>2</v>
@@ -9540,7 +9541,7 @@
       </c>
       <c r="F15" s="108"/>
       <c r="H15" s="112" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I15" s="60">
         <v>14</v>
@@ -9563,7 +9564,7 @@
       </c>
       <c r="F16" s="108"/>
       <c r="H16" s="113" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I16" s="60">
         <v>1</v>
@@ -9571,15 +9572,17 @@
       <c r="J16"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="83"/>
+      <c r="A17" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B17" s="83" t="s">
-        <v>438</v>
+        <v>78</v>
       </c>
       <c r="C17" s="83" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="D17" s="108" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E17" s="83">
         <v>1</v>
@@ -9596,20 +9599,20 @@
     <row r="18" spans="1:10">
       <c r="A18" s="83"/>
       <c r="B18" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C18" s="83" t="s">
         <v>374</v>
       </c>
       <c r="D18" s="108" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E18" s="83">
         <v>1</v>
       </c>
       <c r="F18" s="108"/>
       <c r="H18" s="113" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I18" s="60">
         <v>1</v>
@@ -9627,7 +9630,7 @@
         <v>374</v>
       </c>
       <c r="D19" s="110" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E19" s="83">
         <v>1</v>
@@ -9644,22 +9647,22 @@
     <row r="20" spans="1:10">
       <c r="A20" s="83"/>
       <c r="B20" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C20" s="109" t="s">
         <v>374</v>
       </c>
       <c r="D20" s="110" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E20" s="83">
         <v>1</v>
       </c>
       <c r="F20" s="83" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H20" s="113" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I20" s="60">
         <v>3</v>
@@ -9669,22 +9672,22 @@
     <row r="21" spans="1:10">
       <c r="A21" s="83"/>
       <c r="B21" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C21" s="83" t="s">
+        <v>379</v>
+      </c>
+      <c r="D21" s="108" t="s">
         <v>380</v>
-      </c>
-      <c r="D21" s="108" t="s">
-        <v>381</v>
       </c>
       <c r="E21" s="83">
         <v>1</v>
       </c>
       <c r="F21" s="83" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H21" s="113" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I21" s="60">
         <v>2</v>
@@ -9692,21 +9695,23 @@
       <c r="J21"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="83"/>
+      <c r="A22" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B22" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C22" s="83" t="s">
         <v>95</v>
       </c>
       <c r="D22" s="108" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E22" s="83">
         <v>1</v>
       </c>
       <c r="F22" s="83" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H22" s="113" t="s">
         <v>366</v>
@@ -9721,13 +9726,13 @@
         <v>87</v>
       </c>
       <c r="B23" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C23" s="109" t="s">
+        <v>395</v>
+      </c>
+      <c r="D23" s="110" t="s">
         <v>396</v>
-      </c>
-      <c r="D23" s="110" t="s">
-        <v>397</v>
       </c>
       <c r="E23" s="83">
         <v>1</v>
@@ -9746,20 +9751,20 @@
         <v>87</v>
       </c>
       <c r="B24" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C24" s="101" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D24" s="108" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E24" s="101">
         <v>1</v>
       </c>
       <c r="F24" s="108"/>
       <c r="H24" s="112" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I24" s="60">
         <v>4</v>
@@ -9771,20 +9776,20 @@
         <v>87</v>
       </c>
       <c r="B25" s="83" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C25" s="101" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D25" s="108" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E25" s="81">
         <v>1</v>
       </c>
       <c r="F25" s="111"/>
       <c r="H25" s="113" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I25" s="60">
         <v>1</v>
@@ -9799,17 +9804,17 @@
         <v>78</v>
       </c>
       <c r="C26" s="101" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D26" s="111" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E26" s="81">
         <v>1</v>
       </c>
       <c r="F26" s="111"/>
       <c r="H26" s="113" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I26" s="60">
         <v>3</v>
@@ -9823,10 +9828,10 @@
         <v>78</v>
       </c>
       <c r="C27" s="101" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D27" s="108" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E27" s="83">
         <v>1</v>
@@ -9840,15 +9845,17 @@
       </c>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="83"/>
+      <c r="A28" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B28" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C28" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D28" s="108" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E28" s="83">
         <v>1</v>
@@ -9863,16 +9870,16 @@
     </row>
     <row r="29" spans="1:10">
       <c r="A29" s="83" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="B29" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C29" s="83" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D29" s="108" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E29" s="83">
         <v>1</v>
@@ -9890,13 +9897,13 @@
         <v>87</v>
       </c>
       <c r="B30" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C30" s="83" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D30" s="108" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E30" s="83">
         <v>1</v>
@@ -9910,15 +9917,17 @@
       </c>
     </row>
     <row r="31" spans="1:10">
-      <c r="A31" s="83"/>
+      <c r="A31" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B31" s="83" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C31" s="83" t="s">
+        <v>426</v>
+      </c>
+      <c r="D31" s="108" t="s">
         <v>427</v>
-      </c>
-      <c r="D31" s="108" t="s">
-        <v>428</v>
       </c>
       <c r="E31" s="83">
         <v>1</v>
@@ -9932,44 +9941,48 @@
       </c>
     </row>
     <row r="32" spans="1:10">
-      <c r="A32" s="101"/>
+      <c r="A32" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B32" s="83" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C32" s="90" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D32" s="108" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E32" s="101">
         <v>1</v>
       </c>
       <c r="F32" s="108"/>
       <c r="H32" s="113" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I32" s="60">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="83"/>
+      <c r="A33" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B33" s="83" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C33" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D33" s="108" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E33" s="83">
         <v>1</v>
       </c>
       <c r="F33" s="108"/>
       <c r="H33" s="113" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I33" s="60">
         <v>1</v>
@@ -9983,39 +9996,41 @@
         <v>78</v>
       </c>
       <c r="C34" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D34" s="108" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E34" s="83">
         <v>1</v>
       </c>
       <c r="F34" s="108"/>
       <c r="H34" s="113" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I34" s="60">
         <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="83"/>
+      <c r="A35" s="83" t="s">
+        <v>87</v>
+      </c>
       <c r="B35" s="83" t="s">
         <v>78</v>
       </c>
       <c r="C35" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D35" s="108" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E35" s="83">
         <v>1</v>
       </c>
       <c r="F35" s="108"/>
       <c r="H35" s="113" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I35" s="60">
         <v>1</v>
@@ -10024,13 +10039,13 @@
     <row r="36" spans="1:9">
       <c r="A36" s="83"/>
       <c r="B36" s="83" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D36" s="108" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E36" s="83">
         <v>1</v>
@@ -10051,10 +10066,10 @@
         <v>78</v>
       </c>
       <c r="C37" s="81" t="s">
+        <v>409</v>
+      </c>
+      <c r="D37" s="111" t="s">
         <v>410</v>
-      </c>
-      <c r="D37" s="111" t="s">
-        <v>411</v>
       </c>
       <c r="E37" s="81">
         <v>1</v>
@@ -10067,7 +10082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9">
+    <row r="38" spans="1:9" hidden="1">
       <c r="A38" s="83"/>
       <c r="B38" s="83" t="s">
         <v>78</v>
@@ -10083,13 +10098,13 @@
       </c>
       <c r="F38" s="108"/>
       <c r="H38" s="113" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I38" s="60">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" hidden="1">
       <c r="A39" s="83"/>
       <c r="B39" s="83"/>
       <c r="C39" s="83" t="s">
@@ -10109,14 +10124,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
+    <row r="40" spans="1:9" hidden="1">
       <c r="A40" s="83"/>
       <c r="B40" s="83"/>
       <c r="C40" s="83" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D40" s="108" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E40" s="83">
         <v>2</v>
@@ -10129,14 +10144,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:9">
+    <row r="41" spans="1:9" hidden="1">
       <c r="A41" s="83"/>
       <c r="B41" s="83"/>
       <c r="C41" s="83" t="s">
         <v>95</v>
       </c>
       <c r="D41" s="108" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E41" s="83">
         <v>2</v>
@@ -10149,7 +10164,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9">
+    <row r="42" spans="1:9" hidden="1">
       <c r="A42" s="101" t="s">
         <v>87</v>
       </c>
@@ -10158,7 +10173,7 @@
         <v>238</v>
       </c>
       <c r="D42" s="108" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E42" s="101">
         <v>2</v>
@@ -10171,14 +10186,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9">
+    <row r="43" spans="1:9" hidden="1">
       <c r="A43" s="83"/>
       <c r="B43" s="83"/>
       <c r="C43" s="83" t="s">
+        <v>393</v>
+      </c>
+      <c r="D43" s="108" t="s">
         <v>394</v>
-      </c>
-      <c r="D43" s="108" t="s">
-        <v>395</v>
       </c>
       <c r="E43" s="83">
         <v>2</v>
@@ -10191,14 +10206,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="44" spans="1:9">
+    <row r="44" spans="1:9" hidden="1">
       <c r="A44" s="83"/>
       <c r="B44" s="83"/>
       <c r="C44" s="83" t="s">
+        <v>397</v>
+      </c>
+      <c r="D44" s="108" t="s">
         <v>398</v>
-      </c>
-      <c r="D44" s="108" t="s">
-        <v>399</v>
       </c>
       <c r="E44" s="83">
         <v>2</v>
@@ -10211,14 +10226,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9">
+    <row r="45" spans="1:9" hidden="1">
       <c r="A45" s="83"/>
       <c r="B45" s="83"/>
       <c r="C45" s="83" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D45" s="108" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E45" s="83">
         <v>2</v>
@@ -10231,74 +10246,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:9">
+    <row r="46" spans="1:9" hidden="1">
       <c r="A46" s="83"/>
       <c r="B46" s="83"/>
       <c r="C46" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D46" s="83" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E46" s="83">
         <v>2</v>
       </c>
       <c r="F46" s="108"/>
       <c r="H46" s="113" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I46" s="60">
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:9">
+    <row r="47" spans="1:9" hidden="1">
       <c r="A47" s="83"/>
       <c r="B47" s="83"/>
       <c r="C47" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D47" s="83" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E47" s="83">
         <v>2</v>
       </c>
       <c r="F47" s="108"/>
       <c r="H47" s="113" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I47" s="60">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9">
+    <row r="48" spans="1:9" hidden="1">
       <c r="A48" s="83"/>
       <c r="B48" s="83"/>
       <c r="C48" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D48" s="108" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E48" s="83">
         <v>2</v>
       </c>
       <c r="F48" s="108"/>
       <c r="H48" s="113" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="I48" s="60">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" hidden="1">
       <c r="A49" s="83"/>
       <c r="B49" s="83"/>
       <c r="C49" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D49" s="108" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E49" s="83">
         <v>2</v>
@@ -10311,14 +10326,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" hidden="1">
       <c r="A50" s="101"/>
       <c r="B50" s="101"/>
       <c r="C50" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D50" s="108" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E50" s="101">
         <v>2</v>
@@ -10331,34 +10346,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" hidden="1">
       <c r="A51" s="83"/>
       <c r="B51" s="83"/>
       <c r="C51" s="81" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D51" s="108" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E51" s="83">
         <v>2</v>
       </c>
       <c r="F51" s="108"/>
       <c r="H51" s="113" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I51" s="60">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" hidden="1">
       <c r="A52" s="81"/>
       <c r="B52" s="81"/>
       <c r="C52" s="83" t="s">
+        <v>411</v>
+      </c>
+      <c r="D52" s="108" t="s">
         <v>412</v>
-      </c>
-      <c r="D52" s="108" t="s">
-        <v>413</v>
       </c>
       <c r="E52" s="81">
         <v>2</v>
@@ -10369,14 +10384,14 @@
       </c>
       <c r="I52" s="60"/>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" hidden="1">
       <c r="A53" s="81"/>
       <c r="B53" s="81"/>
       <c r="C53" s="83" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D53" s="108" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E53" s="81">
         <v>2</v>
@@ -10387,14 +10402,14 @@
       </c>
       <c r="I53" s="60"/>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" hidden="1">
       <c r="A54" s="81"/>
       <c r="B54" s="81"/>
       <c r="C54" s="83" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D54" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E54" s="81">
         <v>2</v>
@@ -10405,16 +10420,16 @@
       </c>
       <c r="I54" s="60"/>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" hidden="1">
       <c r="A55" s="81" t="s">
         <v>87</v>
       </c>
       <c r="B55" s="81"/>
       <c r="C55" s="83" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D55" s="108" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E55" s="81">
         <v>2</v>
@@ -10427,7 +10442,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="56" spans="1:9">
+    <row r="56" spans="1:9" hidden="1">
       <c r="A56" s="83" t="s">
         <v>87</v>
       </c>
@@ -10447,7 +10462,7 @@
       <c r="H56"/>
       <c r="I56"/>
     </row>
-    <row r="57" spans="1:9">
+    <row r="57" spans="1:9" hidden="1">
       <c r="A57" s="83"/>
       <c r="B57" s="83" t="s">
         <v>78</v>
@@ -10463,7 +10478,7 @@
       </c>
       <c r="F57" s="85"/>
     </row>
-    <row r="58" spans="1:9">
+    <row r="58" spans="1:9" hidden="1">
       <c r="A58" s="83"/>
       <c r="B58" s="83"/>
       <c r="C58" s="83" t="s">
@@ -10477,7 +10492,7 @@
       </c>
       <c r="F58" s="108"/>
     </row>
-    <row r="59" spans="1:9">
+    <row r="59" spans="1:9" hidden="1">
       <c r="A59" s="83"/>
       <c r="B59" s="83"/>
       <c r="C59" s="83" t="s">
@@ -10491,7 +10506,7 @@
       </c>
       <c r="F59" s="108"/>
     </row>
-    <row r="60" spans="1:9">
+    <row r="60" spans="1:9" hidden="1">
       <c r="A60" s="83"/>
       <c r="B60" s="83" t="s">
         <v>78</v>
@@ -10500,168 +10515,168 @@
         <v>374</v>
       </c>
       <c r="D60" s="108" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E60" s="83">
         <v>3</v>
       </c>
       <c r="F60" s="108"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" hidden="1">
       <c r="A61" s="83"/>
       <c r="B61" s="83"/>
       <c r="C61" s="83" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D61" s="108" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E61" s="83">
         <v>3</v>
       </c>
       <c r="F61" s="108"/>
     </row>
-    <row r="62" spans="1:9">
+    <row r="62" spans="1:9" hidden="1">
       <c r="A62" s="83"/>
       <c r="B62" s="83"/>
       <c r="C62" s="83" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D62" s="108" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E62" s="83">
         <v>3</v>
       </c>
       <c r="F62" s="108"/>
     </row>
-    <row r="63" spans="1:9">
+    <row r="63" spans="1:9" hidden="1">
       <c r="A63" s="83"/>
       <c r="B63" s="83"/>
       <c r="C63" s="83" t="s">
+        <v>384</v>
+      </c>
+      <c r="D63" s="108" t="s">
         <v>385</v>
-      </c>
-      <c r="D63" s="108" t="s">
-        <v>386</v>
       </c>
       <c r="E63" s="83">
         <v>3</v>
       </c>
       <c r="F63" s="108"/>
     </row>
-    <row r="64" spans="1:9">
+    <row r="64" spans="1:9" hidden="1">
       <c r="A64" s="83"/>
       <c r="B64" s="83"/>
       <c r="C64" s="83" t="s">
         <v>95</v>
       </c>
       <c r="D64" s="108" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E64" s="83">
         <v>3</v>
       </c>
       <c r="F64" s="108"/>
     </row>
-    <row r="65" spans="1:18">
+    <row r="65" spans="1:18" hidden="1">
       <c r="A65" s="83"/>
       <c r="B65" s="83"/>
       <c r="C65" s="83" t="s">
         <v>95</v>
       </c>
       <c r="D65" s="108" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E65" s="83">
         <v>3</v>
       </c>
       <c r="F65" s="108"/>
     </row>
-    <row r="66" spans="1:18">
+    <row r="66" spans="1:18" hidden="1">
       <c r="A66" s="83"/>
       <c r="B66" s="83"/>
       <c r="C66" s="83" t="s">
         <v>238</v>
       </c>
       <c r="D66" s="108" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E66" s="83">
         <v>3</v>
       </c>
       <c r="F66" s="108"/>
     </row>
-    <row r="67" spans="1:18">
+    <row r="67" spans="1:18" hidden="1">
       <c r="A67" s="101"/>
       <c r="B67" s="101"/>
       <c r="C67" s="101" t="s">
         <v>238</v>
       </c>
       <c r="D67" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E67" s="101">
         <v>3</v>
       </c>
       <c r="F67" s="108"/>
     </row>
-    <row r="68" spans="1:18">
+    <row r="68" spans="1:18" hidden="1">
       <c r="A68" s="83"/>
       <c r="B68" s="83"/>
       <c r="C68" s="101" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D68" s="108" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E68" s="83">
         <v>3</v>
       </c>
       <c r="F68" s="108"/>
     </row>
-    <row r="69" spans="1:18">
+    <row r="69" spans="1:18" hidden="1">
       <c r="A69" s="81"/>
       <c r="B69" s="81"/>
       <c r="C69" s="90" t="s">
+        <v>406</v>
+      </c>
+      <c r="D69" s="111" t="s">
         <v>407</v>
-      </c>
-      <c r="D69" s="111" t="s">
-        <v>408</v>
       </c>
       <c r="E69" s="81">
         <v>3</v>
       </c>
       <c r="F69" s="111"/>
     </row>
-    <row r="70" spans="1:18">
+    <row r="70" spans="1:18" hidden="1">
       <c r="A70" s="81"/>
       <c r="B70" s="81"/>
       <c r="C70" s="90" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D70" s="111" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E70" s="81">
         <v>3</v>
       </c>
       <c r="F70" s="111"/>
     </row>
-    <row r="71" spans="1:18">
+    <row r="71" spans="1:18" hidden="1">
       <c r="A71" s="81"/>
       <c r="B71" s="81"/>
       <c r="C71" s="83" t="s">
         <v>51</v>
       </c>
       <c r="D71" s="108" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E71" s="81">
         <v>3</v>
       </c>
       <c r="F71" s="111"/>
     </row>
-    <row r="72" spans="1:18">
+    <row r="72" spans="1:18" hidden="1">
       <c r="A72" s="81"/>
       <c r="B72" s="81"/>
       <c r="C72" s="81"/>
@@ -10669,7 +10684,7 @@
       <c r="E72" s="81"/>
       <c r="F72" s="111"/>
     </row>
-    <row r="73" spans="1:18">
+    <row r="73" spans="1:18" hidden="1">
       <c r="A73" s="81"/>
       <c r="B73" s="81"/>
       <c r="C73" s="81"/>
@@ -10677,7 +10692,7 @@
       <c r="E73" s="81"/>
       <c r="F73" s="111"/>
     </row>
-    <row r="74" spans="1:18">
+    <row r="74" spans="1:18" hidden="1">
       <c r="A74" s="81"/>
       <c r="B74" s="81"/>
       <c r="C74" s="81"/>
@@ -10685,7 +10700,7 @@
       <c r="E74" s="81"/>
       <c r="F74" s="111"/>
     </row>
-    <row r="75" spans="1:18">
+    <row r="75" spans="1:18" hidden="1">
       <c r="A75" s="90"/>
       <c r="B75" s="90"/>
       <c r="C75" s="90"/>
@@ -10928,9 +10943,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="44.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2">
@@ -11275,7 +11290,7 @@
         <f>SUM(F42:J42)</f>
         <v>82</v>
       </c>
-      <c r="L42" s="114">
+      <c r="L42" s="116">
         <v>191</v>
       </c>
     </row>
@@ -11300,7 +11315,7 @@
         <f t="shared" ref="K43:K45" si="1">SUM(F43:J43)</f>
         <v>117</v>
       </c>
-      <c r="L43" s="115"/>
+      <c r="L43" s="117"/>
     </row>
     <row r="44" spans="5:12" ht="15">
       <c r="E44" s="36" t="s">
@@ -11491,9 +11506,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="20.44140625" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="32.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" thickBot="1">
@@ -11772,8 +11787,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.375" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6">
@@ -11965,8 +11980,8 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.375" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7">
@@ -12281,9 +12296,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:7">
@@ -12698,8 +12713,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="9.625" customWidth="1"/>
-    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" customWidth="1"/>
     <col min="6" max="6" width="37" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12967,12 +12982,12 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="4.625" customWidth="1"/>
-    <col min="3" max="3" width="9.125" customWidth="1"/>
-    <col min="6" max="6" width="44.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="6" max="6" width="44.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.125" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
@@ -13449,15 +13464,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="3.75" customWidth="1"/>
-    <col min="4" max="4" width="9.125" customWidth="1"/>
-    <col min="5" max="5" width="9.875" customWidth="1"/>
-    <col min="6" max="6" width="47.375" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="1" max="1" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.88671875" customWidth="1"/>
+    <col min="6" max="6" width="47.33203125" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" customWidth="1"/>
     <col min="9" max="9" width="15" customWidth="1"/>
-    <col min="10" max="10" width="9.125" customWidth="1"/>
-    <col min="11" max="12" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" customWidth="1"/>
+    <col min="11" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" thickBot="1">
@@ -13684,7 +13699,7 @@
       <c r="F14" s="57"/>
       <c r="G14" s="56"/>
     </row>
-    <row r="15" spans="2:10" ht="25.5">
+    <row r="15" spans="2:10">
       <c r="B15" s="65">
         <v>2</v>
       </c>
@@ -13768,7 +13783,7 @@
       </c>
       <c r="G19" s="56"/>
     </row>
-    <row r="20" spans="2:7" ht="25.5">
+    <row r="20" spans="2:7">
       <c r="B20" s="65">
         <v>3</v>
       </c>
@@ -13893,8 +13908,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="12.625" customWidth="1"/>
-    <col min="5" max="5" width="9.25" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" customWidth="1"/>
     <col min="6" max="6" width="60" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
12 sprint - zarys
</commit_message>
<xml_diff>
--- a/plan/Backlog.xlsx
+++ b/plan/Backlog.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" activeTab="12"/>
+    <workbookView xWindow="600" yWindow="15" windowWidth="13725" windowHeight="8265" tabRatio="764" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="37" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="09_Sprint" sheetId="46" r:id="rId11"/>
     <sheet name="10_Sprint" sheetId="48" r:id="rId12"/>
     <sheet name="11_Sprint" sheetId="49" r:id="rId13"/>
-    <sheet name="Arkusz1" sheetId="47" r:id="rId14"/>
+    <sheet name="12_Sprint" sheetId="50" r:id="rId14"/>
+    <sheet name="Arkusz1" sheetId="47" r:id="rId15"/>
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId15"/>
-    <pivotCache cacheId="1" r:id="rId16"/>
-    <pivotCache cacheId="2" r:id="rId17"/>
+    <pivotCache cacheId="0" r:id="rId16"/>
+    <pivotCache cacheId="1" r:id="rId17"/>
+    <pivotCache cacheId="2" r:id="rId18"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -621,7 +622,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="522">
   <si>
     <t>Id</t>
   </si>
@@ -2109,6 +2110,84 @@
   </si>
   <si>
     <t>zasłonięcie okien na dole (cokolwiek - papier remontowy)</t>
+  </si>
+  <si>
+    <t>PLAN NA GRUDZIEŃ/STYCZEŃ</t>
+  </si>
+  <si>
+    <t>Podjazd</t>
+  </si>
+  <si>
+    <t>zrobić projekt</t>
+  </si>
+  <si>
+    <t>zdobyć wyceny</t>
+  </si>
+  <si>
+    <t>poszukać ekip</t>
+  </si>
+  <si>
+    <t>spytać Glapy co ze styropianem przed garażem - czy i tak trzeba będzie go wyciąć</t>
+  </si>
+  <si>
+    <t>Rolety</t>
+  </si>
+  <si>
+    <t>pomierzyć okna</t>
+  </si>
+  <si>
+    <t>zebrać wyceny</t>
+  </si>
+  <si>
+    <t>Oświetlenie zewnętrzne</t>
+  </si>
+  <si>
+    <t>Oświetlenie wewnętrzne</t>
+  </si>
+  <si>
+    <t>Schody</t>
+  </si>
+  <si>
+    <t>kupić płytę i szpachlę</t>
+  </si>
+  <si>
+    <t>zaszpachlować</t>
+  </si>
+  <si>
+    <t>górna łazienka</t>
+  </si>
+  <si>
+    <t>kotłownia</t>
+  </si>
+  <si>
+    <t>salon</t>
+  </si>
+  <si>
+    <t>Cokoły</t>
+  </si>
+  <si>
+    <t>salon i hol</t>
+  </si>
+  <si>
+    <t>wiatrołap</t>
+  </si>
+  <si>
+    <t>piętro</t>
+  </si>
+  <si>
+    <t>Sprzątanie</t>
+  </si>
+  <si>
+    <t>cokoły</t>
+  </si>
+  <si>
+    <t>podłogi</t>
+  </si>
+  <si>
+    <t>okna - ramy</t>
+  </si>
+  <si>
+    <t>okna - szyby</t>
   </si>
 </sst>
 </file>
@@ -2844,8 +2923,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2874,80 +2951,13 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="113">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Czcionka tekstu podstawowego"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3128,6 +3138,75 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Czcionka tekstu podstawowego"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -7008,15 +7087,15 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A4:F47" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2" totalsRowBorderDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tabela9" displayName="Tabela9" ref="A4:F47" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="A4:F47"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Status" dataDxfId="10"/>
-    <tableColumn id="2" name="Realizator" dataDxfId="9"/>
-    <tableColumn id="3" name="Zakres" dataDxfId="8"/>
-    <tableColumn id="4" name="Zadanie" dataDxfId="7"/>
-    <tableColumn id="5" name="Priorytet" dataDxfId="6"/>
-    <tableColumn id="6" name="Uwagi" dataDxfId="5"/>
+    <tableColumn id="1" name="Status" dataDxfId="5"/>
+    <tableColumn id="2" name="Realizator" dataDxfId="4"/>
+    <tableColumn id="3" name="Zakres" dataDxfId="3"/>
+    <tableColumn id="4" name="Zadanie" dataDxfId="2"/>
+    <tableColumn id="5" name="Priorytet" dataDxfId="1"/>
+    <tableColumn id="6" name="Uwagi" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11407,7 +11486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -11439,29 +11518,29 @@
       <c r="D4" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="118" t="s">
+      <c r="E4" s="116" t="s">
         <v>1</v>
       </c>
       <c r="F4" s="99" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="102">
-      <c r="A5" s="119"/>
-      <c r="B5" s="120"/>
+    <row r="5" spans="1:6">
+      <c r="A5" s="117"/>
+      <c r="B5" s="118"/>
       <c r="C5" s="83" t="s">
         <v>355</v>
       </c>
       <c r="D5" s="85" t="s">
         <v>443</v>
       </c>
-      <c r="E5" s="121">
+      <c r="E5" s="119">
         <v>2</v>
       </c>
-      <c r="F5" s="122"/>
-    </row>
-    <row r="6" spans="1:6" ht="51">
-      <c r="A6" s="123"/>
+      <c r="F5" s="120"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="121"/>
       <c r="B6" s="83" t="s">
         <v>78</v>
       </c>
@@ -11474,10 +11553,10 @@
       <c r="E6" s="85">
         <v>1</v>
       </c>
-      <c r="F6" s="124"/>
-    </row>
-    <row r="7" spans="1:6" ht="38.25">
-      <c r="A7" s="123"/>
+      <c r="F6" s="122"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="121"/>
       <c r="B7" s="83" t="s">
         <v>78</v>
       </c>
@@ -11490,497 +11569,497 @@
       <c r="E7" s="85">
         <v>1</v>
       </c>
-      <c r="F7" s="124"/>
+      <c r="F7" s="122"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="123"/>
-      <c r="B8" s="125"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="123"/>
       <c r="C8" s="83" t="s">
         <v>355</v>
       </c>
-      <c r="D8" s="125" t="s">
+      <c r="D8" s="123" t="s">
         <v>444</v>
       </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="124"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="122"/>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="123"/>
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
-      <c r="F9" s="124"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="123"/>
+      <c r="C9" s="123"/>
+      <c r="D9" s="123"/>
+      <c r="E9" s="123"/>
+      <c r="F9" s="122"/>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="126"/>
-      <c r="B10" s="127"/>
-      <c r="C10" s="125" t="s">
+      <c r="A10" s="124"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="123" t="s">
         <v>445</v>
       </c>
-      <c r="D10" s="127" t="s">
+      <c r="D10" s="125" t="s">
         <v>446</v>
       </c>
-      <c r="E10" s="127">
+      <c r="E10" s="125">
         <v>2</v>
       </c>
-      <c r="F10" s="128"/>
+      <c r="F10" s="126"/>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="126"/>
-      <c r="B11" s="127"/>
-      <c r="C11" s="125" t="s">
+      <c r="A11" s="124"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="123" t="s">
         <v>445</v>
       </c>
-      <c r="D11" s="127" t="s">
+      <c r="D11" s="125" t="s">
         <v>447</v>
       </c>
-      <c r="E11" s="127">
+      <c r="E11" s="125">
         <v>2</v>
       </c>
-      <c r="F11" s="128"/>
+      <c r="F11" s="126"/>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="126"/>
-      <c r="B12" s="127"/>
-      <c r="C12" s="125" t="s">
+      <c r="A12" s="124"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="123" t="s">
         <v>445</v>
       </c>
-      <c r="D12" s="127" t="s">
+      <c r="D12" s="125" t="s">
         <v>448</v>
       </c>
-      <c r="E12" s="127">
+      <c r="E12" s="125">
         <v>2</v>
       </c>
-      <c r="F12" s="128"/>
+      <c r="F12" s="126"/>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="126"/>
-      <c r="B13" s="127"/>
-      <c r="C13" s="127" t="s">
+      <c r="A13" s="124"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D13" s="127" t="s">
+      <c r="D13" s="125" t="s">
         <v>449</v>
       </c>
-      <c r="E13" s="127">
+      <c r="E13" s="125">
         <v>1</v>
       </c>
-      <c r="F13" s="128"/>
+      <c r="F13" s="126"/>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="126"/>
-      <c r="B14" s="127"/>
-      <c r="C14" s="127" t="s">
+      <c r="A14" s="124"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D14" s="127" t="s">
+      <c r="D14" s="125" t="s">
         <v>450</v>
       </c>
-      <c r="E14" s="127">
+      <c r="E14" s="125">
         <v>1</v>
       </c>
-      <c r="F14" s="128"/>
+      <c r="F14" s="126"/>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="129"/>
-      <c r="B15" s="130"/>
-      <c r="C15" s="127" t="s">
+      <c r="A15" s="127"/>
+      <c r="B15" s="128"/>
+      <c r="C15" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D15" s="130" t="s">
+      <c r="D15" s="128" t="s">
         <v>451</v>
       </c>
-      <c r="E15" s="130"/>
-      <c r="F15" s="131"/>
+      <c r="E15" s="128"/>
+      <c r="F15" s="129"/>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="129"/>
-      <c r="B16" s="130"/>
-      <c r="C16" s="127" t="s">
+      <c r="A16" s="127"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D16" s="130" t="s">
+      <c r="D16" s="128" t="s">
         <v>452</v>
       </c>
-      <c r="E16" s="130">
+      <c r="E16" s="128">
         <v>2</v>
       </c>
-      <c r="F16" s="131"/>
+      <c r="F16" s="129"/>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="126"/>
-      <c r="B17" s="127"/>
-      <c r="C17" s="127" t="s">
+      <c r="A17" s="124"/>
+      <c r="B17" s="125"/>
+      <c r="C17" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D17" s="127" t="s">
+      <c r="D17" s="125" t="s">
         <v>453</v>
       </c>
-      <c r="E17" s="127">
+      <c r="E17" s="125">
         <v>1</v>
       </c>
-      <c r="F17" s="128"/>
+      <c r="F17" s="126"/>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="126"/>
-      <c r="B18" s="127"/>
-      <c r="C18" s="127" t="s">
+      <c r="A18" s="124"/>
+      <c r="B18" s="125"/>
+      <c r="C18" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D18" s="127" t="s">
+      <c r="D18" s="125" t="s">
         <v>454</v>
       </c>
-      <c r="E18" s="127">
+      <c r="E18" s="125">
         <v>1</v>
       </c>
-      <c r="F18" s="128"/>
+      <c r="F18" s="126"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="126"/>
-      <c r="B19" s="127"/>
-      <c r="C19" s="127" t="s">
+      <c r="A19" s="124"/>
+      <c r="B19" s="125"/>
+      <c r="C19" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D19" s="127" t="s">
+      <c r="D19" s="125" t="s">
         <v>455</v>
       </c>
-      <c r="E19" s="127">
+      <c r="E19" s="125">
         <v>1</v>
       </c>
-      <c r="F19" s="128"/>
+      <c r="F19" s="126"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="126"/>
-      <c r="B20" s="127"/>
-      <c r="C20" s="127" t="s">
+      <c r="A20" s="124"/>
+      <c r="B20" s="125"/>
+      <c r="C20" s="125" t="s">
         <v>393</v>
       </c>
-      <c r="D20" s="127" t="s">
+      <c r="D20" s="125" t="s">
         <v>456</v>
       </c>
-      <c r="E20" s="127">
+      <c r="E20" s="125">
         <v>1</v>
       </c>
-      <c r="F20" s="128"/>
+      <c r="F20" s="126"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="126"/>
-      <c r="B21" s="127"/>
-      <c r="C21" s="127" t="s">
+      <c r="A21" s="124"/>
+      <c r="B21" s="125"/>
+      <c r="C21" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D21" s="127" t="s">
+      <c r="D21" s="125" t="s">
         <v>457</v>
       </c>
-      <c r="E21" s="127">
+      <c r="E21" s="125">
         <v>1</v>
       </c>
-      <c r="F21" s="128"/>
+      <c r="F21" s="126"/>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="126"/>
-      <c r="B22" s="127"/>
-      <c r="C22" s="127" t="s">
+      <c r="A22" s="124"/>
+      <c r="B22" s="125"/>
+      <c r="C22" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D22" s="127" t="s">
+      <c r="D22" s="125" t="s">
         <v>458</v>
       </c>
-      <c r="E22" s="127">
+      <c r="E22" s="125">
         <v>1</v>
       </c>
-      <c r="F22" s="128"/>
+      <c r="F22" s="126"/>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="126"/>
-      <c r="B23" s="127"/>
-      <c r="C23" s="127" t="s">
+      <c r="A23" s="124"/>
+      <c r="B23" s="125"/>
+      <c r="C23" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D23" s="127" t="s">
+      <c r="D23" s="125" t="s">
         <v>459</v>
       </c>
-      <c r="E23" s="127">
+      <c r="E23" s="125">
         <v>1</v>
       </c>
-      <c r="F23" s="128"/>
+      <c r="F23" s="126"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="132"/>
-      <c r="B24" s="133"/>
-      <c r="C24" s="127" t="s">
+      <c r="A24" s="130"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D24" s="133" t="s">
+      <c r="D24" s="131" t="s">
         <v>460</v>
       </c>
-      <c r="E24" s="133">
+      <c r="E24" s="131">
         <v>1</v>
       </c>
-      <c r="F24" s="134"/>
+      <c r="F24" s="132"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="129"/>
-      <c r="B25" s="130"/>
-      <c r="C25" s="127" t="s">
+      <c r="A25" s="127"/>
+      <c r="B25" s="128"/>
+      <c r="C25" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D25" s="130" t="s">
+      <c r="D25" s="128" t="s">
         <v>461</v>
       </c>
-      <c r="E25" s="130">
+      <c r="E25" s="128">
         <v>1</v>
       </c>
-      <c r="F25" s="134"/>
+      <c r="F25" s="132"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="129"/>
-      <c r="B26" s="130"/>
-      <c r="C26" s="127" t="s">
+      <c r="A26" s="127"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D26" s="130" t="s">
+      <c r="D26" s="128" t="s">
         <v>462</v>
       </c>
-      <c r="E26" s="130">
+      <c r="E26" s="128">
         <v>1</v>
       </c>
-      <c r="F26" s="134"/>
+      <c r="F26" s="132"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="129"/>
-      <c r="B27" s="130"/>
-      <c r="C27" s="127" t="s">
+      <c r="A27" s="127"/>
+      <c r="B27" s="128"/>
+      <c r="C27" s="125" t="s">
         <v>284</v>
       </c>
-      <c r="D27" s="130" t="s">
+      <c r="D27" s="128" t="s">
         <v>463</v>
       </c>
-      <c r="E27" s="130">
+      <c r="E27" s="128">
         <v>2</v>
       </c>
-      <c r="F27" s="134"/>
+      <c r="F27" s="132"/>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="129"/>
-      <c r="B28" s="130"/>
-      <c r="C28" s="130" t="s">
+      <c r="A28" s="127"/>
+      <c r="B28" s="128"/>
+      <c r="C28" s="128" t="s">
         <v>464</v>
       </c>
-      <c r="D28" s="130" t="s">
+      <c r="D28" s="128" t="s">
         <v>465</v>
       </c>
-      <c r="E28" s="130">
+      <c r="E28" s="128">
         <v>3</v>
       </c>
-      <c r="F28" s="134"/>
+      <c r="F28" s="132"/>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="129"/>
-      <c r="B29" s="130"/>
-      <c r="C29" s="130" t="s">
+      <c r="A29" s="127"/>
+      <c r="B29" s="128"/>
+      <c r="C29" s="128" t="s">
         <v>464</v>
       </c>
-      <c r="D29" s="130" t="s">
+      <c r="D29" s="128" t="s">
         <v>466</v>
       </c>
-      <c r="E29" s="130">
+      <c r="E29" s="128">
         <v>1</v>
       </c>
-      <c r="F29" s="134"/>
+      <c r="F29" s="132"/>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="129"/>
-      <c r="B30" s="130"/>
-      <c r="C30" s="127" t="s">
+      <c r="A30" s="127"/>
+      <c r="B30" s="128"/>
+      <c r="C30" s="125" t="s">
         <v>397</v>
       </c>
-      <c r="D30" s="130" t="s">
+      <c r="D30" s="128" t="s">
         <v>467</v>
       </c>
-      <c r="E30" s="130">
+      <c r="E30" s="128">
         <v>1</v>
       </c>
-      <c r="F30" s="134"/>
+      <c r="F30" s="132"/>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="129"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="127" t="s">
+      <c r="A31" s="127"/>
+      <c r="B31" s="128"/>
+      <c r="C31" s="125" t="s">
         <v>397</v>
       </c>
-      <c r="D31" s="130" t="s">
+      <c r="D31" s="128" t="s">
         <v>468</v>
       </c>
-      <c r="E31" s="130">
+      <c r="E31" s="128">
         <v>1</v>
       </c>
-      <c r="F31" s="131"/>
+      <c r="F31" s="129"/>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="135"/>
-      <c r="B32" s="136"/>
-      <c r="C32" s="136" t="s">
+      <c r="A32" s="133"/>
+      <c r="B32" s="134"/>
+      <c r="C32" s="134" t="s">
         <v>469</v>
       </c>
-      <c r="D32" s="136" t="s">
+      <c r="D32" s="134" t="s">
         <v>470</v>
       </c>
-      <c r="E32" s="136"/>
-      <c r="F32" s="137"/>
+      <c r="E32" s="134"/>
+      <c r="F32" s="135"/>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="129"/>
-      <c r="B33" s="130"/>
-      <c r="C33" s="136" t="s">
+      <c r="A33" s="127"/>
+      <c r="B33" s="128"/>
+      <c r="C33" s="134" t="s">
         <v>469</v>
       </c>
-      <c r="D33" s="130" t="s">
+      <c r="D33" s="128" t="s">
         <v>471</v>
       </c>
-      <c r="E33" s="130"/>
-      <c r="F33" s="131"/>
+      <c r="E33" s="128"/>
+      <c r="F33" s="129"/>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="129"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="136" t="s">
+      <c r="A34" s="127"/>
+      <c r="B34" s="128"/>
+      <c r="C34" s="134" t="s">
         <v>469</v>
       </c>
-      <c r="D34" s="130" t="s">
+      <c r="D34" s="128" t="s">
         <v>472</v>
       </c>
-      <c r="E34" s="130"/>
-      <c r="F34" s="131"/>
+      <c r="E34" s="128"/>
+      <c r="F34" s="129"/>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="129"/>
-      <c r="B35" s="130"/>
-      <c r="C35" s="136" t="s">
+      <c r="A35" s="127"/>
+      <c r="B35" s="128"/>
+      <c r="C35" s="134" t="s">
         <v>469</v>
       </c>
-      <c r="D35" s="130" t="s">
+      <c r="D35" s="128" t="s">
         <v>473</v>
       </c>
-      <c r="E35" s="130"/>
-      <c r="F35" s="131"/>
+      <c r="E35" s="128"/>
+      <c r="F35" s="129"/>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="129"/>
-      <c r="B36" s="130"/>
-      <c r="C36" s="130" t="s">
+      <c r="A36" s="127"/>
+      <c r="B36" s="128"/>
+      <c r="C36" s="128" t="s">
         <v>384</v>
       </c>
-      <c r="D36" s="130" t="s">
+      <c r="D36" s="128" t="s">
         <v>474</v>
       </c>
-      <c r="E36" s="130"/>
-      <c r="F36" s="131"/>
+      <c r="E36" s="128"/>
+      <c r="F36" s="129"/>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="129"/>
-      <c r="B37" s="130"/>
-      <c r="C37" s="130" t="s">
+      <c r="A37" s="127"/>
+      <c r="B37" s="128"/>
+      <c r="C37" s="128" t="s">
         <v>384</v>
       </c>
-      <c r="D37" s="130" t="s">
+      <c r="D37" s="128" t="s">
         <v>475</v>
       </c>
-      <c r="E37" s="130"/>
-      <c r="F37" s="131"/>
+      <c r="E37" s="128"/>
+      <c r="F37" s="129"/>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="135"/>
-      <c r="B38" s="136"/>
-      <c r="C38" s="130" t="s">
+      <c r="A38" s="133"/>
+      <c r="B38" s="134"/>
+      <c r="C38" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="D38" s="136" t="s">
+      <c r="D38" s="134" t="s">
         <v>476</v>
       </c>
-      <c r="E38" s="136"/>
-      <c r="F38" s="137"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="135"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="129"/>
-      <c r="B39" s="130"/>
-      <c r="C39" s="130" t="s">
+      <c r="A39" s="127"/>
+      <c r="B39" s="128"/>
+      <c r="C39" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="130" t="s">
+      <c r="D39" s="128" t="s">
         <v>477</v>
       </c>
-      <c r="E39" s="130"/>
-      <c r="F39" s="137"/>
+      <c r="E39" s="128"/>
+      <c r="F39" s="135"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="129"/>
-      <c r="B40" s="130"/>
-      <c r="C40" s="130" t="s">
+      <c r="A40" s="127"/>
+      <c r="B40" s="128"/>
+      <c r="C40" s="128" t="s">
         <v>121</v>
       </c>
-      <c r="D40" s="130" t="s">
+      <c r="D40" s="128" t="s">
         <v>478</v>
       </c>
-      <c r="E40" s="130"/>
-      <c r="F40" s="137"/>
+      <c r="E40" s="128"/>
+      <c r="F40" s="135"/>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="129"/>
-      <c r="B41" s="130"/>
-      <c r="C41" s="130"/>
-      <c r="D41" s="130"/>
-      <c r="E41" s="130"/>
-      <c r="F41" s="137"/>
+      <c r="A41" s="127"/>
+      <c r="B41" s="128"/>
+      <c r="C41" s="128"/>
+      <c r="D41" s="128"/>
+      <c r="E41" s="128"/>
+      <c r="F41" s="135"/>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="129"/>
-      <c r="B42" s="130"/>
-      <c r="C42" s="130"/>
-      <c r="D42" s="130"/>
-      <c r="E42" s="130"/>
-      <c r="F42" s="137"/>
+      <c r="A42" s="127"/>
+      <c r="B42" s="128"/>
+      <c r="C42" s="128"/>
+      <c r="D42" s="128"/>
+      <c r="E42" s="128"/>
+      <c r="F42" s="135"/>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="129"/>
-      <c r="B43" s="130"/>
-      <c r="C43" s="130"/>
-      <c r="D43" s="130"/>
-      <c r="E43" s="130"/>
-      <c r="F43" s="137"/>
+      <c r="A43" s="127"/>
+      <c r="B43" s="128"/>
+      <c r="C43" s="128"/>
+      <c r="D43" s="128"/>
+      <c r="E43" s="128"/>
+      <c r="F43" s="135"/>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="129"/>
-      <c r="B44" s="130"/>
-      <c r="C44" s="130"/>
-      <c r="D44" s="130"/>
-      <c r="E44" s="130"/>
-      <c r="F44" s="137"/>
+      <c r="A44" s="127"/>
+      <c r="B44" s="128"/>
+      <c r="C44" s="128"/>
+      <c r="D44" s="128"/>
+      <c r="E44" s="128"/>
+      <c r="F44" s="135"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="129"/>
-      <c r="B45" s="130"/>
-      <c r="C45" s="130"/>
-      <c r="D45" s="130"/>
-      <c r="E45" s="130"/>
-      <c r="F45" s="137"/>
+      <c r="A45" s="127"/>
+      <c r="B45" s="128"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="135"/>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="129"/>
-      <c r="B46" s="130"/>
-      <c r="C46" s="130"/>
-      <c r="D46" s="130"/>
-      <c r="E46" s="130"/>
-      <c r="F46" s="137"/>
+      <c r="A46" s="127"/>
+      <c r="B46" s="128"/>
+      <c r="C46" s="128"/>
+      <c r="D46" s="128"/>
+      <c r="E46" s="128"/>
+      <c r="F46" s="135"/>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="129"/>
-      <c r="B47" s="130"/>
-      <c r="C47" s="130"/>
-      <c r="D47" s="130"/>
-      <c r="E47" s="130"/>
-      <c r="F47" s="137"/>
+      <c r="A47" s="127"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="128"/>
+      <c r="E47" s="128"/>
+      <c r="F47" s="135"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
@@ -12076,6 +12155,144 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="2" spans="2:3">
+      <c r="B2" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3">
+      <c r="B4" t="s">
+        <v>497</v>
+      </c>
+      <c r="C4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3">
+      <c r="C5" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="C6" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="C7" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>502</v>
+      </c>
+      <c r="C9" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="C10" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3">
+      <c r="B12" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3">
+      <c r="B13" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3">
+      <c r="B15" t="s">
+        <v>507</v>
+      </c>
+      <c r="C15" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3">
+      <c r="C16" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3">
+      <c r="B18" t="s">
+        <v>434</v>
+      </c>
+      <c r="C18" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="C19" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3">
+      <c r="C20" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3">
+      <c r="B22" t="s">
+        <v>513</v>
+      </c>
+      <c r="C22" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3">
+      <c r="C23" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3">
+      <c r="C24" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3">
+      <c r="B26" t="s">
+        <v>517</v>
+      </c>
+      <c r="C26" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3">
+      <c r="C27" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3">
+      <c r="C28" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3">
+      <c r="C29" t="s">
+        <v>521</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:L60"/>
   <sheetViews>
@@ -12432,7 +12649,7 @@
         <f>SUM(F42:J42)</f>
         <v>82</v>
       </c>
-      <c r="L42" s="116">
+      <c r="L42" s="136">
         <v>191</v>
       </c>
     </row>
@@ -12457,7 +12674,7 @@
         <f t="shared" ref="K43:K45" si="1">SUM(F43:J43)</f>
         <v>117</v>
       </c>
-      <c r="L43" s="117"/>
+      <c r="L43" s="137"/>
     </row>
     <row r="44" spans="5:12" ht="15">
       <c r="E44" s="36" t="s">

</xml_diff>